<commit_message>
Update latest digest: 2024-06-01 → 2025-09-24
</commit_message>
<xml_diff>
--- a/outputs/latest/POGO_Digest.xlsx
+++ b/outputs/latest/POGO_Digest.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q319"/>
+  <dimension ref="A1:Q320"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1258,7 +1258,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Cancún, Mexico - Pokémon GO City Safari</t>
+          <t>Valencia, Spain - Pokémon GO City Safari</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1277,12 +1277,12 @@
       <c r="O16" t="inlineStr"/>
       <c r="P16" t="inlineStr">
         <is>
-          <t>Cancún, Mexico - Pokémon GO City Safari City Safari Starts: Saturday, September 27, 2025, at 10:00 AM Local Time Ends: Sunday, September 28, 2025, at  6:00 PM Local Time Pokémon GO City Safari is coming to Cancún, Mexico, on September 27 and 28, 2025! Set off on a citywide adventure as you discover the vibrant stories, new friends, and exciting Pokémon waiting for you in Cancún! Whether you’re a resident of Cancún or a first-time visitor, your Pokémon GO City Safari will take you across the city in an all-new way—from historic landmarks to local favorites, get ready for a taste of the city with Pokémon GO by your side! One-day Tickets are MX$190 (including any applicable taxes and fees) on either September 27, 2025 or September 28, 2025, from 10 am to 6 pm EST. Bonuses Features Spawns Eggs Research Sales Bonuses Ticket Holder Bonuses Ticket-holding Trainers will receive the following bonuses and rewards between 10:00 a.m. and 6:00 p.m., anywhere in Cancún on their ticketed day! An increased chance of encountering Shiny Pokémon Lure Modules (excluding Golden Lures) activated during the event will last for four hours Up to five Special Trades can be made during the day on your ticket</t>
+          <t xml:space="preserve">Valencia, Spain - Pokémon GO City Safari City Safari Starts: Saturday, September 27, 2025, at 10:00 AM Local Time Ends: Sunday, September 28, 2025, at  6:00 PM Local Time Pokémon GO City Safari is coming to Valencia, Spain, on September 27 and 28, 2025! Set off on a citywide adventure as you discover the vibrant stories, new friends, and exciting Pokémon waiting for you in Valencia! Whether you’re a resident of Valencia or a first-time visitor, your Pokémon GO City Safari will take you across the city in an all-new way—from historic landmarks to local favorites, get ready for a taste of the city with Pokémon GO by your side! One-day Tickets are €10 (including any applicable taxes and fees) on either September 27, 2025 or September 28, 2025, from 10 am to 6 pm CEST. Bonuses Features Spawns Eggs Research Sales Bonuses Ticket Holder Bonuses Ticket-holding Trainers will receive the following bonuses and rewards between 10:00 a.m. and 6:00 p.m., anywhere in Valencia on their ticketed day! An increased chance of encountering Shiny Pokémon Lure Modules (excluding Golden Lures) activated during the event will last for four hours Up to five Special Trades can be made during the day on your </t>
         </is>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>2024-06-01_city-safari-cancn-mexico---pokmon-go-city-safari-sun-sep-28-at-600-pm-local-time-ends-calculating.html</t>
+          <t>2024-06-01_city-safari-valencia-spain---pokmon-go-city-safari-sun-sep-28-at-600-pm-local-time-ends-calculating.html</t>
         </is>
       </c>
     </row>
@@ -1309,7 +1309,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Vancouver, Canada - Pokémon GO City Safari</t>
+          <t>Cancún, Mexico - Pokémon GO City Safari</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1328,12 +1328,12 @@
       <c r="O17" t="inlineStr"/>
       <c r="P17" t="inlineStr">
         <is>
-          <t xml:space="preserve">Vancouver, Canada - Pokémon GO City Safari City Safari Starts: Saturday, September 27, 2025, at 10:00 AM Local Time Ends: Sunday, September 28, 2025, at  6:00 PM Local Time Pokémon GO City Safari is coming to Vancouver, Canada, on September 27 and 28, 2025! Set off on a citywide adventure as you discover the vibrant stories, new friends, and exciting Pokémon waiting for you in Vancouver! Whether you’re a resident of Vancouver or a first-time visitor, your Pokémon GO City Safari will take you across the city in an all-new way—from historic landmarks to local favorites, get ready for a taste of the city with Pokémon GO by your side! One-day Tickets are CA$14 (including any applicable taxes and fees) on either September 27, 2025 or September 28, 2025, from 10 am to 6 pm PDT. Bonuses Features Spawns Eggs Research Sales Bonuses Ticket Holder Bonuses Ticket-holding Trainers will receive the following bonuses and rewards between 10:00 a.m. and 6:00 p.m., anywhere in Vancouver on their ticketed day! An increased chance of encountering Shiny Pokémon Lure Modules (excluding Golden Lures) activated during the event will last for four hours Up to five Special Trades can be made during the day </t>
+          <t>Cancún, Mexico - Pokémon GO City Safari City Safari Starts: Saturday, September 27, 2025, at 10:00 AM Local Time Ends: Sunday, September 28, 2025, at  6:00 PM Local Time Pokémon GO City Safari is coming to Cancún, Mexico, on September 27 and 28, 2025! Set off on a citywide adventure as you discover the vibrant stories, new friends, and exciting Pokémon waiting for you in Cancún! Whether you’re a resident of Cancún or a first-time visitor, your Pokémon GO City Safari will take you across the city in an all-new way—from historic landmarks to local favorites, get ready for a taste of the city with Pokémon GO by your side! One-day Tickets are MX$190 (including any applicable taxes and fees) on either September 27, 2025 or September 28, 2025, from 10 am to 6 pm EST. Bonuses Features Spawns Eggs Research Sales Bonuses Ticket Holder Bonuses Ticket-holding Trainers will receive the following bonuses and rewards between 10:00 a.m. and 6:00 p.m., anywhere in Cancún on their ticketed day! An increased chance of encountering Shiny Pokémon Lure Modules (excluding Golden Lures) activated during the event will last for four hours Up to five Special Trades can be made during the day on your ticket</t>
         </is>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>2024-06-01_city-safari-vancouver-canada---pokmon-go-city-safari-sun-sep-28-at-600-pm-local-time-ends-calculating.html</t>
+          <t>2024-06-01_city-safari-cancn-mexico---pokmon-go-city-safari-sun-sep-28-at-600-pm-local-time-ends-calculating.html</t>
         </is>
       </c>
     </row>
@@ -1350,22 +1350,22 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Mega Camerupt Raid Day</t>
+          <t>Vancouver, Canada - Pokémon GO City Safari</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G18" t="inlineStr"/>
@@ -1379,12 +1379,12 @@
       <c r="O18" t="inlineStr"/>
       <c r="P18" t="inlineStr">
         <is>
-          <t>Mega Camerupt Raid Day Raid Day Starts: Sunday, September 28, 2025, at  2:00 PM Local Time Ends: Sunday, September 28, 2025, at  5:00 PM Local Time Mega Camerupt charges in for its Pokémon GO debut! Bonuses Features Raids Shiny Sales Bonuses Remote Raid Pass limit increased to 20 from Saturday, September 27, at 5:00 p.m. to Sunday, September 28, 2025, at 8:00 p.m. PDT Receive up to five additional free Raid Passes from spinning Gym Photo Discs (for a total of six) Increased chance of encountering Shiny Camerupt from Mega Raids Event Ticket For US$4.99 (or the equivalent pricing tier in your local currency), you can purchase a ticket that grants the following bonuses. Receive up to eight additional free Raid Passes from spinning Gym Photo Discs (for a total of 14) Increased chance to get Rare Candy XL from Raid Battles 50% more XP from Raid Battles 2× Stardust from Raid Battles These bonuses will be effective on Sunday, September 28, 2025, from 2:00 p.m. to 5:00 p.m. local time. Trainers will be able to purchase and gift tickets to any of their Pokémon GO friends that they have achieved a Friendship level of Great Friends or higher with. Please note that purchases—including those ma</t>
+          <t xml:space="preserve">Vancouver, Canada - Pokémon GO City Safari City Safari Starts: Saturday, September 27, 2025, at 10:00 AM Local Time Ends: Sunday, September 28, 2025, at  6:00 PM Local Time Pokémon GO City Safari is coming to Vancouver, Canada, on September 27 and 28, 2025! Set off on a citywide adventure as you discover the vibrant stories, new friends, and exciting Pokémon waiting for you in Vancouver! Whether you’re a resident of Vancouver or a first-time visitor, your Pokémon GO City Safari will take you across the city in an all-new way—from historic landmarks to local favorites, get ready for a taste of the city with Pokémon GO by your side! One-day Tickets are CA$14 (including any applicable taxes and fees) on either September 27, 2025 or September 28, 2025, from 10 am to 6 pm PDT. Bonuses Features Spawns Eggs Research Sales Bonuses Ticket Holder Bonuses Ticket-holding Trainers will receive the following bonuses and rewards between 10:00 a.m. and 6:00 p.m., anywhere in Vancouver on their ticketed day! An increased chance of encountering Shiny Pokémon Lure Modules (excluding Golden Lures) activated during the event will last for four hours Up to five Special Trades can be made during the day </t>
         </is>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>2024-06-01_raid-day-mega-camerupt-raid-day-sun-sep-28-at-500-pm-local-time-ends-calculating.html</t>
+          <t>2024-06-01_city-safari-vancouver-canada---pokmon-go-city-safari-sun-sep-28-at-600-pm-local-time-ends-calculating.html</t>
         </is>
       </c>
     </row>
@@ -1401,22 +1401,22 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Dynamax Beldum during Max Monday</t>
+          <t>Mega Camerupt Raid Day</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G19" t="inlineStr"/>
@@ -1430,12 +1430,12 @@
       <c r="O19" t="inlineStr"/>
       <c r="P19" t="inlineStr">
         <is>
-          <t>Dynamax Beldum during Max Monday Max Mondays Starts: Monday, September 29, 2025, at  6:00 PM Local Time Ends: Monday, September 29, 2025, at  7:00 PM Local Time These Dynamax Pokémon may appear in Max Battles throughout Delightful Days. They will also take over Power Spots for an hour each week on Mondays from 6:00 p.m. to 7:00 p.m. local time! On September 29, 2025 , the featured Dynamax Pokémon is Beldum . Beldum Leek Duck Hey, I'm LeekDuck. I create Pokémon GO graphics, resources and report Pokémon GO news. You can find them on X, Facebook, Instagram, Threads, and Bluesky. You can also find me on Twitch and YouTube!</t>
+          <t>Mega Camerupt Raid Day Raid Day Starts: Sunday, September 28, 2025, at  2:00 PM Local Time Ends: Sunday, September 28, 2025, at  5:00 PM Local Time Mega Camerupt charges in for its Pokémon GO debut! Bonuses Features Raids Shiny Sales Bonuses Remote Raid Pass limit increased to 20 from Saturday, September 27, at 5:00 p.m. to Sunday, September 28, 2025, at 8:00 p.m. PDT Receive up to five additional free Raid Passes from spinning Gym Photo Discs (for a total of six) Increased chance of encountering Shiny Camerupt from Mega Raids Event Ticket For US$4.99 (or the equivalent pricing tier in your local currency), you can purchase a ticket that grants the following bonuses. Receive up to eight additional free Raid Passes from spinning Gym Photo Discs (for a total of 14) Increased chance to get Rare Candy XL from Raid Battles 50% more XP from Raid Battles 2× Stardust from Raid Battles These bonuses will be effective on Sunday, September 28, 2025, from 2:00 p.m. to 5:00 p.m. local time. Trainers will be able to purchase and gift tickets to any of their Pokémon GO friends that they have achieved a Friendship level of Great Friends or higher with. Please note that purchases—including those ma</t>
         </is>
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>2024-06-01_max-mondays-dynamax-beldum-during-max-monday-mon-sep-29-at-700-pm-local-time-ends-calculating.html</t>
+          <t>2024-06-01_raid-day-mega-camerupt-raid-day-sun-sep-28-at-500-pm-local-time-ends-calculating.html</t>
         </is>
       </c>
     </row>
@@ -1452,17 +1452,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Aron Spotlight Hour</t>
+          <t>Dynamax Beldum during Max Monday</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1481,12 +1481,12 @@
       <c r="O20" t="inlineStr"/>
       <c r="P20" t="inlineStr">
         <is>
-          <t>Aron Spotlight Hour Pokémon Spotlight Hour Starts: Tuesday, September 30, 2025, at  6:00 PM Local Time Ends: Tuesday, September 30, 2025, at  7:00 PM Local Time Pokémon Spotlight Hour will feature a different Pokémon and special bonus for one hour at 6:00 p.m. local time on Tuesday during the month of September. September 30 : The featured Pokémon is Aron and the special bonus is 2× Transfer Candy . Spawns The following Pokémon will appear more frequently in the wild. Aron Graphic Leek Duck Hey, I'm LeekDuck. I create Pokémon GO graphics, resources and report Pokémon GO news. You can find them on X, Facebook, Instagram, Threads, and Bluesky. You can also find me on Twitch and YouTube!</t>
+          <t>Dynamax Beldum during Max Monday Max Mondays Starts: Monday, September 29, 2025, at  6:00 PM Local Time Ends: Monday, September 29, 2025, at  7:00 PM Local Time These Dynamax Pokémon may appear in Max Battles throughout Delightful Days. They will also take over Power Spots for an hour each week on Mondays from 6:00 p.m. to 7:00 p.m. local time! On September 29, 2025 , the featured Dynamax Pokémon is Beldum . Beldum Leek Duck Hey, I'm LeekDuck. I create Pokémon GO graphics, resources and report Pokémon GO news. You can find them on X, Facebook, Instagram, Threads, and Bluesky. You can also find me on Twitch and YouTube!</t>
         </is>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>2024-06-01_pokmon-spotlight-hour-aron-spotlight-hour-tue-sep-30-at-700-pm-local-time-ends-calculating.html</t>
+          <t>2024-06-01_max-mondays-dynamax-beldum-during-max-monday-mon-sep-29-at-700-pm-local-time-ends-calculating.html</t>
         </is>
       </c>
     </row>
@@ -1513,12 +1513,12 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Mega Steelix, Scizor, and Lucario in Mega Raids</t>
+          <t>Aron Spotlight Hour</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G21" t="inlineStr"/>
@@ -1532,12 +1532,12 @@
       <c r="O21" t="inlineStr"/>
       <c r="P21" t="inlineStr">
         <is>
-          <t>Mega Steelix, Scizor, and Lucario in Mega Raids Raid Battles Starts: Tuesday, September 30, 2025, at 10:00 AM Local Time Ends: Tuesday, October 7, 2025, at 10:00 AM Local Time Mega Steelix, Mega Scizor, and Mega Lucario return to Mega Raids on September 30, 2025, at 10 am local time. Raids Shiny Raids Mega Steelix, Mega Scizor, and Mega Lucario will be in Mega Raids. Mega Steelix Mega Scizor Mega Lucario Shiny If you’re lucky, you may encounter Shiny Steelix, Scizor, or Lucario. Shiny forms for these Pokémon have previously been available. Steelix Mega Steelix Scizor Mega Scizor Lucario Mega Lucario Leek Duck Hey, I'm LeekDuck. I create Pokémon GO graphics, resources and report Pokémon GO news. You can find them on X, Facebook, Instagram, Threads, and Bluesky. You can also find me on Twitch and YouTube!</t>
+          <t>Aron Spotlight Hour Pokémon Spotlight Hour Starts: Tuesday, September 30, 2025, at  6:00 PM Local Time Ends: Tuesday, September 30, 2025, at  7:00 PM Local Time Pokémon Spotlight Hour will feature a different Pokémon and special bonus for one hour at 6:00 p.m. local time on Tuesday during the month of September. September 30 : The featured Pokémon is Aron and the special bonus is 2× Transfer Candy . Spawns The following Pokémon will appear more frequently in the wild. Aron Graphic Leek Duck Hey, I'm LeekDuck. I create Pokémon GO graphics, resources and report Pokémon GO news. You can find them on X, Facebook, Instagram, Threads, and Bluesky. You can also find me on Twitch and YouTube!</t>
         </is>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>2024-06-01_raid-battles-mega-steelix-scizor-and-lucario-in-mega-raids-tue-oct-7-at-1000-am-local-time-ends-calculating.html</t>
+          <t>2024-06-01_pokmon-spotlight-hour-aron-spotlight-hour-tue-sep-30-at-700-pm-local-time-ends-calculating.html</t>
         </is>
       </c>
     </row>
@@ -1564,12 +1564,12 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation</t>
+          <t>Mega Steelix, Scizor, and Lucario in Mega Raids</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G22" t="inlineStr"/>
@@ -1583,12 +1583,12 @@
       <c r="O22" t="inlineStr"/>
       <c r="P22" t="inlineStr">
         <is>
-          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation GO Battle League Starts: Calculating... Ends: Calculating... The Great League and Fantasy Cup: Great League Edition will run from September 30, 2025, at 1:00 p.m. to October 7, 2025, at 1:00 p.m. PT. Great League Pokémon must be at or below 1,500 CP to enter. Fantasy Cup: Great League Edition Pokémon must be at or below 1,500 CP to enter. Only Dragon-, Steel-, and Fairy-type Pokémon are eligible. Leek Duck Hey, I'm LeekDuck. I create Pokémon GO graphics, resources and report Pokémon GO news. You can find them on X, Facebook, Instagram, Threads, and Bluesky. You can also find me on Twitch and YouTube!</t>
+          <t>Mega Steelix, Scizor, and Lucario in Mega Raids Raid Battles Starts: Tuesday, September 30, 2025, at 10:00 AM Local Time Ends: Tuesday, October 7, 2025, at 10:00 AM Local Time Mega Steelix, Mega Scizor, and Mega Lucario return to Mega Raids on September 30, 2025, at 10 am local time. Raids Shiny Raids Mega Steelix, Mega Scizor, and Mega Lucario will be in Mega Raids. Mega Steelix Mega Scizor Mega Lucario Shiny If you’re lucky, you may encounter Shiny Steelix, Scizor, or Lucario. Shiny forms for these Pokémon have previously been available. Steelix Mega Steelix Scizor Mega Scizor Lucario Mega Lucario Leek Duck Hey, I'm LeekDuck. I create Pokémon GO graphics, resources and report Pokémon GO news. You can find them on X, Facebook, Instagram, Threads, and Bluesky. You can also find me on Twitch and YouTube!</t>
         </is>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>2024-06-01_go-battle-league-great-league-and-fantasy-cup-great-league-edition--tales-of-transformation-calculating-ends-calculating.html</t>
+          <t>2024-06-01_raid-battles-mega-steelix-scizor-and-lucario-in-mega-raids-tue-oct-7-at-1000-am-local-time-ends-calculating.html</t>
         </is>
       </c>
     </row>
@@ -1615,7 +1615,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Great League</t>
+          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1634,7 +1634,7 @@
       <c r="O23" t="inlineStr"/>
       <c r="P23" t="inlineStr">
         <is>
-          <t>The Great League and Fantasy Cup: Great League Edition will run from September 30, 2025, at 1:00 p.m. to October 7, 2025, at 1:00 p.m. PT. Great League Pokémon must be at or below 1,500 CP to enter. Fantasy Cup: Great League Edition Pokémon must be at or below 1,500 CP to enter. Only Dragon-, Steel-, and Fairy-type Pokémon are eligible.</t>
+          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation GO Battle League Starts: Calculating... Ends: Calculating... The Great League and Fantasy Cup: Great League Edition will run from September 30, 2025, at 1:00 p.m. to October 7, 2025, at 1:00 p.m. PT. Great League Pokémon must be at or below 1,500 CP to enter. Fantasy Cup: Great League Edition Pokémon must be at or below 1,500 CP to enter. Only Dragon-, Steel-, and Fairy-type Pokémon are eligible. Leek Duck Hey, I'm LeekDuck. I create Pokémon GO graphics, resources and report Pokémon GO news. You can find them on X, Facebook, Instagram, Threads, and Bluesky. You can also find me on Twitch and YouTube!</t>
         </is>
       </c>
       <c r="Q23" t="inlineStr">
@@ -1666,7 +1666,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Steel Skyline</t>
+          <t>Great League</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1685,12 +1685,12 @@
       <c r="O24" t="inlineStr"/>
       <c r="P24" t="inlineStr">
         <is>
-          <t>Steel Skyline Event Starts: Tuesday, September 30, 2025, at 10:00 AM Local Time Ends: Tuesday, October 7, 2025, at  8:00 PM Local Time Dynamax Duraludon makes its Pokémon GO debut during Steel Skyline! Complete Global Challenges, encounter Steel-type Pokémon, and participate in Max Battles. Features Spawns Raids Research Shiny Sales Features Dynamax Debut The following Pokémon will make its Pokémon GO debut in four-star Max Battles! Duraludon Global Challenges Global Challenges will take place throughout the Steel Skyline event! Work with Trainers around the world to complete Field Research tasks and complete throwing-based challenges to unlock bonuses for all to enjoy! Once a challenge is completed, special bonuses will be unlocked for the remainder of the event and the next Global Challenge will begin. How far can you get? Level 1 Reward Additional Candy for successfully catching Pokémon with Nice, Great, and Excellent Throws Increased chance for Trainers level 31 and up to receive Candy XL for catching Pokémon with Nice, Great, and Excellent Throws Level 2 Rewards Additional 5,000 XP from winning raids Level 3 Rewards One guaranteed Rare Candy XL from winning in-person Max Battl</t>
+          <t>The Great League and Fantasy Cup: Great League Edition will run from September 30, 2025, at 1:00 p.m. to October 7, 2025, at 1:00 p.m. PT. Great League Pokémon must be at or below 1,500 CP to enter. Fantasy Cup: Great League Edition Pokémon must be at or below 1,500 CP to enter. Only Dragon-, Steel-, and Fairy-type Pokémon are eligible.</t>
         </is>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>2024-06-01_event-steel-skyline-tue-oct-7-at-800-pm-local-time-ends-calculating.html</t>
+          <t>2024-06-01_go-battle-league-great-league-and-fantasy-cup-great-league-edition--tales-of-transformation-calculating-ends-calculating.html</t>
         </is>
       </c>
     </row>
@@ -1702,27 +1702,27 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2025-10</t>
+          <t>2025-09</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2025-10-01</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>2025-10-01</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Dialga (Origin Forme) Raid Hour</t>
+          <t>Steel Skyline</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G25" t="inlineStr"/>
@@ -1736,12 +1736,12 @@
       <c r="O25" t="inlineStr"/>
       <c r="P25" t="inlineStr">
         <is>
-          <t>Dialga (Origin Forme) Raid Hour Raid Hour Starts: Wednesday, October 1, 2025, at  6:00 PM Local Time Ends: Wednesday, October 1, 2025, at  7:00 PM Local Time A Raid Hour featuring Dialga (Origin Forme) is scheduled from 6 to 7 pm Local Time. During this hour there will be an increased number of 5-star Raids. Origin Forme Dialga caught during Raid Hour may know the Charged Attack Roar of Time. Leek Duck Hey, I'm LeekDuck. I create Pokémon GO graphics, resources and report Pokémon GO news. You can find them on X, Facebook, Instagram, Threads, and Bluesky. You can also find me on Twitch and YouTube!</t>
+          <t>Steel Skyline Event Starts: Tuesday, September 30, 2025, at 10:00 AM Local Time Ends: Tuesday, October 7, 2025, at  8:00 PM Local Time Dynamax Duraludon makes its Pokémon GO debut during Steel Skyline! Complete Global Challenges, encounter Steel-type Pokémon, and participate in Max Battles. Features Spawns Raids Research Shiny Sales Features Dynamax Debut The following Pokémon will make its Pokémon GO debut in four-star Max Battles! Duraludon Global Challenges Global Challenges will take place throughout the Steel Skyline event! Work with Trainers around the world to complete Field Research tasks and complete throwing-based challenges to unlock bonuses for all to enjoy! Once a challenge is completed, special bonuses will be unlocked for the remainder of the event and the next Global Challenge will begin. How far can you get? Level 1 Reward Additional Candy for successfully catching Pokémon with Nice, Great, and Excellent Throws Increased chance for Trainers level 31 and up to receive Candy XL for catching Pokémon with Nice, Great, and Excellent Throws Level 2 Rewards Additional 5,000 XP from winning raids Level 3 Rewards One guaranteed Rare Candy XL from winning in-person Max Battl</t>
         </is>
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>2024-06-01_raid-hour-dialga-origin-forme-raid-hour-wed-oct-1-at-700-pm-local-time-ends-calculating.html</t>
+          <t>2024-06-01_event-steel-skyline-tue-oct-7-at-800-pm-local-time-ends-calculating.html</t>
         </is>
       </c>
     </row>
@@ -1758,17 +1758,17 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>2025-10-04</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>2025-10-04</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Mega Metagross Raid Day</t>
+          <t>Dialga (Origin Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1787,12 +1787,12 @@
       <c r="O26" t="inlineStr"/>
       <c r="P26" t="inlineStr">
         <is>
-          <t>Mega Metagross Raid Day Raid Day Starts: Saturday, October 4, 2025, at  2:00 PM Local Time Ends: Saturday, October 4, 2025, at  5:00 PM Local Time Link up for a battle of the minds on Mega Metagross Raid Day! Bonuses Features Raids Shiny Sales Bonuses Remote Raid Pass limit increased to 20 from Friday, October 3, at 5:00 p.m. to Saturday, October 4, 2025, at 8:00 p.m. PDT Receive up to five additional free Raid Passes from spinning Gym Photo Discs (for a total of six) Increased chance of encountering Shiny Metagross from Mega Raids Event Ticket For US$4.99 (or the equivalent pricing tier in your local currency), you can purchase a ticket that grants the following bonuses. Receive up to eight additional free Raid Passes from spinning Gym Photo Discs (for a total of 14) Increased chance to get Rare Candy XL from Raid Battles 5,000 XP from Raid Battles 2× Stardust from Raid Battles These bonuses will be effective on Saturday, October 4, 2025, from 2:00 p.m. to 5:00 p.m. local time. *If the Global Challenge during Steel Skyline is complete, Trainers who also have a Mega Metagross Raid Day ticket will earn an additional 5,000 XP from Raid Battles. Trainers will be able to purchase and g</t>
+          <t>Dialga (Origin Forme) Raid Hour Raid Hour Starts: Wednesday, October 1, 2025, at  6:00 PM Local Time Ends: Wednesday, October 1, 2025, at  7:00 PM Local Time A Raid Hour featuring Dialga (Origin Forme) is scheduled from 6 to 7 pm Local Time. During this hour there will be an increased number of 5-star Raids. Origin Forme Dialga caught during Raid Hour may know the Charged Attack Roar of Time. Leek Duck Hey, I'm LeekDuck. I create Pokémon GO graphics, resources and report Pokémon GO news. You can find them on X, Facebook, Instagram, Threads, and Bluesky. You can also find me on Twitch and YouTube!</t>
         </is>
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>2024-06-01_raid-day-mega-metagross-raid-day-sat-oct-4-at-500-pm-local-time-ends-calculating.html</t>
+          <t>2024-06-01_raid-hour-dialga-origin-forme-raid-hour-wed-oct-1-at-700-pm-local-time-ends-calculating.html</t>
         </is>
       </c>
     </row>
@@ -1809,22 +1809,22 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>2025-10-10</t>
+          <t>2025-10-04</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>2025-10-10</t>
+          <t>2025-10-04</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Harvest Festival</t>
+          <t>Mega Metagross Raid Day</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G27" t="inlineStr"/>
@@ -1838,12 +1838,12 @@
       <c r="O27" t="inlineStr"/>
       <c r="P27" t="inlineStr">
         <is>
-          <t>Harvest Festival Event Starts: Friday, October 10, 2025, at 10:00 AM Local Time Ends: Thursday, October 16, 2025, at  8:00 PM Local Time The Harvest Festival returns to Pokémon GO, featuring the debut of Dipplin and Hydrapple! Discover Syrupy Apples and enjoy special bonuses throughout the event! Bonuses Features Spawns Research Shiny Sales Bonuses 2× Candy for catching Pokémon with Pinap Berries and Silver Pinap Berries Increased chance to encounter Shiny Pumpkaboo and Shiny Smoliv Increased chance for apples to appear at PokéStops with an active Mossy Lure Module Features Pokémon Debuts The following Pokémon will make their Pokémon GO debuts! Dipplin Hydrapple You can use 200 Applin Candy and 20 Syrupy Apples to evolve Applin into Dipplin. You can evolve Dipplin into Hydrapple using 400 Applin Candy and by catching seven Dragon-type Pokémon with Dipplin as your buddy. Apples Beginning during the Harvest Festival event, you might discover Syrupy Apples ! Apples have an increased chance of appearing at PokéStops with active Mossy Lure Modules , and tapping on them will award Sweet Apples, Tart Apples, Syrupy Apples, or encounters with Pokémon—including Applin, if you’re lucky! Spaw</t>
+          <t>Mega Metagross Raid Day Raid Day Starts: Saturday, October 4, 2025, at  2:00 PM Local Time Ends: Saturday, October 4, 2025, at  5:00 PM Local Time Link up for a battle of the minds on Mega Metagross Raid Day! Bonuses Features Raids Shiny Sales Bonuses Remote Raid Pass limit increased to 20 from Friday, October 3, at 5:00 p.m. to Saturday, October 4, 2025, at 8:00 p.m. PDT Receive up to five additional free Raid Passes from spinning Gym Photo Discs (for a total of six) Increased chance of encountering Shiny Metagross from Mega Raids Event Ticket For US$4.99 (or the equivalent pricing tier in your local currency), you can purchase a ticket that grants the following bonuses. Receive up to eight additional free Raid Passes from spinning Gym Photo Discs (for a total of 14) Increased chance to get Rare Candy XL from Raid Battles 5,000 XP from Raid Battles 2× Stardust from Raid Battles These bonuses will be effective on Saturday, October 4, 2025, from 2:00 p.m. to 5:00 p.m. local time. *If the Global Challenge during Steel Skyline is complete, Trainers who also have a Mega Metagross Raid Day ticket will earn an additional 5,000 XP from Raid Battles. Trainers will be able to purchase and g</t>
         </is>
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>2024-06-01_event-harvest-festival-thu-oct-16-at-800-pm-local-time-ends-calculating.html</t>
+          <t>2024-06-01_raid-day-mega-metagross-raid-day-sat-oct-4-at-500-pm-local-time-ends-calculating.html</t>
         </is>
       </c>
     </row>
@@ -1860,17 +1860,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>2025-10-12</t>
+          <t>2025-10-10</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>2025-10-12</t>
+          <t>2025-10-10</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Solosis Community Day</t>
+          <t>Harvest Festival</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -1889,12 +1889,12 @@
       <c r="O28" t="inlineStr"/>
       <c r="P28" t="inlineStr">
         <is>
-          <t>Solosis Community Day Community Day Starts: Sunday, October 12, 2025, at  2:00 PM Local Time Ends: Sunday, October 12, 2025, at  5:00 PM Local Time Solosis, the Cell Pokémon, will be featured during October Community Day! Bonuses Features Spawns Research Shiny Sales Graphic Bonuses Increased Spawns 3x Catch Stardust 3-hour Incense** 1-hour Lures*** 2x Catch Candy 2x Chance to receive Candy XL from catching Pokémon One additional Special Trade can be made for a maximum of three for the day* Trades made will require 50% less Stardust* * While most bonuses are only active during the three hours of the event, these bonuses will be active from 2:00 p.m. to 9:00 p.m. local time. ** The three-hour Incense bonus excludes Daily Adventure Incense. *** Lure Modules will last for one hour and may attract the featured Pokémon. Features Featured Attack Evolve Duosion (Solosis’s Evolution) during the event or up to four hours afterwards to get a Reuniclus that knows the Fast Attack Charm. Charm (Fairy-type) Trainer Battles: 13 power Gyms and raids: 20 power Photobomb Take a few snapshots during Community Day for a surprise! During the event you can snap an AR Photo and get photobombed by Solosis.</t>
+          <t>Harvest Festival Event Starts: Friday, October 10, 2025, at 10:00 AM Local Time Ends: Thursday, October 16, 2025, at  8:00 PM Local Time The Harvest Festival returns to Pokémon GO, featuring the debut of Dipplin and Hydrapple! Discover Syrupy Apples and enjoy special bonuses throughout the event! Bonuses Features Spawns Research Shiny Sales Bonuses 2× Candy for catching Pokémon with Pinap Berries and Silver Pinap Berries Increased chance to encounter Shiny Pumpkaboo and Shiny Smoliv Increased chance for apples to appear at PokéStops with an active Mossy Lure Module Features Pokémon Debuts The following Pokémon will make their Pokémon GO debuts! Dipplin Hydrapple You can use 200 Applin Candy and 20 Syrupy Apples to evolve Applin into Dipplin. You can evolve Dipplin into Hydrapple using 400 Applin Candy and by catching seven Dragon-type Pokémon with Dipplin as your buddy. Apples Beginning during the Harvest Festival event, you might discover Syrupy Apples ! Apples have an increased chance of appearing at PokéStops with active Mossy Lure Modules , and tapping on them will award Sweet Apples, Tart Apples, Syrupy Apples, or encounters with Pokémon—including Applin, if you’re lucky! Spaw</t>
         </is>
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>2024-06-01_community-day-solosis-community-day-sun-oct-12-at-500-pm-local-time-ends-calculating.html</t>
+          <t>2024-06-01_event-harvest-festival-thu-oct-16-at-800-pm-local-time-ends-calculating.html</t>
         </is>
       </c>
     </row>
@@ -1911,17 +1911,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-12</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-12</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Master Premier and Great League Remix | Tales of Transformation</t>
+          <t>Solosis Community Day</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -1940,12 +1940,12 @@
       <c r="O29" t="inlineStr"/>
       <c r="P29" t="inlineStr">
         <is>
-          <t>Master Premier and Great League Remix | Tales of Transformation GO Battle League Starts: Calculating... Ends: Calculating... The Master Premier and Great League Remix will run from October 14, 2025, at 1:00 p.m. to October 21, 2025, at 1:00 p.m. PT. Trainers will also receive 4× Stardust from win rewards (this does not include end-of-set rewards). Master Premier No CP limit. Legendary Pokémon, Mythical Pokémon, and Ultra Beasts are not eligible. Great League Remix Pokémon must be at or below 1,500 CP to enter. The 20 Pokémon that are most used by Trainers ranked Ace and above in the Great League are not eligible in the Great League Remix. Check back later for more details. Leek Duck Hey, I'm LeekDuck. I create Pokémon GO graphics, resources and report Pokémon GO news. You can find them on X, Facebook, Instagram, Threads, and Bluesky. You can also find me on Twitch and YouTube!</t>
+          <t>Solosis Community Day Community Day Starts: Sunday, October 12, 2025, at  2:00 PM Local Time Ends: Sunday, October 12, 2025, at  5:00 PM Local Time Solosis, the Cell Pokémon, will be featured during October Community Day! Bonuses Features Spawns Research Shiny Sales Graphic Bonuses Increased Spawns 3x Catch Stardust 3-hour Incense** 1-hour Lures*** 2x Catch Candy 2x Chance to receive Candy XL from catching Pokémon One additional Special Trade can be made for a maximum of three for the day* Trades made will require 50% less Stardust* * While most bonuses are only active during the three hours of the event, these bonuses will be active from 2:00 p.m. to 9:00 p.m. local time. ** The three-hour Incense bonus excludes Daily Adventure Incense. *** Lure Modules will last for one hour and may attract the featured Pokémon. Features Featured Attack Evolve Duosion (Solosis’s Evolution) during the event or up to four hours afterwards to get a Reuniclus that knows the Fast Attack Charm. Charm (Fairy-type) Trainer Battles: 13 power Gyms and raids: 20 power Photobomb Take a few snapshots during Community Day for a surprise! During the event you can snap an AR Photo and get photobombed by Solosis.</t>
         </is>
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>2024-06-01_go-battle-league-master-premier-and-great-league-remix--tales-of-transformation-calculating-ends-calculating.html</t>
+          <t>2024-06-01_community-day-solosis-community-day-sun-oct-12-at-500-pm-local-time-ends-calculating.html</t>
         </is>
       </c>
     </row>
@@ -1972,7 +1972,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Master Premier</t>
+          <t>Master Premier and Great League Remix | Tales of Transformation</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -1991,7 +1991,7 @@
       <c r="O30" t="inlineStr"/>
       <c r="P30" t="inlineStr">
         <is>
-          <t>The Master Premier and Great League Remix will run from October 14, 2025, at 1:00 p.m. to October 21, 2025, at 1:00 p.m. PT. Trainers will also receive 4× Stardust from win rewards (this does not include end-of-set rewards). Master Premier No CP limit. Legendary Pokémon, Mythical Pokémon, and Ultra Beasts are not eligible. Great League Remix Pokémon must be at or below 1,500 CP to enter. The 20 Pokémon that are most used by Trainers ranked Ace and above in the Great League are not eligible in the Great League Remix. Check back later for more details.</t>
+          <t>Master Premier and Great League Remix | Tales of Transformation GO Battle League Starts: Calculating... Ends: Calculating... The Master Premier and Great League Remix will run from October 14, 2025, at 1:00 p.m. to October 21, 2025, at 1:00 p.m. PT. Trainers will also receive 4× Stardust from win rewards (this does not include end-of-set rewards). Master Premier No CP limit. Legendary Pokémon, Mythical Pokémon, and Ultra Beasts are not eligible. Great League Remix Pokémon must be at or below 1,500 CP to enter. The 20 Pokémon that are most used by Trainers ranked Ace and above in the Great League are not eligible in the Great League Remix. Check back later for more details. Leek Duck Hey, I'm LeekDuck. I create Pokémon GO graphics, resources and report Pokémon GO news. You can find them on X, Facebook, Instagram, Threads, and Bluesky. You can also find me on Twitch and YouTube!</t>
         </is>
       </c>
       <c r="Q30" t="inlineStr">
@@ -2013,17 +2013,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>GO Battle Weekend: Tales of Transformation</t>
+          <t>Master Premier</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2042,12 +2042,12 @@
       <c r="O31" t="inlineStr"/>
       <c r="P31" t="inlineStr">
         <is>
-          <t>GO Battle Weekend: Tales of Transformation Event Starts: Saturday, October 25, 2025, at 12:00 AM Local Time Ends: Sunday, October 26, 2025, at 11:59 PM Local Time Bonuses 4× Stardust from win rewards. (This does not include end-of-set rewards.) The maximum number of sets you can play per day will increase from five to 20—for a total of 100 battles—from 12:00 a.m. to 11:59 p.m. local time. Free battle-themed Timed Research will be available. Rewards include glasses for your avatar inspired by Clemont. Pokémon encountered via GO Battle League rewards will have a wider variance of Attack, Defense, and HP. Active Leagues The following leagues will be active. Great League Ultra League Master League Research Sales Research Free battle-themed Timed Research will be available. Rewards include glasses for your avatar inspired by Clemont. Sales Pokémon GO Web Store - Special Boxes Get your party ready for GO Battle Weekend with new deals in the Pokémon GO Web Store! For US$4.99 (or the equivalent pricing tier in your local currency), the GO Battle Weekend Ultra Ticket Box will feature an event ticket and a bonus Premium Battle Pass at no additional cost. For US$19.99 (or the equivalent prici</t>
+          <t>The Master Premier and Great League Remix will run from October 14, 2025, at 1:00 p.m. to October 21, 2025, at 1:00 p.m. PT. Trainers will also receive 4× Stardust from win rewards (this does not include end-of-set rewards). Master Premier No CP limit. Legendary Pokémon, Mythical Pokémon, and Ultra Beasts are not eligible. Great League Remix Pokémon must be at or below 1,500 CP to enter. The 20 Pokémon that are most used by Trainers ranked Ace and above in the Great League are not eligible in the Great League Remix. Check back later for more details.</t>
         </is>
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>2024-06-01_event-go-battle-weekend-tales-of-transformation-sun-oct-26-at-1159-pm-local-time-ends-calculating.html</t>
+          <t>2024-06-01_go-battle-league-master-premier-and-great-league-remix--tales-of-transformation-calculating-ends-calculating.html</t>
         </is>
       </c>
     </row>
@@ -2064,17 +2064,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>2025-10-28</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2025-10-28</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation</t>
+          <t>GO Battle Weekend: Tales of Transformation</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2093,12 +2093,12 @@
       <c r="O32" t="inlineStr"/>
       <c r="P32" t="inlineStr">
         <is>
-          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation GO Battle League Starts: Calculating... Ends: Calculating... The Great League and Halloween Cup: Great League Edition will run from October 28, 2025, at 1:00 p.m. to November 4, 2025, at 1:00 p.m. PT. Great League Pokémon must be at or below 1,500 CP to enter. Halloween Cup: Great League Edition Pokémon must be at or below 1,500 CP to enter. Only Poison-, Bug-, Ghost-, Dark-, and Fairy-type Pokémon are eligible. Leek Duck Hey, I'm LeekDuck. I create Pokémon GO graphics, resources and report Pokémon GO news. You can find them on X, Facebook, Instagram, Threads, and Bluesky. You can also find me on Twitch and YouTube!</t>
+          <t>GO Battle Weekend: Tales of Transformation Event Starts: Saturday, October 25, 2025, at 12:00 AM Local Time Ends: Sunday, October 26, 2025, at 11:59 PM Local Time Bonuses 4× Stardust from win rewards. (This does not include end-of-set rewards.) The maximum number of sets you can play per day will increase from five to 20—for a total of 100 battles—from 12:00 a.m. to 11:59 p.m. local time. Free battle-themed Timed Research will be available. Rewards include glasses for your avatar inspired by Clemont. Pokémon encountered via GO Battle League rewards will have a wider variance of Attack, Defense, and HP. Active Leagues The following leagues will be active. Great League Ultra League Master League Research Sales Research Free battle-themed Timed Research will be available. Rewards include glasses for your avatar inspired by Clemont. Sales Pokémon GO Web Store - Special Boxes Get your party ready for GO Battle Weekend with new deals in the Pokémon GO Web Store! For US$4.99 (or the equivalent pricing tier in your local currency), the GO Battle Weekend Ultra Ticket Box will feature an event ticket and a bonus Premium Battle Pass at no additional cost. For US$19.99 (or the equivalent prici</t>
         </is>
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>2024-06-01_go-battle-league-great-league-and-halloween-cup-great-league-edition--tales-of-transformation-calculating-ends-calculati.html</t>
+          <t>2024-06-01_event-go-battle-weekend-tales-of-transformation-sun-oct-26-at-1159-pm-local-time-ends-calculating.html</t>
         </is>
       </c>
     </row>
@@ -2125,7 +2125,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Great League</t>
+          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2144,7 +2144,7 @@
       <c r="O33" t="inlineStr"/>
       <c r="P33" t="inlineStr">
         <is>
-          <t>The Great League and Halloween Cup: Great League Edition will run from October 28, 2025, at 1:00 p.m. to November 4, 2025, at 1:00 p.m. PT. Great League Pokémon must be at or below 1,500 CP to enter. Halloween Cup: Great League Edition Pokémon must be at or below 1,500 CP to enter. Only Poison-, Bug-, Ghost-, Dark-, and Fairy-type Pokémon are eligible.</t>
+          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation GO Battle League Starts: Calculating... Ends: Calculating... The Great League and Halloween Cup: Great League Edition will run from October 28, 2025, at 1:00 p.m. to November 4, 2025, at 1:00 p.m. PT. Great League Pokémon must be at or below 1,500 CP to enter. Halloween Cup: Great League Edition Pokémon must be at or below 1,500 CP to enter. Only Poison-, Bug-, Ghost-, Dark-, and Fairy-type Pokémon are eligible. Leek Duck Hey, I'm LeekDuck. I create Pokémon GO graphics, resources and report Pokémon GO news. You can find them on X, Facebook, Instagram, Threads, and Bluesky. You can also find me on Twitch and YouTube!</t>
         </is>
       </c>
       <c r="Q33" t="inlineStr">
@@ -2161,22 +2161,22 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>2025-11</t>
+          <t>2025-10</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>2025-11-04</t>
+          <t>2025-10-28</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>2025-11-04</t>
+          <t>2025-10-28</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
+          <t>Great League</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2195,12 +2195,12 @@
       <c r="O34" t="inlineStr"/>
       <c r="P34" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation GO Battle League Starts: Calculating... Ends: Calculating... The Ultra League and Jungle Cup: Great League Edition will run from November 4, 2025, at 1:00 p.m. to November 11, 2025, at 1:00 p.m. PT. Ultra League Pokémon must be at or below 2,500 CP to enter. Jungle Cup: Great League Edition Pokémon must be at or below 1,500 CP to enter. Only Normal-, Grass-, Electric-, Poison-, Ground-, Flying-, Bug-, and Dark-type Pokémon are eligible. The following Pokémon will not be allowed. Gligar Galarian Stunfisk Leek Duck Hey, I'm LeekDuck. I create Pokémon GO graphics, resources and report Pokémon GO news. You can find them on X, Facebook, Instagram, Threads, and Bluesky. You can also find me on Twitch and YouTube!</t>
+          <t>The Great League and Halloween Cup: Great League Edition will run from October 28, 2025, at 1:00 p.m. to November 4, 2025, at 1:00 p.m. PT. Great League Pokémon must be at or below 1,500 CP to enter. Halloween Cup: Great League Edition Pokémon must be at or below 1,500 CP to enter. Only Poison-, Bug-, Ghost-, Dark-, and Fairy-type Pokémon are eligible.</t>
         </is>
       </c>
       <c r="Q34" t="inlineStr">
         <is>
-          <t>2024-06-01_go-battle-league-ultra-league-and-jungle-cup-great-league-edition--tales-of-transformation-calculating-ends-calculating.html</t>
+          <t>2024-06-01_go-battle-league-great-league-and-halloween-cup-great-league-edition--tales-of-transformation-calculating-ends-calculati.html</t>
         </is>
       </c>
     </row>
@@ -2227,7 +2227,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Ultra League</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -2246,7 +2246,7 @@
       <c r="O35" t="inlineStr"/>
       <c r="P35" t="inlineStr">
         <is>
-          <t>The Ultra League and Jungle Cup: Great League Edition will run from November 4, 2025, at 1:00 p.m. to November 11, 2025, at 1:00 p.m. PT. Ultra League Pokémon must be at or below 2,500 CP to enter. Jungle Cup: Great League Edition Pokémon must be at or below 1,500 CP to enter. Only Normal-, Grass-, Electric-, Poison-, Ground-, Flying-, Bug-, and Dark-type Pokémon are eligible. The following Pokémon will not be allowed. Gligar Galarian Stunfisk</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation GO Battle League Starts: Calculating... Ends: Calculating... The Ultra League and Jungle Cup: Great League Edition will run from November 4, 2025, at 1:00 p.m. to November 11, 2025, at 1:00 p.m. PT. Ultra League Pokémon must be at or below 2,500 CP to enter. Jungle Cup: Great League Edition Pokémon must be at or below 1,500 CP to enter. Only Normal-, Grass-, Electric-, Poison-, Ground-, Flying-, Bug-, and Dark-type Pokémon are eligible. The following Pokémon will not be allowed. Gligar Galarian Stunfisk Leek Duck Hey, I'm LeekDuck. I create Pokémon GO graphics, resources and report Pokémon GO news. You can find them on X, Facebook, Instagram, Threads, and Bluesky. You can also find me on Twitch and YouTube!</t>
         </is>
       </c>
       <c r="Q35" t="inlineStr">
@@ -2278,7 +2278,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
+          <t>Ultra League</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -2297,7 +2297,7 @@
       <c r="O36" t="inlineStr"/>
       <c r="P36" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation GO Battle League Starts: Calculating... Ends: Calculating... The Ultra League and Jungle Cup: Great League Edition will run from November 4, 2025, at 1:00 p.m. to November 11, 2025, at 1:00 p.m. PT. Ultra League Pokémon must be at or below 2,500 CP to enter. Jungle Cup: Great League Edition Pokémon must be at or below 1,500 CP to enter. Only Normal-, Grass-, Electric-, Poison-, Ground-, Flying-, Bug-, and Dark-type Pokémon are eligible. The following Pokémon will not be allowed. Gligar Galarian Stunfisk Leek Duck Hey, I'm LeekDuck. I create Pokémon GO graphics, resources and report Pokémon GO news. You can find them on X, Facebook, Instagram, Threads, and Bluesky. You can also find me on Twitch and YouTube!</t>
+          <t>The Ultra League and Jungle Cup: Great League Edition will run from November 4, 2025, at 1:00 p.m. to November 11, 2025, at 1:00 p.m. PT. Ultra League Pokémon must be at or below 2,500 CP to enter. Jungle Cup: Great League Edition Pokémon must be at or below 1,500 CP to enter. Only Normal-, Grass-, Electric-, Poison-, Ground-, Flying-, Bug-, and Dark-type Pokémon are eligible. The following Pokémon will not be allowed. Gligar Galarian Stunfisk</t>
         </is>
       </c>
       <c r="Q36" t="inlineStr">
@@ -2329,7 +2329,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Ultra League</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -2348,7 +2348,7 @@
       <c r="O37" t="inlineStr"/>
       <c r="P37" t="inlineStr">
         <is>
-          <t>The Ultra League and Jungle Cup: Great League Edition will run from November 4, 2025, at 1:00 p.m. to November 11, 2025, at 1:00 p.m. PT. Ultra League Pokémon must be at or below 2,500 CP to enter. Jungle Cup: Great League Edition Pokémon must be at or below 1,500 CP to enter. Only Normal-, Grass-, Electric-, Poison-, Ground-, Flying-, Bug-, and Dark-type Pokémon are eligible. The following Pokémon will not be allowed. Gligar Galarian Stunfisk</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation GO Battle League Starts: Calculating... Ends: Calculating... The Ultra League and Jungle Cup: Great League Edition will run from November 4, 2025, at 1:00 p.m. to November 11, 2025, at 1:00 p.m. PT. Ultra League Pokémon must be at or below 2,500 CP to enter. Jungle Cup: Great League Edition Pokémon must be at or below 1,500 CP to enter. Only Normal-, Grass-, Electric-, Poison-, Ground-, Flying-, Bug-, and Dark-type Pokémon are eligible. The following Pokémon will not be allowed. Gligar Galarian Stunfisk Leek Duck Hey, I'm LeekDuck. I create Pokémon GO graphics, resources and report Pokémon GO news. You can find them on X, Facebook, Instagram, Threads, and Bluesky. You can also find me on Twitch and YouTube!</t>
         </is>
       </c>
       <c r="Q37" t="inlineStr">
@@ -2370,17 +2370,17 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>2025-11-09</t>
+          <t>2025-11-04</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>2025-11-09</t>
+          <t>2025-11-04</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Nagasaki</t>
+          <t>Ultra League</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -2399,12 +2399,12 @@
       <c r="O38" t="inlineStr"/>
       <c r="P38" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Nagasaki Wild Area Location-specific Ticketed Event Starts: Calculating... Ends: Calculating... For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area? In this next chapter of Pokémon GO Wild Area, get ready to test your skills once again as you encounter Dark- and Fairy-type Pokémon, including Grimmsnarl, the Bulk Up Pokémon! Plus, exceptionally powerful Pokémon known as mighty Pokémon are appearing in the wild—use GO Wild Area–exclusive GO Safari Balls to improve your odds of catching these rare Pokémon. All event gameplay is exclusive to ticket holders. Tickets for Pokémon GO Wild Area: Nagasaki are now available on the Niantic events portal . Live Event Ticket - ¥3,600 (including applicable taxes and fees) Location: A citywide experience across Nagasaki City, Japan Dates: November 7, 8, or 9, 2025 Time: 9:00 a.m. – 5:00 p.m. JST Tickets for Pokémon GO Wild Area: Nagasaki include one day of event gameplay, and attendees may purchase add-ons that extend the gameplay for an additional day. One-day tickets are ¥3,600 (or the equivalent pricing tier in your local currency, including applicable taxes and fees). Event game</t>
+          <t>The Ultra League and Jungle Cup: Great League Edition will run from November 4, 2025, at 1:00 p.m. to November 11, 2025, at 1:00 p.m. PT. Ultra League Pokémon must be at or below 2,500 CP to enter. Jungle Cup: Great League Edition Pokémon must be at or below 1,500 CP to enter. Only Normal-, Grass-, Electric-, Poison-, Ground-, Flying-, Bug-, and Dark-type Pokémon are eligible. The following Pokémon will not be allowed. Gligar Galarian Stunfisk</t>
         </is>
       </c>
       <c r="Q38" t="inlineStr">
         <is>
-          <t>2024-06-01_wild-area-pokmon-go-wild-area-nagasaki-calculating-ends-calculating.html</t>
+          <t>2024-06-01_go-battle-league-ultra-league-and-jungle-cup-great-league-edition--tales-of-transformation-calculating-ends-calculating.html</t>
         </is>
       </c>
     </row>
@@ -2421,17 +2421,17 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>2025-11-11</t>
+          <t>2025-11-09</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>2025-11-11</t>
+          <t>2025-11-09</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Pokémon GO Wild Area: Nagasaki</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -2450,12 +2450,12 @@
       <c r="O39" t="inlineStr"/>
       <c r="P39" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation GO Battle League Starts: Calculating... Ends: Calculating... The Great League, Ultra League, and Master League will run from November 11, 2025, at 1:00 p.m. to November 18, 2025, at 1:00 p.m. PT. Trainers will also receive 4× Stardust from win rewards (this does not include end-of-set rewards). Great League Pokémon must be at or below 1,500 CP to enter. Ultra League Pokémon must be at or below 2,500 CP to enter. Master League All Pokémon are eligible. Leek Duck Hey, I'm LeekDuck. I create Pokémon GO graphics, resources and report Pokémon GO news. You can find them on X, Facebook, Instagram, Threads, and Bluesky. You can also find me on Twitch and YouTube!</t>
+          <t>Pokémon GO Wild Area: Nagasaki Wild Area Location-specific Ticketed Event Starts: Calculating... Ends: Calculating... For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area? In this next chapter of Pokémon GO Wild Area, get ready to test your skills once again as you encounter Dark- and Fairy-type Pokémon, including Grimmsnarl, the Bulk Up Pokémon! Plus, exceptionally powerful Pokémon known as mighty Pokémon are appearing in the wild—use GO Wild Area–exclusive GO Safari Balls to improve your odds of catching these rare Pokémon. All event gameplay is exclusive to ticket holders. Tickets for Pokémon GO Wild Area: Nagasaki are now available on the Niantic events portal . Live Event Ticket - ¥3,600 (including applicable taxes and fees) Location: A citywide experience across Nagasaki City, Japan Dates: November 7, 8, or 9, 2025 Time: 9:00 a.m. – 5:00 p.m. JST Tickets for Pokémon GO Wild Area: Nagasaki include one day of event gameplay, and attendees may purchase add-ons that extend the gameplay for an additional day. One-day tickets are ¥3,600 (or the equivalent pricing tier in your local currency, including applicable taxes and fees). Event game</t>
         </is>
       </c>
       <c r="Q39" t="inlineStr">
         <is>
-          <t>2024-06-01_go-battle-league-great-league-ultra-league-and-master-league--tales-of-transformation-calculating-ends-calculating.html</t>
+          <t>2024-06-01_wild-area-pokmon-go-wild-area-nagasaki-calculating-ends-calculating.html</t>
         </is>
       </c>
     </row>
@@ -2482,7 +2482,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Great League</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -2501,7 +2501,7 @@
       <c r="O40" t="inlineStr"/>
       <c r="P40" t="inlineStr">
         <is>
-          <t>The Great League, Ultra League, and Master League will run from November 11, 2025, at 1:00 p.m. to November 18, 2025, at 1:00 p.m. PT. Trainers will also receive 4× Stardust from win rewards (this does not include end-of-set rewards). Great League Pokémon must be at or below 1,500 CP to enter. Ultra League Pokémon must be at or below 2,500 CP to enter. Master League All Pokémon are eligible.</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation GO Battle League Starts: Calculating... Ends: Calculating... The Great League, Ultra League, and Master League will run from November 11, 2025, at 1:00 p.m. to November 18, 2025, at 1:00 p.m. PT. Trainers will also receive 4× Stardust from win rewards (this does not include end-of-set rewards). Great League Pokémon must be at or below 1,500 CP to enter. Ultra League Pokémon must be at or below 2,500 CP to enter. Master League All Pokémon are eligible. Leek Duck Hey, I'm LeekDuck. I create Pokémon GO graphics, resources and report Pokémon GO news. You can find them on X, Facebook, Instagram, Threads, and Bluesky. You can also find me on Twitch and YouTube!</t>
         </is>
       </c>
       <c r="Q40" t="inlineStr">
@@ -2533,7 +2533,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Great League</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -2552,7 +2552,7 @@
       <c r="O41" t="inlineStr"/>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation GO Battle League Starts: Calculating... Ends: Calculating... The Great League, Ultra League, and Master League will run from November 11, 2025, at 1:00 p.m. to November 18, 2025, at 1:00 p.m. PT. Trainers will also receive 4× Stardust from win rewards (this does not include end-of-set rewards). Great League Pokémon must be at or below 1,500 CP to enter. Ultra League Pokémon must be at or below 2,500 CP to enter. Master League All Pokémon are eligible. Leek Duck Hey, I'm LeekDuck. I create Pokémon GO graphics, resources and report Pokémon GO news. You can find them on X, Facebook, Instagram, Threads, and Bluesky. You can also find me on Twitch and YouTube!</t>
+          <t>The Great League, Ultra League, and Master League will run from November 11, 2025, at 1:00 p.m. to November 18, 2025, at 1:00 p.m. PT. Trainers will also receive 4× Stardust from win rewards (this does not include end-of-set rewards). Great League Pokémon must be at or below 1,500 CP to enter. Ultra League Pokémon must be at or below 2,500 CP to enter. Master League All Pokémon are eligible.</t>
         </is>
       </c>
       <c r="Q41" t="inlineStr">
@@ -2584,7 +2584,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Great League</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -2603,7 +2603,7 @@
       <c r="O42" t="inlineStr"/>
       <c r="P42" t="inlineStr">
         <is>
-          <t>The Great League, Ultra League, and Master League will run from November 11, 2025, at 1:00 p.m. to November 18, 2025, at 1:00 p.m. PT. Trainers will also receive 4× Stardust from win rewards (this does not include end-of-set rewards). Great League Pokémon must be at or below 1,500 CP to enter. Ultra League Pokémon must be at or below 2,500 CP to enter. Master League All Pokémon are eligible.</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation GO Battle League Starts: Calculating... Ends: Calculating... The Great League, Ultra League, and Master League will run from November 11, 2025, at 1:00 p.m. to November 18, 2025, at 1:00 p.m. PT. Trainers will also receive 4× Stardust from win rewards (this does not include end-of-set rewards). Great League Pokémon must be at or below 1,500 CP to enter. Ultra League Pokémon must be at or below 2,500 CP to enter. Master League All Pokémon are eligible. Leek Duck Hey, I'm LeekDuck. I create Pokémon GO graphics, resources and report Pokémon GO news. You can find them on X, Facebook, Instagram, Threads, and Bluesky. You can also find me on Twitch and YouTube!</t>
         </is>
       </c>
       <c r="Q42" t="inlineStr">
@@ -2635,7 +2635,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Great League</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -2654,7 +2654,7 @@
       <c r="O43" t="inlineStr"/>
       <c r="P43" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation GO Battle League Starts: Calculating... Ends: Calculating... The Great League, Ultra League, and Master League will run from November 11, 2025, at 1:00 p.m. to November 18, 2025, at 1:00 p.m. PT. Trainers will also receive 4× Stardust from win rewards (this does not include end-of-set rewards). Great League Pokémon must be at or below 1,500 CP to enter. Ultra League Pokémon must be at or below 2,500 CP to enter. Master League All Pokémon are eligible. Leek Duck Hey, I'm LeekDuck. I create Pokémon GO graphics, resources and report Pokémon GO news. You can find them on X, Facebook, Instagram, Threads, and Bluesky. You can also find me on Twitch and YouTube!</t>
+          <t>The Great League, Ultra League, and Master League will run from November 11, 2025, at 1:00 p.m. to November 18, 2025, at 1:00 p.m. PT. Trainers will also receive 4× Stardust from win rewards (this does not include end-of-set rewards). Great League Pokémon must be at or below 1,500 CP to enter. Ultra League Pokémon must be at or below 2,500 CP to enter. Master League All Pokémon are eligible.</t>
         </is>
       </c>
       <c r="Q43" t="inlineStr">
@@ -2686,7 +2686,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Great League</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -2705,7 +2705,7 @@
       <c r="O44" t="inlineStr"/>
       <c r="P44" t="inlineStr">
         <is>
-          <t>The Great League, Ultra League, and Master League will run from November 11, 2025, at 1:00 p.m. to November 18, 2025, at 1:00 p.m. PT. Trainers will also receive 4× Stardust from win rewards (this does not include end-of-set rewards). Great League Pokémon must be at or below 1,500 CP to enter. Ultra League Pokémon must be at or below 2,500 CP to enter. Master League All Pokémon are eligible.</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation GO Battle League Starts: Calculating... Ends: Calculating... The Great League, Ultra League, and Master League will run from November 11, 2025, at 1:00 p.m. to November 18, 2025, at 1:00 p.m. PT. Trainers will also receive 4× Stardust from win rewards (this does not include end-of-set rewards). Great League Pokémon must be at or below 1,500 CP to enter. Ultra League Pokémon must be at or below 2,500 CP to enter. Master League All Pokémon are eligible. Leek Duck Hey, I'm LeekDuck. I create Pokémon GO graphics, resources and report Pokémon GO news. You can find them on X, Facebook, Instagram, Threads, and Bluesky. You can also find me on Twitch and YouTube!</t>
         </is>
       </c>
       <c r="Q44" t="inlineStr">
@@ -2727,17 +2727,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>2025-11-15</t>
+          <t>2025-11-11</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>2025-11-15</t>
+          <t>2025-11-11</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Global</t>
+          <t>Great League</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -2756,12 +2756,12 @@
       <c r="O45" t="inlineStr"/>
       <c r="P45" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Global Wild Area Ticketed Event Starts: Saturday, November 15, 2025, at 10:00 AM Local Time Ends: Sunday, November 16, 2025, at  6:00 PM Local Time For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area? Trainers around the world can gear up for a worldwide adventure during Pokémon GO Wild Area: Global, available in-game for two days only! Looking to enhance your GO Wild Area weekend with exclusive Special Research, additional bonuses, and an increased chance of encountering Shiny Pokémon? Purchase a global event ticket from the Pokémon GO Web Store! Event Tickets Tickets for Pokémon GO Wild Area: Global are available now in the in-game Shop and Pokémon Go Web Store for $11.99 USD . Purchase your ticket on the Pokémon GO Web Store for a new avatar item! Trainers who purchase their Pokémon GO Wild Area: Global ticket on the Pokémon GO Web Store will receive a special avatar item—the Flower Crown! You can purchase your ticket on the web store until the last day of the event to receive this avatar item. Pokémon GO Wild Area: Nagasaki For details on the in-person event in Nagasaki, Japan, click here . Bonuses Features Spawn</t>
+          <t>The Great League, Ultra League, and Master League will run from November 11, 2025, at 1:00 p.m. to November 18, 2025, at 1:00 p.m. PT. Trainers will also receive 4× Stardust from win rewards (this does not include end-of-set rewards). Great League Pokémon must be at or below 1,500 CP to enter. Ultra League Pokémon must be at or below 2,500 CP to enter. Master League All Pokémon are eligible.</t>
         </is>
       </c>
       <c r="Q45" t="inlineStr">
         <is>
-          <t>2024-06-01_wild-area-pokmon-go-wild-area-global-sun-nov-16-at-600-pm-local-time-ends-calculating.html</t>
+          <t>2024-06-01_go-battle-league-great-league-ultra-league-and-master-league--tales-of-transformation-calculating-ends-calculating.html</t>
         </is>
       </c>
     </row>
@@ -2778,22 +2778,22 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>2025-11-18</t>
+          <t>2025-11-15</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>2025-11-18</t>
+          <t>2025-11-15</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation</t>
+          <t>Pokémon GO Wild Area: Global</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G46" t="inlineStr"/>
@@ -2807,12 +2807,12 @@
       <c r="O46" t="inlineStr"/>
       <c r="P46" t="inlineStr">
         <is>
-          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation GO Battle League Starts: Calculating... Ends: Calculating... The 2025 Championship Series Cup and Master League: Mega Edition will run from November 18, 2025, at 1:00 p.m. to November 25, 2025, at 1:00 p.m. PT. Trainers will also receive 4× Stardust from win rewards (this does not include end-of-set rewards). 2025 Championship Series Cup Pokémon must be at or below 1,500 CP to enter. Only Ice-, Flying-, Psychic-, Ghost-, and Dragon-type Pokémon are eligible. Legendary Pokémon, Mythical Pokémon, Shadow Pokémon, and Ultra Beasts are not eligible. The following Pokémon will not be allowed. Alolan Sandshrew Alolan Sandslash Alolan Ninetales Lapras Galarian Corsola Kingdra Jellicent Honedge Doublade Corviknight Master League: Mega Edition No CP limit. Mega-Evolved Pokémon are allowed. Leek Duck Hey, I'm LeekDuck. I create Pokémon GO graphics, resources and report Pokémon GO news. You can find them on X, Facebook, Instagram, Threads, and Bluesky. You can also find me on Twitch and YouTube!</t>
+          <t>Pokémon GO Wild Area: Global Wild Area Ticketed Event Starts: Saturday, November 15, 2025, at 10:00 AM Local Time Ends: Sunday, November 16, 2025, at  6:00 PM Local Time For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area? Trainers around the world can gear up for a worldwide adventure during Pokémon GO Wild Area: Global, available in-game for two days only! Looking to enhance your GO Wild Area weekend with exclusive Special Research, additional bonuses, and an increased chance of encountering Shiny Pokémon? Purchase a global event ticket from the Pokémon GO Web Store! Event Tickets Tickets for Pokémon GO Wild Area: Global are available now in the in-game Shop and Pokémon Go Web Store for $11.99 USD . Purchase your ticket on the Pokémon GO Web Store for a new avatar item! Trainers who purchase their Pokémon GO Wild Area: Global ticket on the Pokémon GO Web Store will receive a special avatar item—the Flower Crown! You can purchase your ticket on the web store until the last day of the event to receive this avatar item. Pokémon GO Wild Area: Nagasaki For details on the in-person event in Nagasaki, Japan, click here . Bonuses Features Spawn</t>
         </is>
       </c>
       <c r="Q46" t="inlineStr">
         <is>
-          <t>2024-06-01_go-battle-league-2025-championship-series-cup-and-master-league-mega-edition--tales-of-transformation-calculating-ends-c.html</t>
+          <t>2024-06-01_wild-area-pokmon-go-wild-area-global-sun-nov-16-at-600-pm-local-time-ends-calculating.html</t>
         </is>
       </c>
     </row>
@@ -2839,12 +2839,12 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>2025 Championship Series Cup</t>
+          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G47" t="inlineStr"/>
@@ -2858,7 +2858,7 @@
       <c r="O47" t="inlineStr"/>
       <c r="P47" t="inlineStr">
         <is>
-          <t>The 2025 Championship Series Cup and Master League: Mega Edition will run from November 18, 2025, at 1:00 p.m. to November 25, 2025, at 1:00 p.m. PT. Trainers will also receive 4× Stardust from win rewards (this does not include end-of-set rewards). 2025 Championship Series Cup Pokémon must be at or below 1,500 CP to enter. Only Ice-, Flying-, Psychic-, Ghost-, and Dragon-type Pokémon are eligible. Legendary Pokémon, Mythical Pokémon, Shadow Pokémon, and Ultra Beasts are not eligible. The following Pokémon will not be allowed. Alolan Sandshrew Alolan Sandslash Alolan Ninetales Lapras Galarian Corsola Kingdra Jellicent Honedge Doublade Corviknight Master League: Mega Edition No CP limit. Mega-Evolved Pokémon are allowed.</t>
+          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation GO Battle League Starts: Calculating... Ends: Calculating... The 2025 Championship Series Cup and Master League: Mega Edition will run from November 18, 2025, at 1:00 p.m. to November 25, 2025, at 1:00 p.m. PT. Trainers will also receive 4× Stardust from win rewards (this does not include end-of-set rewards). 2025 Championship Series Cup Pokémon must be at or below 1,500 CP to enter. Only Ice-, Flying-, Psychic-, Ghost-, and Dragon-type Pokémon are eligible. Legendary Pokémon, Mythical Pokémon, Shadow Pokémon, and Ultra Beasts are not eligible. The following Pokémon will not be allowed. Alolan Sandshrew Alolan Sandslash Alolan Ninetales Lapras Galarian Corsola Kingdra Jellicent Honedge Doublade Corviknight Master League: Mega Edition No CP limit. Mega-Evolved Pokémon are allowed. Leek Duck Hey, I'm LeekDuck. I create Pokémon GO graphics, resources and report Pokémon GO news. You can find them on X, Facebook, Instagram, Threads, and Bluesky. You can also find me on Twitch and YouTube!</t>
         </is>
       </c>
       <c r="Q47" t="inlineStr">
@@ -2880,17 +2880,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-18</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-18</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation</t>
+          <t>2025 Championship Series Cup</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -2909,12 +2909,12 @@
       <c r="O48" t="inlineStr"/>
       <c r="P48" t="inlineStr">
         <is>
-          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation GO Battle League Starts: Calculating... Ends: Calculating... The Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League will run from November 25, 2025, at 1:00 p.m. to December 2, 2025, at 1:00 p.m. PT. Trainers will also receive 4× Stardust from win rewards (this does not include end-of-set rewards). Catch Cup: Tales of Transformation: Great Edition Pokémon must be at or below 1,500 CP to enter. Only Pokémon caught during the Tales of Transformation Season are eligible. Pokémon must be caught between September 2, 2025, at 1:00 p.m. and December 2, 2025, at 1:00 p.m. local time. Ultra League Pokémon must be at or below 2,500 CP to enter. Master League All Pokémon are eligible. Leek Duck Hey, I'm LeekDuck. I create Pokémon GO graphics, resources and report Pokémon GO news. You can find them on X, Facebook, Instagram, Threads, and Bluesky. You can also find me on Twitch and YouTube!</t>
+          <t>The 2025 Championship Series Cup and Master League: Mega Edition will run from November 18, 2025, at 1:00 p.m. to November 25, 2025, at 1:00 p.m. PT. Trainers will also receive 4× Stardust from win rewards (this does not include end-of-set rewards). 2025 Championship Series Cup Pokémon must be at or below 1,500 CP to enter. Only Ice-, Flying-, Psychic-, Ghost-, and Dragon-type Pokémon are eligible. Legendary Pokémon, Mythical Pokémon, Shadow Pokémon, and Ultra Beasts are not eligible. The following Pokémon will not be allowed. Alolan Sandshrew Alolan Sandslash Alolan Ninetales Lapras Galarian Corsola Kingdra Jellicent Honedge Doublade Corviknight Master League: Mega Edition No CP limit. Mega-Evolved Pokémon are allowed.</t>
         </is>
       </c>
       <c r="Q48" t="inlineStr">
         <is>
-          <t>2024-06-01_go-battle-league-catch-cup-tales-of-transformation-great-edition-ultra-league-and-master-league--tales-of-transformation.html</t>
+          <t>2024-06-01_go-battle-league-2025-championship-series-cup-and-master-league-mega-edition--tales-of-transformation-calculating-ends-c.html</t>
         </is>
       </c>
     </row>
@@ -2941,7 +2941,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Catch Cup: Tales of Transformation: Great Edition</t>
+          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -2960,7 +2960,7 @@
       <c r="O49" t="inlineStr"/>
       <c r="P49" t="inlineStr">
         <is>
-          <t>The Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League will run from November 25, 2025, at 1:00 p.m. to December 2, 2025, at 1:00 p.m. PT. Trainers will also receive 4× Stardust from win rewards (this does not include end-of-set rewards). Catch Cup: Tales of Transformation: Great Edition Pokémon must be at or below 1,500 CP to enter. Only Pokémon caught during the Tales of Transformation Season are eligible. Pokémon must be caught between September 2, 2025, at 1:00 p.m. and December 2, 2025, at 1:00 p.m. local time. Ultra League Pokémon must be at or below 2,500 CP to enter. Master League All Pokémon are eligible.</t>
+          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation GO Battle League Starts: Calculating... Ends: Calculating... The Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League will run from November 25, 2025, at 1:00 p.m. to December 2, 2025, at 1:00 p.m. PT. Trainers will also receive 4× Stardust from win rewards (this does not include end-of-set rewards). Catch Cup: Tales of Transformation: Great Edition Pokémon must be at or below 1,500 CP to enter. Only Pokémon caught during the Tales of Transformation Season are eligible. Pokémon must be caught between September 2, 2025, at 1:00 p.m. and December 2, 2025, at 1:00 p.m. local time. Ultra League Pokémon must be at or below 2,500 CP to enter. Master League All Pokémon are eligible. Leek Duck Hey, I'm LeekDuck. I create Pokémon GO graphics, resources and report Pokémon GO news. You can find them on X, Facebook, Instagram, Threads, and Bluesky. You can also find me on Twitch and YouTube!</t>
         </is>
       </c>
       <c r="Q49" t="inlineStr">
@@ -2982,17 +2982,17 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>November Community Day</t>
+          <t>Catch Cup: Tales of Transformation: Great Edition</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -3011,12 +3011,12 @@
       <c r="O50" t="inlineStr"/>
       <c r="P50" t="inlineStr">
         <is>
-          <t>November Community Day Community Day Starts: Sunday, November 30, 2025, at  2:00 PM Local Time Ends: Sunday, November 30, 2025, at  5:00 PM Local Time November Community Day is on November 30, 2025. Stay tuned for the announcement of the featured Pokémon. Leek Duck Hey, I'm LeekDuck. I create Pokémon GO graphics, resources and report Pokémon GO news. You can find them on X, Facebook, Instagram, Threads, and Bluesky. You can also find me on Twitch and YouTube!</t>
+          <t>The Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League will run from November 25, 2025, at 1:00 p.m. to December 2, 2025, at 1:00 p.m. PT. Trainers will also receive 4× Stardust from win rewards (this does not include end-of-set rewards). Catch Cup: Tales of Transformation: Great Edition Pokémon must be at or below 1,500 CP to enter. Only Pokémon caught during the Tales of Transformation Season are eligible. Pokémon must be caught between September 2, 2025, at 1:00 p.m. and December 2, 2025, at 1:00 p.m. local time. Ultra League Pokémon must be at or below 2,500 CP to enter. Master League All Pokémon are eligible.</t>
         </is>
       </c>
       <c r="Q50" t="inlineStr">
         <is>
-          <t>2024-06-01_community-day-november-community-day-sun-nov-30-at-500-pm-local-time-ends-calculating.html</t>
+          <t>2024-06-01_go-battle-league-catch-cup-tales-of-transformation-great-edition-ultra-league-and-master-league--tales-of-transformation.html</t>
         </is>
       </c>
     </row>
@@ -3026,17 +3026,29 @@
           <t>Leek Duck</t>
         </is>
       </c>
-      <c r="B51" t="inlineStr"/>
-      <c r="C51" t="inlineStr"/>
-      <c r="D51" t="inlineStr"/>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>2025-11</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>2025-11-30</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>2025-11-30</t>
+        </is>
+      </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Dialga (Origin Forme) Raid Hour</t>
+          <t>November Community Day</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G51" t="inlineStr"/>
@@ -3050,12 +3062,12 @@
       <c r="O51" t="inlineStr"/>
       <c r="P51" t="inlineStr">
         <is>
-          <t>Raid Hour Dialga (Origin Forme) Raid Hour Wed, Sep 24, at 7:00 PM Local Time Ends: Calculating... PokéStop Showcase Ditto, Dunsparce, Dudunsparce PokéStop Showcases Wed, Sep 24, at 8:00 PM Local Time Ends: Calculating... Event Completely Normal Sat, Sep 27, at 8:00 PM Local Time Ends: Calculating... City Safari Bangkok, Thailand - Pokémon GO City Safari Sun, Sep 28, at 6:00 PM Local Time Ends: Calculating... City Safari Amsterdam, Netherlands - Pokémon GO City Safari Sun, Sep 28, at 6:00 PM Local Time Ends: Calculating... City Safari Valencia, Spain - Pokémon GO City Safari Sun, Sep 28, at 6:00 PM Local Time Ends: Calculating... City Safari Cancún, Mexico - Pokémon GO City Safari Sun, Sep 28, at 6:00 PM Local Time Ends: Calculating... City Safari Vancouver, Canada - Pokémon GO City Safari Sun, Sep 28, at 6:00 PM Local Time Ends: Calculating... Raid Day Mega Camerupt Raid Day Sun, Sep 28, at 5:00 PM Local Time Ends: Calculating... Max Mondays Dynamax Beldum during Max Monday Mon, Sep 29, at 7:00 PM Local Time Ends: Calculating... Raid Battles Mega Kangaskhan and Mega Lopunny in Mega Raids Tue, Sep 30, at 10:00 AM Local Time Ends: Calculating... GO Battle League Great League, Ultra L</t>
+          <t>November Community Day Community Day Starts: Sunday, November 30, 2025, at  2:00 PM Local Time Ends: Sunday, November 30, 2025, at  5:00 PM Local Time November Community Day is on November 30, 2025. Stay tuned for the announcement of the featured Pokémon. Leek Duck Hey, I'm LeekDuck. I create Pokémon GO graphics, resources and report Pokémon GO news. You can find them on X, Facebook, Instagram, Threads, and Bluesky. You can also find me on Twitch and YouTube!</t>
         </is>
       </c>
       <c r="Q51" t="inlineStr">
         <is>
-          <t>2024-06-01_events.html</t>
+          <t>2024-06-01_community-day-november-community-day-sun-nov-30-at-500-pm-local-time-ends-calculating.html</t>
         </is>
       </c>
     </row>
@@ -3089,7 +3101,7 @@
       <c r="O52" t="inlineStr"/>
       <c r="P52" t="inlineStr">
         <is>
-          <t>Raid Hour Dialga (Origin Forme) Raid Hour Wed, Sep 24, at 7:00 PM Local Time Ends: Calculating...</t>
+          <t>Raid Hour Dialga (Origin Forme) Raid Hour Wed, Sep 24, at 7:00 PM Local Time Ends: Calculating... PokéStop Showcase Ditto, Dunsparce, Dudunsparce PokéStop Showcases Wed, Sep 24, at 8:00 PM Local Time Ends: Calculating... Event Completely Normal Sat, Sep 27, at 8:00 PM Local Time Ends: Calculating... City Safari Bangkok, Thailand - Pokémon GO City Safari Sun, Sep 28, at 6:00 PM Local Time Ends: Calculating... City Safari Amsterdam, Netherlands - Pokémon GO City Safari Sun, Sep 28, at 6:00 PM Local Time Ends: Calculating... City Safari Valencia, Spain - Pokémon GO City Safari Sun, Sep 28, at 6:00 PM Local Time Ends: Calculating... City Safari Cancún, Mexico - Pokémon GO City Safari Sun, Sep 28, at 6:00 PM Local Time Ends: Calculating... City Safari Vancouver, Canada - Pokémon GO City Safari Sun, Sep 28, at 6:00 PM Local Time Ends: Calculating... Raid Day Mega Camerupt Raid Day Sun, Sep 28, at 5:00 PM Local Time Ends: Calculating... Max Mondays Dynamax Beldum during Max Monday Mon, Sep 29, at 7:00 PM Local Time Ends: Calculating... Raid Battles Mega Kangaskhan and Mega Lopunny in Mega Raids Tue, Sep 30, at 10:00 AM Local Time Ends: Calculating... GO Battle League Great League, Ultra L</t>
         </is>
       </c>
       <c r="Q52" t="inlineStr">
@@ -3128,7 +3140,7 @@
       <c r="O53" t="inlineStr"/>
       <c r="P53" t="inlineStr">
         <is>
-          <t>Dialga (Origin Forme) Raid Hour Wed, Sep 24, at 7:00 PM Local Time Ends: Calculating...</t>
+          <t>Raid Hour Dialga (Origin Forme) Raid Hour Wed, Sep 24, at 7:00 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q53" t="inlineStr">
@@ -3206,7 +3218,7 @@
       <c r="O55" t="inlineStr"/>
       <c r="P55" t="inlineStr">
         <is>
-          <t>Dialga (Origin Forme) Raid Hour Wed, Sep 24, at 7:00 PM Local Time</t>
+          <t>Dialga (Origin Forme) Raid Hour Wed, Sep 24, at 7:00 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q55" t="inlineStr">
@@ -3226,12 +3238,12 @@
       <c r="D56" t="inlineStr"/>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Ditto, Dunsparce, Dudunsparce PokéStop Showcases</t>
+          <t>Dialga (Origin Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G56" t="inlineStr"/>
@@ -3245,7 +3257,7 @@
       <c r="O56" t="inlineStr"/>
       <c r="P56" t="inlineStr">
         <is>
-          <t>PokéStop Showcase Ditto, Dunsparce, Dudunsparce PokéStop Showcases Wed, Sep 24, at 8:00 PM Local Time Ends: Calculating...</t>
+          <t>Dialga (Origin Forme) Raid Hour Wed, Sep 24, at 7:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q56" t="inlineStr">
@@ -3284,7 +3296,7 @@
       <c r="O57" t="inlineStr"/>
       <c r="P57" t="inlineStr">
         <is>
-          <t>Ditto, Dunsparce, Dudunsparce PokéStop Showcases Wed, Sep 24, at 8:00 PM Local Time Ends: Calculating...</t>
+          <t>PokéStop Showcase Ditto, Dunsparce, Dudunsparce PokéStop Showcases Wed, Sep 24, at 8:00 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q57" t="inlineStr">
@@ -3362,7 +3374,7 @@
       <c r="O59" t="inlineStr"/>
       <c r="P59" t="inlineStr">
         <is>
-          <t>Ditto, Dunsparce, Dudunsparce PokéStop Showcases Wed, Sep 24, at 8:00 PM Local Time</t>
+          <t>Ditto, Dunsparce, Dudunsparce PokéStop Showcases Wed, Sep 24, at 8:00 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q59" t="inlineStr">
@@ -3382,7 +3394,7 @@
       <c r="D60" t="inlineStr"/>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Completely Normal</t>
+          <t>Ditto, Dunsparce, Dudunsparce PokéStop Showcases</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -3401,7 +3413,7 @@
       <c r="O60" t="inlineStr"/>
       <c r="P60" t="inlineStr">
         <is>
-          <t>Event Completely Normal Sat, Sep 27, at 8:00 PM Local Time Ends: Calculating...</t>
+          <t>Ditto, Dunsparce, Dudunsparce PokéStop Showcases Wed, Sep 24, at 8:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q60" t="inlineStr">
@@ -3440,7 +3452,7 @@
       <c r="O61" t="inlineStr"/>
       <c r="P61" t="inlineStr">
         <is>
-          <t>Completely Normal Sat, Sep 27, at 8:00 PM Local Time Ends: Calculating...</t>
+          <t>Event Completely Normal Sat, Sep 27, at 8:00 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q61" t="inlineStr">
@@ -3518,7 +3530,7 @@
       <c r="O63" t="inlineStr"/>
       <c r="P63" t="inlineStr">
         <is>
-          <t>Completely Normal Sat, Sep 27, at 8:00 PM Local Time</t>
+          <t>Completely Normal Sat, Sep 27, at 8:00 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q63" t="inlineStr">
@@ -3538,7 +3550,7 @@
       <c r="D64" t="inlineStr"/>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Bangkok, Thailand - Pokémon GO City Safari</t>
+          <t>Completely Normal</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -3557,7 +3569,7 @@
       <c r="O64" t="inlineStr"/>
       <c r="P64" t="inlineStr">
         <is>
-          <t>City Safari Bangkok, Thailand - Pokémon GO City Safari Sun, Sep 28, at 6:00 PM Local Time Ends: Calculating...</t>
+          <t>Completely Normal Sat, Sep 27, at 8:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q64" t="inlineStr">
@@ -3596,7 +3608,7 @@
       <c r="O65" t="inlineStr"/>
       <c r="P65" t="inlineStr">
         <is>
-          <t>Bangkok, Thailand - Pokémon GO City Safari Sun, Sep 28, at 6:00 PM Local Time Ends: Calculating...</t>
+          <t>City Safari Bangkok, Thailand - Pokémon GO City Safari Sun, Sep 28, at 6:00 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q65" t="inlineStr">
@@ -3674,7 +3686,7 @@
       <c r="O67" t="inlineStr"/>
       <c r="P67" t="inlineStr">
         <is>
-          <t>Bangkok, Thailand - Pokémon GO City Safari Sun, Sep 28, at 6:00 PM Local Time</t>
+          <t>Bangkok, Thailand - Pokémon GO City Safari Sun, Sep 28, at 6:00 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q67" t="inlineStr">
@@ -3694,7 +3706,7 @@
       <c r="D68" t="inlineStr"/>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Amsterdam, Netherlands - Pokémon GO City Safari</t>
+          <t>Bangkok, Thailand - Pokémon GO City Safari</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -3713,7 +3725,7 @@
       <c r="O68" t="inlineStr"/>
       <c r="P68" t="inlineStr">
         <is>
-          <t>City Safari Amsterdam, Netherlands - Pokémon GO City Safari Sun, Sep 28, at 6:00 PM Local Time Ends: Calculating...</t>
+          <t>Bangkok, Thailand - Pokémon GO City Safari Sun, Sep 28, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q68" t="inlineStr">
@@ -3752,7 +3764,7 @@
       <c r="O69" t="inlineStr"/>
       <c r="P69" t="inlineStr">
         <is>
-          <t>Amsterdam, Netherlands - Pokémon GO City Safari Sun, Sep 28, at 6:00 PM Local Time Ends: Calculating...</t>
+          <t>City Safari Amsterdam, Netherlands - Pokémon GO City Safari Sun, Sep 28, at 6:00 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q69" t="inlineStr">
@@ -3830,7 +3842,7 @@
       <c r="O71" t="inlineStr"/>
       <c r="P71" t="inlineStr">
         <is>
-          <t>Amsterdam, Netherlands - Pokémon GO City Safari Sun, Sep 28, at 6:00 PM Local Time</t>
+          <t>Amsterdam, Netherlands - Pokémon GO City Safari Sun, Sep 28, at 6:00 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q71" t="inlineStr">
@@ -3850,7 +3862,7 @@
       <c r="D72" t="inlineStr"/>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Valencia, Spain - Pokémon GO City Safari</t>
+          <t>Amsterdam, Netherlands - Pokémon GO City Safari</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -3869,7 +3881,7 @@
       <c r="O72" t="inlineStr"/>
       <c r="P72" t="inlineStr">
         <is>
-          <t>City Safari Valencia, Spain - Pokémon GO City Safari Sun, Sep 28, at 6:00 PM Local Time Ends: Calculating...</t>
+          <t>Amsterdam, Netherlands - Pokémon GO City Safari Sun, Sep 28, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q72" t="inlineStr">
@@ -3908,7 +3920,7 @@
       <c r="O73" t="inlineStr"/>
       <c r="P73" t="inlineStr">
         <is>
-          <t>Valencia, Spain - Pokémon GO City Safari Sun, Sep 28, at 6:00 PM Local Time Ends: Calculating...</t>
+          <t>City Safari Valencia, Spain - Pokémon GO City Safari Sun, Sep 28, at 6:00 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q73" t="inlineStr">
@@ -3986,7 +3998,7 @@
       <c r="O75" t="inlineStr"/>
       <c r="P75" t="inlineStr">
         <is>
-          <t>Valencia, Spain - Pokémon GO City Safari Sun, Sep 28, at 6:00 PM Local Time</t>
+          <t>Valencia, Spain - Pokémon GO City Safari Sun, Sep 28, at 6:00 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q75" t="inlineStr">
@@ -4006,7 +4018,7 @@
       <c r="D76" t="inlineStr"/>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Cancún, Mexico - Pokémon GO City Safari</t>
+          <t>Valencia, Spain - Pokémon GO City Safari</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -4025,7 +4037,7 @@
       <c r="O76" t="inlineStr"/>
       <c r="P76" t="inlineStr">
         <is>
-          <t>City Safari Cancún, Mexico - Pokémon GO City Safari Sun, Sep 28, at 6:00 PM Local Time Ends: Calculating...</t>
+          <t>Valencia, Spain - Pokémon GO City Safari Sun, Sep 28, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q76" t="inlineStr">
@@ -4064,7 +4076,7 @@
       <c r="O77" t="inlineStr"/>
       <c r="P77" t="inlineStr">
         <is>
-          <t>Cancún, Mexico - Pokémon GO City Safari Sun, Sep 28, at 6:00 PM Local Time Ends: Calculating...</t>
+          <t>City Safari Cancún, Mexico - Pokémon GO City Safari Sun, Sep 28, at 6:00 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q77" t="inlineStr">
@@ -4142,7 +4154,7 @@
       <c r="O79" t="inlineStr"/>
       <c r="P79" t="inlineStr">
         <is>
-          <t>Cancún, Mexico - Pokémon GO City Safari Sun, Sep 28, at 6:00 PM Local Time</t>
+          <t>Cancún, Mexico - Pokémon GO City Safari Sun, Sep 28, at 6:00 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q79" t="inlineStr">
@@ -4162,7 +4174,7 @@
       <c r="D80" t="inlineStr"/>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Vancouver, Canada - Pokémon GO City Safari</t>
+          <t>Cancún, Mexico - Pokémon GO City Safari</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -4181,7 +4193,7 @@
       <c r="O80" t="inlineStr"/>
       <c r="P80" t="inlineStr">
         <is>
-          <t>City Safari Vancouver, Canada - Pokémon GO City Safari Sun, Sep 28, at 6:00 PM Local Time Ends: Calculating...</t>
+          <t>Cancún, Mexico - Pokémon GO City Safari Sun, Sep 28, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q80" t="inlineStr">
@@ -4220,7 +4232,7 @@
       <c r="O81" t="inlineStr"/>
       <c r="P81" t="inlineStr">
         <is>
-          <t>Vancouver, Canada - Pokémon GO City Safari Sun, Sep 28, at 6:00 PM Local Time Ends: Calculating...</t>
+          <t>City Safari Vancouver, Canada - Pokémon GO City Safari Sun, Sep 28, at 6:00 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q81" t="inlineStr">
@@ -4298,7 +4310,7 @@
       <c r="O83" t="inlineStr"/>
       <c r="P83" t="inlineStr">
         <is>
-          <t>Vancouver, Canada - Pokémon GO City Safari Sun, Sep 28, at 6:00 PM Local Time</t>
+          <t>Vancouver, Canada - Pokémon GO City Safari Sun, Sep 28, at 6:00 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q83" t="inlineStr">
@@ -4318,12 +4330,12 @@
       <c r="D84" t="inlineStr"/>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Mega Camerupt Raid Day</t>
+          <t>Vancouver, Canada - Pokémon GO City Safari</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G84" t="inlineStr"/>
@@ -4337,7 +4349,7 @@
       <c r="O84" t="inlineStr"/>
       <c r="P84" t="inlineStr">
         <is>
-          <t>Raid Day Mega Camerupt Raid Day Sun, Sep 28, at 5:00 PM Local Time Ends: Calculating...</t>
+          <t>Vancouver, Canada - Pokémon GO City Safari Sun, Sep 28, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q84" t="inlineStr">
@@ -4376,7 +4388,7 @@
       <c r="O85" t="inlineStr"/>
       <c r="P85" t="inlineStr">
         <is>
-          <t>Mega Camerupt Raid Day Sun, Sep 28, at 5:00 PM Local Time Ends: Calculating...</t>
+          <t>Raid Day Mega Camerupt Raid Day Sun, Sep 28, at 5:00 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q85" t="inlineStr">
@@ -4454,7 +4466,7 @@
       <c r="O87" t="inlineStr"/>
       <c r="P87" t="inlineStr">
         <is>
-          <t>Mega Camerupt Raid Day Sun, Sep 28, at 5:00 PM Local Time</t>
+          <t>Mega Camerupt Raid Day Sun, Sep 28, at 5:00 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q87" t="inlineStr">
@@ -4474,12 +4486,12 @@
       <c r="D88" t="inlineStr"/>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Dynamax Beldum during Max Monday</t>
+          <t>Mega Camerupt Raid Day</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G88" t="inlineStr"/>
@@ -4493,7 +4505,7 @@
       <c r="O88" t="inlineStr"/>
       <c r="P88" t="inlineStr">
         <is>
-          <t>Max Mondays Dynamax Beldum during Max Monday Mon, Sep 29, at 7:00 PM Local Time Ends: Calculating...</t>
+          <t>Mega Camerupt Raid Day Sun, Sep 28, at 5:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q88" t="inlineStr">
@@ -4532,7 +4544,7 @@
       <c r="O89" t="inlineStr"/>
       <c r="P89" t="inlineStr">
         <is>
-          <t>Dynamax Beldum during Max Monday Mon, Sep 29, at 7:00 PM Local Time Ends: Calculating...</t>
+          <t>Max Mondays Dynamax Beldum during Max Monday Mon, Sep 29, at 7:00 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q89" t="inlineStr">
@@ -4610,7 +4622,7 @@
       <c r="O91" t="inlineStr"/>
       <c r="P91" t="inlineStr">
         <is>
-          <t>Dynamax Beldum during Max Monday Mon, Sep 29, at 7:00 PM Local Time</t>
+          <t>Dynamax Beldum during Max Monday Mon, Sep 29, at 7:00 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q91" t="inlineStr">
@@ -4630,12 +4642,12 @@
       <c r="D92" t="inlineStr"/>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Mega Kangaskhan and Mega Lopunny in Mega Raids</t>
+          <t>Dynamax Beldum during Max Monday</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G92" t="inlineStr"/>
@@ -4649,7 +4661,7 @@
       <c r="O92" t="inlineStr"/>
       <c r="P92" t="inlineStr">
         <is>
-          <t>Raid Battles Mega Kangaskhan and Mega Lopunny in Mega Raids Tue, Sep 30, at 10:00 AM Local Time Ends: Calculating...</t>
+          <t>Dynamax Beldum during Max Monday Mon, Sep 29, at 7:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q92" t="inlineStr">
@@ -4688,7 +4700,7 @@
       <c r="O93" t="inlineStr"/>
       <c r="P93" t="inlineStr">
         <is>
-          <t>Mega Kangaskhan and Mega Lopunny in Mega Raids Tue, Sep 30, at 10:00 AM Local Time Ends: Calculating...</t>
+          <t>Raid Battles Mega Kangaskhan and Mega Lopunny in Mega Raids Tue, Sep 30, at 10:00 AM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q93" t="inlineStr">
@@ -4766,7 +4778,7 @@
       <c r="O95" t="inlineStr"/>
       <c r="P95" t="inlineStr">
         <is>
-          <t>Mega Kangaskhan and Mega Lopunny in Mega Raids Tue, Sep 30, at 10:00 AM Local Time</t>
+          <t>Mega Kangaskhan and Mega Lopunny in Mega Raids Tue, Sep 30, at 10:00 AM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q95" t="inlineStr">
@@ -4786,12 +4798,12 @@
       <c r="D96" t="inlineStr"/>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Mega Kangaskhan and Mega Lopunny in Mega Raids</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G96" t="inlineStr"/>
@@ -4805,7 +4817,7 @@
       <c r="O96" t="inlineStr"/>
       <c r="P96" t="inlineStr">
         <is>
-          <t>GO Battle League Great League, Ultra League, and Master League | Tales of Transformation Calculating... Ends: Calculating...</t>
+          <t>Mega Kangaskhan and Mega Lopunny in Mega Raids Tue, Sep 30, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q96" t="inlineStr">
@@ -4844,7 +4856,7 @@
       <c r="O97" t="inlineStr"/>
       <c r="P97" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Ends: Calculating...</t>
+          <t>GO Battle League Great League, Ultra League, and Master League | Tales of Transformation Calculating... Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q97" t="inlineStr">
@@ -4922,7 +4934,7 @@
       <c r="O99" t="inlineStr"/>
       <c r="P99" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating...</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q99" t="inlineStr">
@@ -4942,12 +4954,12 @@
       <c r="D100" t="inlineStr"/>
       <c r="E100" t="inlineStr">
         <is>
-          <t>Aron Spotlight Hour</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G100" t="inlineStr"/>
@@ -4961,7 +4973,7 @@
       <c r="O100" t="inlineStr"/>
       <c r="P100" t="inlineStr">
         <is>
-          <t>Pokémon Spotlight Hour Aron Spotlight Hour Tue, Sep 30, at 7:00 PM Local Time Ends: Calculating...</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q100" t="inlineStr">
@@ -5000,7 +5012,7 @@
       <c r="O101" t="inlineStr"/>
       <c r="P101" t="inlineStr">
         <is>
-          <t>Aron Spotlight Hour Tue, Sep 30, at 7:00 PM Local Time Ends: Calculating...</t>
+          <t>Pokémon Spotlight Hour Aron Spotlight Hour Tue, Sep 30, at 7:00 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q101" t="inlineStr">
@@ -5078,7 +5090,7 @@
       <c r="O103" t="inlineStr"/>
       <c r="P103" t="inlineStr">
         <is>
-          <t>Aron Spotlight Hour Tue, Sep 30, at 7:00 PM Local Time</t>
+          <t>Aron Spotlight Hour Tue, Sep 30, at 7:00 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q103" t="inlineStr">
@@ -5098,12 +5110,12 @@
       <c r="D104" t="inlineStr"/>
       <c r="E104" t="inlineStr">
         <is>
-          <t>Dialga (Origin Forme) Raid Hour</t>
+          <t>Aron Spotlight Hour</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G104" t="inlineStr"/>
@@ -5117,7 +5129,7 @@
       <c r="O104" t="inlineStr"/>
       <c r="P104" t="inlineStr">
         <is>
-          <t>Raid Hour Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 7:00 PM Local Time Ends: Calculating...</t>
+          <t>Aron Spotlight Hour Tue, Sep 30, at 7:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q104" t="inlineStr">
@@ -5156,7 +5168,7 @@
       <c r="O105" t="inlineStr"/>
       <c r="P105" t="inlineStr">
         <is>
-          <t>Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 7:00 PM Local Time Ends: Calculating...</t>
+          <t>Raid Hour Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 7:00 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q105" t="inlineStr">
@@ -5234,7 +5246,7 @@
       <c r="O107" t="inlineStr"/>
       <c r="P107" t="inlineStr">
         <is>
-          <t>Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 7:00 PM Local Time</t>
+          <t>Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 7:00 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q107" t="inlineStr">
@@ -5254,7 +5266,7 @@
       <c r="D108" t="inlineStr"/>
       <c r="E108" t="inlineStr">
         <is>
-          <t>Mega Metagross Raid Day</t>
+          <t>Dialga (Origin Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
@@ -5273,7 +5285,7 @@
       <c r="O108" t="inlineStr"/>
       <c r="P108" t="inlineStr">
         <is>
-          <t>Raid Day Mega Metagross Raid Day Sat, Oct 4, at 5:00 PM Local Time Ends: Calculating...</t>
+          <t>Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 7:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q108" t="inlineStr">
@@ -5312,7 +5324,7 @@
       <c r="O109" t="inlineStr"/>
       <c r="P109" t="inlineStr">
         <is>
-          <t>Mega Metagross Raid Day Sat, Oct 4, at 5:00 PM Local Time Ends: Calculating...</t>
+          <t>Raid Day Mega Metagross Raid Day Sat, Oct 4, at 5:00 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q109" t="inlineStr">
@@ -5390,7 +5402,7 @@
       <c r="O111" t="inlineStr"/>
       <c r="P111" t="inlineStr">
         <is>
-          <t>Mega Metagross Raid Day Sat, Oct 4, at 5:00 PM Local Time</t>
+          <t>Mega Metagross Raid Day Sat, Oct 4, at 5:00 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q111" t="inlineStr">
@@ -5410,12 +5422,12 @@
       <c r="D112" t="inlineStr"/>
       <c r="E112" t="inlineStr">
         <is>
-          <t>GO Pass: September</t>
+          <t>Mega Metagross Raid Day</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G112" t="inlineStr"/>
@@ -5429,7 +5441,7 @@
       <c r="O112" t="inlineStr"/>
       <c r="P112" t="inlineStr">
         <is>
-          <t>GO Pass GO Pass: September Tue, Oct 7, at 10:00 AM Local Time Ends: Calculating...</t>
+          <t>Mega Metagross Raid Day Sat, Oct 4, at 5:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q112" t="inlineStr">
@@ -5468,7 +5480,7 @@
       <c r="O113" t="inlineStr"/>
       <c r="P113" t="inlineStr">
         <is>
-          <t>GO Pass: September Tue, Oct 7, at 10:00 AM Local Time Ends: Calculating...</t>
+          <t>GO Pass GO Pass: September Tue, Oct 7, at 10:00 AM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q113" t="inlineStr">
@@ -5546,7 +5558,7 @@
       <c r="O115" t="inlineStr"/>
       <c r="P115" t="inlineStr">
         <is>
-          <t>GO Pass: September Tue, Oct 7, at 10:00 AM Local Time</t>
+          <t>GO Pass: September Tue, Oct 7, at 10:00 AM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q115" t="inlineStr">
@@ -5566,12 +5578,12 @@
       <c r="D116" t="inlineStr"/>
       <c r="E116" t="inlineStr">
         <is>
-          <t>Dialga in 5-star Raid Battles</t>
+          <t>GO Pass: September</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G116" t="inlineStr"/>
@@ -5585,7 +5597,7 @@
       <c r="O116" t="inlineStr"/>
       <c r="P116" t="inlineStr">
         <is>
-          <t>Raid Battles Dialga in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time Ends: Calculating...</t>
+          <t>GO Pass: September Tue, Oct 7, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q116" t="inlineStr">
@@ -5624,7 +5636,7 @@
       <c r="O117" t="inlineStr"/>
       <c r="P117" t="inlineStr">
         <is>
-          <t>Dialga in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time Ends: Calculating...</t>
+          <t>Raid Battles Dialga in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q117" t="inlineStr">
@@ -5702,7 +5714,7 @@
       <c r="O119" t="inlineStr"/>
       <c r="P119" t="inlineStr">
         <is>
-          <t>Dialga in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time</t>
+          <t>Dialga in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q119" t="inlineStr">
@@ -5722,7 +5734,7 @@
       <c r="D120" t="inlineStr"/>
       <c r="E120" t="inlineStr">
         <is>
-          <t>Mega Steelix, Scizor, and Lucario in Mega Raids</t>
+          <t>Dialga in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
@@ -5741,7 +5753,7 @@
       <c r="O120" t="inlineStr"/>
       <c r="P120" t="inlineStr">
         <is>
-          <t>Raid Battles Mega Steelix, Scizor, and Lucario in Mega Raids Tue, Oct 7, at 10:00 AM Local Time Ends: Calculating...</t>
+          <t>Dialga in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q120" t="inlineStr">
@@ -5780,7 +5792,7 @@
       <c r="O121" t="inlineStr"/>
       <c r="P121" t="inlineStr">
         <is>
-          <t>Mega Steelix, Scizor, and Lucario in Mega Raids Tue, Oct 7, at 10:00 AM Local Time Ends: Calculating...</t>
+          <t>Raid Battles Mega Steelix, Scizor, and Lucario in Mega Raids Tue, Oct 7, at 10:00 AM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q121" t="inlineStr">
@@ -5858,7 +5870,7 @@
       <c r="O123" t="inlineStr"/>
       <c r="P123" t="inlineStr">
         <is>
-          <t>Mega Steelix, Scizor, and Lucario in Mega Raids Tue, Oct 7, at 10:00 AM Local Time</t>
+          <t>Mega Steelix, Scizor, and Lucario in Mega Raids Tue, Oct 7, at 10:00 AM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q123" t="inlineStr">
@@ -5878,12 +5890,12 @@
       <c r="D124" t="inlineStr"/>
       <c r="E124" t="inlineStr">
         <is>
-          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation</t>
+          <t>Mega Steelix, Scizor, and Lucario in Mega Raids</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G124" t="inlineStr"/>
@@ -5897,7 +5909,7 @@
       <c r="O124" t="inlineStr"/>
       <c r="P124" t="inlineStr">
         <is>
-          <t>GO Battle League Great League and Fantasy Cup: Great League Edition | Tales of Transformation Calculating... Ends: Calculating...</t>
+          <t>Mega Steelix, Scizor, and Lucario in Mega Raids Tue, Oct 7, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q124" t="inlineStr">
@@ -5936,7 +5948,7 @@
       <c r="O125" t="inlineStr"/>
       <c r="P125" t="inlineStr">
         <is>
-          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation Calculating... Ends: Calculating...</t>
+          <t>GO Battle League Great League and Fantasy Cup: Great League Edition | Tales of Transformation Calculating... Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q125" t="inlineStr">
@@ -6014,7 +6026,7 @@
       <c r="O127" t="inlineStr"/>
       <c r="P127" t="inlineStr">
         <is>
-          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation Calculating...</t>
+          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation Calculating... Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q127" t="inlineStr">
@@ -6034,7 +6046,7 @@
       <c r="D128" t="inlineStr"/>
       <c r="E128" t="inlineStr">
         <is>
-          <t>Steel Skyline</t>
+          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
@@ -6053,7 +6065,7 @@
       <c r="O128" t="inlineStr"/>
       <c r="P128" t="inlineStr">
         <is>
-          <t>Event Steel Skyline Tue, Oct 7, at 8:00 PM Local Time Ends: Calculating...</t>
+          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q128" t="inlineStr">
@@ -6092,7 +6104,7 @@
       <c r="O129" t="inlineStr"/>
       <c r="P129" t="inlineStr">
         <is>
-          <t>Steel Skyline Tue, Oct 7, at 8:00 PM Local Time Ends: Calculating...</t>
+          <t>Event Steel Skyline Tue, Oct 7, at 8:00 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q129" t="inlineStr">
@@ -6170,7 +6182,7 @@
       <c r="O131" t="inlineStr"/>
       <c r="P131" t="inlineStr">
         <is>
-          <t>Steel Skyline Tue, Oct 7, at 8:00 PM Local Time</t>
+          <t>Steel Skyline Tue, Oct 7, at 8:00 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q131" t="inlineStr">
@@ -6190,12 +6202,12 @@
       <c r="D132" t="inlineStr"/>
       <c r="E132" t="inlineStr">
         <is>
-          <t>Solosis Community Day</t>
+          <t>Steel Skyline</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
         <is>
-          <t>Community Day</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G132" t="inlineStr"/>
@@ -6209,7 +6221,7 @@
       <c r="O132" t="inlineStr"/>
       <c r="P132" t="inlineStr">
         <is>
-          <t>Community Day Solosis Community Day Sun, Oct 12, at 5:00 PM Local Time Ends: Calculating...</t>
+          <t>Steel Skyline Tue, Oct 7, at 8:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q132" t="inlineStr">
@@ -6248,7 +6260,7 @@
       <c r="O133" t="inlineStr"/>
       <c r="P133" t="inlineStr">
         <is>
-          <t>Solosis Community Day Sun, Oct 12, at 5:00 PM Local Time Ends: Calculating...</t>
+          <t>Community Day Solosis Community Day Sun, Oct 12, at 5:00 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q133" t="inlineStr">
@@ -6326,7 +6338,7 @@
       <c r="O135" t="inlineStr"/>
       <c r="P135" t="inlineStr">
         <is>
-          <t>Solosis Community Day Sun, Oct 12, at 5:00 PM Local Time</t>
+          <t>Solosis Community Day Sun, Oct 12, at 5:00 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q135" t="inlineStr">
@@ -6346,12 +6358,12 @@
       <c r="D136" t="inlineStr"/>
       <c r="E136" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
+          <t>Solosis Community Day</t>
         </is>
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Community Day</t>
         </is>
       </c>
       <c r="G136" t="inlineStr"/>
@@ -6365,7 +6377,7 @@
       <c r="O136" t="inlineStr"/>
       <c r="P136" t="inlineStr">
         <is>
-          <t>GO Battle League Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Ends: Calculating...</t>
+          <t>Solosis Community Day Sun, Oct 12, at 5:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q136" t="inlineStr">
@@ -6404,7 +6416,7 @@
       <c r="O137" t="inlineStr"/>
       <c r="P137" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Ends: Calculating...</t>
+          <t>GO Battle League Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q137" t="inlineStr">
@@ -6482,7 +6494,7 @@
       <c r="O139" t="inlineStr"/>
       <c r="P139" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating...</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q139" t="inlineStr">
@@ -6502,7 +6514,7 @@
       <c r="D140" t="inlineStr"/>
       <c r="E140" t="inlineStr">
         <is>
-          <t>XP Celebration</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F140" t="inlineStr">
@@ -6521,7 +6533,7 @@
       <c r="O140" t="inlineStr"/>
       <c r="P140" t="inlineStr">
         <is>
-          <t>Event XP Celebration Tue, Oct 14, at 11:59 PM Local Time Ends: Calculating...</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q140" t="inlineStr">
@@ -6560,7 +6572,7 @@
       <c r="O141" t="inlineStr"/>
       <c r="P141" t="inlineStr">
         <is>
-          <t>XP Celebration Tue, Oct 14, at 11:59 PM Local Time Ends: Calculating...</t>
+          <t>Event XP Celebration Tue, Oct 14, at 11:59 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q141" t="inlineStr">
@@ -6638,7 +6650,7 @@
       <c r="O143" t="inlineStr"/>
       <c r="P143" t="inlineStr">
         <is>
-          <t>XP Celebration Tue, Oct 14, at 11:59 PM Local Time</t>
+          <t>XP Celebration Tue, Oct 14, at 11:59 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q143" t="inlineStr">
@@ -6658,7 +6670,7 @@
       <c r="D144" t="inlineStr"/>
       <c r="E144" t="inlineStr">
         <is>
-          <t>Harvest Festival</t>
+          <t>XP Celebration</t>
         </is>
       </c>
       <c r="F144" t="inlineStr">
@@ -6677,7 +6689,7 @@
       <c r="O144" t="inlineStr"/>
       <c r="P144" t="inlineStr">
         <is>
-          <t>Event Harvest Festival Thu, Oct 16, at 8:00 PM Local Time Ends: Calculating...</t>
+          <t>XP Celebration Tue, Oct 14, at 11:59 PM Local Time</t>
         </is>
       </c>
       <c r="Q144" t="inlineStr">
@@ -6716,7 +6728,7 @@
       <c r="O145" t="inlineStr"/>
       <c r="P145" t="inlineStr">
         <is>
-          <t>Harvest Festival Thu, Oct 16, at 8:00 PM Local Time Ends: Calculating...</t>
+          <t>Event Harvest Festival Thu, Oct 16, at 8:00 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q145" t="inlineStr">
@@ -6794,7 +6806,7 @@
       <c r="O147" t="inlineStr"/>
       <c r="P147" t="inlineStr">
         <is>
-          <t>Harvest Festival Thu, Oct 16, at 8:00 PM Local Time</t>
+          <t>Harvest Festival Thu, Oct 16, at 8:00 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q147" t="inlineStr">
@@ -6814,7 +6826,7 @@
       <c r="D148" t="inlineStr"/>
       <c r="E148" t="inlineStr">
         <is>
-          <t>Master Premier and Great League Remix | Tales of Transformation</t>
+          <t>Harvest Festival</t>
         </is>
       </c>
       <c r="F148" t="inlineStr">
@@ -6833,7 +6845,7 @@
       <c r="O148" t="inlineStr"/>
       <c r="P148" t="inlineStr">
         <is>
-          <t>GO Battle League Master Premier and Great League Remix | Tales of Transformation Calculating... Ends: Calculating...</t>
+          <t>Harvest Festival Thu, Oct 16, at 8:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q148" t="inlineStr">
@@ -6872,7 +6884,7 @@
       <c r="O149" t="inlineStr"/>
       <c r="P149" t="inlineStr">
         <is>
-          <t>Master Premier and Great League Remix | Tales of Transformation Calculating... Ends: Calculating...</t>
+          <t>GO Battle League Master Premier and Great League Remix | Tales of Transformation Calculating... Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q149" t="inlineStr">
@@ -6950,7 +6962,7 @@
       <c r="O151" t="inlineStr"/>
       <c r="P151" t="inlineStr">
         <is>
-          <t>Master Premier and Great League Remix | Tales of Transformation Calculating...</t>
+          <t>Master Premier and Great League Remix | Tales of Transformation Calculating... Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q151" t="inlineStr">
@@ -6970,7 +6982,7 @@
       <c r="D152" t="inlineStr"/>
       <c r="E152" t="inlineStr">
         <is>
-          <t>GO Battle Weekend: Tales of Transformation</t>
+          <t>Master Premier and Great League Remix | Tales of Transformation</t>
         </is>
       </c>
       <c r="F152" t="inlineStr">
@@ -6989,7 +7001,7 @@
       <c r="O152" t="inlineStr"/>
       <c r="P152" t="inlineStr">
         <is>
-          <t>Event GO Battle Weekend: Tales of Transformation Sun, Oct 26, at 11:59 PM Local Time Ends: Calculating...</t>
+          <t>Master Premier and Great League Remix | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q152" t="inlineStr">
@@ -7028,7 +7040,7 @@
       <c r="O153" t="inlineStr"/>
       <c r="P153" t="inlineStr">
         <is>
-          <t>GO Battle Weekend: Tales of Transformation Sun, Oct 26, at 11:59 PM Local Time Ends: Calculating...</t>
+          <t>Event GO Battle Weekend: Tales of Transformation Sun, Oct 26, at 11:59 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q153" t="inlineStr">
@@ -7106,7 +7118,7 @@
       <c r="O155" t="inlineStr"/>
       <c r="P155" t="inlineStr">
         <is>
-          <t>GO Battle Weekend: Tales of Transformation Sun, Oct 26, at 11:59 PM Local Time</t>
+          <t>GO Battle Weekend: Tales of Transformation Sun, Oct 26, at 11:59 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q155" t="inlineStr">
@@ -7126,7 +7138,7 @@
       <c r="D156" t="inlineStr"/>
       <c r="E156" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>GO Battle Weekend: Tales of Transformation</t>
         </is>
       </c>
       <c r="F156" t="inlineStr">
@@ -7145,7 +7157,7 @@
       <c r="O156" t="inlineStr"/>
       <c r="P156" t="inlineStr">
         <is>
-          <t>GO Battle League Great League, Ultra League, and Master League | Tales of Transformation Calculating... Ends: Calculating...</t>
+          <t>GO Battle Weekend: Tales of Transformation Sun, Oct 26, at 11:59 PM Local Time</t>
         </is>
       </c>
       <c r="Q156" t="inlineStr">
@@ -7184,7 +7196,7 @@
       <c r="O157" t="inlineStr"/>
       <c r="P157" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Ends: Calculating...</t>
+          <t>GO Battle League Great League, Ultra League, and Master League | Tales of Transformation Calculating... Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q157" t="inlineStr">
@@ -7262,7 +7274,7 @@
       <c r="O159" t="inlineStr"/>
       <c r="P159" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating...</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q159" t="inlineStr">
@@ -7282,7 +7294,7 @@
       <c r="D160" t="inlineStr"/>
       <c r="E160" t="inlineStr">
         <is>
-          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F160" t="inlineStr">
@@ -7301,7 +7313,7 @@
       <c r="O160" t="inlineStr"/>
       <c r="P160" t="inlineStr">
         <is>
-          <t>GO Battle League Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating... Ends: Calculating...</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q160" t="inlineStr">
@@ -7340,7 +7352,7 @@
       <c r="O161" t="inlineStr"/>
       <c r="P161" t="inlineStr">
         <is>
-          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating... Ends: Calculating...</t>
+          <t>GO Battle League Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating... Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q161" t="inlineStr">
@@ -7418,7 +7430,7 @@
       <c r="O163" t="inlineStr"/>
       <c r="P163" t="inlineStr">
         <is>
-          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating...</t>
+          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating... Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q163" t="inlineStr">
@@ -7438,7 +7450,7 @@
       <c r="D164" t="inlineStr"/>
       <c r="E164" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Nagasaki</t>
+          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F164" t="inlineStr">
@@ -7457,7 +7469,7 @@
       <c r="O164" t="inlineStr"/>
       <c r="P164" t="inlineStr">
         <is>
-          <t>Wild Area Pokémon GO Wild Area: Nagasaki Calculating... Ends: Calculating...</t>
+          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q164" t="inlineStr">
@@ -7496,7 +7508,7 @@
       <c r="O165" t="inlineStr"/>
       <c r="P165" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Nagasaki Calculating... Ends: Calculating...</t>
+          <t>Wild Area Pokémon GO Wild Area: Nagasaki Calculating... Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q165" t="inlineStr">
@@ -7574,7 +7586,7 @@
       <c r="O167" t="inlineStr"/>
       <c r="P167" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Nagasaki Calculating...</t>
+          <t>Pokémon GO Wild Area: Nagasaki Calculating... Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q167" t="inlineStr">
@@ -7594,7 +7606,7 @@
       <c r="D168" t="inlineStr"/>
       <c r="E168" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
+          <t>Pokémon GO Wild Area: Nagasaki</t>
         </is>
       </c>
       <c r="F168" t="inlineStr">
@@ -7613,7 +7625,7 @@
       <c r="O168" t="inlineStr"/>
       <c r="P168" t="inlineStr">
         <is>
-          <t>GO Battle League Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Ends: Calculating...</t>
+          <t>Pokémon GO Wild Area: Nagasaki Calculating...</t>
         </is>
       </c>
       <c r="Q168" t="inlineStr">
@@ -7652,7 +7664,7 @@
       <c r="O169" t="inlineStr"/>
       <c r="P169" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Ends: Calculating...</t>
+          <t>GO Battle League Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q169" t="inlineStr">
@@ -7730,7 +7742,7 @@
       <c r="O171" t="inlineStr"/>
       <c r="P171" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating...</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q171" t="inlineStr">
@@ -7750,7 +7762,7 @@
       <c r="D172" t="inlineStr"/>
       <c r="E172" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Global</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F172" t="inlineStr">
@@ -7769,7 +7781,7 @@
       <c r="O172" t="inlineStr"/>
       <c r="P172" t="inlineStr">
         <is>
-          <t>Wild Area Pokémon GO Wild Area: Global Sun, Nov 16, at 6:00 PM Local Time Ends: Calculating...</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q172" t="inlineStr">
@@ -7808,7 +7820,7 @@
       <c r="O173" t="inlineStr"/>
       <c r="P173" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Global Sun, Nov 16, at 6:00 PM Local Time Ends: Calculating...</t>
+          <t>Wild Area Pokémon GO Wild Area: Global Sun, Nov 16, at 6:00 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q173" t="inlineStr">
@@ -7886,7 +7898,7 @@
       <c r="O175" t="inlineStr"/>
       <c r="P175" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Global Sun, Nov 16, at 6:00 PM Local Time</t>
+          <t>Pokémon GO Wild Area: Global Sun, Nov 16, at 6:00 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q175" t="inlineStr">
@@ -7906,7 +7918,7 @@
       <c r="D176" t="inlineStr"/>
       <c r="E176" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Pokémon GO Wild Area: Global</t>
         </is>
       </c>
       <c r="F176" t="inlineStr">
@@ -7925,7 +7937,7 @@
       <c r="O176" t="inlineStr"/>
       <c r="P176" t="inlineStr">
         <is>
-          <t>GO Battle League Great League, Ultra League, and Master League | Tales of Transformation Calculating... Ends: Calculating...</t>
+          <t>Pokémon GO Wild Area: Global Sun, Nov 16, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q176" t="inlineStr">
@@ -7964,7 +7976,7 @@
       <c r="O177" t="inlineStr"/>
       <c r="P177" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Ends: Calculating...</t>
+          <t>GO Battle League Great League, Ultra League, and Master League | Tales of Transformation Calculating... Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q177" t="inlineStr">
@@ -8042,7 +8054,7 @@
       <c r="O179" t="inlineStr"/>
       <c r="P179" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating...</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q179" t="inlineStr">
@@ -8062,12 +8074,12 @@
       <c r="D180" t="inlineStr"/>
       <c r="E180" t="inlineStr">
         <is>
-          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F180" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G180" t="inlineStr"/>
@@ -8081,7 +8093,7 @@
       <c r="O180" t="inlineStr"/>
       <c r="P180" t="inlineStr">
         <is>
-          <t>GO Battle League 2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating... Ends: Calculating...</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q180" t="inlineStr">
@@ -8120,7 +8132,7 @@
       <c r="O181" t="inlineStr"/>
       <c r="P181" t="inlineStr">
         <is>
-          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating... Ends: Calculating...</t>
+          <t>GO Battle League 2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating... Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q181" t="inlineStr">
@@ -8198,7 +8210,7 @@
       <c r="O183" t="inlineStr"/>
       <c r="P183" t="inlineStr">
         <is>
-          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating...</t>
+          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating... Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q183" t="inlineStr">
@@ -8218,12 +8230,12 @@
       <c r="D184" t="inlineStr"/>
       <c r="E184" t="inlineStr">
         <is>
-          <t>November Community Day</t>
+          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F184" t="inlineStr">
         <is>
-          <t>Community Day</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G184" t="inlineStr"/>
@@ -8237,7 +8249,7 @@
       <c r="O184" t="inlineStr"/>
       <c r="P184" t="inlineStr">
         <is>
-          <t>Community Day November Community Day Sun, Nov 30, at 5:00 PM Local Time Ends: Calculating...</t>
+          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q184" t="inlineStr">
@@ -8276,7 +8288,7 @@
       <c r="O185" t="inlineStr"/>
       <c r="P185" t="inlineStr">
         <is>
-          <t>November Community Day Sun, Nov 30, at 5:00 PM Local Time Ends: Calculating...</t>
+          <t>Community Day November Community Day Sun, Nov 30, at 5:00 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q185" t="inlineStr">
@@ -8354,7 +8366,7 @@
       <c r="O187" t="inlineStr"/>
       <c r="P187" t="inlineStr">
         <is>
-          <t>November Community Day Sun, Nov 30, at 5:00 PM Local Time</t>
+          <t>November Community Day Sun, Nov 30, at 5:00 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q187" t="inlineStr">
@@ -8374,12 +8386,12 @@
       <c r="D188" t="inlineStr"/>
       <c r="E188" t="inlineStr">
         <is>
-          <t>Trade Days | Tales of Transformation</t>
+          <t>November Community Day</t>
         </is>
       </c>
       <c r="F188" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Community Day</t>
         </is>
       </c>
       <c r="G188" t="inlineStr"/>
@@ -8393,7 +8405,7 @@
       <c r="O188" t="inlineStr"/>
       <c r="P188" t="inlineStr">
         <is>
-          <t>Event Trade Days | Tales of Transformation Sun, Nov 30, at 11:59 PM Local Time Ends: Calculating...</t>
+          <t>November Community Day Sun, Nov 30, at 5:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q188" t="inlineStr">
@@ -8432,7 +8444,7 @@
       <c r="O189" t="inlineStr"/>
       <c r="P189" t="inlineStr">
         <is>
-          <t>Trade Days | Tales of Transformation Sun, Nov 30, at 11:59 PM Local Time Ends: Calculating...</t>
+          <t>Event Trade Days | Tales of Transformation Sun, Nov 30, at 11:59 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q189" t="inlineStr">
@@ -8510,7 +8522,7 @@
       <c r="O191" t="inlineStr"/>
       <c r="P191" t="inlineStr">
         <is>
-          <t>Trade Days | Tales of Transformation Sun, Nov 30, at 11:59 PM Local Time</t>
+          <t>Trade Days | Tales of Transformation Sun, Nov 30, at 11:59 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q191" t="inlineStr">
@@ -8530,7 +8542,7 @@
       <c r="D192" t="inlineStr"/>
       <c r="E192" t="inlineStr">
         <is>
-          <t>Tales of Transformation</t>
+          <t>Trade Days | Tales of Transformation</t>
         </is>
       </c>
       <c r="F192" t="inlineStr">
@@ -8549,7 +8561,7 @@
       <c r="O192" t="inlineStr"/>
       <c r="P192" t="inlineStr">
         <is>
-          <t>Season Tales of Transformation Tue, Dec 2, at 10:00 AM Local Time Ends: Calculating...</t>
+          <t>Trade Days | Tales of Transformation Sun, Nov 30, at 11:59 PM Local Time</t>
         </is>
       </c>
       <c r="Q192" t="inlineStr">
@@ -8588,7 +8600,7 @@
       <c r="O193" t="inlineStr"/>
       <c r="P193" t="inlineStr">
         <is>
-          <t>Tales of Transformation Tue, Dec 2, at 10:00 AM Local Time Ends: Calculating...</t>
+          <t>Season Tales of Transformation Tue, Dec 2, at 10:00 AM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q193" t="inlineStr">
@@ -8666,7 +8678,7 @@
       <c r="O195" t="inlineStr"/>
       <c r="P195" t="inlineStr">
         <is>
-          <t>Tales of Transformation Tue, Dec 2, at 10:00 AM Local Time</t>
+          <t>Tales of Transformation Tue, Dec 2, at 10:00 AM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q195" t="inlineStr">
@@ -8686,7 +8698,7 @@
       <c r="D196" t="inlineStr"/>
       <c r="E196" t="inlineStr">
         <is>
-          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Tales of Transformation</t>
         </is>
       </c>
       <c r="F196" t="inlineStr">
@@ -8705,7 +8717,7 @@
       <c r="O196" t="inlineStr"/>
       <c r="P196" t="inlineStr">
         <is>
-          <t>GO Battle League Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating... Ends: Calculating...</t>
+          <t>Tales of Transformation Tue, Dec 2, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q196" t="inlineStr">
@@ -8744,7 +8756,7 @@
       <c r="O197" t="inlineStr"/>
       <c r="P197" t="inlineStr">
         <is>
-          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating... Ends: Calculating...</t>
+          <t>GO Battle League Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating... Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q197" t="inlineStr">
@@ -8822,7 +8834,7 @@
       <c r="O199" t="inlineStr"/>
       <c r="P199" t="inlineStr">
         <is>
-          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating...</t>
+          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating... Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q199" t="inlineStr">
@@ -8842,12 +8854,12 @@
       <c r="D200" t="inlineStr"/>
       <c r="E200" t="inlineStr">
         <is>
-          <t>Dialga (Origin Forme) Raid Hour</t>
+          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F200" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G200" t="inlineStr"/>
@@ -8861,7 +8873,7 @@
       <c r="O200" t="inlineStr"/>
       <c r="P200" t="inlineStr">
         <is>
-          <t>Raid Hour Dialga (Origin Forme) Raid Hour Wed, Sep 24, at 6:00 PM Local Time Starts: Calculating... City Safari Bangkok, Thailand - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating... City Safari Amsterdam, Netherlands - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating... City Safari Valencia, Spain - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating... City Safari Cancún, Mexico - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating... City Safari Vancouver, Canada - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating... Raid Day Mega Camerupt Raid Day Sun, Sep 28, at 2:00 PM Local Time Starts: Calculating... Max Mondays Dynamax Beldum during Max Monday Mon, Sep 29, at 6:00 PM Local Time Starts: Calculating... Raid Battles Mega Steelix, Scizor, and Lucario in Mega Raids Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating... Event Steel Skyline Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating... GO Battle League Great League and Fantasy Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating... Pokémo</t>
+          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q200" t="inlineStr">
@@ -8900,7 +8912,7 @@
       <c r="O201" t="inlineStr"/>
       <c r="P201" t="inlineStr">
         <is>
-          <t>Raid Hour Dialga (Origin Forme) Raid Hour Wed, Sep 24, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Raid Hour Dialga (Origin Forme) Raid Hour Wed, Sep 24, at 6:00 PM Local Time Starts: Calculating... City Safari Bangkok, Thailand - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating... City Safari Amsterdam, Netherlands - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating... City Safari Valencia, Spain - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating... City Safari Cancún, Mexico - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating... City Safari Vancouver, Canada - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating... Raid Day Mega Camerupt Raid Day Sun, Sep 28, at 2:00 PM Local Time Starts: Calculating... Max Mondays Dynamax Beldum during Max Monday Mon, Sep 29, at 6:00 PM Local Time Starts: Calculating... Raid Battles Mega Steelix, Scizor, and Lucario in Mega Raids Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating... Event Steel Skyline Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating... GO Battle League Great League and Fantasy Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating... Pokémo</t>
         </is>
       </c>
       <c r="Q201" t="inlineStr">
@@ -8939,7 +8951,7 @@
       <c r="O202" t="inlineStr"/>
       <c r="P202" t="inlineStr">
         <is>
-          <t>Dialga (Origin Forme) Raid Hour Wed, Sep 24, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Raid Hour Dialga (Origin Forme) Raid Hour Wed, Sep 24, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q202" t="inlineStr">
@@ -9017,7 +9029,7 @@
       <c r="O204" t="inlineStr"/>
       <c r="P204" t="inlineStr">
         <is>
-          <t>Dialga (Origin Forme) Raid Hour Wed, Sep 24, at 6:00 PM Local Time</t>
+          <t>Dialga (Origin Forme) Raid Hour Wed, Sep 24, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q204" t="inlineStr">
@@ -9037,12 +9049,12 @@
       <c r="D205" t="inlineStr"/>
       <c r="E205" t="inlineStr">
         <is>
-          <t>Bangkok, Thailand - Pokémon GO City Safari</t>
+          <t>Dialga (Origin Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F205" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G205" t="inlineStr"/>
@@ -9056,7 +9068,7 @@
       <c r="O205" t="inlineStr"/>
       <c r="P205" t="inlineStr">
         <is>
-          <t>City Safari Bangkok, Thailand - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Dialga (Origin Forme) Raid Hour Wed, Sep 24, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q205" t="inlineStr">
@@ -9095,7 +9107,7 @@
       <c r="O206" t="inlineStr"/>
       <c r="P206" t="inlineStr">
         <is>
-          <t>Bangkok, Thailand - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>City Safari Bangkok, Thailand - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q206" t="inlineStr">
@@ -9173,7 +9185,7 @@
       <c r="O208" t="inlineStr"/>
       <c r="P208" t="inlineStr">
         <is>
-          <t>Bangkok, Thailand - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time</t>
+          <t>Bangkok, Thailand - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q208" t="inlineStr">
@@ -9193,7 +9205,7 @@
       <c r="D209" t="inlineStr"/>
       <c r="E209" t="inlineStr">
         <is>
-          <t>Amsterdam, Netherlands - Pokémon GO City Safari</t>
+          <t>Bangkok, Thailand - Pokémon GO City Safari</t>
         </is>
       </c>
       <c r="F209" t="inlineStr">
@@ -9212,7 +9224,7 @@
       <c r="O209" t="inlineStr"/>
       <c r="P209" t="inlineStr">
         <is>
-          <t>City Safari Amsterdam, Netherlands - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Bangkok, Thailand - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q209" t="inlineStr">
@@ -9251,7 +9263,7 @@
       <c r="O210" t="inlineStr"/>
       <c r="P210" t="inlineStr">
         <is>
-          <t>Amsterdam, Netherlands - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>City Safari Amsterdam, Netherlands - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q210" t="inlineStr">
@@ -9329,7 +9341,7 @@
       <c r="O212" t="inlineStr"/>
       <c r="P212" t="inlineStr">
         <is>
-          <t>Amsterdam, Netherlands - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time</t>
+          <t>Amsterdam, Netherlands - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q212" t="inlineStr">
@@ -9349,7 +9361,7 @@
       <c r="D213" t="inlineStr"/>
       <c r="E213" t="inlineStr">
         <is>
-          <t>Valencia, Spain - Pokémon GO City Safari</t>
+          <t>Amsterdam, Netherlands - Pokémon GO City Safari</t>
         </is>
       </c>
       <c r="F213" t="inlineStr">
@@ -9368,7 +9380,7 @@
       <c r="O213" t="inlineStr"/>
       <c r="P213" t="inlineStr">
         <is>
-          <t>City Safari Valencia, Spain - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Amsterdam, Netherlands - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q213" t="inlineStr">
@@ -9407,7 +9419,7 @@
       <c r="O214" t="inlineStr"/>
       <c r="P214" t="inlineStr">
         <is>
-          <t>Valencia, Spain - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>City Safari Valencia, Spain - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q214" t="inlineStr">
@@ -9485,7 +9497,7 @@
       <c r="O216" t="inlineStr"/>
       <c r="P216" t="inlineStr">
         <is>
-          <t>Valencia, Spain - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time</t>
+          <t>Valencia, Spain - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q216" t="inlineStr">
@@ -9505,7 +9517,7 @@
       <c r="D217" t="inlineStr"/>
       <c r="E217" t="inlineStr">
         <is>
-          <t>Cancún, Mexico - Pokémon GO City Safari</t>
+          <t>Valencia, Spain - Pokémon GO City Safari</t>
         </is>
       </c>
       <c r="F217" t="inlineStr">
@@ -9524,7 +9536,7 @@
       <c r="O217" t="inlineStr"/>
       <c r="P217" t="inlineStr">
         <is>
-          <t>City Safari Cancún, Mexico - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Valencia, Spain - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q217" t="inlineStr">
@@ -9563,7 +9575,7 @@
       <c r="O218" t="inlineStr"/>
       <c r="P218" t="inlineStr">
         <is>
-          <t>Cancún, Mexico - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>City Safari Cancún, Mexico - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q218" t="inlineStr">
@@ -9641,7 +9653,7 @@
       <c r="O220" t="inlineStr"/>
       <c r="P220" t="inlineStr">
         <is>
-          <t>Cancún, Mexico - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time</t>
+          <t>Cancún, Mexico - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q220" t="inlineStr">
@@ -9661,7 +9673,7 @@
       <c r="D221" t="inlineStr"/>
       <c r="E221" t="inlineStr">
         <is>
-          <t>Vancouver, Canada - Pokémon GO City Safari</t>
+          <t>Cancún, Mexico - Pokémon GO City Safari</t>
         </is>
       </c>
       <c r="F221" t="inlineStr">
@@ -9680,7 +9692,7 @@
       <c r="O221" t="inlineStr"/>
       <c r="P221" t="inlineStr">
         <is>
-          <t>City Safari Vancouver, Canada - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Cancún, Mexico - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q221" t="inlineStr">
@@ -9719,7 +9731,7 @@
       <c r="O222" t="inlineStr"/>
       <c r="P222" t="inlineStr">
         <is>
-          <t>Vancouver, Canada - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>City Safari Vancouver, Canada - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q222" t="inlineStr">
@@ -9797,7 +9809,7 @@
       <c r="O224" t="inlineStr"/>
       <c r="P224" t="inlineStr">
         <is>
-          <t>Vancouver, Canada - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time</t>
+          <t>Vancouver, Canada - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q224" t="inlineStr">
@@ -9817,12 +9829,12 @@
       <c r="D225" t="inlineStr"/>
       <c r="E225" t="inlineStr">
         <is>
-          <t>Mega Camerupt Raid Day</t>
+          <t>Vancouver, Canada - Pokémon GO City Safari</t>
         </is>
       </c>
       <c r="F225" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G225" t="inlineStr"/>
@@ -9836,7 +9848,7 @@
       <c r="O225" t="inlineStr"/>
       <c r="P225" t="inlineStr">
         <is>
-          <t>Raid Day Mega Camerupt Raid Day Sun, Sep 28, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Vancouver, Canada - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q225" t="inlineStr">
@@ -9875,7 +9887,7 @@
       <c r="O226" t="inlineStr"/>
       <c r="P226" t="inlineStr">
         <is>
-          <t>Mega Camerupt Raid Day Sun, Sep 28, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Raid Day Mega Camerupt Raid Day Sun, Sep 28, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q226" t="inlineStr">
@@ -9953,7 +9965,7 @@
       <c r="O228" t="inlineStr"/>
       <c r="P228" t="inlineStr">
         <is>
-          <t>Mega Camerupt Raid Day Sun, Sep 28, at 2:00 PM Local Time</t>
+          <t>Mega Camerupt Raid Day Sun, Sep 28, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q228" t="inlineStr">
@@ -9973,12 +9985,12 @@
       <c r="D229" t="inlineStr"/>
       <c r="E229" t="inlineStr">
         <is>
-          <t>Dynamax Beldum during Max Monday</t>
+          <t>Mega Camerupt Raid Day</t>
         </is>
       </c>
       <c r="F229" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G229" t="inlineStr"/>
@@ -9992,7 +10004,7 @@
       <c r="O229" t="inlineStr"/>
       <c r="P229" t="inlineStr">
         <is>
-          <t>Max Mondays Dynamax Beldum during Max Monday Mon, Sep 29, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Mega Camerupt Raid Day Sun, Sep 28, at 2:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q229" t="inlineStr">
@@ -10031,7 +10043,7 @@
       <c r="O230" t="inlineStr"/>
       <c r="P230" t="inlineStr">
         <is>
-          <t>Dynamax Beldum during Max Monday Mon, Sep 29, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Max Mondays Dynamax Beldum during Max Monday Mon, Sep 29, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q230" t="inlineStr">
@@ -10109,7 +10121,7 @@
       <c r="O232" t="inlineStr"/>
       <c r="P232" t="inlineStr">
         <is>
-          <t>Dynamax Beldum during Max Monday Mon, Sep 29, at 6:00 PM Local Time</t>
+          <t>Dynamax Beldum during Max Monday Mon, Sep 29, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q232" t="inlineStr">
@@ -10129,12 +10141,12 @@
       <c r="D233" t="inlineStr"/>
       <c r="E233" t="inlineStr">
         <is>
-          <t>Mega Steelix, Scizor, and Lucario in Mega Raids</t>
+          <t>Dynamax Beldum during Max Monday</t>
         </is>
       </c>
       <c r="F233" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G233" t="inlineStr"/>
@@ -10148,7 +10160,7 @@
       <c r="O233" t="inlineStr"/>
       <c r="P233" t="inlineStr">
         <is>
-          <t>Raid Battles Mega Steelix, Scizor, and Lucario in Mega Raids Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Dynamax Beldum during Max Monday Mon, Sep 29, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q233" t="inlineStr">
@@ -10187,7 +10199,7 @@
       <c r="O234" t="inlineStr"/>
       <c r="P234" t="inlineStr">
         <is>
-          <t>Mega Steelix, Scizor, and Lucario in Mega Raids Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Raid Battles Mega Steelix, Scizor, and Lucario in Mega Raids Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q234" t="inlineStr">
@@ -10265,7 +10277,7 @@
       <c r="O236" t="inlineStr"/>
       <c r="P236" t="inlineStr">
         <is>
-          <t>Mega Steelix, Scizor, and Lucario in Mega Raids Tue, Sep 30, at 10:00 AM Local Time</t>
+          <t>Mega Steelix, Scizor, and Lucario in Mega Raids Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q236" t="inlineStr">
@@ -10285,12 +10297,12 @@
       <c r="D237" t="inlineStr"/>
       <c r="E237" t="inlineStr">
         <is>
-          <t>Steel Skyline</t>
+          <t>Mega Steelix, Scizor, and Lucario in Mega Raids</t>
         </is>
       </c>
       <c r="F237" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G237" t="inlineStr"/>
@@ -10304,7 +10316,7 @@
       <c r="O237" t="inlineStr"/>
       <c r="P237" t="inlineStr">
         <is>
-          <t>Event Steel Skyline Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Mega Steelix, Scizor, and Lucario in Mega Raids Tue, Sep 30, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q237" t="inlineStr">
@@ -10343,7 +10355,7 @@
       <c r="O238" t="inlineStr"/>
       <c r="P238" t="inlineStr">
         <is>
-          <t>Steel Skyline Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Event Steel Skyline Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q238" t="inlineStr">
@@ -10421,7 +10433,7 @@
       <c r="O240" t="inlineStr"/>
       <c r="P240" t="inlineStr">
         <is>
-          <t>Steel Skyline Tue, Sep 30, at 10:00 AM Local Time</t>
+          <t>Steel Skyline Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q240" t="inlineStr">
@@ -10441,7 +10453,7 @@
       <c r="D241" t="inlineStr"/>
       <c r="E241" t="inlineStr">
         <is>
-          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation</t>
+          <t>Steel Skyline</t>
         </is>
       </c>
       <c r="F241" t="inlineStr">
@@ -10460,7 +10472,7 @@
       <c r="O241" t="inlineStr"/>
       <c r="P241" t="inlineStr">
         <is>
-          <t>GO Battle League Great League and Fantasy Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Steel Skyline Tue, Sep 30, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q241" t="inlineStr">
@@ -10499,7 +10511,7 @@
       <c r="O242" t="inlineStr"/>
       <c r="P242" t="inlineStr">
         <is>
-          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>GO Battle League Great League and Fantasy Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q242" t="inlineStr">
@@ -10577,7 +10589,7 @@
       <c r="O244" t="inlineStr"/>
       <c r="P244" t="inlineStr">
         <is>
-          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation Calculating...</t>
+          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q244" t="inlineStr">
@@ -10597,12 +10609,12 @@
       <c r="D245" t="inlineStr"/>
       <c r="E245" t="inlineStr">
         <is>
-          <t>Aron Spotlight Hour</t>
+          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F245" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G245" t="inlineStr"/>
@@ -10616,7 +10628,7 @@
       <c r="O245" t="inlineStr"/>
       <c r="P245" t="inlineStr">
         <is>
-          <t>Pokémon Spotlight Hour Aron Spotlight Hour Tue, Sep 30, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q245" t="inlineStr">
@@ -10655,7 +10667,7 @@
       <c r="O246" t="inlineStr"/>
       <c r="P246" t="inlineStr">
         <is>
-          <t>Aron Spotlight Hour Tue, Sep 30, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Pokémon Spotlight Hour Aron Spotlight Hour Tue, Sep 30, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q246" t="inlineStr">
@@ -10733,7 +10745,7 @@
       <c r="O248" t="inlineStr"/>
       <c r="P248" t="inlineStr">
         <is>
-          <t>Aron Spotlight Hour Tue, Sep 30, at 6:00 PM Local Time</t>
+          <t>Aron Spotlight Hour Tue, Sep 30, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q248" t="inlineStr">
@@ -10753,12 +10765,12 @@
       <c r="D249" t="inlineStr"/>
       <c r="E249" t="inlineStr">
         <is>
-          <t>Dialga (Origin Forme) Raid Hour</t>
+          <t>Aron Spotlight Hour</t>
         </is>
       </c>
       <c r="F249" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G249" t="inlineStr"/>
@@ -10772,7 +10784,7 @@
       <c r="O249" t="inlineStr"/>
       <c r="P249" t="inlineStr">
         <is>
-          <t>Raid Hour Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Aron Spotlight Hour Tue, Sep 30, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q249" t="inlineStr">
@@ -10811,7 +10823,7 @@
       <c r="O250" t="inlineStr"/>
       <c r="P250" t="inlineStr">
         <is>
-          <t>Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Raid Hour Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q250" t="inlineStr">
@@ -10889,7 +10901,7 @@
       <c r="O252" t="inlineStr"/>
       <c r="P252" t="inlineStr">
         <is>
-          <t>Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 6:00 PM Local Time</t>
+          <t>Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q252" t="inlineStr">
@@ -10909,7 +10921,7 @@
       <c r="D253" t="inlineStr"/>
       <c r="E253" t="inlineStr">
         <is>
-          <t>Mega Metagross Raid Day</t>
+          <t>Dialga (Origin Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F253" t="inlineStr">
@@ -10928,7 +10940,7 @@
       <c r="O253" t="inlineStr"/>
       <c r="P253" t="inlineStr">
         <is>
-          <t>Raid Day Mega Metagross Raid Day Sat, Oct 4, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q253" t="inlineStr">
@@ -10967,7 +10979,7 @@
       <c r="O254" t="inlineStr"/>
       <c r="P254" t="inlineStr">
         <is>
-          <t>Mega Metagross Raid Day Sat, Oct 4, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Raid Day Mega Metagross Raid Day Sat, Oct 4, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q254" t="inlineStr">
@@ -11045,7 +11057,7 @@
       <c r="O256" t="inlineStr"/>
       <c r="P256" t="inlineStr">
         <is>
-          <t>Mega Metagross Raid Day Sat, Oct 4, at 2:00 PM Local Time</t>
+          <t>Mega Metagross Raid Day Sat, Oct 4, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q256" t="inlineStr">
@@ -11065,12 +11077,12 @@
       <c r="D257" t="inlineStr"/>
       <c r="E257" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
+          <t>Mega Metagross Raid Day</t>
         </is>
       </c>
       <c r="F257" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G257" t="inlineStr"/>
@@ -11084,7 +11096,7 @@
       <c r="O257" t="inlineStr"/>
       <c r="P257" t="inlineStr">
         <is>
-          <t>GO Battle League Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Mega Metagross Raid Day Sat, Oct 4, at 2:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q257" t="inlineStr">
@@ -11123,7 +11135,7 @@
       <c r="O258" t="inlineStr"/>
       <c r="P258" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>GO Battle League Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q258" t="inlineStr">
@@ -11201,7 +11213,7 @@
       <c r="O260" t="inlineStr"/>
       <c r="P260" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating...</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q260" t="inlineStr">
@@ -11221,7 +11233,7 @@
       <c r="D261" t="inlineStr"/>
       <c r="E261" t="inlineStr">
         <is>
-          <t>Harvest Festival</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F261" t="inlineStr">
@@ -11240,7 +11252,7 @@
       <c r="O261" t="inlineStr"/>
       <c r="P261" t="inlineStr">
         <is>
-          <t>Event Harvest Festival Fri, Oct 10, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q261" t="inlineStr">
@@ -11279,7 +11291,7 @@
       <c r="O262" t="inlineStr"/>
       <c r="P262" t="inlineStr">
         <is>
-          <t>Harvest Festival Fri, Oct 10, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Event Harvest Festival Fri, Oct 10, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q262" t="inlineStr">
@@ -11357,7 +11369,7 @@
       <c r="O264" t="inlineStr"/>
       <c r="P264" t="inlineStr">
         <is>
-          <t>Harvest Festival Fri, Oct 10, at 10:00 AM Local Time</t>
+          <t>Harvest Festival Fri, Oct 10, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q264" t="inlineStr">
@@ -11377,12 +11389,12 @@
       <c r="D265" t="inlineStr"/>
       <c r="E265" t="inlineStr">
         <is>
-          <t>Solosis Community Day</t>
+          <t>Harvest Festival</t>
         </is>
       </c>
       <c r="F265" t="inlineStr">
         <is>
-          <t>Community Day</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G265" t="inlineStr"/>
@@ -11396,7 +11408,7 @@
       <c r="O265" t="inlineStr"/>
       <c r="P265" t="inlineStr">
         <is>
-          <t>Community Day Solosis Community Day Sun, Oct 12, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Harvest Festival Fri, Oct 10, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q265" t="inlineStr">
@@ -11435,7 +11447,7 @@
       <c r="O266" t="inlineStr"/>
       <c r="P266" t="inlineStr">
         <is>
-          <t>Solosis Community Day Sun, Oct 12, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Community Day Solosis Community Day Sun, Oct 12, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q266" t="inlineStr">
@@ -11513,7 +11525,7 @@
       <c r="O268" t="inlineStr"/>
       <c r="P268" t="inlineStr">
         <is>
-          <t>Solosis Community Day Sun, Oct 12, at 2:00 PM Local Time</t>
+          <t>Solosis Community Day Sun, Oct 12, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q268" t="inlineStr">
@@ -11533,12 +11545,12 @@
       <c r="D269" t="inlineStr"/>
       <c r="E269" t="inlineStr">
         <is>
-          <t>Master Premier and Great League Remix | Tales of Transformation</t>
+          <t>Solosis Community Day</t>
         </is>
       </c>
       <c r="F269" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Community Day</t>
         </is>
       </c>
       <c r="G269" t="inlineStr"/>
@@ -11552,7 +11564,7 @@
       <c r="O269" t="inlineStr"/>
       <c r="P269" t="inlineStr">
         <is>
-          <t>GO Battle League Master Premier and Great League Remix | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Solosis Community Day Sun, Oct 12, at 2:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q269" t="inlineStr">
@@ -11591,7 +11603,7 @@
       <c r="O270" t="inlineStr"/>
       <c r="P270" t="inlineStr">
         <is>
-          <t>Master Premier and Great League Remix | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>GO Battle League Master Premier and Great League Remix | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q270" t="inlineStr">
@@ -11669,7 +11681,7 @@
       <c r="O272" t="inlineStr"/>
       <c r="P272" t="inlineStr">
         <is>
-          <t>Master Premier and Great League Remix | Tales of Transformation Calculating...</t>
+          <t>Master Premier and Great League Remix | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q272" t="inlineStr">
@@ -11689,7 +11701,7 @@
       <c r="D273" t="inlineStr"/>
       <c r="E273" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Master Premier and Great League Remix | Tales of Transformation</t>
         </is>
       </c>
       <c r="F273" t="inlineStr">
@@ -11708,7 +11720,7 @@
       <c r="O273" t="inlineStr"/>
       <c r="P273" t="inlineStr">
         <is>
-          <t>GO Battle League Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Master Premier and Great League Remix | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q273" t="inlineStr">
@@ -11747,7 +11759,7 @@
       <c r="O274" t="inlineStr"/>
       <c r="P274" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>GO Battle League Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q274" t="inlineStr">
@@ -11825,7 +11837,7 @@
       <c r="O276" t="inlineStr"/>
       <c r="P276" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating...</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q276" t="inlineStr">
@@ -11845,7 +11857,7 @@
       <c r="D277" t="inlineStr"/>
       <c r="E277" t="inlineStr">
         <is>
-          <t>GO Battle Weekend: Tales of Transformation</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F277" t="inlineStr">
@@ -11864,7 +11876,7 @@
       <c r="O277" t="inlineStr"/>
       <c r="P277" t="inlineStr">
         <is>
-          <t>Event GO Battle Weekend: Tales of Transformation Sat, Oct 25, at 12:00 AM Local Time Starts: Calculating...</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q277" t="inlineStr">
@@ -11903,7 +11915,7 @@
       <c r="O278" t="inlineStr"/>
       <c r="P278" t="inlineStr">
         <is>
-          <t>GO Battle Weekend: Tales of Transformation Sat, Oct 25, at 12:00 AM Local Time Starts: Calculating...</t>
+          <t>Event GO Battle Weekend: Tales of Transformation Sat, Oct 25, at 12:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q278" t="inlineStr">
@@ -11981,7 +11993,7 @@
       <c r="O280" t="inlineStr"/>
       <c r="P280" t="inlineStr">
         <is>
-          <t>GO Battle Weekend: Tales of Transformation Sat, Oct 25, at 12:00 AM Local Time</t>
+          <t>GO Battle Weekend: Tales of Transformation Sat, Oct 25, at 12:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q280" t="inlineStr">
@@ -12001,7 +12013,7 @@
       <c r="D281" t="inlineStr"/>
       <c r="E281" t="inlineStr">
         <is>
-          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation</t>
+          <t>GO Battle Weekend: Tales of Transformation</t>
         </is>
       </c>
       <c r="F281" t="inlineStr">
@@ -12020,7 +12032,7 @@
       <c r="O281" t="inlineStr"/>
       <c r="P281" t="inlineStr">
         <is>
-          <t>GO Battle League Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>GO Battle Weekend: Tales of Transformation Sat, Oct 25, at 12:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q281" t="inlineStr">
@@ -12059,7 +12071,7 @@
       <c r="O282" t="inlineStr"/>
       <c r="P282" t="inlineStr">
         <is>
-          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>GO Battle League Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q282" t="inlineStr">
@@ -12137,7 +12149,7 @@
       <c r="O284" t="inlineStr"/>
       <c r="P284" t="inlineStr">
         <is>
-          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating...</t>
+          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q284" t="inlineStr">
@@ -12157,7 +12169,7 @@
       <c r="D285" t="inlineStr"/>
       <c r="E285" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
+          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F285" t="inlineStr">
@@ -12176,7 +12188,7 @@
       <c r="O285" t="inlineStr"/>
       <c r="P285" t="inlineStr">
         <is>
-          <t>GO Battle League Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q285" t="inlineStr">
@@ -12215,7 +12227,7 @@
       <c r="O286" t="inlineStr"/>
       <c r="P286" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>GO Battle League Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q286" t="inlineStr">
@@ -12293,7 +12305,7 @@
       <c r="O288" t="inlineStr"/>
       <c r="P288" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating...</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q288" t="inlineStr">
@@ -12313,7 +12325,7 @@
       <c r="D289" t="inlineStr"/>
       <c r="E289" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Nagasaki</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F289" t="inlineStr">
@@ -12332,7 +12344,7 @@
       <c r="O289" t="inlineStr"/>
       <c r="P289" t="inlineStr">
         <is>
-          <t>Wild Area Pokémon GO Wild Area: Nagasaki Calculating... Starts: Calculating...</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q289" t="inlineStr">
@@ -12371,7 +12383,7 @@
       <c r="O290" t="inlineStr"/>
       <c r="P290" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Nagasaki Calculating... Starts: Calculating...</t>
+          <t>Wild Area Pokémon GO Wild Area: Nagasaki Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q290" t="inlineStr">
@@ -12449,7 +12461,7 @@
       <c r="O292" t="inlineStr"/>
       <c r="P292" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Nagasaki Calculating...</t>
+          <t>Pokémon GO Wild Area: Nagasaki Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q292" t="inlineStr">
@@ -12469,7 +12481,7 @@
       <c r="D293" t="inlineStr"/>
       <c r="E293" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Pokémon GO Wild Area: Nagasaki</t>
         </is>
       </c>
       <c r="F293" t="inlineStr">
@@ -12488,7 +12500,7 @@
       <c r="O293" t="inlineStr"/>
       <c r="P293" t="inlineStr">
         <is>
-          <t>GO Battle League Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Pokémon GO Wild Area: Nagasaki Calculating...</t>
         </is>
       </c>
       <c r="Q293" t="inlineStr">
@@ -12527,7 +12539,7 @@
       <c r="O294" t="inlineStr"/>
       <c r="P294" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>GO Battle League Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q294" t="inlineStr">
@@ -12605,7 +12617,7 @@
       <c r="O296" t="inlineStr"/>
       <c r="P296" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating...</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q296" t="inlineStr">
@@ -12625,7 +12637,7 @@
       <c r="D297" t="inlineStr"/>
       <c r="E297" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Global</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F297" t="inlineStr">
@@ -12644,7 +12656,7 @@
       <c r="O297" t="inlineStr"/>
       <c r="P297" t="inlineStr">
         <is>
-          <t>Wild Area Pokémon GO Wild Area: Global Sat, Nov 15, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q297" t="inlineStr">
@@ -12683,7 +12695,7 @@
       <c r="O298" t="inlineStr"/>
       <c r="P298" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Global Sat, Nov 15, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Wild Area Pokémon GO Wild Area: Global Sat, Nov 15, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q298" t="inlineStr">
@@ -12761,7 +12773,7 @@
       <c r="O300" t="inlineStr"/>
       <c r="P300" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Global Sat, Nov 15, at 10:00 AM Local Time</t>
+          <t>Pokémon GO Wild Area: Global Sat, Nov 15, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q300" t="inlineStr">
@@ -12781,12 +12793,12 @@
       <c r="D301" t="inlineStr"/>
       <c r="E301" t="inlineStr">
         <is>
-          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation</t>
+          <t>Pokémon GO Wild Area: Global</t>
         </is>
       </c>
       <c r="F301" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G301" t="inlineStr"/>
@@ -12800,7 +12812,7 @@
       <c r="O301" t="inlineStr"/>
       <c r="P301" t="inlineStr">
         <is>
-          <t>GO Battle League 2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Pokémon GO Wild Area: Global Sat, Nov 15, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q301" t="inlineStr">
@@ -12839,7 +12851,7 @@
       <c r="O302" t="inlineStr"/>
       <c r="P302" t="inlineStr">
         <is>
-          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>GO Battle League 2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q302" t="inlineStr">
@@ -12917,7 +12929,7 @@
       <c r="O304" t="inlineStr"/>
       <c r="P304" t="inlineStr">
         <is>
-          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating...</t>
+          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q304" t="inlineStr">
@@ -12937,12 +12949,12 @@
       <c r="D305" t="inlineStr"/>
       <c r="E305" t="inlineStr">
         <is>
-          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation</t>
+          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F305" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G305" t="inlineStr"/>
@@ -12956,7 +12968,7 @@
       <c r="O305" t="inlineStr"/>
       <c r="P305" t="inlineStr">
         <is>
-          <t>GO Battle League Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q305" t="inlineStr">
@@ -12995,7 +13007,7 @@
       <c r="O306" t="inlineStr"/>
       <c r="P306" t="inlineStr">
         <is>
-          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>GO Battle League Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q306" t="inlineStr">
@@ -13073,7 +13085,7 @@
       <c r="O308" t="inlineStr"/>
       <c r="P308" t="inlineStr">
         <is>
-          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating...</t>
+          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q308" t="inlineStr">
@@ -13093,12 +13105,12 @@
       <c r="D309" t="inlineStr"/>
       <c r="E309" t="inlineStr">
         <is>
-          <t>November Community Day</t>
+          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F309" t="inlineStr">
         <is>
-          <t>Community Day</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G309" t="inlineStr"/>
@@ -13112,7 +13124,7 @@
       <c r="O309" t="inlineStr"/>
       <c r="P309" t="inlineStr">
         <is>
-          <t>Community Day November Community Day Sun, Nov 30, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q309" t="inlineStr">
@@ -13151,7 +13163,7 @@
       <c r="O310" t="inlineStr"/>
       <c r="P310" t="inlineStr">
         <is>
-          <t>November Community Day Sun, Nov 30, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Community Day November Community Day Sun, Nov 30, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q310" t="inlineStr">
@@ -13229,7 +13241,7 @@
       <c r="O312" t="inlineStr"/>
       <c r="P312" t="inlineStr">
         <is>
-          <t>November Community Day Sun, Nov 30, at 2:00 PM Local Time</t>
+          <t>November Community Day Sun, Nov 30, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q312" t="inlineStr">
@@ -13249,12 +13261,12 @@
       <c r="D313" t="inlineStr"/>
       <c r="E313" t="inlineStr">
         <is>
-          <t>Raid NOW</t>
+          <t>November Community Day</t>
         </is>
       </c>
       <c r="F313" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Community Day</t>
         </is>
       </c>
       <c r="G313" t="inlineStr"/>
@@ -13268,12 +13280,12 @@
       <c r="O313" t="inlineStr"/>
       <c r="P313" t="inlineStr">
         <is>
-          <t>Raid NOW From Leek Duck | Powered by GO FRIEND General Information It has been reported that the registration information (Trainer Name, Trainer Level, Trainer Code) is incorrect. Please check again. HOST HOST Auto join Raids you are joining (Latest 2) MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rpl_maxuser'] }} {{ val1['cnt'] }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} No.{{ val1['rpl_id'] }} No.{{ val1['rpl_id'] }} TL{{ val1['rpl_level'] }} {{ val1['rpl_glevel'] }} {{ ((val1['rpl_gescore'] == -1)?0:val1['rpl_gescore']) }} {{ aryPokemon[value]['raidbbs_short_name_en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} FULL Host TL 5 30 35 40 45 Host Rating - 0 {{ i }} MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['ti</t>
+          <t>November Community Day Sun, Nov 30, at 2:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q313" t="inlineStr">
         <is>
-          <t>2024-06-01_raid-now.html</t>
+          <t>2024-06-01_events.html</t>
         </is>
       </c>
     </row>
@@ -13288,7 +13300,7 @@
       <c r="D314" t="inlineStr"/>
       <c r="E314" t="inlineStr">
         <is>
-          <t>Raids you are joining (Latest 2)</t>
+          <t>Raid NOW</t>
         </is>
       </c>
       <c r="F314" t="inlineStr">
@@ -13307,7 +13319,7 @@
       <c r="O314" t="inlineStr"/>
       <c r="P314" t="inlineStr">
         <is>
-          <t>General Information It has been reported that the registration information (Trainer Name, Trainer Level, Trainer Code) is incorrect. Please check again. HOST HOST Auto join Raids you are joining (Latest 2) MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rpl_maxuser'] }} {{ val1['cnt'] }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} No.{{ val1['rpl_id'] }} No.{{ val1['rpl_id'] }} TL{{ val1['rpl_level'] }} {{ val1['rpl_glevel'] }} {{ ((val1['rpl_gescore'] == -1)?0:val1['rpl_gescore']) }} {{ aryPokemon[value]['raidbbs_short_name_en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} FULL Host TL 5 30 35 40 45 Host Rating - 0 {{ i }} MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rp</t>
+          <t>Raid NOW From Leek Duck | Powered by GO FRIEND General Information It has been reported that the registration information (Trainer Name, Trainer Level, Trainer Code) is incorrect. Please check again. HOST HOST Auto join Raids you are joining (Latest 2) MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rpl_maxuser'] }} {{ val1['cnt'] }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} No.{{ val1['rpl_id'] }} No.{{ val1['rpl_id'] }} TL{{ val1['rpl_level'] }} {{ val1['rpl_glevel'] }} {{ ((val1['rpl_gescore'] == -1)?0:val1['rpl_gescore']) }} {{ aryPokemon[value]['raidbbs_short_name_en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} FULL Host TL 5 30 35 40 45 Host Rating - 0 {{ i }} MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['ti</t>
         </is>
       </c>
       <c r="Q314" t="inlineStr">
@@ -13346,7 +13358,7 @@
       <c r="O315" t="inlineStr"/>
       <c r="P315" t="inlineStr">
         <is>
-          <t>Raids you are joining (Latest 2) MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rpl_maxuser'] }} {{ val1['cnt'] }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} No.{{ val1['rpl_id'] }} No.{{ val1['rpl_id'] }} TL{{ val1['rpl_level'] }} {{ val1['rpl_glevel'] }} {{ ((val1['rpl_gescore'] == -1)?0:val1['rpl_gescore']) }}</t>
+          <t>General Information It has been reported that the registration information (Trainer Name, Trainer Level, Trainer Code) is incorrect. Please check again. HOST HOST Auto join Raids you are joining (Latest 2) MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rpl_maxuser'] }} {{ val1['cnt'] }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} No.{{ val1['rpl_id'] }} No.{{ val1['rpl_id'] }} TL{{ val1['rpl_level'] }} {{ val1['rpl_glevel'] }} {{ ((val1['rpl_gescore'] == -1)?0:val1['rpl_gescore']) }} {{ aryPokemon[value]['raidbbs_short_name_en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} FULL Host TL 5 30 35 40 45 Host Rating - 0 {{ i }} MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rp</t>
         </is>
       </c>
       <c r="Q315" t="inlineStr">
@@ -13366,12 +13378,12 @@
       <c r="D316" t="inlineStr"/>
       <c r="E316" t="inlineStr">
         <is>
-          <t>まとめて評価</t>
+          <t>Raids you are joining (Latest 2)</t>
         </is>
       </c>
       <c r="F316" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G316" t="inlineStr"/>
@@ -13385,7 +13397,7 @@
       <c r="O316" t="inlineStr"/>
       <c r="P316" t="inlineStr">
         <is>
-          <t>まとめて評価 Can't rate</t>
+          <t>Raids you are joining (Latest 2) MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rpl_maxuser'] }} {{ val1['cnt'] }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} No.{{ val1['rpl_id'] }} No.{{ val1['rpl_id'] }} TL{{ val1['rpl_level'] }} {{ val1['rpl_glevel'] }} {{ ((val1['rpl_gescore'] == -1)?0:val1['rpl_gescore']) }}</t>
         </is>
       </c>
       <c r="Q316" t="inlineStr">
@@ -13405,7 +13417,7 @@
       <c r="D317" t="inlineStr"/>
       <c r="E317" t="inlineStr">
         <is>
-          <t>Bonuses</t>
+          <t>まとめて評価</t>
         </is>
       </c>
       <c r="F317" t="inlineStr">
@@ -13424,12 +13436,12 @@
       <c r="O317" t="inlineStr"/>
       <c r="P317" t="inlineStr">
         <is>
-          <t>Bonuses 4× Stardust from win rewards. (This does not include end-of-set rewards.) The maximum number of sets you can play per day will increase from five to 20—for a total of 100 battles—from 12:00 a.m. to 11:59 p.m. local time. Free battle-themed Timed Research will be available. Rewards include glasses for your avatar inspired by Clemont. Pokémon encountered via GO Battle League rewards will have a wider variance of Attack, Defense, and HP. Active Leagues The following leagues will be active. Great League Ultra League Master League</t>
+          <t>まとめて評価 Can't rate</t>
         </is>
       </c>
       <c r="Q317" t="inlineStr">
         <is>
-          <t>2024-06-01_event-go-battle-weekend-tales-of-transformation-sun-oct-26-at-1159-pm-local-time-ends-calculating.html</t>
+          <t>2024-06-01_raid-now.html</t>
         </is>
       </c>
     </row>
@@ -13444,7 +13456,7 @@
       <c r="D318" t="inlineStr"/>
       <c r="E318" t="inlineStr">
         <is>
-          <t>For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area?</t>
+          <t>Bonuses</t>
         </is>
       </c>
       <c r="F318" t="inlineStr">
@@ -13463,12 +13475,12 @@
       <c r="O318" t="inlineStr"/>
       <c r="P318" t="inlineStr">
         <is>
-          <t xml:space="preserve">For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area? In this next chapter of Pokémon GO Wild Area, get ready to test your skills once again as you encounter Dark- and Fairy-type Pokémon, including Grimmsnarl, the Bulk Up Pokémon! Plus, exceptionally powerful Pokémon known as mighty Pokémon are appearing in the wild—use GO Wild Area–exclusive GO Safari Balls to improve your odds of catching these rare Pokémon. All event gameplay is exclusive to ticket holders. Tickets for Pokémon GO Wild Area: Nagasaki are now available on the Niantic events portal . Live Event Ticket - ¥3,600 (including applicable taxes and fees) Location: A citywide experience across Nagasaki City, Japan Dates: November 7, 8, or 9, 2025 Time: 9:00 a.m. – 5:00 p.m. JST Tickets for Pokémon GO Wild Area: Nagasaki include one day of event gameplay, and attendees may purchase add-ons that extend the gameplay for an additional day. One-day tickets are ¥3,600 (or the equivalent pricing tier in your local currency, including applicable taxes and fees). Event gameplay will be available only at the date, time, and location specified on your ticket. Note: Tickets to this event are </t>
+          <t>Bonuses 4× Stardust from win rewards. (This does not include end-of-set rewards.) The maximum number of sets you can play per day will increase from five to 20—for a total of 100 battles—from 12:00 a.m. to 11:59 p.m. local time. Free battle-themed Timed Research will be available. Rewards include glasses for your avatar inspired by Clemont. Pokémon encountered via GO Battle League rewards will have a wider variance of Attack, Defense, and HP. Active Leagues The following leagues will be active. Great League Ultra League Master League</t>
         </is>
       </c>
       <c r="Q318" t="inlineStr">
         <is>
-          <t>2024-06-01_wild-area-pokmon-go-wild-area-nagasaki-calculating-ends-calculating.html</t>
+          <t>2024-06-01_event-go-battle-weekend-tales-of-transformation-sun-oct-26-at-1159-pm-local-time-ends-calculating.html</t>
         </is>
       </c>
     </row>
@@ -13502,10 +13514,49 @@
       <c r="O319" t="inlineStr"/>
       <c r="P319" t="inlineStr">
         <is>
+          <t xml:space="preserve">For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area? In this next chapter of Pokémon GO Wild Area, get ready to test your skills once again as you encounter Dark- and Fairy-type Pokémon, including Grimmsnarl, the Bulk Up Pokémon! Plus, exceptionally powerful Pokémon known as mighty Pokémon are appearing in the wild—use GO Wild Area–exclusive GO Safari Balls to improve your odds of catching these rare Pokémon. All event gameplay is exclusive to ticket holders. Tickets for Pokémon GO Wild Area: Nagasaki are now available on the Niantic events portal . Live Event Ticket - ¥3,600 (including applicable taxes and fees) Location: A citywide experience across Nagasaki City, Japan Dates: November 7, 8, or 9, 2025 Time: 9:00 a.m. – 5:00 p.m. JST Tickets for Pokémon GO Wild Area: Nagasaki include one day of event gameplay, and attendees may purchase add-ons that extend the gameplay for an additional day. One-day tickets are ¥3,600 (or the equivalent pricing tier in your local currency, including applicable taxes and fees). Event gameplay will be available only at the date, time, and location specified on your ticket. Note: Tickets to this event are </t>
+        </is>
+      </c>
+      <c r="Q319" t="inlineStr">
+        <is>
+          <t>2024-06-01_wild-area-pokmon-go-wild-area-nagasaki-calculating-ends-calculating.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>Leek Duck</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr"/>
+      <c r="C320" t="inlineStr"/>
+      <c r="D320" t="inlineStr"/>
+      <c r="E320" t="inlineStr">
+        <is>
+          <t>For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area?</t>
+        </is>
+      </c>
+      <c r="F320" t="inlineStr">
+        <is>
+          <t>Event/News</t>
+        </is>
+      </c>
+      <c r="G320" t="inlineStr"/>
+      <c r="H320" t="inlineStr"/>
+      <c r="I320" t="inlineStr"/>
+      <c r="J320" t="inlineStr"/>
+      <c r="K320" t="inlineStr"/>
+      <c r="L320" t="inlineStr"/>
+      <c r="M320" t="inlineStr"/>
+      <c r="N320" t="inlineStr"/>
+      <c r="O320" t="inlineStr"/>
+      <c r="P320" t="inlineStr">
+        <is>
           <t>For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area? Trainers around the world can gear up for a worldwide adventure during Pokémon GO Wild Area: Global, available in-game for two days only! Looking to enhance your GO Wild Area weekend with exclusive Special Research, additional bonuses, and an increased chance of encountering Shiny Pokémon? Purchase a global event ticket from the Pokémon GO Web Store! Event Tickets Tickets for Pokémon GO Wild Area: Global are available now in the in-game Shop and Pokémon Go Web Store for $11.99 USD . Purchase your ticket on the Pokémon GO Web Store for a new avatar item! Trainers who purchase their Pokémon GO Wild Area: Global ticket on the Pokémon GO Web Store will receive a special avatar item—the Flower Crown! You can purchase your ticket on the web store until the last day of the event to receive this avatar item. Pokémon GO Wild Area: Nagasaki For details on the in-person event in Nagasaki, Japan, click here .</t>
         </is>
       </c>
-      <c r="Q319" t="inlineStr">
+      <c r="Q320" t="inlineStr">
         <is>
           <t>2024-06-01_wild-area-pokmon-go-wild-area-global-sun-nov-16-at-600-pm-local-time-ends-calculating.html</t>
         </is>

</xml_diff>

<commit_message>
Update latest digest: 2024-06-01 → 2025-09-26
</commit_message>
<xml_diff>
--- a/outputs/latest/POGO_Digest.xlsx
+++ b/outputs/latest/POGO_Digest.xlsx
@@ -1328,7 +1328,7 @@
       <c r="O17" t="inlineStr"/>
       <c r="P17" t="inlineStr">
         <is>
-          <t>Mega Camerupt Raid Day Raid Day Starts: Sunday, September 28, 2025, at  2:00 PM Local Time Ends: Sunday, September 28, 2025, at  5:00 PM Local Time Mega Camerupt charges in for its Pokémon GO debut! Bonuses Features Raids Shiny Sales Bonuses Remote Raid Pass limit increased to 20 from Saturday, September 27, at 5:00 p.m. to Sunday, September 28, 2025, at 8:00 p.m. PDT Receive up to five additional free Raid Passes from spinning Gym Photo Discs (for a total of six) Increased chance of encountering Shiny Camerupt from Mega Raids Event Ticket For US$4.99 (or the equivalent pricing tier in your local currency), you can purchase a ticket that grants the following bonuses. Receive up to eight additional free Raid Passes from spinning Gym Photo Discs (for a total of 14) Increased chance to get Rare Candy XL from Raid Battles 50% more XP from Raid Battles 2× Stardust from Raid Battles These bonuses will be effective on Sunday, September 28, 2025, from 2:00 p.m. to 5:00 p.m. local time. Trainers will be able to purchase and gift tickets to any of their Pokémon GO friends that they have achieved a Friendship level of Great Friends or higher with. Please note that purchases—including those ma</t>
+          <t xml:space="preserve">Mega Camerupt Raid Day Raid Day Starts: Sunday, September 28, 2025, at  2:00 PM Local Time Ends: Sunday, September 28, 2025, at  5:00 PM Local Time Mega Camerupt charges in for its Pokémon GO debut! Bonuses Features Raids Shiny Sales Graphic Bonuses Remote Raid Pass limit increased to 20 from Saturday, September 27, at 5:00 p.m. to Sunday, September 28, 2025, at 8:00 p.m. PDT Receive up to five additional free Raid Passes from spinning Gym Photo Discs (for a total of six) Increased chance of encountering Shiny Camerupt from Mega Raids Event Ticket For US$4.99 (or the equivalent pricing tier in your local currency), you can purchase a ticket that grants the following bonuses. Receive up to eight additional free Raid Passes from spinning Gym Photo Discs (for a total of 14) Increased chance to get Rare Candy XL from Raid Battles 50% more XP from Raid Battles 2× Stardust from Raid Battles These bonuses will be effective on Sunday, September 28, 2025, from 2:00 p.m. to 5:00 p.m. local time. Trainers will be able to purchase and gift tickets to any of their Pokémon GO friends that they have achieved a Friendship level of Great Friends or higher with. Please note that purchases—including </t>
         </is>
       </c>
       <c r="Q17" t="inlineStr">
@@ -2635,7 +2635,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Mega Raid Day</t>
+          <t>Mega Rayquaza Raid Day</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -2654,12 +2654,12 @@
       <c r="O43" t="inlineStr"/>
       <c r="P43" t="inlineStr">
         <is>
-          <t>Mega Raid Day Raid Day Starts: Saturday, October 18, 2025, at 10:00 AM Local Time Ends: Saturday, October 18, 2025, at  8:00 PM Local Time The Mega Raid Day event will take place on October 18, 2025 from 10 am to 8 pm. Stay tuned for more details. Leek Duck Hey, I'm LeekDuck. I create Pokémon GO graphics, resources and report Pokémon GO news. You can find them on X, Facebook, Instagram, Threads, and Bluesky. You can also find me on Twitch and YouTube!</t>
+          <t>Mega Rayquaza Raid Day Raid Day Starts: Saturday, October 18, 2025, at 10:00 AM Local Time Ends: Saturday, October 18, 2025, at  8:00 PM Local Time The Mega Rayquaza Raid Day event will take place on October 18, 2025 from 10 am to 8 pm. Stay tuned for more details. Leek Duck Hey, I'm LeekDuck. I create Pokémon GO graphics, resources and report Pokémon GO news. You can find them on X, Facebook, Instagram, Threads, and Bluesky. You can also find me on Twitch and YouTube!</t>
         </is>
       </c>
       <c r="Q43" t="inlineStr">
         <is>
-          <t>2024-06-01_raid-day-mega-raid-day-sat-oct-18-at-800-pm-local-time-ends-calculating.html</t>
+          <t>2024-06-01_raid-day-mega-rayquaza-raid-day-sat-oct-18-at-800-pm-local-time-ends-calculating.html</t>
         </is>
       </c>
     </row>
@@ -8971,7 +8971,7 @@
       <c r="D195" t="inlineStr"/>
       <c r="E195" t="inlineStr">
         <is>
-          <t>Mega Raid Day</t>
+          <t>Mega Rayquaza Raid Day</t>
         </is>
       </c>
       <c r="F195" t="inlineStr">
@@ -8990,7 +8990,7 @@
       <c r="O195" t="inlineStr"/>
       <c r="P195" t="inlineStr">
         <is>
-          <t>Raid Day Mega Raid Day Sat, Oct 18, at 8:00 PM Local Time Ends: Calculating...</t>
+          <t>Raid Day Mega Rayquaza Raid Day Sat, Oct 18, at 8:00 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q195" t="inlineStr">
@@ -9010,7 +9010,7 @@
       <c r="D196" t="inlineStr"/>
       <c r="E196" t="inlineStr">
         <is>
-          <t>Mega Raid Day</t>
+          <t>Mega Rayquaza Raid Day</t>
         </is>
       </c>
       <c r="F196" t="inlineStr">
@@ -9029,7 +9029,7 @@
       <c r="O196" t="inlineStr"/>
       <c r="P196" t="inlineStr">
         <is>
-          <t>Mega Raid Day Sat, Oct 18, at 8:00 PM Local Time Ends: Calculating...</t>
+          <t>Mega Rayquaza Raid Day Sat, Oct 18, at 8:00 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q196" t="inlineStr">
@@ -9049,7 +9049,7 @@
       <c r="D197" t="inlineStr"/>
       <c r="E197" t="inlineStr">
         <is>
-          <t>Mega Raid Day</t>
+          <t>Mega Rayquaza Raid Day</t>
         </is>
       </c>
       <c r="F197" t="inlineStr">
@@ -9068,7 +9068,7 @@
       <c r="O197" t="inlineStr"/>
       <c r="P197" t="inlineStr">
         <is>
-          <t>Mega Raid Day Sat, Oct 18, at 8:00 PM Local Time Ends: Calculating...</t>
+          <t>Mega Rayquaza Raid Day Sat, Oct 18, at 8:00 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q197" t="inlineStr">
@@ -9088,7 +9088,7 @@
       <c r="D198" t="inlineStr"/>
       <c r="E198" t="inlineStr">
         <is>
-          <t>Mega Raid Day</t>
+          <t>Mega Rayquaza Raid Day</t>
         </is>
       </c>
       <c r="F198" t="inlineStr">
@@ -9107,7 +9107,7 @@
       <c r="O198" t="inlineStr"/>
       <c r="P198" t="inlineStr">
         <is>
-          <t>Mega Raid Day Sat, Oct 18, at 8:00 PM Local Time</t>
+          <t>Mega Rayquaza Raid Day Sat, Oct 18, at 8:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q198" t="inlineStr">
@@ -18058,7 +18058,7 @@
       <c r="D428" t="inlineStr"/>
       <c r="E428" t="inlineStr">
         <is>
-          <t>Mega Raid Day</t>
+          <t>Mega Rayquaza Raid Day</t>
         </is>
       </c>
       <c r="F428" t="inlineStr">
@@ -18077,7 +18077,7 @@
       <c r="O428" t="inlineStr"/>
       <c r="P428" t="inlineStr">
         <is>
-          <t>Raid Day Mega Raid Day Sat, Oct 18, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Raid Day Mega Rayquaza Raid Day Sat, Oct 18, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q428" t="inlineStr">
@@ -18097,7 +18097,7 @@
       <c r="D429" t="inlineStr"/>
       <c r="E429" t="inlineStr">
         <is>
-          <t>Mega Raid Day</t>
+          <t>Mega Rayquaza Raid Day</t>
         </is>
       </c>
       <c r="F429" t="inlineStr">
@@ -18116,7 +18116,7 @@
       <c r="O429" t="inlineStr"/>
       <c r="P429" t="inlineStr">
         <is>
-          <t>Mega Raid Day Sat, Oct 18, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Mega Rayquaza Raid Day Sat, Oct 18, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q429" t="inlineStr">
@@ -18136,7 +18136,7 @@
       <c r="D430" t="inlineStr"/>
       <c r="E430" t="inlineStr">
         <is>
-          <t>Mega Raid Day</t>
+          <t>Mega Rayquaza Raid Day</t>
         </is>
       </c>
       <c r="F430" t="inlineStr">
@@ -18155,7 +18155,7 @@
       <c r="O430" t="inlineStr"/>
       <c r="P430" t="inlineStr">
         <is>
-          <t>Mega Raid Day Sat, Oct 18, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Mega Rayquaza Raid Day Sat, Oct 18, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q430" t="inlineStr">
@@ -18175,7 +18175,7 @@
       <c r="D431" t="inlineStr"/>
       <c r="E431" t="inlineStr">
         <is>
-          <t>Mega Raid Day</t>
+          <t>Mega Rayquaza Raid Day</t>
         </is>
       </c>
       <c r="F431" t="inlineStr">
@@ -18194,7 +18194,7 @@
       <c r="O431" t="inlineStr"/>
       <c r="P431" t="inlineStr">
         <is>
-          <t>Mega Raid Day Sat, Oct 18, at 10:00 AM Local Time</t>
+          <t>Mega Rayquaza Raid Day Sat, Oct 18, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q431" t="inlineStr">

</xml_diff>

<commit_message>
Update latest digest: 2024-06-01 → 2025-09-27
</commit_message>
<xml_diff>
--- a/outputs/latest/POGO_Digest.xlsx
+++ b/outputs/latest/POGO_Digest.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q535"/>
+  <dimension ref="A1:Q531"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13858,7 +13858,7 @@
       <c r="D320" t="inlineStr"/>
       <c r="E320" t="inlineStr">
         <is>
-          <t>Bangkok, Thailand - Pokémon GO City Safari</t>
+          <t>Amsterdam, Netherlands - Pokémon GO City Safari</t>
         </is>
       </c>
       <c r="F320" t="inlineStr">
@@ -13877,7 +13877,7 @@
       <c r="O320" t="inlineStr"/>
       <c r="P320" t="inlineStr">
         <is>
-          <t xml:space="preserve">City Safari Bangkok, Thailand - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating... City Safari Amsterdam, Netherlands - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating... City Safari Valencia, Spain - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating... City Safari Cancún, Mexico - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating... City Safari Vancouver, Canada - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating... PokéStop Showcase Camerupt and Dudunsparce PokéStop Showcases Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating... Raid Day Mega Camerupt Raid Day Sun, Sep 28, at 2:00 PM Local Time Starts: Calculating... Max Mondays Dynamax Beldum during Max Monday Mon, Sep 29, at 6:00 PM Local Time Starts: Calculating... Raid Battles Mega Steelix, Scizor, and Lucario in Mega Raids Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating... Event Steel Skyline Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating... GO Battle League Great League and Fantasy Cup: Great League Edition | Tales of Transformation Calculating... Starts: </t>
+          <t>City Safari Amsterdam, Netherlands - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating... City Safari Valencia, Spain - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating... City Safari Cancún, Mexico - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating... City Safari Vancouver, Canada - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating... PokéStop Showcase Camerupt and Dudunsparce PokéStop Showcases Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating... Raid Day Mega Camerupt Raid Day Sun, Sep 28, at 2:00 PM Local Time Starts: Calculating... Max Mondays Dynamax Beldum during Max Monday Mon, Sep 29, at 6:00 PM Local Time Starts: Calculating... Raid Battles Mega Steelix, Scizor, and Lucario in Mega Raids Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating... Event Steel Skyline Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating... GO Battle League Great League and Fantasy Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating... Pokémon Spotlight Hour Aron Spotlight Hour Tue, Sep 30, at 6:00 PM Local Time Starts: Calculating..</t>
         </is>
       </c>
       <c r="Q320" t="inlineStr">
@@ -13897,7 +13897,7 @@
       <c r="D321" t="inlineStr"/>
       <c r="E321" t="inlineStr">
         <is>
-          <t>Bangkok, Thailand - Pokémon GO City Safari</t>
+          <t>Amsterdam, Netherlands - Pokémon GO City Safari</t>
         </is>
       </c>
       <c r="F321" t="inlineStr">
@@ -13916,7 +13916,7 @@
       <c r="O321" t="inlineStr"/>
       <c r="P321" t="inlineStr">
         <is>
-          <t>City Safari Bangkok, Thailand - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>City Safari Amsterdam, Netherlands - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q321" t="inlineStr">
@@ -13936,7 +13936,7 @@
       <c r="D322" t="inlineStr"/>
       <c r="E322" t="inlineStr">
         <is>
-          <t>Bangkok, Thailand - Pokémon GO City Safari</t>
+          <t>Amsterdam, Netherlands - Pokémon GO City Safari</t>
         </is>
       </c>
       <c r="F322" t="inlineStr">
@@ -13955,7 +13955,7 @@
       <c r="O322" t="inlineStr"/>
       <c r="P322" t="inlineStr">
         <is>
-          <t>Bangkok, Thailand - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Amsterdam, Netherlands - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q322" t="inlineStr">
@@ -13975,7 +13975,7 @@
       <c r="D323" t="inlineStr"/>
       <c r="E323" t="inlineStr">
         <is>
-          <t>Bangkok, Thailand - Pokémon GO City Safari</t>
+          <t>Amsterdam, Netherlands - Pokémon GO City Safari</t>
         </is>
       </c>
       <c r="F323" t="inlineStr">
@@ -13994,7 +13994,7 @@
       <c r="O323" t="inlineStr"/>
       <c r="P323" t="inlineStr">
         <is>
-          <t>Bangkok, Thailand - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Amsterdam, Netherlands - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q323" t="inlineStr">
@@ -14014,7 +14014,7 @@
       <c r="D324" t="inlineStr"/>
       <c r="E324" t="inlineStr">
         <is>
-          <t>Bangkok, Thailand - Pokémon GO City Safari</t>
+          <t>Amsterdam, Netherlands - Pokémon GO City Safari</t>
         </is>
       </c>
       <c r="F324" t="inlineStr">
@@ -14033,7 +14033,7 @@
       <c r="O324" t="inlineStr"/>
       <c r="P324" t="inlineStr">
         <is>
-          <t>Bangkok, Thailand - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time</t>
+          <t>Amsterdam, Netherlands - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q324" t="inlineStr">
@@ -14053,7 +14053,7 @@
       <c r="D325" t="inlineStr"/>
       <c r="E325" t="inlineStr">
         <is>
-          <t>Amsterdam, Netherlands - Pokémon GO City Safari</t>
+          <t>Valencia, Spain - Pokémon GO City Safari</t>
         </is>
       </c>
       <c r="F325" t="inlineStr">
@@ -14072,7 +14072,7 @@
       <c r="O325" t="inlineStr"/>
       <c r="P325" t="inlineStr">
         <is>
-          <t>City Safari Amsterdam, Netherlands - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>City Safari Valencia, Spain - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q325" t="inlineStr">
@@ -14092,7 +14092,7 @@
       <c r="D326" t="inlineStr"/>
       <c r="E326" t="inlineStr">
         <is>
-          <t>Amsterdam, Netherlands - Pokémon GO City Safari</t>
+          <t>Valencia, Spain - Pokémon GO City Safari</t>
         </is>
       </c>
       <c r="F326" t="inlineStr">
@@ -14111,7 +14111,7 @@
       <c r="O326" t="inlineStr"/>
       <c r="P326" t="inlineStr">
         <is>
-          <t>Amsterdam, Netherlands - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Valencia, Spain - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q326" t="inlineStr">
@@ -14131,7 +14131,7 @@
       <c r="D327" t="inlineStr"/>
       <c r="E327" t="inlineStr">
         <is>
-          <t>Amsterdam, Netherlands - Pokémon GO City Safari</t>
+          <t>Valencia, Spain - Pokémon GO City Safari</t>
         </is>
       </c>
       <c r="F327" t="inlineStr">
@@ -14150,7 +14150,7 @@
       <c r="O327" t="inlineStr"/>
       <c r="P327" t="inlineStr">
         <is>
-          <t>Amsterdam, Netherlands - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Valencia, Spain - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q327" t="inlineStr">
@@ -14170,7 +14170,7 @@
       <c r="D328" t="inlineStr"/>
       <c r="E328" t="inlineStr">
         <is>
-          <t>Amsterdam, Netherlands - Pokémon GO City Safari</t>
+          <t>Valencia, Spain - Pokémon GO City Safari</t>
         </is>
       </c>
       <c r="F328" t="inlineStr">
@@ -14189,7 +14189,7 @@
       <c r="O328" t="inlineStr"/>
       <c r="P328" t="inlineStr">
         <is>
-          <t>Amsterdam, Netherlands - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time</t>
+          <t>Valencia, Spain - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q328" t="inlineStr">
@@ -14209,7 +14209,7 @@
       <c r="D329" t="inlineStr"/>
       <c r="E329" t="inlineStr">
         <is>
-          <t>Valencia, Spain - Pokémon GO City Safari</t>
+          <t>Cancún, Mexico - Pokémon GO City Safari</t>
         </is>
       </c>
       <c r="F329" t="inlineStr">
@@ -14228,7 +14228,7 @@
       <c r="O329" t="inlineStr"/>
       <c r="P329" t="inlineStr">
         <is>
-          <t>City Safari Valencia, Spain - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>City Safari Cancún, Mexico - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q329" t="inlineStr">
@@ -14248,7 +14248,7 @@
       <c r="D330" t="inlineStr"/>
       <c r="E330" t="inlineStr">
         <is>
-          <t>Valencia, Spain - Pokémon GO City Safari</t>
+          <t>Cancún, Mexico - Pokémon GO City Safari</t>
         </is>
       </c>
       <c r="F330" t="inlineStr">
@@ -14267,7 +14267,7 @@
       <c r="O330" t="inlineStr"/>
       <c r="P330" t="inlineStr">
         <is>
-          <t>Valencia, Spain - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Cancún, Mexico - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q330" t="inlineStr">
@@ -14287,7 +14287,7 @@
       <c r="D331" t="inlineStr"/>
       <c r="E331" t="inlineStr">
         <is>
-          <t>Valencia, Spain - Pokémon GO City Safari</t>
+          <t>Cancún, Mexico - Pokémon GO City Safari</t>
         </is>
       </c>
       <c r="F331" t="inlineStr">
@@ -14306,7 +14306,7 @@
       <c r="O331" t="inlineStr"/>
       <c r="P331" t="inlineStr">
         <is>
-          <t>Valencia, Spain - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Cancún, Mexico - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q331" t="inlineStr">
@@ -14326,7 +14326,7 @@
       <c r="D332" t="inlineStr"/>
       <c r="E332" t="inlineStr">
         <is>
-          <t>Valencia, Spain - Pokémon GO City Safari</t>
+          <t>Cancún, Mexico - Pokémon GO City Safari</t>
         </is>
       </c>
       <c r="F332" t="inlineStr">
@@ -14345,7 +14345,7 @@
       <c r="O332" t="inlineStr"/>
       <c r="P332" t="inlineStr">
         <is>
-          <t>Valencia, Spain - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time</t>
+          <t>Cancún, Mexico - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q332" t="inlineStr">
@@ -14365,7 +14365,7 @@
       <c r="D333" t="inlineStr"/>
       <c r="E333" t="inlineStr">
         <is>
-          <t>Cancún, Mexico - Pokémon GO City Safari</t>
+          <t>Vancouver, Canada - Pokémon GO City Safari</t>
         </is>
       </c>
       <c r="F333" t="inlineStr">
@@ -14384,7 +14384,7 @@
       <c r="O333" t="inlineStr"/>
       <c r="P333" t="inlineStr">
         <is>
-          <t>City Safari Cancún, Mexico - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>City Safari Vancouver, Canada - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q333" t="inlineStr">
@@ -14404,7 +14404,7 @@
       <c r="D334" t="inlineStr"/>
       <c r="E334" t="inlineStr">
         <is>
-          <t>Cancún, Mexico - Pokémon GO City Safari</t>
+          <t>Vancouver, Canada - Pokémon GO City Safari</t>
         </is>
       </c>
       <c r="F334" t="inlineStr">
@@ -14423,7 +14423,7 @@
       <c r="O334" t="inlineStr"/>
       <c r="P334" t="inlineStr">
         <is>
-          <t>Cancún, Mexico - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Vancouver, Canada - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q334" t="inlineStr">
@@ -14443,7 +14443,7 @@
       <c r="D335" t="inlineStr"/>
       <c r="E335" t="inlineStr">
         <is>
-          <t>Cancún, Mexico - Pokémon GO City Safari</t>
+          <t>Vancouver, Canada - Pokémon GO City Safari</t>
         </is>
       </c>
       <c r="F335" t="inlineStr">
@@ -14462,7 +14462,7 @@
       <c r="O335" t="inlineStr"/>
       <c r="P335" t="inlineStr">
         <is>
-          <t>Cancún, Mexico - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Vancouver, Canada - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q335" t="inlineStr">
@@ -14482,7 +14482,7 @@
       <c r="D336" t="inlineStr"/>
       <c r="E336" t="inlineStr">
         <is>
-          <t>Cancún, Mexico - Pokémon GO City Safari</t>
+          <t>Vancouver, Canada - Pokémon GO City Safari</t>
         </is>
       </c>
       <c r="F336" t="inlineStr">
@@ -14501,7 +14501,7 @@
       <c r="O336" t="inlineStr"/>
       <c r="P336" t="inlineStr">
         <is>
-          <t>Cancún, Mexico - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time</t>
+          <t>Vancouver, Canada - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q336" t="inlineStr">
@@ -14521,7 +14521,7 @@
       <c r="D337" t="inlineStr"/>
       <c r="E337" t="inlineStr">
         <is>
-          <t>Vancouver, Canada - Pokémon GO City Safari</t>
+          <t>Camerupt and Dudunsparce PokéStop Showcases</t>
         </is>
       </c>
       <c r="F337" t="inlineStr">
@@ -14540,7 +14540,7 @@
       <c r="O337" t="inlineStr"/>
       <c r="P337" t="inlineStr">
         <is>
-          <t>City Safari Vancouver, Canada - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>PokéStop Showcase Camerupt and Dudunsparce PokéStop Showcases Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q337" t="inlineStr">
@@ -14560,7 +14560,7 @@
       <c r="D338" t="inlineStr"/>
       <c r="E338" t="inlineStr">
         <is>
-          <t>Vancouver, Canada - Pokémon GO City Safari</t>
+          <t>Camerupt and Dudunsparce PokéStop Showcases</t>
         </is>
       </c>
       <c r="F338" t="inlineStr">
@@ -14579,7 +14579,7 @@
       <c r="O338" t="inlineStr"/>
       <c r="P338" t="inlineStr">
         <is>
-          <t>Vancouver, Canada - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Camerupt and Dudunsparce PokéStop Showcases Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q338" t="inlineStr">
@@ -14599,7 +14599,7 @@
       <c r="D339" t="inlineStr"/>
       <c r="E339" t="inlineStr">
         <is>
-          <t>Vancouver, Canada - Pokémon GO City Safari</t>
+          <t>Camerupt and Dudunsparce PokéStop Showcases</t>
         </is>
       </c>
       <c r="F339" t="inlineStr">
@@ -14618,7 +14618,7 @@
       <c r="O339" t="inlineStr"/>
       <c r="P339" t="inlineStr">
         <is>
-          <t>Vancouver, Canada - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Camerupt and Dudunsparce PokéStop Showcases Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q339" t="inlineStr">
@@ -14638,7 +14638,7 @@
       <c r="D340" t="inlineStr"/>
       <c r="E340" t="inlineStr">
         <is>
-          <t>Vancouver, Canada - Pokémon GO City Safari</t>
+          <t>Camerupt and Dudunsparce PokéStop Showcases</t>
         </is>
       </c>
       <c r="F340" t="inlineStr">
@@ -14657,7 +14657,7 @@
       <c r="O340" t="inlineStr"/>
       <c r="P340" t="inlineStr">
         <is>
-          <t>Vancouver, Canada - Pokémon GO City Safari Sat, Sep 27, at 10:00 AM Local Time</t>
+          <t>Camerupt and Dudunsparce PokéStop Showcases Sat, Sep 27, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q340" t="inlineStr">
@@ -14677,12 +14677,12 @@
       <c r="D341" t="inlineStr"/>
       <c r="E341" t="inlineStr">
         <is>
-          <t>Camerupt and Dudunsparce PokéStop Showcases</t>
+          <t>Mega Camerupt Raid Day</t>
         </is>
       </c>
       <c r="F341" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G341" t="inlineStr"/>
@@ -14696,7 +14696,7 @@
       <c r="O341" t="inlineStr"/>
       <c r="P341" t="inlineStr">
         <is>
-          <t>PokéStop Showcase Camerupt and Dudunsparce PokéStop Showcases Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Raid Day Mega Camerupt Raid Day Sun, Sep 28, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q341" t="inlineStr">
@@ -14716,12 +14716,12 @@
       <c r="D342" t="inlineStr"/>
       <c r="E342" t="inlineStr">
         <is>
-          <t>Camerupt and Dudunsparce PokéStop Showcases</t>
+          <t>Mega Camerupt Raid Day</t>
         </is>
       </c>
       <c r="F342" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G342" t="inlineStr"/>
@@ -14735,7 +14735,7 @@
       <c r="O342" t="inlineStr"/>
       <c r="P342" t="inlineStr">
         <is>
-          <t>Camerupt and Dudunsparce PokéStop Showcases Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Mega Camerupt Raid Day Sun, Sep 28, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q342" t="inlineStr">
@@ -14755,12 +14755,12 @@
       <c r="D343" t="inlineStr"/>
       <c r="E343" t="inlineStr">
         <is>
-          <t>Camerupt and Dudunsparce PokéStop Showcases</t>
+          <t>Mega Camerupt Raid Day</t>
         </is>
       </c>
       <c r="F343" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G343" t="inlineStr"/>
@@ -14774,7 +14774,7 @@
       <c r="O343" t="inlineStr"/>
       <c r="P343" t="inlineStr">
         <is>
-          <t>Camerupt and Dudunsparce PokéStop Showcases Sat, Sep 27, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Mega Camerupt Raid Day Sun, Sep 28, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q343" t="inlineStr">
@@ -14794,12 +14794,12 @@
       <c r="D344" t="inlineStr"/>
       <c r="E344" t="inlineStr">
         <is>
-          <t>Camerupt and Dudunsparce PokéStop Showcases</t>
+          <t>Mega Camerupt Raid Day</t>
         </is>
       </c>
       <c r="F344" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G344" t="inlineStr"/>
@@ -14813,7 +14813,7 @@
       <c r="O344" t="inlineStr"/>
       <c r="P344" t="inlineStr">
         <is>
-          <t>Camerupt and Dudunsparce PokéStop Showcases Sat, Sep 27, at 10:00 AM Local Time</t>
+          <t>Mega Camerupt Raid Day Sun, Sep 28, at 2:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q344" t="inlineStr">
@@ -14833,12 +14833,12 @@
       <c r="D345" t="inlineStr"/>
       <c r="E345" t="inlineStr">
         <is>
-          <t>Mega Camerupt Raid Day</t>
+          <t>Dynamax Beldum during Max Monday</t>
         </is>
       </c>
       <c r="F345" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G345" t="inlineStr"/>
@@ -14852,7 +14852,7 @@
       <c r="O345" t="inlineStr"/>
       <c r="P345" t="inlineStr">
         <is>
-          <t>Raid Day Mega Camerupt Raid Day Sun, Sep 28, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Max Mondays Dynamax Beldum during Max Monday Mon, Sep 29, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q345" t="inlineStr">
@@ -14872,12 +14872,12 @@
       <c r="D346" t="inlineStr"/>
       <c r="E346" t="inlineStr">
         <is>
-          <t>Mega Camerupt Raid Day</t>
+          <t>Dynamax Beldum during Max Monday</t>
         </is>
       </c>
       <c r="F346" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G346" t="inlineStr"/>
@@ -14891,7 +14891,7 @@
       <c r="O346" t="inlineStr"/>
       <c r="P346" t="inlineStr">
         <is>
-          <t>Mega Camerupt Raid Day Sun, Sep 28, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Dynamax Beldum during Max Monday Mon, Sep 29, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q346" t="inlineStr">
@@ -14911,12 +14911,12 @@
       <c r="D347" t="inlineStr"/>
       <c r="E347" t="inlineStr">
         <is>
-          <t>Mega Camerupt Raid Day</t>
+          <t>Dynamax Beldum during Max Monday</t>
         </is>
       </c>
       <c r="F347" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G347" t="inlineStr"/>
@@ -14930,7 +14930,7 @@
       <c r="O347" t="inlineStr"/>
       <c r="P347" t="inlineStr">
         <is>
-          <t>Mega Camerupt Raid Day Sun, Sep 28, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Dynamax Beldum during Max Monday Mon, Sep 29, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q347" t="inlineStr">
@@ -14950,12 +14950,12 @@
       <c r="D348" t="inlineStr"/>
       <c r="E348" t="inlineStr">
         <is>
-          <t>Mega Camerupt Raid Day</t>
+          <t>Dynamax Beldum during Max Monday</t>
         </is>
       </c>
       <c r="F348" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G348" t="inlineStr"/>
@@ -14969,7 +14969,7 @@
       <c r="O348" t="inlineStr"/>
       <c r="P348" t="inlineStr">
         <is>
-          <t>Mega Camerupt Raid Day Sun, Sep 28, at 2:00 PM Local Time</t>
+          <t>Dynamax Beldum during Max Monday Mon, Sep 29, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q348" t="inlineStr">
@@ -14989,12 +14989,12 @@
       <c r="D349" t="inlineStr"/>
       <c r="E349" t="inlineStr">
         <is>
-          <t>Dynamax Beldum during Max Monday</t>
+          <t>Mega Steelix, Scizor, and Lucario in Mega Raids</t>
         </is>
       </c>
       <c r="F349" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G349" t="inlineStr"/>
@@ -15008,7 +15008,7 @@
       <c r="O349" t="inlineStr"/>
       <c r="P349" t="inlineStr">
         <is>
-          <t>Max Mondays Dynamax Beldum during Max Monday Mon, Sep 29, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Raid Battles Mega Steelix, Scizor, and Lucario in Mega Raids Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q349" t="inlineStr">
@@ -15028,12 +15028,12 @@
       <c r="D350" t="inlineStr"/>
       <c r="E350" t="inlineStr">
         <is>
-          <t>Dynamax Beldum during Max Monday</t>
+          <t>Mega Steelix, Scizor, and Lucario in Mega Raids</t>
         </is>
       </c>
       <c r="F350" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G350" t="inlineStr"/>
@@ -15047,7 +15047,7 @@
       <c r="O350" t="inlineStr"/>
       <c r="P350" t="inlineStr">
         <is>
-          <t>Dynamax Beldum during Max Monday Mon, Sep 29, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Mega Steelix, Scizor, and Lucario in Mega Raids Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q350" t="inlineStr">
@@ -15067,12 +15067,12 @@
       <c r="D351" t="inlineStr"/>
       <c r="E351" t="inlineStr">
         <is>
-          <t>Dynamax Beldum during Max Monday</t>
+          <t>Mega Steelix, Scizor, and Lucario in Mega Raids</t>
         </is>
       </c>
       <c r="F351" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G351" t="inlineStr"/>
@@ -15086,7 +15086,7 @@
       <c r="O351" t="inlineStr"/>
       <c r="P351" t="inlineStr">
         <is>
-          <t>Dynamax Beldum during Max Monday Mon, Sep 29, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Mega Steelix, Scizor, and Lucario in Mega Raids Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q351" t="inlineStr">
@@ -15106,12 +15106,12 @@
       <c r="D352" t="inlineStr"/>
       <c r="E352" t="inlineStr">
         <is>
-          <t>Dynamax Beldum during Max Monday</t>
+          <t>Mega Steelix, Scizor, and Lucario in Mega Raids</t>
         </is>
       </c>
       <c r="F352" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G352" t="inlineStr"/>
@@ -15125,7 +15125,7 @@
       <c r="O352" t="inlineStr"/>
       <c r="P352" t="inlineStr">
         <is>
-          <t>Dynamax Beldum during Max Monday Mon, Sep 29, at 6:00 PM Local Time</t>
+          <t>Mega Steelix, Scizor, and Lucario in Mega Raids Tue, Sep 30, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q352" t="inlineStr">
@@ -15145,12 +15145,12 @@
       <c r="D353" t="inlineStr"/>
       <c r="E353" t="inlineStr">
         <is>
-          <t>Mega Steelix, Scizor, and Lucario in Mega Raids</t>
+          <t>Steel Skyline</t>
         </is>
       </c>
       <c r="F353" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G353" t="inlineStr"/>
@@ -15164,7 +15164,7 @@
       <c r="O353" t="inlineStr"/>
       <c r="P353" t="inlineStr">
         <is>
-          <t>Raid Battles Mega Steelix, Scizor, and Lucario in Mega Raids Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Event Steel Skyline Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q353" t="inlineStr">
@@ -15184,12 +15184,12 @@
       <c r="D354" t="inlineStr"/>
       <c r="E354" t="inlineStr">
         <is>
-          <t>Mega Steelix, Scizor, and Lucario in Mega Raids</t>
+          <t>Steel Skyline</t>
         </is>
       </c>
       <c r="F354" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G354" t="inlineStr"/>
@@ -15203,7 +15203,7 @@
       <c r="O354" t="inlineStr"/>
       <c r="P354" t="inlineStr">
         <is>
-          <t>Mega Steelix, Scizor, and Lucario in Mega Raids Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Steel Skyline Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q354" t="inlineStr">
@@ -15223,12 +15223,12 @@
       <c r="D355" t="inlineStr"/>
       <c r="E355" t="inlineStr">
         <is>
-          <t>Mega Steelix, Scizor, and Lucario in Mega Raids</t>
+          <t>Steel Skyline</t>
         </is>
       </c>
       <c r="F355" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G355" t="inlineStr"/>
@@ -15242,7 +15242,7 @@
       <c r="O355" t="inlineStr"/>
       <c r="P355" t="inlineStr">
         <is>
-          <t>Mega Steelix, Scizor, and Lucario in Mega Raids Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Steel Skyline Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q355" t="inlineStr">
@@ -15262,12 +15262,12 @@
       <c r="D356" t="inlineStr"/>
       <c r="E356" t="inlineStr">
         <is>
-          <t>Mega Steelix, Scizor, and Lucario in Mega Raids</t>
+          <t>Steel Skyline</t>
         </is>
       </c>
       <c r="F356" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G356" t="inlineStr"/>
@@ -15281,7 +15281,7 @@
       <c r="O356" t="inlineStr"/>
       <c r="P356" t="inlineStr">
         <is>
-          <t>Mega Steelix, Scizor, and Lucario in Mega Raids Tue, Sep 30, at 10:00 AM Local Time</t>
+          <t>Steel Skyline Tue, Sep 30, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q356" t="inlineStr">
@@ -15301,7 +15301,7 @@
       <c r="D357" t="inlineStr"/>
       <c r="E357" t="inlineStr">
         <is>
-          <t>Steel Skyline</t>
+          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F357" t="inlineStr">
@@ -15320,7 +15320,7 @@
       <c r="O357" t="inlineStr"/>
       <c r="P357" t="inlineStr">
         <is>
-          <t>Event Steel Skyline Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>GO Battle League Great League and Fantasy Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q357" t="inlineStr">
@@ -15340,7 +15340,7 @@
       <c r="D358" t="inlineStr"/>
       <c r="E358" t="inlineStr">
         <is>
-          <t>Steel Skyline</t>
+          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F358" t="inlineStr">
@@ -15359,7 +15359,7 @@
       <c r="O358" t="inlineStr"/>
       <c r="P358" t="inlineStr">
         <is>
-          <t>Steel Skyline Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q358" t="inlineStr">
@@ -15379,7 +15379,7 @@
       <c r="D359" t="inlineStr"/>
       <c r="E359" t="inlineStr">
         <is>
-          <t>Steel Skyline</t>
+          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F359" t="inlineStr">
@@ -15398,7 +15398,7 @@
       <c r="O359" t="inlineStr"/>
       <c r="P359" t="inlineStr">
         <is>
-          <t>Steel Skyline Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q359" t="inlineStr">
@@ -15418,7 +15418,7 @@
       <c r="D360" t="inlineStr"/>
       <c r="E360" t="inlineStr">
         <is>
-          <t>Steel Skyline</t>
+          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F360" t="inlineStr">
@@ -15437,7 +15437,7 @@
       <c r="O360" t="inlineStr"/>
       <c r="P360" t="inlineStr">
         <is>
-          <t>Steel Skyline Tue, Sep 30, at 10:00 AM Local Time</t>
+          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q360" t="inlineStr">
@@ -15457,12 +15457,12 @@
       <c r="D361" t="inlineStr"/>
       <c r="E361" t="inlineStr">
         <is>
-          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation</t>
+          <t>Aron Spotlight Hour</t>
         </is>
       </c>
       <c r="F361" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G361" t="inlineStr"/>
@@ -15476,7 +15476,7 @@
       <c r="O361" t="inlineStr"/>
       <c r="P361" t="inlineStr">
         <is>
-          <t>GO Battle League Great League and Fantasy Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Pokémon Spotlight Hour Aron Spotlight Hour Tue, Sep 30, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q361" t="inlineStr">
@@ -15496,12 +15496,12 @@
       <c r="D362" t="inlineStr"/>
       <c r="E362" t="inlineStr">
         <is>
-          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation</t>
+          <t>Aron Spotlight Hour</t>
         </is>
       </c>
       <c r="F362" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G362" t="inlineStr"/>
@@ -15515,7 +15515,7 @@
       <c r="O362" t="inlineStr"/>
       <c r="P362" t="inlineStr">
         <is>
-          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Aron Spotlight Hour Tue, Sep 30, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q362" t="inlineStr">
@@ -15535,12 +15535,12 @@
       <c r="D363" t="inlineStr"/>
       <c r="E363" t="inlineStr">
         <is>
-          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation</t>
+          <t>Aron Spotlight Hour</t>
         </is>
       </c>
       <c r="F363" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G363" t="inlineStr"/>
@@ -15554,7 +15554,7 @@
       <c r="O363" t="inlineStr"/>
       <c r="P363" t="inlineStr">
         <is>
-          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Aron Spotlight Hour Tue, Sep 30, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q363" t="inlineStr">
@@ -15574,12 +15574,12 @@
       <c r="D364" t="inlineStr"/>
       <c r="E364" t="inlineStr">
         <is>
-          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation</t>
+          <t>Aron Spotlight Hour</t>
         </is>
       </c>
       <c r="F364" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G364" t="inlineStr"/>
@@ -15593,7 +15593,7 @@
       <c r="O364" t="inlineStr"/>
       <c r="P364" t="inlineStr">
         <is>
-          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation Calculating...</t>
+          <t>Aron Spotlight Hour Tue, Sep 30, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q364" t="inlineStr">
@@ -15613,12 +15613,12 @@
       <c r="D365" t="inlineStr"/>
       <c r="E365" t="inlineStr">
         <is>
-          <t>Aron Spotlight Hour</t>
+          <t>Dialga (Origin Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F365" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G365" t="inlineStr"/>
@@ -15632,7 +15632,7 @@
       <c r="O365" t="inlineStr"/>
       <c r="P365" t="inlineStr">
         <is>
-          <t>Pokémon Spotlight Hour Aron Spotlight Hour Tue, Sep 30, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Raid Hour Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q365" t="inlineStr">
@@ -15652,12 +15652,12 @@
       <c r="D366" t="inlineStr"/>
       <c r="E366" t="inlineStr">
         <is>
-          <t>Aron Spotlight Hour</t>
+          <t>Dialga (Origin Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F366" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G366" t="inlineStr"/>
@@ -15671,7 +15671,7 @@
       <c r="O366" t="inlineStr"/>
       <c r="P366" t="inlineStr">
         <is>
-          <t>Aron Spotlight Hour Tue, Sep 30, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q366" t="inlineStr">
@@ -15691,12 +15691,12 @@
       <c r="D367" t="inlineStr"/>
       <c r="E367" t="inlineStr">
         <is>
-          <t>Aron Spotlight Hour</t>
+          <t>Dialga (Origin Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F367" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G367" t="inlineStr"/>
@@ -15710,7 +15710,7 @@
       <c r="O367" t="inlineStr"/>
       <c r="P367" t="inlineStr">
         <is>
-          <t>Aron Spotlight Hour Tue, Sep 30, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q367" t="inlineStr">
@@ -15730,12 +15730,12 @@
       <c r="D368" t="inlineStr"/>
       <c r="E368" t="inlineStr">
         <is>
-          <t>Aron Spotlight Hour</t>
+          <t>Dialga (Origin Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F368" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G368" t="inlineStr"/>
@@ -15749,7 +15749,7 @@
       <c r="O368" t="inlineStr"/>
       <c r="P368" t="inlineStr">
         <is>
-          <t>Aron Spotlight Hour Tue, Sep 30, at 6:00 PM Local Time</t>
+          <t>Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q368" t="inlineStr">
@@ -15769,7 +15769,7 @@
       <c r="D369" t="inlineStr"/>
       <c r="E369" t="inlineStr">
         <is>
-          <t>Dialga (Origin Forme) Raid Hour</t>
+          <t>Mega Metagross Raid Day</t>
         </is>
       </c>
       <c r="F369" t="inlineStr">
@@ -15788,7 +15788,7 @@
       <c r="O369" t="inlineStr"/>
       <c r="P369" t="inlineStr">
         <is>
-          <t>Raid Hour Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Raid Day Mega Metagross Raid Day Sat, Oct 4, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q369" t="inlineStr">
@@ -15808,7 +15808,7 @@
       <c r="D370" t="inlineStr"/>
       <c r="E370" t="inlineStr">
         <is>
-          <t>Dialga (Origin Forme) Raid Hour</t>
+          <t>Mega Metagross Raid Day</t>
         </is>
       </c>
       <c r="F370" t="inlineStr">
@@ -15827,7 +15827,7 @@
       <c r="O370" t="inlineStr"/>
       <c r="P370" t="inlineStr">
         <is>
-          <t>Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Mega Metagross Raid Day Sat, Oct 4, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q370" t="inlineStr">
@@ -15847,7 +15847,7 @@
       <c r="D371" t="inlineStr"/>
       <c r="E371" t="inlineStr">
         <is>
-          <t>Dialga (Origin Forme) Raid Hour</t>
+          <t>Mega Metagross Raid Day</t>
         </is>
       </c>
       <c r="F371" t="inlineStr">
@@ -15866,7 +15866,7 @@
       <c r="O371" t="inlineStr"/>
       <c r="P371" t="inlineStr">
         <is>
-          <t>Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Mega Metagross Raid Day Sat, Oct 4, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q371" t="inlineStr">
@@ -15886,7 +15886,7 @@
       <c r="D372" t="inlineStr"/>
       <c r="E372" t="inlineStr">
         <is>
-          <t>Dialga (Origin Forme) Raid Hour</t>
+          <t>Mega Metagross Raid Day</t>
         </is>
       </c>
       <c r="F372" t="inlineStr">
@@ -15905,7 +15905,7 @@
       <c r="O372" t="inlineStr"/>
       <c r="P372" t="inlineStr">
         <is>
-          <t>Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 6:00 PM Local Time</t>
+          <t>Mega Metagross Raid Day Sat, Oct 4, at 2:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q372" t="inlineStr">
@@ -15925,12 +15925,12 @@
       <c r="D373" t="inlineStr"/>
       <c r="E373" t="inlineStr">
         <is>
-          <t>Mega Metagross Raid Day</t>
+          <t>Dynamax Drilbur during Max Monday</t>
         </is>
       </c>
       <c r="F373" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G373" t="inlineStr"/>
@@ -15944,7 +15944,7 @@
       <c r="O373" t="inlineStr"/>
       <c r="P373" t="inlineStr">
         <is>
-          <t>Raid Day Mega Metagross Raid Day Sat, Oct 4, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Max Mondays Dynamax Drilbur during Max Monday Mon, Oct 6, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q373" t="inlineStr">
@@ -15964,12 +15964,12 @@
       <c r="D374" t="inlineStr"/>
       <c r="E374" t="inlineStr">
         <is>
-          <t>Mega Metagross Raid Day</t>
+          <t>Dynamax Drilbur during Max Monday</t>
         </is>
       </c>
       <c r="F374" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G374" t="inlineStr"/>
@@ -15983,7 +15983,7 @@
       <c r="O374" t="inlineStr"/>
       <c r="P374" t="inlineStr">
         <is>
-          <t>Mega Metagross Raid Day Sat, Oct 4, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Dynamax Drilbur during Max Monday Mon, Oct 6, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q374" t="inlineStr">
@@ -16003,12 +16003,12 @@
       <c r="D375" t="inlineStr"/>
       <c r="E375" t="inlineStr">
         <is>
-          <t>Mega Metagross Raid Day</t>
+          <t>Dynamax Drilbur during Max Monday</t>
         </is>
       </c>
       <c r="F375" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G375" t="inlineStr"/>
@@ -16022,7 +16022,7 @@
       <c r="O375" t="inlineStr"/>
       <c r="P375" t="inlineStr">
         <is>
-          <t>Mega Metagross Raid Day Sat, Oct 4, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Dynamax Drilbur during Max Monday Mon, Oct 6, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q375" t="inlineStr">
@@ -16042,12 +16042,12 @@
       <c r="D376" t="inlineStr"/>
       <c r="E376" t="inlineStr">
         <is>
-          <t>Mega Metagross Raid Day</t>
+          <t>Dynamax Drilbur during Max Monday</t>
         </is>
       </c>
       <c r="F376" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G376" t="inlineStr"/>
@@ -16061,7 +16061,7 @@
       <c r="O376" t="inlineStr"/>
       <c r="P376" t="inlineStr">
         <is>
-          <t>Mega Metagross Raid Day Sat, Oct 4, at 2:00 PM Local Time</t>
+          <t>Dynamax Drilbur during Max Monday Mon, Oct 6, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q376" t="inlineStr">
@@ -16081,12 +16081,12 @@
       <c r="D377" t="inlineStr"/>
       <c r="E377" t="inlineStr">
         <is>
-          <t>Dynamax Drilbur during Max Monday</t>
+          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F377" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G377" t="inlineStr"/>
@@ -16100,7 +16100,7 @@
       <c r="O377" t="inlineStr"/>
       <c r="P377" t="inlineStr">
         <is>
-          <t>Max Mondays Dynamax Drilbur during Max Monday Mon, Oct 6, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Raid Battles Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q377" t="inlineStr">
@@ -16120,12 +16120,12 @@
       <c r="D378" t="inlineStr"/>
       <c r="E378" t="inlineStr">
         <is>
-          <t>Dynamax Drilbur during Max Monday</t>
+          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F378" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G378" t="inlineStr"/>
@@ -16139,7 +16139,7 @@
       <c r="O378" t="inlineStr"/>
       <c r="P378" t="inlineStr">
         <is>
-          <t>Dynamax Drilbur during Max Monday Mon, Oct 6, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q378" t="inlineStr">
@@ -16159,12 +16159,12 @@
       <c r="D379" t="inlineStr"/>
       <c r="E379" t="inlineStr">
         <is>
-          <t>Dynamax Drilbur during Max Monday</t>
+          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F379" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G379" t="inlineStr"/>
@@ -16178,7 +16178,7 @@
       <c r="O379" t="inlineStr"/>
       <c r="P379" t="inlineStr">
         <is>
-          <t>Dynamax Drilbur during Max Monday Mon, Oct 6, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q379" t="inlineStr">
@@ -16198,12 +16198,12 @@
       <c r="D380" t="inlineStr"/>
       <c r="E380" t="inlineStr">
         <is>
-          <t>Dynamax Drilbur during Max Monday</t>
+          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F380" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G380" t="inlineStr"/>
@@ -16217,7 +16217,7 @@
       <c r="O380" t="inlineStr"/>
       <c r="P380" t="inlineStr">
         <is>
-          <t>Dynamax Drilbur during Max Monday Mon, Oct 6, at 6:00 PM Local Time</t>
+          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q380" t="inlineStr">
@@ -16237,7 +16237,7 @@
       <c r="D381" t="inlineStr"/>
       <c r="E381" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles</t>
+          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids</t>
         </is>
       </c>
       <c r="F381" t="inlineStr">
@@ -16256,7 +16256,7 @@
       <c r="O381" t="inlineStr"/>
       <c r="P381" t="inlineStr">
         <is>
-          <t>Raid Battles Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Raid Battles Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q381" t="inlineStr">
@@ -16276,7 +16276,7 @@
       <c r="D382" t="inlineStr"/>
       <c r="E382" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles</t>
+          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids</t>
         </is>
       </c>
       <c r="F382" t="inlineStr">
@@ -16295,7 +16295,7 @@
       <c r="O382" t="inlineStr"/>
       <c r="P382" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q382" t="inlineStr">
@@ -16315,7 +16315,7 @@
       <c r="D383" t="inlineStr"/>
       <c r="E383" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles</t>
+          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids</t>
         </is>
       </c>
       <c r="F383" t="inlineStr">
@@ -16334,7 +16334,7 @@
       <c r="O383" t="inlineStr"/>
       <c r="P383" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q383" t="inlineStr">
@@ -16354,7 +16354,7 @@
       <c r="D384" t="inlineStr"/>
       <c r="E384" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles</t>
+          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids</t>
         </is>
       </c>
       <c r="F384" t="inlineStr">
@@ -16373,7 +16373,7 @@
       <c r="O384" t="inlineStr"/>
       <c r="P384" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time</t>
+          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids Tue, Oct 7, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q384" t="inlineStr">
@@ -16393,12 +16393,12 @@
       <c r="D385" t="inlineStr"/>
       <c r="E385" t="inlineStr">
         <is>
-          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F385" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G385" t="inlineStr"/>
@@ -16412,7 +16412,7 @@
       <c r="O385" t="inlineStr"/>
       <c r="P385" t="inlineStr">
         <is>
-          <t>Raid Battles Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>GO Battle League Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q385" t="inlineStr">
@@ -16432,12 +16432,12 @@
       <c r="D386" t="inlineStr"/>
       <c r="E386" t="inlineStr">
         <is>
-          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F386" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G386" t="inlineStr"/>
@@ -16451,7 +16451,7 @@
       <c r="O386" t="inlineStr"/>
       <c r="P386" t="inlineStr">
         <is>
-          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q386" t="inlineStr">
@@ -16471,12 +16471,12 @@
       <c r="D387" t="inlineStr"/>
       <c r="E387" t="inlineStr">
         <is>
-          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F387" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G387" t="inlineStr"/>
@@ -16490,7 +16490,7 @@
       <c r="O387" t="inlineStr"/>
       <c r="P387" t="inlineStr">
         <is>
-          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q387" t="inlineStr">
@@ -16510,12 +16510,12 @@
       <c r="D388" t="inlineStr"/>
       <c r="E388" t="inlineStr">
         <is>
-          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F388" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G388" t="inlineStr"/>
@@ -16529,7 +16529,7 @@
       <c r="O388" t="inlineStr"/>
       <c r="P388" t="inlineStr">
         <is>
-          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids Tue, Oct 7, at 10:00 AM Local Time</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q388" t="inlineStr">
@@ -16549,12 +16549,12 @@
       <c r="D389" t="inlineStr"/>
       <c r="E389" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
+          <t>Ferroseed Spotlight Hour</t>
         </is>
       </c>
       <c r="F389" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G389" t="inlineStr"/>
@@ -16568,7 +16568,7 @@
       <c r="O389" t="inlineStr"/>
       <c r="P389" t="inlineStr">
         <is>
-          <t>GO Battle League Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Pokémon Spotlight Hour Ferroseed Spotlight Hour Tue, Oct 7, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q389" t="inlineStr">
@@ -16588,12 +16588,12 @@
       <c r="D390" t="inlineStr"/>
       <c r="E390" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
+          <t>Ferroseed Spotlight Hour</t>
         </is>
       </c>
       <c r="F390" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G390" t="inlineStr"/>
@@ -16607,7 +16607,7 @@
       <c r="O390" t="inlineStr"/>
       <c r="P390" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Ferroseed Spotlight Hour Tue, Oct 7, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q390" t="inlineStr">
@@ -16627,12 +16627,12 @@
       <c r="D391" t="inlineStr"/>
       <c r="E391" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
+          <t>Ferroseed Spotlight Hour</t>
         </is>
       </c>
       <c r="F391" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G391" t="inlineStr"/>
@@ -16646,7 +16646,7 @@
       <c r="O391" t="inlineStr"/>
       <c r="P391" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Ferroseed Spotlight Hour Tue, Oct 7, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q391" t="inlineStr">
@@ -16666,12 +16666,12 @@
       <c r="D392" t="inlineStr"/>
       <c r="E392" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
+          <t>Ferroseed Spotlight Hour</t>
         </is>
       </c>
       <c r="F392" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G392" t="inlineStr"/>
@@ -16685,7 +16685,7 @@
       <c r="O392" t="inlineStr"/>
       <c r="P392" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating...</t>
+          <t>Ferroseed Spotlight Hour Tue, Oct 7, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q392" t="inlineStr">
@@ -16705,12 +16705,12 @@
       <c r="D393" t="inlineStr"/>
       <c r="E393" t="inlineStr">
         <is>
-          <t>Ferroseed Spotlight Hour</t>
+          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F393" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G393" t="inlineStr"/>
@@ -16724,7 +16724,7 @@
       <c r="O393" t="inlineStr"/>
       <c r="P393" t="inlineStr">
         <is>
-          <t>Pokémon Spotlight Hour Ferroseed Spotlight Hour Tue, Oct 7, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Raid Hour Deoxys (Normal &amp; Defense Forme) Raid Hour Wed, Oct 8, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q393" t="inlineStr">
@@ -16744,12 +16744,12 @@
       <c r="D394" t="inlineStr"/>
       <c r="E394" t="inlineStr">
         <is>
-          <t>Ferroseed Spotlight Hour</t>
+          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F394" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G394" t="inlineStr"/>
@@ -16763,7 +16763,7 @@
       <c r="O394" t="inlineStr"/>
       <c r="P394" t="inlineStr">
         <is>
-          <t>Ferroseed Spotlight Hour Tue, Oct 7, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour Wed, Oct 8, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q394" t="inlineStr">
@@ -16783,12 +16783,12 @@
       <c r="D395" t="inlineStr"/>
       <c r="E395" t="inlineStr">
         <is>
-          <t>Ferroseed Spotlight Hour</t>
+          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F395" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G395" t="inlineStr"/>
@@ -16802,7 +16802,7 @@
       <c r="O395" t="inlineStr"/>
       <c r="P395" t="inlineStr">
         <is>
-          <t>Ferroseed Spotlight Hour Tue, Oct 7, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour Wed, Oct 8, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q395" t="inlineStr">
@@ -16822,12 +16822,12 @@
       <c r="D396" t="inlineStr"/>
       <c r="E396" t="inlineStr">
         <is>
-          <t>Ferroseed Spotlight Hour</t>
+          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F396" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G396" t="inlineStr"/>
@@ -16841,7 +16841,7 @@
       <c r="O396" t="inlineStr"/>
       <c r="P396" t="inlineStr">
         <is>
-          <t>Ferroseed Spotlight Hour Tue, Oct 7, at 6:00 PM Local Time</t>
+          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour Wed, Oct 8, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q396" t="inlineStr">
@@ -16861,12 +16861,12 @@
       <c r="D397" t="inlineStr"/>
       <c r="E397" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour</t>
+          <t>Harvest Festival</t>
         </is>
       </c>
       <c r="F397" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G397" t="inlineStr"/>
@@ -16880,7 +16880,7 @@
       <c r="O397" t="inlineStr"/>
       <c r="P397" t="inlineStr">
         <is>
-          <t>Raid Hour Deoxys (Normal &amp; Defense Forme) Raid Hour Wed, Oct 8, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Event Harvest Festival Fri, Oct 10, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q397" t="inlineStr">
@@ -16900,12 +16900,12 @@
       <c r="D398" t="inlineStr"/>
       <c r="E398" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour</t>
+          <t>Harvest Festival</t>
         </is>
       </c>
       <c r="F398" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G398" t="inlineStr"/>
@@ -16919,7 +16919,7 @@
       <c r="O398" t="inlineStr"/>
       <c r="P398" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour Wed, Oct 8, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Harvest Festival Fri, Oct 10, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q398" t="inlineStr">
@@ -16939,12 +16939,12 @@
       <c r="D399" t="inlineStr"/>
       <c r="E399" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour</t>
+          <t>Harvest Festival</t>
         </is>
       </c>
       <c r="F399" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G399" t="inlineStr"/>
@@ -16958,7 +16958,7 @@
       <c r="O399" t="inlineStr"/>
       <c r="P399" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour Wed, Oct 8, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Harvest Festival Fri, Oct 10, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q399" t="inlineStr">
@@ -16978,12 +16978,12 @@
       <c r="D400" t="inlineStr"/>
       <c r="E400" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour</t>
+          <t>Harvest Festival</t>
         </is>
       </c>
       <c r="F400" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G400" t="inlineStr"/>
@@ -16997,7 +16997,7 @@
       <c r="O400" t="inlineStr"/>
       <c r="P400" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour Wed, Oct 8, at 6:00 PM Local Time</t>
+          <t>Harvest Festival Fri, Oct 10, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q400" t="inlineStr">
@@ -17017,12 +17017,12 @@
       <c r="D401" t="inlineStr"/>
       <c r="E401" t="inlineStr">
         <is>
-          <t>Harvest Festival</t>
+          <t>Solosis Community Day</t>
         </is>
       </c>
       <c r="F401" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Community Day</t>
         </is>
       </c>
       <c r="G401" t="inlineStr"/>
@@ -17036,7 +17036,7 @@
       <c r="O401" t="inlineStr"/>
       <c r="P401" t="inlineStr">
         <is>
-          <t>Event Harvest Festival Fri, Oct 10, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Community Day Solosis Community Day Sun, Oct 12, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q401" t="inlineStr">
@@ -17056,12 +17056,12 @@
       <c r="D402" t="inlineStr"/>
       <c r="E402" t="inlineStr">
         <is>
-          <t>Harvest Festival</t>
+          <t>Solosis Community Day</t>
         </is>
       </c>
       <c r="F402" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Community Day</t>
         </is>
       </c>
       <c r="G402" t="inlineStr"/>
@@ -17075,7 +17075,7 @@
       <c r="O402" t="inlineStr"/>
       <c r="P402" t="inlineStr">
         <is>
-          <t>Harvest Festival Fri, Oct 10, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Solosis Community Day Sun, Oct 12, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q402" t="inlineStr">
@@ -17095,12 +17095,12 @@
       <c r="D403" t="inlineStr"/>
       <c r="E403" t="inlineStr">
         <is>
-          <t>Harvest Festival</t>
+          <t>Solosis Community Day</t>
         </is>
       </c>
       <c r="F403" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Community Day</t>
         </is>
       </c>
       <c r="G403" t="inlineStr"/>
@@ -17114,7 +17114,7 @@
       <c r="O403" t="inlineStr"/>
       <c r="P403" t="inlineStr">
         <is>
-          <t>Harvest Festival Fri, Oct 10, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Solosis Community Day Sun, Oct 12, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q403" t="inlineStr">
@@ -17134,12 +17134,12 @@
       <c r="D404" t="inlineStr"/>
       <c r="E404" t="inlineStr">
         <is>
-          <t>Harvest Festival</t>
+          <t>Solosis Community Day</t>
         </is>
       </c>
       <c r="F404" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Community Day</t>
         </is>
       </c>
       <c r="G404" t="inlineStr"/>
@@ -17153,7 +17153,7 @@
       <c r="O404" t="inlineStr"/>
       <c r="P404" t="inlineStr">
         <is>
-          <t>Harvest Festival Fri, Oct 10, at 10:00 AM Local Time</t>
+          <t>Solosis Community Day Sun, Oct 12, at 2:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q404" t="inlineStr">
@@ -17173,12 +17173,12 @@
       <c r="D405" t="inlineStr"/>
       <c r="E405" t="inlineStr">
         <is>
-          <t>Solosis Community Day</t>
+          <t>Dynamax Bounsweet during Max Monday</t>
         </is>
       </c>
       <c r="F405" t="inlineStr">
         <is>
-          <t>Community Day</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G405" t="inlineStr"/>
@@ -17192,7 +17192,7 @@
       <c r="O405" t="inlineStr"/>
       <c r="P405" t="inlineStr">
         <is>
-          <t>Community Day Solosis Community Day Sun, Oct 12, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Max Mondays Dynamax Bounsweet during Max Monday Mon, Oct 13, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q405" t="inlineStr">
@@ -17212,12 +17212,12 @@
       <c r="D406" t="inlineStr"/>
       <c r="E406" t="inlineStr">
         <is>
-          <t>Solosis Community Day</t>
+          <t>Dynamax Bounsweet during Max Monday</t>
         </is>
       </c>
       <c r="F406" t="inlineStr">
         <is>
-          <t>Community Day</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G406" t="inlineStr"/>
@@ -17231,7 +17231,7 @@
       <c r="O406" t="inlineStr"/>
       <c r="P406" t="inlineStr">
         <is>
-          <t>Solosis Community Day Sun, Oct 12, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Dynamax Bounsweet during Max Monday Mon, Oct 13, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q406" t="inlineStr">
@@ -17251,12 +17251,12 @@
       <c r="D407" t="inlineStr"/>
       <c r="E407" t="inlineStr">
         <is>
-          <t>Solosis Community Day</t>
+          <t>Dynamax Bounsweet during Max Monday</t>
         </is>
       </c>
       <c r="F407" t="inlineStr">
         <is>
-          <t>Community Day</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G407" t="inlineStr"/>
@@ -17270,7 +17270,7 @@
       <c r="O407" t="inlineStr"/>
       <c r="P407" t="inlineStr">
         <is>
-          <t>Solosis Community Day Sun, Oct 12, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Dynamax Bounsweet during Max Monday Mon, Oct 13, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q407" t="inlineStr">
@@ -17290,12 +17290,12 @@
       <c r="D408" t="inlineStr"/>
       <c r="E408" t="inlineStr">
         <is>
-          <t>Solosis Community Day</t>
+          <t>Dynamax Bounsweet during Max Monday</t>
         </is>
       </c>
       <c r="F408" t="inlineStr">
         <is>
-          <t>Community Day</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G408" t="inlineStr"/>
@@ -17309,7 +17309,7 @@
       <c r="O408" t="inlineStr"/>
       <c r="P408" t="inlineStr">
         <is>
-          <t>Solosis Community Day Sun, Oct 12, at 2:00 PM Local Time</t>
+          <t>Dynamax Bounsweet during Max Monday Mon, Oct 13, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q408" t="inlineStr">
@@ -17329,12 +17329,12 @@
       <c r="D409" t="inlineStr"/>
       <c r="E409" t="inlineStr">
         <is>
-          <t>Dynamax Bounsweet during Max Monday</t>
+          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F409" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G409" t="inlineStr"/>
@@ -17348,7 +17348,7 @@
       <c r="O409" t="inlineStr"/>
       <c r="P409" t="inlineStr">
         <is>
-          <t>Max Mondays Dynamax Bounsweet during Max Monday Mon, Oct 13, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Raid Battles Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q409" t="inlineStr">
@@ -17368,12 +17368,12 @@
       <c r="D410" t="inlineStr"/>
       <c r="E410" t="inlineStr">
         <is>
-          <t>Dynamax Bounsweet during Max Monday</t>
+          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F410" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G410" t="inlineStr"/>
@@ -17387,7 +17387,7 @@
       <c r="O410" t="inlineStr"/>
       <c r="P410" t="inlineStr">
         <is>
-          <t>Dynamax Bounsweet during Max Monday Mon, Oct 13, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q410" t="inlineStr">
@@ -17407,12 +17407,12 @@
       <c r="D411" t="inlineStr"/>
       <c r="E411" t="inlineStr">
         <is>
-          <t>Dynamax Bounsweet during Max Monday</t>
+          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F411" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G411" t="inlineStr"/>
@@ -17426,7 +17426,7 @@
       <c r="O411" t="inlineStr"/>
       <c r="P411" t="inlineStr">
         <is>
-          <t>Dynamax Bounsweet during Max Monday Mon, Oct 13, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q411" t="inlineStr">
@@ -17446,12 +17446,12 @@
       <c r="D412" t="inlineStr"/>
       <c r="E412" t="inlineStr">
         <is>
-          <t>Dynamax Bounsweet during Max Monday</t>
+          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F412" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G412" t="inlineStr"/>
@@ -17465,7 +17465,7 @@
       <c r="O412" t="inlineStr"/>
       <c r="P412" t="inlineStr">
         <is>
-          <t>Dynamax Bounsweet during Max Monday Mon, Oct 13, at 6:00 PM Local Time</t>
+          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles Tue, Oct 14, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q412" t="inlineStr">
@@ -17485,7 +17485,7 @@
       <c r="D413" t="inlineStr"/>
       <c r="E413" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles</t>
+          <t>Mega Mawile and Mega Salamence in Mega Raids</t>
         </is>
       </c>
       <c r="F413" t="inlineStr">
@@ -17504,7 +17504,7 @@
       <c r="O413" t="inlineStr"/>
       <c r="P413" t="inlineStr">
         <is>
-          <t>Raid Battles Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Raid Battles Mega Mawile and Mega Salamence in Mega Raids Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q413" t="inlineStr">
@@ -17524,7 +17524,7 @@
       <c r="D414" t="inlineStr"/>
       <c r="E414" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles</t>
+          <t>Mega Mawile and Mega Salamence in Mega Raids</t>
         </is>
       </c>
       <c r="F414" t="inlineStr">
@@ -17543,7 +17543,7 @@
       <c r="O414" t="inlineStr"/>
       <c r="P414" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Mega Mawile and Mega Salamence in Mega Raids Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q414" t="inlineStr">
@@ -17563,7 +17563,7 @@
       <c r="D415" t="inlineStr"/>
       <c r="E415" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles</t>
+          <t>Mega Mawile and Mega Salamence in Mega Raids</t>
         </is>
       </c>
       <c r="F415" t="inlineStr">
@@ -17582,7 +17582,7 @@
       <c r="O415" t="inlineStr"/>
       <c r="P415" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Mega Mawile and Mega Salamence in Mega Raids Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q415" t="inlineStr">
@@ -17602,7 +17602,7 @@
       <c r="D416" t="inlineStr"/>
       <c r="E416" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles</t>
+          <t>Mega Mawile and Mega Salamence in Mega Raids</t>
         </is>
       </c>
       <c r="F416" t="inlineStr">
@@ -17621,7 +17621,7 @@
       <c r="O416" t="inlineStr"/>
       <c r="P416" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles Tue, Oct 14, at 10:00 AM Local Time</t>
+          <t>Mega Mawile and Mega Salamence in Mega Raids Tue, Oct 14, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q416" t="inlineStr">
@@ -17641,12 +17641,12 @@
       <c r="D417" t="inlineStr"/>
       <c r="E417" t="inlineStr">
         <is>
-          <t>Mega Mawile and Mega Salamence in Mega Raids</t>
+          <t>Master Premier and Great League Remix | Tales of Transformation</t>
         </is>
       </c>
       <c r="F417" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G417" t="inlineStr"/>
@@ -17660,7 +17660,7 @@
       <c r="O417" t="inlineStr"/>
       <c r="P417" t="inlineStr">
         <is>
-          <t>Raid Battles Mega Mawile and Mega Salamence in Mega Raids Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>GO Battle League Master Premier and Great League Remix | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q417" t="inlineStr">
@@ -17680,12 +17680,12 @@
       <c r="D418" t="inlineStr"/>
       <c r="E418" t="inlineStr">
         <is>
-          <t>Mega Mawile and Mega Salamence in Mega Raids</t>
+          <t>Master Premier and Great League Remix | Tales of Transformation</t>
         </is>
       </c>
       <c r="F418" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G418" t="inlineStr"/>
@@ -17699,7 +17699,7 @@
       <c r="O418" t="inlineStr"/>
       <c r="P418" t="inlineStr">
         <is>
-          <t>Mega Mawile and Mega Salamence in Mega Raids Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Master Premier and Great League Remix | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q418" t="inlineStr">
@@ -17719,12 +17719,12 @@
       <c r="D419" t="inlineStr"/>
       <c r="E419" t="inlineStr">
         <is>
-          <t>Mega Mawile and Mega Salamence in Mega Raids</t>
+          <t>Master Premier and Great League Remix | Tales of Transformation</t>
         </is>
       </c>
       <c r="F419" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G419" t="inlineStr"/>
@@ -17738,7 +17738,7 @@
       <c r="O419" t="inlineStr"/>
       <c r="P419" t="inlineStr">
         <is>
-          <t>Mega Mawile and Mega Salamence in Mega Raids Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Master Premier and Great League Remix | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q419" t="inlineStr">
@@ -17758,12 +17758,12 @@
       <c r="D420" t="inlineStr"/>
       <c r="E420" t="inlineStr">
         <is>
-          <t>Mega Mawile and Mega Salamence in Mega Raids</t>
+          <t>Master Premier and Great League Remix | Tales of Transformation</t>
         </is>
       </c>
       <c r="F420" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G420" t="inlineStr"/>
@@ -17777,7 +17777,7 @@
       <c r="O420" t="inlineStr"/>
       <c r="P420" t="inlineStr">
         <is>
-          <t>Mega Mawile and Mega Salamence in Mega Raids Tue, Oct 14, at 10:00 AM Local Time</t>
+          <t>Master Premier and Great League Remix | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q420" t="inlineStr">
@@ -17797,12 +17797,12 @@
       <c r="D421" t="inlineStr"/>
       <c r="E421" t="inlineStr">
         <is>
-          <t>Master Premier and Great League Remix | Tales of Transformation</t>
+          <t>Petilil Spotlight Hour</t>
         </is>
       </c>
       <c r="F421" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G421" t="inlineStr"/>
@@ -17816,7 +17816,7 @@
       <c r="O421" t="inlineStr"/>
       <c r="P421" t="inlineStr">
         <is>
-          <t>GO Battle League Master Premier and Great League Remix | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Pokémon Spotlight Hour Petilil Spotlight Hour Tue, Oct 14, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q421" t="inlineStr">
@@ -17836,12 +17836,12 @@
       <c r="D422" t="inlineStr"/>
       <c r="E422" t="inlineStr">
         <is>
-          <t>Master Premier and Great League Remix | Tales of Transformation</t>
+          <t>Petilil Spotlight Hour</t>
         </is>
       </c>
       <c r="F422" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G422" t="inlineStr"/>
@@ -17855,7 +17855,7 @@
       <c r="O422" t="inlineStr"/>
       <c r="P422" t="inlineStr">
         <is>
-          <t>Master Premier and Great League Remix | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Petilil Spotlight Hour Tue, Oct 14, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q422" t="inlineStr">
@@ -17875,12 +17875,12 @@
       <c r="D423" t="inlineStr"/>
       <c r="E423" t="inlineStr">
         <is>
-          <t>Master Premier and Great League Remix | Tales of Transformation</t>
+          <t>Petilil Spotlight Hour</t>
         </is>
       </c>
       <c r="F423" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G423" t="inlineStr"/>
@@ -17894,7 +17894,7 @@
       <c r="O423" t="inlineStr"/>
       <c r="P423" t="inlineStr">
         <is>
-          <t>Master Premier and Great League Remix | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Petilil Spotlight Hour Tue, Oct 14, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q423" t="inlineStr">
@@ -17914,12 +17914,12 @@
       <c r="D424" t="inlineStr"/>
       <c r="E424" t="inlineStr">
         <is>
-          <t>Master Premier and Great League Remix | Tales of Transformation</t>
+          <t>Petilil Spotlight Hour</t>
         </is>
       </c>
       <c r="F424" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G424" t="inlineStr"/>
@@ -17933,7 +17933,7 @@
       <c r="O424" t="inlineStr"/>
       <c r="P424" t="inlineStr">
         <is>
-          <t>Master Premier and Great League Remix | Tales of Transformation Calculating...</t>
+          <t>Petilil Spotlight Hour Tue, Oct 14, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q424" t="inlineStr">
@@ -17953,12 +17953,12 @@
       <c r="D425" t="inlineStr"/>
       <c r="E425" t="inlineStr">
         <is>
-          <t>Petilil Spotlight Hour</t>
+          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F425" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G425" t="inlineStr"/>
@@ -17972,7 +17972,7 @@
       <c r="O425" t="inlineStr"/>
       <c r="P425" t="inlineStr">
         <is>
-          <t>Pokémon Spotlight Hour Petilil Spotlight Hour Tue, Oct 14, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Raid Hour Deoxys (Attack &amp; Speed Forme) Raid Hour Wed, Oct 15, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q425" t="inlineStr">
@@ -17992,12 +17992,12 @@
       <c r="D426" t="inlineStr"/>
       <c r="E426" t="inlineStr">
         <is>
-          <t>Petilil Spotlight Hour</t>
+          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F426" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G426" t="inlineStr"/>
@@ -18011,7 +18011,7 @@
       <c r="O426" t="inlineStr"/>
       <c r="P426" t="inlineStr">
         <is>
-          <t>Petilil Spotlight Hour Tue, Oct 14, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour Wed, Oct 15, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q426" t="inlineStr">
@@ -18031,12 +18031,12 @@
       <c r="D427" t="inlineStr"/>
       <c r="E427" t="inlineStr">
         <is>
-          <t>Petilil Spotlight Hour</t>
+          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F427" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G427" t="inlineStr"/>
@@ -18050,7 +18050,7 @@
       <c r="O427" t="inlineStr"/>
       <c r="P427" t="inlineStr">
         <is>
-          <t>Petilil Spotlight Hour Tue, Oct 14, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour Wed, Oct 15, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q427" t="inlineStr">
@@ -18070,12 +18070,12 @@
       <c r="D428" t="inlineStr"/>
       <c r="E428" t="inlineStr">
         <is>
-          <t>Petilil Spotlight Hour</t>
+          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F428" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G428" t="inlineStr"/>
@@ -18089,7 +18089,7 @@
       <c r="O428" t="inlineStr"/>
       <c r="P428" t="inlineStr">
         <is>
-          <t>Petilil Spotlight Hour Tue, Oct 14, at 6:00 PM Local Time</t>
+          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour Wed, Oct 15, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q428" t="inlineStr">
@@ -18109,12 +18109,12 @@
       <c r="D429" t="inlineStr"/>
       <c r="E429" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour</t>
+          <t>Pokémon Legends: Z-A Celebration Event</t>
         </is>
       </c>
       <c r="F429" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G429" t="inlineStr"/>
@@ -18128,7 +18128,7 @@
       <c r="O429" t="inlineStr"/>
       <c r="P429" t="inlineStr">
         <is>
-          <t>Raid Hour Deoxys (Attack &amp; Speed Forme) Raid Hour Wed, Oct 15, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Event Pokémon Legends: Z-A Celebration Event Thu, Oct 16, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q429" t="inlineStr">
@@ -18148,12 +18148,12 @@
       <c r="D430" t="inlineStr"/>
       <c r="E430" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour</t>
+          <t>Pokémon Legends: Z-A Celebration Event</t>
         </is>
       </c>
       <c r="F430" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G430" t="inlineStr"/>
@@ -18167,7 +18167,7 @@
       <c r="O430" t="inlineStr"/>
       <c r="P430" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour Wed, Oct 15, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Pokémon Legends: Z-A Celebration Event Thu, Oct 16, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q430" t="inlineStr">
@@ -18187,12 +18187,12 @@
       <c r="D431" t="inlineStr"/>
       <c r="E431" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour</t>
+          <t>Pokémon Legends: Z-A Celebration Event</t>
         </is>
       </c>
       <c r="F431" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G431" t="inlineStr"/>
@@ -18206,7 +18206,7 @@
       <c r="O431" t="inlineStr"/>
       <c r="P431" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour Wed, Oct 15, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Pokémon Legends: Z-A Celebration Event Thu, Oct 16, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q431" t="inlineStr">
@@ -18226,12 +18226,12 @@
       <c r="D432" t="inlineStr"/>
       <c r="E432" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour</t>
+          <t>Pokémon Legends: Z-A Celebration Event</t>
         </is>
       </c>
       <c r="F432" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G432" t="inlineStr"/>
@@ -18245,7 +18245,7 @@
       <c r="O432" t="inlineStr"/>
       <c r="P432" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour Wed, Oct 15, at 6:00 PM Local Time</t>
+          <t>Pokémon Legends: Z-A Celebration Event Thu, Oct 16, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q432" t="inlineStr">
@@ -18265,12 +18265,12 @@
       <c r="D433" t="inlineStr"/>
       <c r="E433" t="inlineStr">
         <is>
-          <t>Pokémon Legends: Z-A Celebration Event</t>
+          <t>Mega Rayquaza Raid Day</t>
         </is>
       </c>
       <c r="F433" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G433" t="inlineStr"/>
@@ -18284,7 +18284,7 @@
       <c r="O433" t="inlineStr"/>
       <c r="P433" t="inlineStr">
         <is>
-          <t>Event Pokémon Legends: Z-A Celebration Event Thu, Oct 16, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Raid Day Mega Rayquaza Raid Day Sat, Oct 18, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q433" t="inlineStr">
@@ -18304,12 +18304,12 @@
       <c r="D434" t="inlineStr"/>
       <c r="E434" t="inlineStr">
         <is>
-          <t>Pokémon Legends: Z-A Celebration Event</t>
+          <t>Mega Rayquaza Raid Day</t>
         </is>
       </c>
       <c r="F434" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G434" t="inlineStr"/>
@@ -18323,7 +18323,7 @@
       <c r="O434" t="inlineStr"/>
       <c r="P434" t="inlineStr">
         <is>
-          <t>Pokémon Legends: Z-A Celebration Event Thu, Oct 16, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Mega Rayquaza Raid Day Sat, Oct 18, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q434" t="inlineStr">
@@ -18343,12 +18343,12 @@
       <c r="D435" t="inlineStr"/>
       <c r="E435" t="inlineStr">
         <is>
-          <t>Pokémon Legends: Z-A Celebration Event</t>
+          <t>Mega Rayquaza Raid Day</t>
         </is>
       </c>
       <c r="F435" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G435" t="inlineStr"/>
@@ -18362,7 +18362,7 @@
       <c r="O435" t="inlineStr"/>
       <c r="P435" t="inlineStr">
         <is>
-          <t>Pokémon Legends: Z-A Celebration Event Thu, Oct 16, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Mega Rayquaza Raid Day Sat, Oct 18, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q435" t="inlineStr">
@@ -18382,12 +18382,12 @@
       <c r="D436" t="inlineStr"/>
       <c r="E436" t="inlineStr">
         <is>
-          <t>Pokémon Legends: Z-A Celebration Event</t>
+          <t>Mega Rayquaza Raid Day</t>
         </is>
       </c>
       <c r="F436" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G436" t="inlineStr"/>
@@ -18401,7 +18401,7 @@
       <c r="O436" t="inlineStr"/>
       <c r="P436" t="inlineStr">
         <is>
-          <t>Pokémon Legends: Z-A Celebration Event Thu, Oct 16, at 10:00 AM Local Time</t>
+          <t>Mega Rayquaza Raid Day Sat, Oct 18, at 2:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q436" t="inlineStr">
@@ -18421,12 +18421,12 @@
       <c r="D437" t="inlineStr"/>
       <c r="E437" t="inlineStr">
         <is>
-          <t>Mega Rayquaza Raid Day</t>
+          <t>Dynamax Gastly during Max Monday</t>
         </is>
       </c>
       <c r="F437" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G437" t="inlineStr"/>
@@ -18440,7 +18440,7 @@
       <c r="O437" t="inlineStr"/>
       <c r="P437" t="inlineStr">
         <is>
-          <t>Raid Day Mega Rayquaza Raid Day Sat, Oct 18, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Max Mondays Dynamax Gastly during Max Monday Mon, Oct 20, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q437" t="inlineStr">
@@ -18460,12 +18460,12 @@
       <c r="D438" t="inlineStr"/>
       <c r="E438" t="inlineStr">
         <is>
-          <t>Mega Rayquaza Raid Day</t>
+          <t>Dynamax Gastly during Max Monday</t>
         </is>
       </c>
       <c r="F438" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G438" t="inlineStr"/>
@@ -18479,7 +18479,7 @@
       <c r="O438" t="inlineStr"/>
       <c r="P438" t="inlineStr">
         <is>
-          <t>Mega Rayquaza Raid Day Sat, Oct 18, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Dynamax Gastly during Max Monday Mon, Oct 20, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q438" t="inlineStr">
@@ -18499,12 +18499,12 @@
       <c r="D439" t="inlineStr"/>
       <c r="E439" t="inlineStr">
         <is>
-          <t>Mega Rayquaza Raid Day</t>
+          <t>Dynamax Gastly during Max Monday</t>
         </is>
       </c>
       <c r="F439" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G439" t="inlineStr"/>
@@ -18518,7 +18518,7 @@
       <c r="O439" t="inlineStr"/>
       <c r="P439" t="inlineStr">
         <is>
-          <t>Mega Rayquaza Raid Day Sat, Oct 18, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Dynamax Gastly during Max Monday Mon, Oct 20, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q439" t="inlineStr">
@@ -18538,12 +18538,12 @@
       <c r="D440" t="inlineStr"/>
       <c r="E440" t="inlineStr">
         <is>
-          <t>Mega Rayquaza Raid Day</t>
+          <t>Dynamax Gastly during Max Monday</t>
         </is>
       </c>
       <c r="F440" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G440" t="inlineStr"/>
@@ -18557,7 +18557,7 @@
       <c r="O440" t="inlineStr"/>
       <c r="P440" t="inlineStr">
         <is>
-          <t>Mega Rayquaza Raid Day Sat, Oct 18, at 2:00 PM Local Time</t>
+          <t>Dynamax Gastly during Max Monday Mon, Oct 20, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q440" t="inlineStr">
@@ -18577,7 +18577,7 @@
       <c r="D441" t="inlineStr"/>
       <c r="E441" t="inlineStr">
         <is>
-          <t>Dynamax Gastly during Max Monday</t>
+          <t>Halloween 2025 Part I</t>
         </is>
       </c>
       <c r="F441" t="inlineStr">
@@ -18596,7 +18596,7 @@
       <c r="O441" t="inlineStr"/>
       <c r="P441" t="inlineStr">
         <is>
-          <t>Max Mondays Dynamax Gastly during Max Monday Mon, Oct 20, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Event Halloween 2025 Part I Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q441" t="inlineStr">
@@ -18616,7 +18616,7 @@
       <c r="D442" t="inlineStr"/>
       <c r="E442" t="inlineStr">
         <is>
-          <t>Dynamax Gastly during Max Monday</t>
+          <t>Halloween 2025 Part I</t>
         </is>
       </c>
       <c r="F442" t="inlineStr">
@@ -18635,7 +18635,7 @@
       <c r="O442" t="inlineStr"/>
       <c r="P442" t="inlineStr">
         <is>
-          <t>Dynamax Gastly during Max Monday Mon, Oct 20, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Halloween 2025 Part I Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q442" t="inlineStr">
@@ -18655,7 +18655,7 @@
       <c r="D443" t="inlineStr"/>
       <c r="E443" t="inlineStr">
         <is>
-          <t>Dynamax Gastly during Max Monday</t>
+          <t>Halloween 2025 Part I</t>
         </is>
       </c>
       <c r="F443" t="inlineStr">
@@ -18674,7 +18674,7 @@
       <c r="O443" t="inlineStr"/>
       <c r="P443" t="inlineStr">
         <is>
-          <t>Dynamax Gastly during Max Monday Mon, Oct 20, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Halloween 2025 Part I Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q443" t="inlineStr">
@@ -18694,7 +18694,7 @@
       <c r="D444" t="inlineStr"/>
       <c r="E444" t="inlineStr">
         <is>
-          <t>Dynamax Gastly during Max Monday</t>
+          <t>Halloween 2025 Part I</t>
         </is>
       </c>
       <c r="F444" t="inlineStr">
@@ -18713,7 +18713,7 @@
       <c r="O444" t="inlineStr"/>
       <c r="P444" t="inlineStr">
         <is>
-          <t>Dynamax Gastly during Max Monday Mon, Oct 20, at 6:00 PM Local Time</t>
+          <t>Halloween 2025 Part I Tue, Oct 21, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q444" t="inlineStr">
@@ -18733,12 +18733,12 @@
       <c r="D445" t="inlineStr"/>
       <c r="E445" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part I</t>
+          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F445" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G445" t="inlineStr"/>
@@ -18752,7 +18752,7 @@
       <c r="O445" t="inlineStr"/>
       <c r="P445" t="inlineStr">
         <is>
-          <t>Event Halloween 2025 Part I Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Raid Battles Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q445" t="inlineStr">
@@ -18772,12 +18772,12 @@
       <c r="D446" t="inlineStr"/>
       <c r="E446" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part I</t>
+          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F446" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G446" t="inlineStr"/>
@@ -18791,7 +18791,7 @@
       <c r="O446" t="inlineStr"/>
       <c r="P446" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part I Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q446" t="inlineStr">
@@ -18811,12 +18811,12 @@
       <c r="D447" t="inlineStr"/>
       <c r="E447" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part I</t>
+          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F447" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G447" t="inlineStr"/>
@@ -18830,7 +18830,7 @@
       <c r="O447" t="inlineStr"/>
       <c r="P447" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part I Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q447" t="inlineStr">
@@ -18850,12 +18850,12 @@
       <c r="D448" t="inlineStr"/>
       <c r="E448" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part I</t>
+          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F448" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G448" t="inlineStr"/>
@@ -18869,7 +18869,7 @@
       <c r="O448" t="inlineStr"/>
       <c r="P448" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part I Tue, Oct 21, at 10:00 AM Local Time</t>
+          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles Tue, Oct 21, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q448" t="inlineStr">
@@ -18889,7 +18889,7 @@
       <c r="D449" t="inlineStr"/>
       <c r="E449" t="inlineStr">
         <is>
-          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles</t>
+          <t>Mega Houndoom and Mega Absol in Mega Raids</t>
         </is>
       </c>
       <c r="F449" t="inlineStr">
@@ -18908,7 +18908,7 @@
       <c r="O449" t="inlineStr"/>
       <c r="P449" t="inlineStr">
         <is>
-          <t>Raid Battles Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Raid Battles Mega Houndoom and Mega Absol in Mega Raids Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q449" t="inlineStr">
@@ -18928,7 +18928,7 @@
       <c r="D450" t="inlineStr"/>
       <c r="E450" t="inlineStr">
         <is>
-          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles</t>
+          <t>Mega Houndoom and Mega Absol in Mega Raids</t>
         </is>
       </c>
       <c r="F450" t="inlineStr">
@@ -18947,7 +18947,7 @@
       <c r="O450" t="inlineStr"/>
       <c r="P450" t="inlineStr">
         <is>
-          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Mega Houndoom and Mega Absol in Mega Raids Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q450" t="inlineStr">
@@ -18967,7 +18967,7 @@
       <c r="D451" t="inlineStr"/>
       <c r="E451" t="inlineStr">
         <is>
-          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles</t>
+          <t>Mega Houndoom and Mega Absol in Mega Raids</t>
         </is>
       </c>
       <c r="F451" t="inlineStr">
@@ -18986,7 +18986,7 @@
       <c r="O451" t="inlineStr"/>
       <c r="P451" t="inlineStr">
         <is>
-          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Mega Houndoom and Mega Absol in Mega Raids Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q451" t="inlineStr">
@@ -19006,7 +19006,7 @@
       <c r="D452" t="inlineStr"/>
       <c r="E452" t="inlineStr">
         <is>
-          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles</t>
+          <t>Mega Houndoom and Mega Absol in Mega Raids</t>
         </is>
       </c>
       <c r="F452" t="inlineStr">
@@ -19025,7 +19025,7 @@
       <c r="O452" t="inlineStr"/>
       <c r="P452" t="inlineStr">
         <is>
-          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles Tue, Oct 21, at 10:00 AM Local Time</t>
+          <t>Mega Houndoom and Mega Absol in Mega Raids Tue, Oct 21, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q452" t="inlineStr">
@@ -19045,12 +19045,12 @@
       <c r="D453" t="inlineStr"/>
       <c r="E453" t="inlineStr">
         <is>
-          <t>Mega Houndoom and Mega Absol in Mega Raids</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F453" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G453" t="inlineStr"/>
@@ -19064,7 +19064,7 @@
       <c r="O453" t="inlineStr"/>
       <c r="P453" t="inlineStr">
         <is>
-          <t>Raid Battles Mega Houndoom and Mega Absol in Mega Raids Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>GO Battle League Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q453" t="inlineStr">
@@ -19084,12 +19084,12 @@
       <c r="D454" t="inlineStr"/>
       <c r="E454" t="inlineStr">
         <is>
-          <t>Mega Houndoom and Mega Absol in Mega Raids</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F454" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G454" t="inlineStr"/>
@@ -19103,7 +19103,7 @@
       <c r="O454" t="inlineStr"/>
       <c r="P454" t="inlineStr">
         <is>
-          <t>Mega Houndoom and Mega Absol in Mega Raids Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q454" t="inlineStr">
@@ -19123,12 +19123,12 @@
       <c r="D455" t="inlineStr"/>
       <c r="E455" t="inlineStr">
         <is>
-          <t>Mega Houndoom and Mega Absol in Mega Raids</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F455" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G455" t="inlineStr"/>
@@ -19142,7 +19142,7 @@
       <c r="O455" t="inlineStr"/>
       <c r="P455" t="inlineStr">
         <is>
-          <t>Mega Houndoom and Mega Absol in Mega Raids Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q455" t="inlineStr">
@@ -19162,12 +19162,12 @@
       <c r="D456" t="inlineStr"/>
       <c r="E456" t="inlineStr">
         <is>
-          <t>Mega Houndoom and Mega Absol in Mega Raids</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F456" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G456" t="inlineStr"/>
@@ -19181,7 +19181,7 @@
       <c r="O456" t="inlineStr"/>
       <c r="P456" t="inlineStr">
         <is>
-          <t>Mega Houndoom and Mega Absol in Mega Raids Tue, Oct 21, at 10:00 AM Local Time</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q456" t="inlineStr">
@@ -19201,12 +19201,12 @@
       <c r="D457" t="inlineStr"/>
       <c r="E457" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Gastly Spotlight Hour</t>
         </is>
       </c>
       <c r="F457" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G457" t="inlineStr"/>
@@ -19220,7 +19220,7 @@
       <c r="O457" t="inlineStr"/>
       <c r="P457" t="inlineStr">
         <is>
-          <t>GO Battle League Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Pokémon Spotlight Hour Gastly Spotlight Hour Tue, Oct 21, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q457" t="inlineStr">
@@ -19240,12 +19240,12 @@
       <c r="D458" t="inlineStr"/>
       <c r="E458" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Gastly Spotlight Hour</t>
         </is>
       </c>
       <c r="F458" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G458" t="inlineStr"/>
@@ -19259,7 +19259,7 @@
       <c r="O458" t="inlineStr"/>
       <c r="P458" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Gastly Spotlight Hour Tue, Oct 21, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q458" t="inlineStr">
@@ -19279,12 +19279,12 @@
       <c r="D459" t="inlineStr"/>
       <c r="E459" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Gastly Spotlight Hour</t>
         </is>
       </c>
       <c r="F459" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G459" t="inlineStr"/>
@@ -19298,7 +19298,7 @@
       <c r="O459" t="inlineStr"/>
       <c r="P459" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Gastly Spotlight Hour Tue, Oct 21, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q459" t="inlineStr">
@@ -19318,12 +19318,12 @@
       <c r="D460" t="inlineStr"/>
       <c r="E460" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Gastly Spotlight Hour</t>
         </is>
       </c>
       <c r="F460" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G460" t="inlineStr"/>
@@ -19337,7 +19337,7 @@
       <c r="O460" t="inlineStr"/>
       <c r="P460" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating...</t>
+          <t>Gastly Spotlight Hour Tue, Oct 21, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q460" t="inlineStr">
@@ -19357,12 +19357,12 @@
       <c r="D461" t="inlineStr"/>
       <c r="E461" t="inlineStr">
         <is>
-          <t>Gastly Spotlight Hour</t>
+          <t>Genesect Raid Hour</t>
         </is>
       </c>
       <c r="F461" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G461" t="inlineStr"/>
@@ -19376,7 +19376,7 @@
       <c r="O461" t="inlineStr"/>
       <c r="P461" t="inlineStr">
         <is>
-          <t>Pokémon Spotlight Hour Gastly Spotlight Hour Tue, Oct 21, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Raid Hour Genesect Raid Hour Wed, Oct 22, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q461" t="inlineStr">
@@ -19396,12 +19396,12 @@
       <c r="D462" t="inlineStr"/>
       <c r="E462" t="inlineStr">
         <is>
-          <t>Gastly Spotlight Hour</t>
+          <t>Genesect Raid Hour</t>
         </is>
       </c>
       <c r="F462" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G462" t="inlineStr"/>
@@ -19415,7 +19415,7 @@
       <c r="O462" t="inlineStr"/>
       <c r="P462" t="inlineStr">
         <is>
-          <t>Gastly Spotlight Hour Tue, Oct 21, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Genesect Raid Hour Wed, Oct 22, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q462" t="inlineStr">
@@ -19435,12 +19435,12 @@
       <c r="D463" t="inlineStr"/>
       <c r="E463" t="inlineStr">
         <is>
-          <t>Gastly Spotlight Hour</t>
+          <t>Genesect Raid Hour</t>
         </is>
       </c>
       <c r="F463" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G463" t="inlineStr"/>
@@ -19454,7 +19454,7 @@
       <c r="O463" t="inlineStr"/>
       <c r="P463" t="inlineStr">
         <is>
-          <t>Gastly Spotlight Hour Tue, Oct 21, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Genesect Raid Hour Wed, Oct 22, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q463" t="inlineStr">
@@ -19474,12 +19474,12 @@
       <c r="D464" t="inlineStr"/>
       <c r="E464" t="inlineStr">
         <is>
-          <t>Gastly Spotlight Hour</t>
+          <t>Genesect Raid Hour</t>
         </is>
       </c>
       <c r="F464" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G464" t="inlineStr"/>
@@ -19493,7 +19493,7 @@
       <c r="O464" t="inlineStr"/>
       <c r="P464" t="inlineStr">
         <is>
-          <t>Gastly Spotlight Hour Tue, Oct 21, at 6:00 PM Local Time</t>
+          <t>Genesect Raid Hour Wed, Oct 22, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q464" t="inlineStr">
@@ -19513,12 +19513,12 @@
       <c r="D465" t="inlineStr"/>
       <c r="E465" t="inlineStr">
         <is>
-          <t>Genesect Raid Hour</t>
+          <t>GO Battle Weekend: Tales of Transformation</t>
         </is>
       </c>
       <c r="F465" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G465" t="inlineStr"/>
@@ -19532,7 +19532,7 @@
       <c r="O465" t="inlineStr"/>
       <c r="P465" t="inlineStr">
         <is>
-          <t>Raid Hour Genesect Raid Hour Wed, Oct 22, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Event GO Battle Weekend: Tales of Transformation Sat, Oct 25, at 12:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q465" t="inlineStr">
@@ -19552,12 +19552,12 @@
       <c r="D466" t="inlineStr"/>
       <c r="E466" t="inlineStr">
         <is>
-          <t>Genesect Raid Hour</t>
+          <t>GO Battle Weekend: Tales of Transformation</t>
         </is>
       </c>
       <c r="F466" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G466" t="inlineStr"/>
@@ -19571,7 +19571,7 @@
       <c r="O466" t="inlineStr"/>
       <c r="P466" t="inlineStr">
         <is>
-          <t>Genesect Raid Hour Wed, Oct 22, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>GO Battle Weekend: Tales of Transformation Sat, Oct 25, at 12:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q466" t="inlineStr">
@@ -19591,12 +19591,12 @@
       <c r="D467" t="inlineStr"/>
       <c r="E467" t="inlineStr">
         <is>
-          <t>Genesect Raid Hour</t>
+          <t>GO Battle Weekend: Tales of Transformation</t>
         </is>
       </c>
       <c r="F467" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G467" t="inlineStr"/>
@@ -19610,7 +19610,7 @@
       <c r="O467" t="inlineStr"/>
       <c r="P467" t="inlineStr">
         <is>
-          <t>Genesect Raid Hour Wed, Oct 22, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>GO Battle Weekend: Tales of Transformation Sat, Oct 25, at 12:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q467" t="inlineStr">
@@ -19630,12 +19630,12 @@
       <c r="D468" t="inlineStr"/>
       <c r="E468" t="inlineStr">
         <is>
-          <t>Genesect Raid Hour</t>
+          <t>GO Battle Weekend: Tales of Transformation</t>
         </is>
       </c>
       <c r="F468" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G468" t="inlineStr"/>
@@ -19649,7 +19649,7 @@
       <c r="O468" t="inlineStr"/>
       <c r="P468" t="inlineStr">
         <is>
-          <t>Genesect Raid Hour Wed, Oct 22, at 6:00 PM Local Time</t>
+          <t>GO Battle Weekend: Tales of Transformation Sat, Oct 25, at 12:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q468" t="inlineStr">
@@ -19669,7 +19669,7 @@
       <c r="D469" t="inlineStr"/>
       <c r="E469" t="inlineStr">
         <is>
-          <t>GO Battle Weekend: Tales of Transformation</t>
+          <t>Halloween 2025 Part II</t>
         </is>
       </c>
       <c r="F469" t="inlineStr">
@@ -19688,7 +19688,7 @@
       <c r="O469" t="inlineStr"/>
       <c r="P469" t="inlineStr">
         <is>
-          <t>Event GO Battle Weekend: Tales of Transformation Sat, Oct 25, at 12:00 AM Local Time Starts: Calculating...</t>
+          <t>Event Halloween 2025 Part II Mon, Oct 27, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q469" t="inlineStr">
@@ -19708,7 +19708,7 @@
       <c r="D470" t="inlineStr"/>
       <c r="E470" t="inlineStr">
         <is>
-          <t>GO Battle Weekend: Tales of Transformation</t>
+          <t>Halloween 2025 Part II</t>
         </is>
       </c>
       <c r="F470" t="inlineStr">
@@ -19727,7 +19727,7 @@
       <c r="O470" t="inlineStr"/>
       <c r="P470" t="inlineStr">
         <is>
-          <t>GO Battle Weekend: Tales of Transformation Sat, Oct 25, at 12:00 AM Local Time Starts: Calculating...</t>
+          <t>Halloween 2025 Part II Mon, Oct 27, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q470" t="inlineStr">
@@ -19747,7 +19747,7 @@
       <c r="D471" t="inlineStr"/>
       <c r="E471" t="inlineStr">
         <is>
-          <t>GO Battle Weekend: Tales of Transformation</t>
+          <t>Halloween 2025 Part II</t>
         </is>
       </c>
       <c r="F471" t="inlineStr">
@@ -19766,7 +19766,7 @@
       <c r="O471" t="inlineStr"/>
       <c r="P471" t="inlineStr">
         <is>
-          <t>GO Battle Weekend: Tales of Transformation Sat, Oct 25, at 12:00 AM Local Time Starts: Calculating...</t>
+          <t>Halloween 2025 Part II Mon, Oct 27, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q471" t="inlineStr">
@@ -19786,7 +19786,7 @@
       <c r="D472" t="inlineStr"/>
       <c r="E472" t="inlineStr">
         <is>
-          <t>GO Battle Weekend: Tales of Transformation</t>
+          <t>Halloween 2025 Part II</t>
         </is>
       </c>
       <c r="F472" t="inlineStr">
@@ -19805,7 +19805,7 @@
       <c r="O472" t="inlineStr"/>
       <c r="P472" t="inlineStr">
         <is>
-          <t>GO Battle Weekend: Tales of Transformation Sat, Oct 25, at 12:00 AM Local Time</t>
+          <t>Halloween 2025 Part II Mon, Oct 27, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q472" t="inlineStr">
@@ -19825,7 +19825,7 @@
       <c r="D473" t="inlineStr"/>
       <c r="E473" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part II</t>
+          <t>Dynamax Woobat during Max Monday</t>
         </is>
       </c>
       <c r="F473" t="inlineStr">
@@ -19844,7 +19844,7 @@
       <c r="O473" t="inlineStr"/>
       <c r="P473" t="inlineStr">
         <is>
-          <t>Event Halloween 2025 Part II Mon, Oct 27, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Max Mondays Dynamax Woobat during Max Monday Mon, Oct 27, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q473" t="inlineStr">
@@ -19864,7 +19864,7 @@
       <c r="D474" t="inlineStr"/>
       <c r="E474" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part II</t>
+          <t>Dynamax Woobat during Max Monday</t>
         </is>
       </c>
       <c r="F474" t="inlineStr">
@@ -19883,7 +19883,7 @@
       <c r="O474" t="inlineStr"/>
       <c r="P474" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part II Mon, Oct 27, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Dynamax Woobat during Max Monday Mon, Oct 27, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q474" t="inlineStr">
@@ -19903,7 +19903,7 @@
       <c r="D475" t="inlineStr"/>
       <c r="E475" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part II</t>
+          <t>Dynamax Woobat during Max Monday</t>
         </is>
       </c>
       <c r="F475" t="inlineStr">
@@ -19922,7 +19922,7 @@
       <c r="O475" t="inlineStr"/>
       <c r="P475" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part II Mon, Oct 27, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Dynamax Woobat during Max Monday Mon, Oct 27, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q475" t="inlineStr">
@@ -19942,7 +19942,7 @@
       <c r="D476" t="inlineStr"/>
       <c r="E476" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part II</t>
+          <t>Dynamax Woobat during Max Monday</t>
         </is>
       </c>
       <c r="F476" t="inlineStr">
@@ -19961,7 +19961,7 @@
       <c r="O476" t="inlineStr"/>
       <c r="P476" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part II Mon, Oct 27, at 10:00 AM Local Time</t>
+          <t>Dynamax Woobat during Max Monday Mon, Oct 27, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q476" t="inlineStr">
@@ -19981,12 +19981,12 @@
       <c r="D477" t="inlineStr"/>
       <c r="E477" t="inlineStr">
         <is>
-          <t>Dynamax Woobat during Max Monday</t>
+          <t>Giratina (Altered Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F477" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G477" t="inlineStr"/>
@@ -20000,7 +20000,7 @@
       <c r="O477" t="inlineStr"/>
       <c r="P477" t="inlineStr">
         <is>
-          <t>Max Mondays Dynamax Woobat during Max Monday Mon, Oct 27, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Raid Battles Giratina (Altered Forme) in 5-star Raid Battles Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q477" t="inlineStr">
@@ -20020,12 +20020,12 @@
       <c r="D478" t="inlineStr"/>
       <c r="E478" t="inlineStr">
         <is>
-          <t>Dynamax Woobat during Max Monday</t>
+          <t>Giratina (Altered Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F478" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G478" t="inlineStr"/>
@@ -20039,7 +20039,7 @@
       <c r="O478" t="inlineStr"/>
       <c r="P478" t="inlineStr">
         <is>
-          <t>Dynamax Woobat during Max Monday Mon, Oct 27, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Giratina (Altered Forme) in 5-star Raid Battles Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q478" t="inlineStr">
@@ -20059,12 +20059,12 @@
       <c r="D479" t="inlineStr"/>
       <c r="E479" t="inlineStr">
         <is>
-          <t>Dynamax Woobat during Max Monday</t>
+          <t>Giratina (Altered Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F479" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G479" t="inlineStr"/>
@@ -20078,7 +20078,7 @@
       <c r="O479" t="inlineStr"/>
       <c r="P479" t="inlineStr">
         <is>
-          <t>Dynamax Woobat during Max Monday Mon, Oct 27, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Giratina (Altered Forme) in 5-star Raid Battles Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q479" t="inlineStr">
@@ -20098,12 +20098,12 @@
       <c r="D480" t="inlineStr"/>
       <c r="E480" t="inlineStr">
         <is>
-          <t>Dynamax Woobat during Max Monday</t>
+          <t>Giratina (Altered Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F480" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G480" t="inlineStr"/>
@@ -20117,7 +20117,7 @@
       <c r="O480" t="inlineStr"/>
       <c r="P480" t="inlineStr">
         <is>
-          <t>Dynamax Woobat during Max Monday Mon, Oct 27, at 6:00 PM Local Time</t>
+          <t>Giratina (Altered Forme) in 5-star Raid Battles Tue, Oct 28, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q480" t="inlineStr">
@@ -20137,7 +20137,7 @@
       <c r="D481" t="inlineStr"/>
       <c r="E481" t="inlineStr">
         <is>
-          <t>Giratina (Altered Forme) in 5-star Raid Battles</t>
+          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids</t>
         </is>
       </c>
       <c r="F481" t="inlineStr">
@@ -20156,7 +20156,7 @@
       <c r="O481" t="inlineStr"/>
       <c r="P481" t="inlineStr">
         <is>
-          <t>Raid Battles Giratina (Altered Forme) in 5-star Raid Battles Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Raid Battles Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q481" t="inlineStr">
@@ -20176,7 +20176,7 @@
       <c r="D482" t="inlineStr"/>
       <c r="E482" t="inlineStr">
         <is>
-          <t>Giratina (Altered Forme) in 5-star Raid Battles</t>
+          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids</t>
         </is>
       </c>
       <c r="F482" t="inlineStr">
@@ -20195,7 +20195,7 @@
       <c r="O482" t="inlineStr"/>
       <c r="P482" t="inlineStr">
         <is>
-          <t>Giratina (Altered Forme) in 5-star Raid Battles Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q482" t="inlineStr">
@@ -20215,7 +20215,7 @@
       <c r="D483" t="inlineStr"/>
       <c r="E483" t="inlineStr">
         <is>
-          <t>Giratina (Altered Forme) in 5-star Raid Battles</t>
+          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids</t>
         </is>
       </c>
       <c r="F483" t="inlineStr">
@@ -20234,7 +20234,7 @@
       <c r="O483" t="inlineStr"/>
       <c r="P483" t="inlineStr">
         <is>
-          <t>Giratina (Altered Forme) in 5-star Raid Battles Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q483" t="inlineStr">
@@ -20254,7 +20254,7 @@
       <c r="D484" t="inlineStr"/>
       <c r="E484" t="inlineStr">
         <is>
-          <t>Giratina (Altered Forme) in 5-star Raid Battles</t>
+          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids</t>
         </is>
       </c>
       <c r="F484" t="inlineStr">
@@ -20273,7 +20273,7 @@
       <c r="O484" t="inlineStr"/>
       <c r="P484" t="inlineStr">
         <is>
-          <t>Giratina (Altered Forme) in 5-star Raid Battles Tue, Oct 28, at 10:00 AM Local Time</t>
+          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids Tue, Oct 28, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q484" t="inlineStr">
@@ -20293,12 +20293,12 @@
       <c r="D485" t="inlineStr"/>
       <c r="E485" t="inlineStr">
         <is>
-          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids</t>
+          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F485" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G485" t="inlineStr"/>
@@ -20312,7 +20312,7 @@
       <c r="O485" t="inlineStr"/>
       <c r="P485" t="inlineStr">
         <is>
-          <t>Raid Battles Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>GO Battle League Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q485" t="inlineStr">
@@ -20332,12 +20332,12 @@
       <c r="D486" t="inlineStr"/>
       <c r="E486" t="inlineStr">
         <is>
-          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids</t>
+          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F486" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G486" t="inlineStr"/>
@@ -20351,7 +20351,7 @@
       <c r="O486" t="inlineStr"/>
       <c r="P486" t="inlineStr">
         <is>
-          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q486" t="inlineStr">
@@ -20371,12 +20371,12 @@
       <c r="D487" t="inlineStr"/>
       <c r="E487" t="inlineStr">
         <is>
-          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids</t>
+          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F487" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G487" t="inlineStr"/>
@@ -20390,7 +20390,7 @@
       <c r="O487" t="inlineStr"/>
       <c r="P487" t="inlineStr">
         <is>
-          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q487" t="inlineStr">
@@ -20410,12 +20410,12 @@
       <c r="D488" t="inlineStr"/>
       <c r="E488" t="inlineStr">
         <is>
-          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids</t>
+          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F488" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G488" t="inlineStr"/>
@@ -20429,7 +20429,7 @@
       <c r="O488" t="inlineStr"/>
       <c r="P488" t="inlineStr">
         <is>
-          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids Tue, Oct 28, at 10:00 AM Local Time</t>
+          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q488" t="inlineStr">
@@ -20449,12 +20449,12 @@
       <c r="D489" t="inlineStr"/>
       <c r="E489" t="inlineStr">
         <is>
-          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation</t>
+          <t>Sinistea Spotlight Hour</t>
         </is>
       </c>
       <c r="F489" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G489" t="inlineStr"/>
@@ -20468,7 +20468,7 @@
       <c r="O489" t="inlineStr"/>
       <c r="P489" t="inlineStr">
         <is>
-          <t>GO Battle League Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Pokémon Spotlight Hour Sinistea Spotlight Hour Tue, Oct 28, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q489" t="inlineStr">
@@ -20488,12 +20488,12 @@
       <c r="D490" t="inlineStr"/>
       <c r="E490" t="inlineStr">
         <is>
-          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation</t>
+          <t>Sinistea Spotlight Hour</t>
         </is>
       </c>
       <c r="F490" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G490" t="inlineStr"/>
@@ -20507,7 +20507,7 @@
       <c r="O490" t="inlineStr"/>
       <c r="P490" t="inlineStr">
         <is>
-          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Sinistea Spotlight Hour Tue, Oct 28, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q490" t="inlineStr">
@@ -20527,12 +20527,12 @@
       <c r="D491" t="inlineStr"/>
       <c r="E491" t="inlineStr">
         <is>
-          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation</t>
+          <t>Sinistea Spotlight Hour</t>
         </is>
       </c>
       <c r="F491" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G491" t="inlineStr"/>
@@ -20546,7 +20546,7 @@
       <c r="O491" t="inlineStr"/>
       <c r="P491" t="inlineStr">
         <is>
-          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Sinistea Spotlight Hour Tue, Oct 28, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q491" t="inlineStr">
@@ -20566,12 +20566,12 @@
       <c r="D492" t="inlineStr"/>
       <c r="E492" t="inlineStr">
         <is>
-          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation</t>
+          <t>Sinistea Spotlight Hour</t>
         </is>
       </c>
       <c r="F492" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G492" t="inlineStr"/>
@@ -20585,7 +20585,7 @@
       <c r="O492" t="inlineStr"/>
       <c r="P492" t="inlineStr">
         <is>
-          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating...</t>
+          <t>Sinistea Spotlight Hour Tue, Oct 28, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q492" t="inlineStr">
@@ -20605,12 +20605,12 @@
       <c r="D493" t="inlineStr"/>
       <c r="E493" t="inlineStr">
         <is>
-          <t>Sinistea Spotlight Hour</t>
+          <t>Giratina (Origin Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F493" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G493" t="inlineStr"/>
@@ -20624,7 +20624,7 @@
       <c r="O493" t="inlineStr"/>
       <c r="P493" t="inlineStr">
         <is>
-          <t>Pokémon Spotlight Hour Sinistea Spotlight Hour Tue, Oct 28, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Raid Hour Giratina (Origin Forme) Raid Hour Wed, Oct 29, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q493" t="inlineStr">
@@ -20644,12 +20644,12 @@
       <c r="D494" t="inlineStr"/>
       <c r="E494" t="inlineStr">
         <is>
-          <t>Sinistea Spotlight Hour</t>
+          <t>Giratina (Origin Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F494" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G494" t="inlineStr"/>
@@ -20663,7 +20663,7 @@
       <c r="O494" t="inlineStr"/>
       <c r="P494" t="inlineStr">
         <is>
-          <t>Sinistea Spotlight Hour Tue, Oct 28, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Giratina (Origin Forme) Raid Hour Wed, Oct 29, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q494" t="inlineStr">
@@ -20683,12 +20683,12 @@
       <c r="D495" t="inlineStr"/>
       <c r="E495" t="inlineStr">
         <is>
-          <t>Sinistea Spotlight Hour</t>
+          <t>Giratina (Origin Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F495" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G495" t="inlineStr"/>
@@ -20702,7 +20702,7 @@
       <c r="O495" t="inlineStr"/>
       <c r="P495" t="inlineStr">
         <is>
-          <t>Sinistea Spotlight Hour Tue, Oct 28, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Giratina (Origin Forme) Raid Hour Wed, Oct 29, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q495" t="inlineStr">
@@ -20722,12 +20722,12 @@
       <c r="D496" t="inlineStr"/>
       <c r="E496" t="inlineStr">
         <is>
-          <t>Sinistea Spotlight Hour</t>
+          <t>Giratina (Origin Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F496" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G496" t="inlineStr"/>
@@ -20741,7 +20741,7 @@
       <c r="O496" t="inlineStr"/>
       <c r="P496" t="inlineStr">
         <is>
-          <t>Sinistea Spotlight Hour Tue, Oct 28, at 6:00 PM Local Time</t>
+          <t>Giratina (Origin Forme) Raid Hour Wed, Oct 29, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q496" t="inlineStr">
@@ -20761,12 +20761,12 @@
       <c r="D497" t="inlineStr"/>
       <c r="E497" t="inlineStr">
         <is>
-          <t>Giratina (Origin Forme) Raid Hour</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F497" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G497" t="inlineStr"/>
@@ -20780,7 +20780,7 @@
       <c r="O497" t="inlineStr"/>
       <c r="P497" t="inlineStr">
         <is>
-          <t>Raid Hour Giratina (Origin Forme) Raid Hour Wed, Oct 29, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>GO Battle League Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q497" t="inlineStr">
@@ -20800,12 +20800,12 @@
       <c r="D498" t="inlineStr"/>
       <c r="E498" t="inlineStr">
         <is>
-          <t>Giratina (Origin Forme) Raid Hour</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F498" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G498" t="inlineStr"/>
@@ -20819,7 +20819,7 @@
       <c r="O498" t="inlineStr"/>
       <c r="P498" t="inlineStr">
         <is>
-          <t>Giratina (Origin Forme) Raid Hour Wed, Oct 29, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q498" t="inlineStr">
@@ -20839,12 +20839,12 @@
       <c r="D499" t="inlineStr"/>
       <c r="E499" t="inlineStr">
         <is>
-          <t>Giratina (Origin Forme) Raid Hour</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F499" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G499" t="inlineStr"/>
@@ -20858,7 +20858,7 @@
       <c r="O499" t="inlineStr"/>
       <c r="P499" t="inlineStr">
         <is>
-          <t>Giratina (Origin Forme) Raid Hour Wed, Oct 29, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q499" t="inlineStr">
@@ -20878,12 +20878,12 @@
       <c r="D500" t="inlineStr"/>
       <c r="E500" t="inlineStr">
         <is>
-          <t>Giratina (Origin Forme) Raid Hour</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F500" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G500" t="inlineStr"/>
@@ -20897,7 +20897,7 @@
       <c r="O500" t="inlineStr"/>
       <c r="P500" t="inlineStr">
         <is>
-          <t>Giratina (Origin Forme) Raid Hour Wed, Oct 29, at 6:00 PM Local Time</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q500" t="inlineStr">
@@ -20917,7 +20917,7 @@
       <c r="D501" t="inlineStr"/>
       <c r="E501" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
+          <t>Pokémon GO Wild Area: Nagasaki</t>
         </is>
       </c>
       <c r="F501" t="inlineStr">
@@ -20936,7 +20936,7 @@
       <c r="O501" t="inlineStr"/>
       <c r="P501" t="inlineStr">
         <is>
-          <t>GO Battle League Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Wild Area Pokémon GO Wild Area: Nagasaki Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q501" t="inlineStr">
@@ -20956,7 +20956,7 @@
       <c r="D502" t="inlineStr"/>
       <c r="E502" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
+          <t>Pokémon GO Wild Area: Nagasaki</t>
         </is>
       </c>
       <c r="F502" t="inlineStr">
@@ -20975,7 +20975,7 @@
       <c r="O502" t="inlineStr"/>
       <c r="P502" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Pokémon GO Wild Area: Nagasaki Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q502" t="inlineStr">
@@ -20995,7 +20995,7 @@
       <c r="D503" t="inlineStr"/>
       <c r="E503" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
+          <t>Pokémon GO Wild Area: Nagasaki</t>
         </is>
       </c>
       <c r="F503" t="inlineStr">
@@ -21014,7 +21014,7 @@
       <c r="O503" t="inlineStr"/>
       <c r="P503" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Pokémon GO Wild Area: Nagasaki Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q503" t="inlineStr">
@@ -21034,7 +21034,7 @@
       <c r="D504" t="inlineStr"/>
       <c r="E504" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
+          <t>Pokémon GO Wild Area: Nagasaki</t>
         </is>
       </c>
       <c r="F504" t="inlineStr">
@@ -21053,7 +21053,7 @@
       <c r="O504" t="inlineStr"/>
       <c r="P504" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating...</t>
+          <t>Pokémon GO Wild Area: Nagasaki Calculating...</t>
         </is>
       </c>
       <c r="Q504" t="inlineStr">
@@ -21073,7 +21073,7 @@
       <c r="D505" t="inlineStr"/>
       <c r="E505" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Nagasaki</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F505" t="inlineStr">
@@ -21092,7 +21092,7 @@
       <c r="O505" t="inlineStr"/>
       <c r="P505" t="inlineStr">
         <is>
-          <t>Wild Area Pokémon GO Wild Area: Nagasaki Calculating... Starts: Calculating...</t>
+          <t>GO Battle League Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q505" t="inlineStr">
@@ -21112,7 +21112,7 @@
       <c r="D506" t="inlineStr"/>
       <c r="E506" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Nagasaki</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F506" t="inlineStr">
@@ -21131,7 +21131,7 @@
       <c r="O506" t="inlineStr"/>
       <c r="P506" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Nagasaki Calculating... Starts: Calculating...</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q506" t="inlineStr">
@@ -21151,7 +21151,7 @@
       <c r="D507" t="inlineStr"/>
       <c r="E507" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Nagasaki</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F507" t="inlineStr">
@@ -21170,7 +21170,7 @@
       <c r="O507" t="inlineStr"/>
       <c r="P507" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Nagasaki Calculating... Starts: Calculating...</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q507" t="inlineStr">
@@ -21190,7 +21190,7 @@
       <c r="D508" t="inlineStr"/>
       <c r="E508" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Nagasaki</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F508" t="inlineStr">
@@ -21209,7 +21209,7 @@
       <c r="O508" t="inlineStr"/>
       <c r="P508" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Nagasaki Calculating...</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q508" t="inlineStr">
@@ -21229,7 +21229,7 @@
       <c r="D509" t="inlineStr"/>
       <c r="E509" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Pokémon GO Wild Area: Global</t>
         </is>
       </c>
       <c r="F509" t="inlineStr">
@@ -21248,7 +21248,7 @@
       <c r="O509" t="inlineStr"/>
       <c r="P509" t="inlineStr">
         <is>
-          <t>GO Battle League Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Wild Area Pokémon GO Wild Area: Global Sat, Nov 15, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q509" t="inlineStr">
@@ -21268,7 +21268,7 @@
       <c r="D510" t="inlineStr"/>
       <c r="E510" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Pokémon GO Wild Area: Global</t>
         </is>
       </c>
       <c r="F510" t="inlineStr">
@@ -21287,7 +21287,7 @@
       <c r="O510" t="inlineStr"/>
       <c r="P510" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Pokémon GO Wild Area: Global Sat, Nov 15, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q510" t="inlineStr">
@@ -21307,7 +21307,7 @@
       <c r="D511" t="inlineStr"/>
       <c r="E511" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Pokémon GO Wild Area: Global</t>
         </is>
       </c>
       <c r="F511" t="inlineStr">
@@ -21326,7 +21326,7 @@
       <c r="O511" t="inlineStr"/>
       <c r="P511" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Pokémon GO Wild Area: Global Sat, Nov 15, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q511" t="inlineStr">
@@ -21346,7 +21346,7 @@
       <c r="D512" t="inlineStr"/>
       <c r="E512" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Pokémon GO Wild Area: Global</t>
         </is>
       </c>
       <c r="F512" t="inlineStr">
@@ -21365,7 +21365,7 @@
       <c r="O512" t="inlineStr"/>
       <c r="P512" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating...</t>
+          <t>Pokémon GO Wild Area: Global Sat, Nov 15, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q512" t="inlineStr">
@@ -21385,12 +21385,12 @@
       <c r="D513" t="inlineStr"/>
       <c r="E513" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Global</t>
+          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F513" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G513" t="inlineStr"/>
@@ -21404,7 +21404,7 @@
       <c r="O513" t="inlineStr"/>
       <c r="P513" t="inlineStr">
         <is>
-          <t>Wild Area Pokémon GO Wild Area: Global Sat, Nov 15, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>GO Battle League 2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q513" t="inlineStr">
@@ -21424,12 +21424,12 @@
       <c r="D514" t="inlineStr"/>
       <c r="E514" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Global</t>
+          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F514" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G514" t="inlineStr"/>
@@ -21443,7 +21443,7 @@
       <c r="O514" t="inlineStr"/>
       <c r="P514" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Global Sat, Nov 15, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q514" t="inlineStr">
@@ -21463,12 +21463,12 @@
       <c r="D515" t="inlineStr"/>
       <c r="E515" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Global</t>
+          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F515" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G515" t="inlineStr"/>
@@ -21482,7 +21482,7 @@
       <c r="O515" t="inlineStr"/>
       <c r="P515" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Global Sat, Nov 15, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q515" t="inlineStr">
@@ -21502,12 +21502,12 @@
       <c r="D516" t="inlineStr"/>
       <c r="E516" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Global</t>
+          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F516" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G516" t="inlineStr"/>
@@ -21521,7 +21521,7 @@
       <c r="O516" t="inlineStr"/>
       <c r="P516" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Global Sat, Nov 15, at 10:00 AM Local Time</t>
+          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q516" t="inlineStr">
@@ -21541,12 +21541,12 @@
       <c r="D517" t="inlineStr"/>
       <c r="E517" t="inlineStr">
         <is>
-          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation</t>
+          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F517" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G517" t="inlineStr"/>
@@ -21560,7 +21560,7 @@
       <c r="O517" t="inlineStr"/>
       <c r="P517" t="inlineStr">
         <is>
-          <t>GO Battle League 2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>GO Battle League Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q517" t="inlineStr">
@@ -21580,12 +21580,12 @@
       <c r="D518" t="inlineStr"/>
       <c r="E518" t="inlineStr">
         <is>
-          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation</t>
+          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F518" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G518" t="inlineStr"/>
@@ -21599,7 +21599,7 @@
       <c r="O518" t="inlineStr"/>
       <c r="P518" t="inlineStr">
         <is>
-          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q518" t="inlineStr">
@@ -21619,12 +21619,12 @@
       <c r="D519" t="inlineStr"/>
       <c r="E519" t="inlineStr">
         <is>
-          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation</t>
+          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F519" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G519" t="inlineStr"/>
@@ -21638,7 +21638,7 @@
       <c r="O519" t="inlineStr"/>
       <c r="P519" t="inlineStr">
         <is>
-          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q519" t="inlineStr">
@@ -21658,12 +21658,12 @@
       <c r="D520" t="inlineStr"/>
       <c r="E520" t="inlineStr">
         <is>
-          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation</t>
+          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F520" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G520" t="inlineStr"/>
@@ -21677,7 +21677,7 @@
       <c r="O520" t="inlineStr"/>
       <c r="P520" t="inlineStr">
         <is>
-          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating...</t>
+          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q520" t="inlineStr">
@@ -21697,12 +21697,12 @@
       <c r="D521" t="inlineStr"/>
       <c r="E521" t="inlineStr">
         <is>
-          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation</t>
+          <t>November Community Day</t>
         </is>
       </c>
       <c r="F521" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Community Day</t>
         </is>
       </c>
       <c r="G521" t="inlineStr"/>
@@ -21716,7 +21716,7 @@
       <c r="O521" t="inlineStr"/>
       <c r="P521" t="inlineStr">
         <is>
-          <t>GO Battle League Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Community Day November Community Day Sun, Nov 30, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q521" t="inlineStr">
@@ -21736,12 +21736,12 @@
       <c r="D522" t="inlineStr"/>
       <c r="E522" t="inlineStr">
         <is>
-          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation</t>
+          <t>November Community Day</t>
         </is>
       </c>
       <c r="F522" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Community Day</t>
         </is>
       </c>
       <c r="G522" t="inlineStr"/>
@@ -21755,7 +21755,7 @@
       <c r="O522" t="inlineStr"/>
       <c r="P522" t="inlineStr">
         <is>
-          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>November Community Day Sun, Nov 30, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q522" t="inlineStr">
@@ -21775,12 +21775,12 @@
       <c r="D523" t="inlineStr"/>
       <c r="E523" t="inlineStr">
         <is>
-          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation</t>
+          <t>November Community Day</t>
         </is>
       </c>
       <c r="F523" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Community Day</t>
         </is>
       </c>
       <c r="G523" t="inlineStr"/>
@@ -21794,7 +21794,7 @@
       <c r="O523" t="inlineStr"/>
       <c r="P523" t="inlineStr">
         <is>
-          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>November Community Day Sun, Nov 30, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q523" t="inlineStr">
@@ -21814,12 +21814,12 @@
       <c r="D524" t="inlineStr"/>
       <c r="E524" t="inlineStr">
         <is>
-          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation</t>
+          <t>November Community Day</t>
         </is>
       </c>
       <c r="F524" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Community Day</t>
         </is>
       </c>
       <c r="G524" t="inlineStr"/>
@@ -21833,7 +21833,7 @@
       <c r="O524" t="inlineStr"/>
       <c r="P524" t="inlineStr">
         <is>
-          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating...</t>
+          <t>November Community Day Sun, Nov 30, at 2:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q524" t="inlineStr">
@@ -21853,12 +21853,12 @@
       <c r="D525" t="inlineStr"/>
       <c r="E525" t="inlineStr">
         <is>
-          <t>November Community Day</t>
+          <t>Raid NOW</t>
         </is>
       </c>
       <c r="F525" t="inlineStr">
         <is>
-          <t>Community Day</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G525" t="inlineStr"/>
@@ -21872,12 +21872,12 @@
       <c r="O525" t="inlineStr"/>
       <c r="P525" t="inlineStr">
         <is>
-          <t>Community Day November Community Day Sun, Nov 30, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Raid NOW From Leek Duck | Powered by GO FRIEND General Information It has been reported that the registration information (Trainer Name, Trainer Level, Trainer Code) is incorrect. Please check again. HOST HOST Auto join Raids you are joining (Latest 2) MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rpl_maxuser'] }} {{ val1['cnt'] }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} No.{{ val1['rpl_id'] }} No.{{ val1['rpl_id'] }} TL{{ val1['rpl_level'] }} {{ val1['rpl_glevel'] }} {{ ((val1['rpl_gescore'] == -1)?0:val1['rpl_gescore']) }} {{ aryPokemon[value]['raidbbs_short_name_en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} FULL Host TL 5 30 35 40 45 Host Rating - 0 {{ i }} MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['ti</t>
         </is>
       </c>
       <c r="Q525" t="inlineStr">
         <is>
-          <t>2024-06-01_events.html</t>
+          <t>2024-06-01_raid-now.html</t>
         </is>
       </c>
     </row>
@@ -21892,12 +21892,12 @@
       <c r="D526" t="inlineStr"/>
       <c r="E526" t="inlineStr">
         <is>
-          <t>November Community Day</t>
+          <t>Raids you are joining (Latest 2)</t>
         </is>
       </c>
       <c r="F526" t="inlineStr">
         <is>
-          <t>Community Day</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G526" t="inlineStr"/>
@@ -21911,12 +21911,12 @@
       <c r="O526" t="inlineStr"/>
       <c r="P526" t="inlineStr">
         <is>
-          <t>November Community Day Sun, Nov 30, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>General Information It has been reported that the registration information (Trainer Name, Trainer Level, Trainer Code) is incorrect. Please check again. HOST HOST Auto join Raids you are joining (Latest 2) MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rpl_maxuser'] }} {{ val1['cnt'] }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} No.{{ val1['rpl_id'] }} No.{{ val1['rpl_id'] }} TL{{ val1['rpl_level'] }} {{ val1['rpl_glevel'] }} {{ ((val1['rpl_gescore'] == -1)?0:val1['rpl_gescore']) }} {{ aryPokemon[value]['raidbbs_short_name_en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} FULL Host TL 5 30 35 40 45 Host Rating - 0 {{ i }} MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rp</t>
         </is>
       </c>
       <c r="Q526" t="inlineStr">
         <is>
-          <t>2024-06-01_events.html</t>
+          <t>2024-06-01_raid-now.html</t>
         </is>
       </c>
     </row>
@@ -21931,12 +21931,12 @@
       <c r="D527" t="inlineStr"/>
       <c r="E527" t="inlineStr">
         <is>
-          <t>November Community Day</t>
+          <t>Raids you are joining (Latest 2)</t>
         </is>
       </c>
       <c r="F527" t="inlineStr">
         <is>
-          <t>Community Day</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G527" t="inlineStr"/>
@@ -21950,12 +21950,12 @@
       <c r="O527" t="inlineStr"/>
       <c r="P527" t="inlineStr">
         <is>
-          <t>November Community Day Sun, Nov 30, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Raids you are joining (Latest 2) MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rpl_maxuser'] }} {{ val1['cnt'] }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} No.{{ val1['rpl_id'] }} No.{{ val1['rpl_id'] }} TL{{ val1['rpl_level'] }} {{ val1['rpl_glevel'] }} {{ ((val1['rpl_gescore'] == -1)?0:val1['rpl_gescore']) }}</t>
         </is>
       </c>
       <c r="Q527" t="inlineStr">
         <is>
-          <t>2024-06-01_events.html</t>
+          <t>2024-06-01_raid-now.html</t>
         </is>
       </c>
     </row>
@@ -21970,12 +21970,12 @@
       <c r="D528" t="inlineStr"/>
       <c r="E528" t="inlineStr">
         <is>
-          <t>November Community Day</t>
+          <t>まとめて評価</t>
         </is>
       </c>
       <c r="F528" t="inlineStr">
         <is>
-          <t>Community Day</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G528" t="inlineStr"/>
@@ -21989,12 +21989,12 @@
       <c r="O528" t="inlineStr"/>
       <c r="P528" t="inlineStr">
         <is>
-          <t>November Community Day Sun, Nov 30, at 2:00 PM Local Time</t>
+          <t>まとめて評価 Can't rate</t>
         </is>
       </c>
       <c r="Q528" t="inlineStr">
         <is>
-          <t>2024-06-01_events.html</t>
+          <t>2024-06-01_raid-now.html</t>
         </is>
       </c>
     </row>
@@ -22009,12 +22009,12 @@
       <c r="D529" t="inlineStr"/>
       <c r="E529" t="inlineStr">
         <is>
-          <t>Raid NOW</t>
+          <t>Bonuses</t>
         </is>
       </c>
       <c r="F529" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G529" t="inlineStr"/>
@@ -22028,12 +22028,12 @@
       <c r="O529" t="inlineStr"/>
       <c r="P529" t="inlineStr">
         <is>
-          <t>Raid NOW From Leek Duck | Powered by GO FRIEND General Information It has been reported that the registration information (Trainer Name, Trainer Level, Trainer Code) is incorrect. Please check again. HOST HOST Auto join Raids you are joining (Latest 2) MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rpl_maxuser'] }} {{ val1['cnt'] }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} No.{{ val1['rpl_id'] }} No.{{ val1['rpl_id'] }} TL{{ val1['rpl_level'] }} {{ val1['rpl_glevel'] }} {{ ((val1['rpl_gescore'] == -1)?0:val1['rpl_gescore']) }} {{ aryPokemon[value]['raidbbs_short_name_en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} FULL Host TL 5 30 35 40 45 Host Rating - 0 {{ i }} MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['ti</t>
+          <t>Bonuses 4× Stardust from win rewards. (This does not include end-of-set rewards.) The maximum number of sets you can play per day will increase from five to 20—for a total of 100 battles—from 12:00 a.m. to 11:59 p.m. local time. Free battle-themed Timed Research will be available. Rewards include glasses for your avatar inspired by Clemont. Pokémon encountered via GO Battle League rewards will have a wider variance of Attack, Defense, and HP. Active Leagues The following leagues will be active. Great League Ultra League Master League</t>
         </is>
       </c>
       <c r="Q529" t="inlineStr">
         <is>
-          <t>2024-06-01_raid-now.html</t>
+          <t>2024-06-01_event-go-battle-weekend-tales-of-transformation-sun-oct-26-at-1159-pm-local-time-ends-calculating.html</t>
         </is>
       </c>
     </row>
@@ -22048,12 +22048,12 @@
       <c r="D530" t="inlineStr"/>
       <c r="E530" t="inlineStr">
         <is>
-          <t>Raids you are joining (Latest 2)</t>
+          <t>For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area?</t>
         </is>
       </c>
       <c r="F530" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G530" t="inlineStr"/>
@@ -22067,12 +22067,12 @@
       <c r="O530" t="inlineStr"/>
       <c r="P530" t="inlineStr">
         <is>
-          <t>General Information It has been reported that the registration information (Trainer Name, Trainer Level, Trainer Code) is incorrect. Please check again. HOST HOST Auto join Raids you are joining (Latest 2) MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rpl_maxuser'] }} {{ val1['cnt'] }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} No.{{ val1['rpl_id'] }} No.{{ val1['rpl_id'] }} TL{{ val1['rpl_level'] }} {{ val1['rpl_glevel'] }} {{ ((val1['rpl_gescore'] == -1)?0:val1['rpl_gescore']) }} {{ aryPokemon[value]['raidbbs_short_name_en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} FULL Host TL 5 30 35 40 45 Host Rating - 0 {{ i }} MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rp</t>
+          <t xml:space="preserve">For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area? In this next chapter of Pokémon GO Wild Area, get ready to test your skills once again as you encounter Dark- and Fairy-type Pokémon, including Grimmsnarl, the Bulk Up Pokémon! Plus, exceptionally powerful Pokémon known as mighty Pokémon are appearing in the wild—use GO Wild Area–exclusive GO Safari Balls to improve your odds of catching these rare Pokémon. All event gameplay is exclusive to ticket holders. Tickets for Pokémon GO Wild Area: Nagasaki are now available on the Niantic events portal . Live Event Ticket - ¥3,600 (including applicable taxes and fees) Location: A citywide experience across Nagasaki City, Japan Dates: November 7, 8, or 9, 2025 Time: 9:00 a.m. – 5:00 p.m. JST Tickets for Pokémon GO Wild Area: Nagasaki include one day of event gameplay, and attendees may purchase add-ons that extend the gameplay for an additional day. One-day tickets are ¥3,600 (or the equivalent pricing tier in your local currency, including applicable taxes and fees). Event gameplay will be available only at the date, time, and location specified on your ticket. Note: Tickets to this event are </t>
         </is>
       </c>
       <c r="Q530" t="inlineStr">
         <is>
-          <t>2024-06-01_raid-now.html</t>
+          <t>2024-06-01_wild-area-pokmon-go-wild-area-nagasaki-calculating-ends-calculating.html</t>
         </is>
       </c>
     </row>
@@ -22087,12 +22087,12 @@
       <c r="D531" t="inlineStr"/>
       <c r="E531" t="inlineStr">
         <is>
-          <t>Raids you are joining (Latest 2)</t>
+          <t>For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area?</t>
         </is>
       </c>
       <c r="F531" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G531" t="inlineStr"/>
@@ -22106,166 +22106,10 @@
       <c r="O531" t="inlineStr"/>
       <c r="P531" t="inlineStr">
         <is>
-          <t>Raids you are joining (Latest 2) MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rpl_maxuser'] }} {{ val1['cnt'] }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} No.{{ val1['rpl_id'] }} No.{{ val1['rpl_id'] }} TL{{ val1['rpl_level'] }} {{ val1['rpl_glevel'] }} {{ ((val1['rpl_gescore'] == -1)?0:val1['rpl_gescore']) }}</t>
+          <t>For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area? Trainers around the world can gear up for a worldwide adventure during Pokémon GO Wild Area: Global, available in-game for two days only! Looking to enhance your GO Wild Area weekend with exclusive Special Research, additional bonuses, and an increased chance of encountering Shiny Pokémon? Purchase a global event ticket from the Pokémon GO Web Store! Event Tickets Tickets for Pokémon GO Wild Area: Global are available now in the in-game Shop and Pokémon Go Web Store for $11.99 USD . Purchase your ticket on the Pokémon GO Web Store for a new avatar item! Trainers who purchase their Pokémon GO Wild Area: Global ticket on the Pokémon GO Web Store will receive a special avatar item—the Flower Crown! You can purchase your ticket on the web store until the last day of the event to receive this avatar item. Pokémon GO Wild Area: Nagasaki For details on the in-person event in Nagasaki, Japan, click here .</t>
         </is>
       </c>
       <c r="Q531" t="inlineStr">
-        <is>
-          <t>2024-06-01_raid-now.html</t>
-        </is>
-      </c>
-    </row>
-    <row r="532">
-      <c r="A532" t="inlineStr">
-        <is>
-          <t>Leek Duck</t>
-        </is>
-      </c>
-      <c r="B532" t="inlineStr"/>
-      <c r="C532" t="inlineStr"/>
-      <c r="D532" t="inlineStr"/>
-      <c r="E532" t="inlineStr">
-        <is>
-          <t>まとめて評価</t>
-        </is>
-      </c>
-      <c r="F532" t="inlineStr">
-        <is>
-          <t>Event/News</t>
-        </is>
-      </c>
-      <c r="G532" t="inlineStr"/>
-      <c r="H532" t="inlineStr"/>
-      <c r="I532" t="inlineStr"/>
-      <c r="J532" t="inlineStr"/>
-      <c r="K532" t="inlineStr"/>
-      <c r="L532" t="inlineStr"/>
-      <c r="M532" t="inlineStr"/>
-      <c r="N532" t="inlineStr"/>
-      <c r="O532" t="inlineStr"/>
-      <c r="P532" t="inlineStr">
-        <is>
-          <t>まとめて評価 Can't rate</t>
-        </is>
-      </c>
-      <c r="Q532" t="inlineStr">
-        <is>
-          <t>2024-06-01_raid-now.html</t>
-        </is>
-      </c>
-    </row>
-    <row r="533">
-      <c r="A533" t="inlineStr">
-        <is>
-          <t>Leek Duck</t>
-        </is>
-      </c>
-      <c r="B533" t="inlineStr"/>
-      <c r="C533" t="inlineStr"/>
-      <c r="D533" t="inlineStr"/>
-      <c r="E533" t="inlineStr">
-        <is>
-          <t>Bonuses</t>
-        </is>
-      </c>
-      <c r="F533" t="inlineStr">
-        <is>
-          <t>Event/News</t>
-        </is>
-      </c>
-      <c r="G533" t="inlineStr"/>
-      <c r="H533" t="inlineStr"/>
-      <c r="I533" t="inlineStr"/>
-      <c r="J533" t="inlineStr"/>
-      <c r="K533" t="inlineStr"/>
-      <c r="L533" t="inlineStr"/>
-      <c r="M533" t="inlineStr"/>
-      <c r="N533" t="inlineStr"/>
-      <c r="O533" t="inlineStr"/>
-      <c r="P533" t="inlineStr">
-        <is>
-          <t>Bonuses 4× Stardust from win rewards. (This does not include end-of-set rewards.) The maximum number of sets you can play per day will increase from five to 20—for a total of 100 battles—from 12:00 a.m. to 11:59 p.m. local time. Free battle-themed Timed Research will be available. Rewards include glasses for your avatar inspired by Clemont. Pokémon encountered via GO Battle League rewards will have a wider variance of Attack, Defense, and HP. Active Leagues The following leagues will be active. Great League Ultra League Master League</t>
-        </is>
-      </c>
-      <c r="Q533" t="inlineStr">
-        <is>
-          <t>2024-06-01_event-go-battle-weekend-tales-of-transformation-sun-oct-26-at-1159-pm-local-time-ends-calculating.html</t>
-        </is>
-      </c>
-    </row>
-    <row r="534">
-      <c r="A534" t="inlineStr">
-        <is>
-          <t>Leek Duck</t>
-        </is>
-      </c>
-      <c r="B534" t="inlineStr"/>
-      <c r="C534" t="inlineStr"/>
-      <c r="D534" t="inlineStr"/>
-      <c r="E534" t="inlineStr">
-        <is>
-          <t>For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area?</t>
-        </is>
-      </c>
-      <c r="F534" t="inlineStr">
-        <is>
-          <t>Event/News</t>
-        </is>
-      </c>
-      <c r="G534" t="inlineStr"/>
-      <c r="H534" t="inlineStr"/>
-      <c r="I534" t="inlineStr"/>
-      <c r="J534" t="inlineStr"/>
-      <c r="K534" t="inlineStr"/>
-      <c r="L534" t="inlineStr"/>
-      <c r="M534" t="inlineStr"/>
-      <c r="N534" t="inlineStr"/>
-      <c r="O534" t="inlineStr"/>
-      <c r="P534" t="inlineStr">
-        <is>
-          <t xml:space="preserve">For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area? In this next chapter of Pokémon GO Wild Area, get ready to test your skills once again as you encounter Dark- and Fairy-type Pokémon, including Grimmsnarl, the Bulk Up Pokémon! Plus, exceptionally powerful Pokémon known as mighty Pokémon are appearing in the wild—use GO Wild Area–exclusive GO Safari Balls to improve your odds of catching these rare Pokémon. All event gameplay is exclusive to ticket holders. Tickets for Pokémon GO Wild Area: Nagasaki are now available on the Niantic events portal . Live Event Ticket - ¥3,600 (including applicable taxes and fees) Location: A citywide experience across Nagasaki City, Japan Dates: November 7, 8, or 9, 2025 Time: 9:00 a.m. – 5:00 p.m. JST Tickets for Pokémon GO Wild Area: Nagasaki include one day of event gameplay, and attendees may purchase add-ons that extend the gameplay for an additional day. One-day tickets are ¥3,600 (or the equivalent pricing tier in your local currency, including applicable taxes and fees). Event gameplay will be available only at the date, time, and location specified on your ticket. Note: Tickets to this event are </t>
-        </is>
-      </c>
-      <c r="Q534" t="inlineStr">
-        <is>
-          <t>2024-06-01_wild-area-pokmon-go-wild-area-nagasaki-calculating-ends-calculating.html</t>
-        </is>
-      </c>
-    </row>
-    <row r="535">
-      <c r="A535" t="inlineStr">
-        <is>
-          <t>Leek Duck</t>
-        </is>
-      </c>
-      <c r="B535" t="inlineStr"/>
-      <c r="C535" t="inlineStr"/>
-      <c r="D535" t="inlineStr"/>
-      <c r="E535" t="inlineStr">
-        <is>
-          <t>For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area?</t>
-        </is>
-      </c>
-      <c r="F535" t="inlineStr">
-        <is>
-          <t>Event/News</t>
-        </is>
-      </c>
-      <c r="G535" t="inlineStr"/>
-      <c r="H535" t="inlineStr"/>
-      <c r="I535" t="inlineStr"/>
-      <c r="J535" t="inlineStr"/>
-      <c r="K535" t="inlineStr"/>
-      <c r="L535" t="inlineStr"/>
-      <c r="M535" t="inlineStr"/>
-      <c r="N535" t="inlineStr"/>
-      <c r="O535" t="inlineStr"/>
-      <c r="P535" t="inlineStr">
-        <is>
-          <t>For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area? Trainers around the world can gear up for a worldwide adventure during Pokémon GO Wild Area: Global, available in-game for two days only! Looking to enhance your GO Wild Area weekend with exclusive Special Research, additional bonuses, and an increased chance of encountering Shiny Pokémon? Purchase a global event ticket from the Pokémon GO Web Store! Event Tickets Tickets for Pokémon GO Wild Area: Global are available now in the in-game Shop and Pokémon Go Web Store for $11.99 USD . Purchase your ticket on the Pokémon GO Web Store for a new avatar item! Trainers who purchase their Pokémon GO Wild Area: Global ticket on the Pokémon GO Web Store will receive a special avatar item—the Flower Crown! You can purchase your ticket on the web store until the last day of the event to receive this avatar item. Pokémon GO Wild Area: Nagasaki For details on the in-person event in Nagasaki, Japan, click here .</t>
-        </is>
-      </c>
-      <c r="Q535" t="inlineStr">
         <is>
           <t>2024-06-01_wild-area-pokmon-go-wild-area-global-sun-nov-16-at-600-pm-local-time-ends-calculating.html</t>
         </is>

</xml_diff>

<commit_message>
Update latest digest: 2024-06-01 → 2025-09-29
</commit_message>
<xml_diff>
--- a/outputs/latest/POGO_Digest.xlsx
+++ b/outputs/latest/POGO_Digest.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q472"/>
+  <dimension ref="A1:Q476"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -614,7 +614,7 @@
       <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Events Updated on August 28, 2025 Happening Now PokéStop Showcase Camerupt and Dudunsparce PokéStop Showcases Sun, Sep 28, at 8:00 PM Local Time Ends: Calculating... Raid Battles Mega Kangaskhan and Mega Lopunny in Mega Raids Tue, Sep 30, at 10:00 AM Local Time Ends: Calculating... GO Battle League Great League, Ultra League, and Master League | Tales of Transformation Calculating... Ends: Calculating... Pokémon Spotlight Hour Aron Spotlight Hour Tue, Sep 30, at 7:00 PM Local Time Ends: Calculating... Raid Hour Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 7:00 PM Local Time Ends: Calculating... Raid Day Mega Metagross Raid Day Sat, Oct 4, at 5:00 PM Local Time Ends: Calculating... Max Mondays Dynamax Beldum during Max Monday Sun, Oct 5, at 7:00 PM Local Time Ends: Calculating... GO Pass GO Pass: September Tue, Oct 7, at 10:00 AM Local Time Ends: Calculating... Raid Battles Dialga in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time Ends: Calculating... Raid Battles Mega Steelix, Scizor, and Lucario in Mega Raids Tue, Oct 7, at 10:00 AM Local Time Ends: Calculating... GO Battle League Great League and Fantasy Cup: Great League Edition | Tales of Transformation Calculating... </t>
+          <t>Events Updated on August 28, 2025 Happening Now Raid Battles Mega Kangaskhan and Mega Lopunny in Mega Raids Tue, Sep 30, at 10:00 AM Local Time Ends: Calculating... GO Battle League Great League, Ultra League, and Master League | Tales of Transformation Calculating... Ends: Calculating... Pokémon Spotlight Hour Aron Spotlight Hour Tue, Sep 30, at 7:00 PM Local Time Ends: Calculating... Raid Hour Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 7:00 PM Local Time Ends: Calculating... PokéStop Showcase Steel-type PokéStop Showcases Wed, Oct 1, at 8:00 PM Local Time Ends: Calculating... Raid Day Mega Metagross Raid Day Sat, Oct 4, at 5:00 PM Local Time Ends: Calculating... Max Mondays Dynamax Beldum during Max Monday Sun, Oct 5, at 7:00 PM Local Time Ends: Calculating... GO Pass GO Pass: September Tue, Oct 7, at 10:00 AM Local Time Ends: Calculating... Raid Battles Dialga in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time Ends: Calculating... Raid Battles Mega Steelix, Scizor, and Lucario in Mega Raids Tue, Oct 7, at 10:00 AM Local Time Ends: Calculating... GO Battle League Great League and Fantasy Cup: Great League Edition | Tales of Transformation Calculating... Ends: Calculati</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
@@ -993,17 +993,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Camerupt and Dudunsparce PokéStop Showcases</t>
+          <t>Steel-type PokéStop Showcases</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1022,12 +1022,12 @@
       <c r="O11" t="inlineStr"/>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Camerupt and Dudunsparce PokéStop Showcases PokéStop Showcase Starts: Saturday, September 27, 2025, at 10:00 AM Local Time Ends: Sunday, September 28, 2025, at  8:00 PM Local Time There will be PokéStop Showcases featuring Camerupt and Dudunsparce. Top the leaderboard to win rewards including Premium Items! Camerupt Dudunsparce Leek Duck Hey, I'm LeekDuck. I create Pokémon GO graphics, resources and report Pokémon GO news. You can find them on X, Facebook, Instagram, Threads, and Bluesky. You can also find me on Twitch and YouTube!</t>
+          <t>Steel-type PokéStop Showcases PokéStop Showcase Starts: Monday, September 29, 2025, at 10:00 AM Local Time Ends: Wednesday, October 1, 2025, at  8:00 PM Local Time There will be PokéStop Showcases featuring Steel-type Pokémon. Top the leaderboard to win rewards including Premium Items! Leek Duck Hey, I'm LeekDuck. I create Pokémon GO graphics, resources and report Pokémon GO news. You can find them on X, Facebook, Instagram, Threads, and Bluesky. You can also find me on Twitch and YouTube!</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>2024-06-01_pokstop-showcase-camerupt-and-dudunsparce-pokstop-showcases-sun-sep-28-at-800-pm-local-time-ends-calculating.html</t>
+          <t>2024-06-01_pokstop-showcase-steel-type-pokstop-showcases-wed-oct-1-at-800-pm-local-time-ends-calculating.html</t>
         </is>
       </c>
     </row>
@@ -4102,12 +4102,12 @@
       <c r="D72" t="inlineStr"/>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Camerupt and Dudunsparce PokéStop Showcases</t>
+          <t>Mega Kangaskhan and Mega Lopunny in Mega Raids</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G72" t="inlineStr"/>
@@ -4121,7 +4121,7 @@
       <c r="O72" t="inlineStr"/>
       <c r="P72" t="inlineStr">
         <is>
-          <t>PokéStop Showcase Camerupt and Dudunsparce PokéStop Showcases Sun, Sep 28, at 8:00 PM Local Time Ends: Calculating... Raid Battles Mega Kangaskhan and Mega Lopunny in Mega Raids Tue, Sep 30, at 10:00 AM Local Time Ends: Calculating... GO Battle League Great League, Ultra League, and Master League | Tales of Transformation Calculating... Ends: Calculating... Pokémon Spotlight Hour Aron Spotlight Hour Tue, Sep 30, at 7:00 PM Local Time Ends: Calculating... Raid Hour Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 7:00 PM Local Time Ends: Calculating... Raid Day Mega Metagross Raid Day Sat, Oct 4, at 5:00 PM Local Time Ends: Calculating... Max Mondays Dynamax Beldum during Max Monday Sun, Oct 5, at 7:00 PM Local Time Ends: Calculating... GO Pass GO Pass: September Tue, Oct 7, at 10:00 AM Local Time Ends: Calculating... Raid Battles Dialga in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time Ends: Calculating... Raid Battles Mega Steelix, Scizor, and Lucario in Mega Raids Tue, Oct 7, at 10:00 AM Local Time Ends: Calculating... GO Battle League Great League and Fantasy Cup: Great League Edition | Tales of Transformation Calculating... Ends: Calculating... Pokémon Spotlight Hour Ferr</t>
+          <t>Raid Battles Mega Kangaskhan and Mega Lopunny in Mega Raids Tue, Sep 30, at 10:00 AM Local Time Ends: Calculating... GO Battle League Great League, Ultra League, and Master League | Tales of Transformation Calculating... Ends: Calculating... Pokémon Spotlight Hour Aron Spotlight Hour Tue, Sep 30, at 7:00 PM Local Time Ends: Calculating... Raid Hour Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 7:00 PM Local Time Ends: Calculating... PokéStop Showcase Steel-type PokéStop Showcases Wed, Oct 1, at 8:00 PM Local Time Ends: Calculating... Raid Day Mega Metagross Raid Day Sat, Oct 4, at 5:00 PM Local Time Ends: Calculating... Max Mondays Dynamax Beldum during Max Monday Sun, Oct 5, at 7:00 PM Local Time Ends: Calculating... GO Pass GO Pass: September Tue, Oct 7, at 10:00 AM Local Time Ends: Calculating... Raid Battles Dialga in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time Ends: Calculating... Raid Battles Mega Steelix, Scizor, and Lucario in Mega Raids Tue, Oct 7, at 10:00 AM Local Time Ends: Calculating... GO Battle League Great League and Fantasy Cup: Great League Edition | Tales of Transformation Calculating... Ends: Calculating... Pokémon Spotlight Hour Ferroseed Spotlight</t>
         </is>
       </c>
       <c r="Q72" t="inlineStr">
@@ -4141,12 +4141,12 @@
       <c r="D73" t="inlineStr"/>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Camerupt and Dudunsparce PokéStop Showcases</t>
+          <t>Mega Kangaskhan and Mega Lopunny in Mega Raids</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G73" t="inlineStr"/>
@@ -4160,7 +4160,7 @@
       <c r="O73" t="inlineStr"/>
       <c r="P73" t="inlineStr">
         <is>
-          <t>PokéStop Showcase Camerupt and Dudunsparce PokéStop Showcases Sun, Sep 28, at 8:00 PM Local Time Ends: Calculating...</t>
+          <t>Raid Battles Mega Kangaskhan and Mega Lopunny in Mega Raids Tue, Sep 30, at 10:00 AM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q73" t="inlineStr">
@@ -4180,12 +4180,12 @@
       <c r="D74" t="inlineStr"/>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Camerupt and Dudunsparce PokéStop Showcases</t>
+          <t>Mega Kangaskhan and Mega Lopunny in Mega Raids</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G74" t="inlineStr"/>
@@ -4199,7 +4199,7 @@
       <c r="O74" t="inlineStr"/>
       <c r="P74" t="inlineStr">
         <is>
-          <t>Camerupt and Dudunsparce PokéStop Showcases Sun, Sep 28, at 8:00 PM Local Time Ends: Calculating...</t>
+          <t>Mega Kangaskhan and Mega Lopunny in Mega Raids Tue, Sep 30, at 10:00 AM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q74" t="inlineStr">
@@ -4219,12 +4219,12 @@
       <c r="D75" t="inlineStr"/>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Camerupt and Dudunsparce PokéStop Showcases</t>
+          <t>Mega Kangaskhan and Mega Lopunny in Mega Raids</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G75" t="inlineStr"/>
@@ -4238,7 +4238,7 @@
       <c r="O75" t="inlineStr"/>
       <c r="P75" t="inlineStr">
         <is>
-          <t>Camerupt and Dudunsparce PokéStop Showcases Sun, Sep 28, at 8:00 PM Local Time Ends: Calculating...</t>
+          <t>Mega Kangaskhan and Mega Lopunny in Mega Raids Tue, Sep 30, at 10:00 AM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q75" t="inlineStr">
@@ -4258,12 +4258,12 @@
       <c r="D76" t="inlineStr"/>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Camerupt and Dudunsparce PokéStop Showcases</t>
+          <t>Mega Kangaskhan and Mega Lopunny in Mega Raids</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G76" t="inlineStr"/>
@@ -4277,7 +4277,7 @@
       <c r="O76" t="inlineStr"/>
       <c r="P76" t="inlineStr">
         <is>
-          <t>Camerupt and Dudunsparce PokéStop Showcases Sun, Sep 28, at 8:00 PM Local Time</t>
+          <t>Mega Kangaskhan and Mega Lopunny in Mega Raids Tue, Sep 30, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q76" t="inlineStr">
@@ -4297,12 +4297,12 @@
       <c r="D77" t="inlineStr"/>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Mega Kangaskhan and Mega Lopunny in Mega Raids</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G77" t="inlineStr"/>
@@ -4316,7 +4316,7 @@
       <c r="O77" t="inlineStr"/>
       <c r="P77" t="inlineStr">
         <is>
-          <t>Raid Battles Mega Kangaskhan and Mega Lopunny in Mega Raids Tue, Sep 30, at 10:00 AM Local Time Ends: Calculating...</t>
+          <t>GO Battle League Great League, Ultra League, and Master League | Tales of Transformation Calculating... Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q77" t="inlineStr">
@@ -4336,12 +4336,12 @@
       <c r="D78" t="inlineStr"/>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Mega Kangaskhan and Mega Lopunny in Mega Raids</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G78" t="inlineStr"/>
@@ -4355,7 +4355,7 @@
       <c r="O78" t="inlineStr"/>
       <c r="P78" t="inlineStr">
         <is>
-          <t>Mega Kangaskhan and Mega Lopunny in Mega Raids Tue, Sep 30, at 10:00 AM Local Time Ends: Calculating...</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q78" t="inlineStr">
@@ -4375,12 +4375,12 @@
       <c r="D79" t="inlineStr"/>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Mega Kangaskhan and Mega Lopunny in Mega Raids</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G79" t="inlineStr"/>
@@ -4394,7 +4394,7 @@
       <c r="O79" t="inlineStr"/>
       <c r="P79" t="inlineStr">
         <is>
-          <t>Mega Kangaskhan and Mega Lopunny in Mega Raids Tue, Sep 30, at 10:00 AM Local Time Ends: Calculating...</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q79" t="inlineStr">
@@ -4414,12 +4414,12 @@
       <c r="D80" t="inlineStr"/>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Mega Kangaskhan and Mega Lopunny in Mega Raids</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G80" t="inlineStr"/>
@@ -4433,7 +4433,7 @@
       <c r="O80" t="inlineStr"/>
       <c r="P80" t="inlineStr">
         <is>
-          <t>Mega Kangaskhan and Mega Lopunny in Mega Raids Tue, Sep 30, at 10:00 AM Local Time</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q80" t="inlineStr">
@@ -4453,12 +4453,12 @@
       <c r="D81" t="inlineStr"/>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Aron Spotlight Hour</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G81" t="inlineStr"/>
@@ -4472,7 +4472,7 @@
       <c r="O81" t="inlineStr"/>
       <c r="P81" t="inlineStr">
         <is>
-          <t>GO Battle League Great League, Ultra League, and Master League | Tales of Transformation Calculating... Ends: Calculating...</t>
+          <t>Pokémon Spotlight Hour Aron Spotlight Hour Tue, Sep 30, at 7:00 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q81" t="inlineStr">
@@ -4492,12 +4492,12 @@
       <c r="D82" t="inlineStr"/>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Aron Spotlight Hour</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G82" t="inlineStr"/>
@@ -4511,7 +4511,7 @@
       <c r="O82" t="inlineStr"/>
       <c r="P82" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Ends: Calculating...</t>
+          <t>Aron Spotlight Hour Tue, Sep 30, at 7:00 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q82" t="inlineStr">
@@ -4531,12 +4531,12 @@
       <c r="D83" t="inlineStr"/>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Aron Spotlight Hour</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G83" t="inlineStr"/>
@@ -4550,7 +4550,7 @@
       <c r="O83" t="inlineStr"/>
       <c r="P83" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Ends: Calculating...</t>
+          <t>Aron Spotlight Hour Tue, Sep 30, at 7:00 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q83" t="inlineStr">
@@ -4570,12 +4570,12 @@
       <c r="D84" t="inlineStr"/>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Aron Spotlight Hour</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G84" t="inlineStr"/>
@@ -4589,7 +4589,7 @@
       <c r="O84" t="inlineStr"/>
       <c r="P84" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating...</t>
+          <t>Aron Spotlight Hour Tue, Sep 30, at 7:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q84" t="inlineStr">
@@ -4609,12 +4609,12 @@
       <c r="D85" t="inlineStr"/>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Aron Spotlight Hour</t>
+          <t>Dialga (Origin Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G85" t="inlineStr"/>
@@ -4628,7 +4628,7 @@
       <c r="O85" t="inlineStr"/>
       <c r="P85" t="inlineStr">
         <is>
-          <t>Pokémon Spotlight Hour Aron Spotlight Hour Tue, Sep 30, at 7:00 PM Local Time Ends: Calculating...</t>
+          <t>Raid Hour Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 7:00 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q85" t="inlineStr">
@@ -4648,12 +4648,12 @@
       <c r="D86" t="inlineStr"/>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Aron Spotlight Hour</t>
+          <t>Dialga (Origin Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G86" t="inlineStr"/>
@@ -4667,7 +4667,7 @@
       <c r="O86" t="inlineStr"/>
       <c r="P86" t="inlineStr">
         <is>
-          <t>Aron Spotlight Hour Tue, Sep 30, at 7:00 PM Local Time Ends: Calculating...</t>
+          <t>Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 7:00 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q86" t="inlineStr">
@@ -4687,12 +4687,12 @@
       <c r="D87" t="inlineStr"/>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Aron Spotlight Hour</t>
+          <t>Dialga (Origin Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G87" t="inlineStr"/>
@@ -4706,7 +4706,7 @@
       <c r="O87" t="inlineStr"/>
       <c r="P87" t="inlineStr">
         <is>
-          <t>Aron Spotlight Hour Tue, Sep 30, at 7:00 PM Local Time Ends: Calculating...</t>
+          <t>Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 7:00 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q87" t="inlineStr">
@@ -4726,12 +4726,12 @@
       <c r="D88" t="inlineStr"/>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Aron Spotlight Hour</t>
+          <t>Dialga (Origin Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G88" t="inlineStr"/>
@@ -4745,7 +4745,7 @@
       <c r="O88" t="inlineStr"/>
       <c r="P88" t="inlineStr">
         <is>
-          <t>Aron Spotlight Hour Tue, Sep 30, at 7:00 PM Local Time</t>
+          <t>Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 7:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q88" t="inlineStr">
@@ -4765,12 +4765,12 @@
       <c r="D89" t="inlineStr"/>
       <c r="E89" t="inlineStr">
         <is>
-          <t>Dialga (Origin Forme) Raid Hour</t>
+          <t>Steel-type PokéStop Showcases</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G89" t="inlineStr"/>
@@ -4784,7 +4784,7 @@
       <c r="O89" t="inlineStr"/>
       <c r="P89" t="inlineStr">
         <is>
-          <t>Raid Hour Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 7:00 PM Local Time Ends: Calculating...</t>
+          <t>PokéStop Showcase Steel-type PokéStop Showcases Wed, Oct 1, at 8:00 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q89" t="inlineStr">
@@ -4804,12 +4804,12 @@
       <c r="D90" t="inlineStr"/>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Dialga (Origin Forme) Raid Hour</t>
+          <t>Steel-type PokéStop Showcases</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G90" t="inlineStr"/>
@@ -4823,7 +4823,7 @@
       <c r="O90" t="inlineStr"/>
       <c r="P90" t="inlineStr">
         <is>
-          <t>Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 7:00 PM Local Time Ends: Calculating...</t>
+          <t>Steel-type PokéStop Showcases Wed, Oct 1, at 8:00 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q90" t="inlineStr">
@@ -4843,12 +4843,12 @@
       <c r="D91" t="inlineStr"/>
       <c r="E91" t="inlineStr">
         <is>
-          <t>Dialga (Origin Forme) Raid Hour</t>
+          <t>Steel-type PokéStop Showcases</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G91" t="inlineStr"/>
@@ -4862,7 +4862,7 @@
       <c r="O91" t="inlineStr"/>
       <c r="P91" t="inlineStr">
         <is>
-          <t>Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 7:00 PM Local Time Ends: Calculating...</t>
+          <t>Steel-type PokéStop Showcases Wed, Oct 1, at 8:00 PM Local Time Ends: Calculating...</t>
         </is>
       </c>
       <c r="Q91" t="inlineStr">
@@ -4882,12 +4882,12 @@
       <c r="D92" t="inlineStr"/>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Dialga (Origin Forme) Raid Hour</t>
+          <t>Steel-type PokéStop Showcases</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G92" t="inlineStr"/>
@@ -4901,7 +4901,7 @@
       <c r="O92" t="inlineStr"/>
       <c r="P92" t="inlineStr">
         <is>
-          <t>Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 7:00 PM Local Time</t>
+          <t>Steel-type PokéStop Showcases Wed, Oct 1, at 8:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q92" t="inlineStr">
@@ -12409,7 +12409,7 @@
       <c r="D285" t="inlineStr"/>
       <c r="E285" t="inlineStr">
         <is>
-          <t>Dynamax Beldum during Max Monday</t>
+          <t>Steel-type PokéStop Showcases</t>
         </is>
       </c>
       <c r="F285" t="inlineStr">
@@ -12428,7 +12428,7 @@
       <c r="O285" t="inlineStr"/>
       <c r="P285" t="inlineStr">
         <is>
-          <t>Max Mondays Dynamax Beldum during Max Monday Mon, Sep 29, at 6:00 PM Local Time Starts: Calculating... Raid Battles Mega Steelix, Scizor, and Lucario in Mega Raids Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating... Event Steel Skyline Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating... GO Battle League Great League and Fantasy Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating... Pokémon Spotlight Hour Aron Spotlight Hour Tue, Sep 30, at 6:00 PM Local Time Starts: Calculating... Raid Hour Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 6:00 PM Local Time Starts: Calculating... Raid Day Mega Metagross Raid Day Sat, Oct 4, at 2:00 PM Local Time Starts: Calculating... Max Mondays Dynamax Drilbur during Max Monday Mon, Oct 6, at 6:00 PM Local Time Starts: Calculating... Raid Battles Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating... Raid Battles Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating... GO Battle League Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts</t>
+          <t>PokéStop Showcase Steel-type PokéStop Showcases Mon, Sep 29, at 10:00 AM Local Time Starts: Calculating... Max Mondays Dynamax Beldum during Max Monday Mon, Sep 29, at 6:00 PM Local Time Starts: Calculating... Raid Battles Mega Steelix, Scizor, and Lucario in Mega Raids Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating... Event Steel Skyline Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating... GO Battle League Great League and Fantasy Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating... Pokémon Spotlight Hour Aron Spotlight Hour Tue, Sep 30, at 6:00 PM Local Time Starts: Calculating... Raid Hour Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 6:00 PM Local Time Starts: Calculating... Raid Day Mega Metagross Raid Day Sat, Oct 4, at 2:00 PM Local Time Starts: Calculating... Max Mondays Dynamax Drilbur during Max Monday Mon, Oct 6, at 6:00 PM Local Time Starts: Calculating... Raid Battles Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating... Raid Battles Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating... GO Batt</t>
         </is>
       </c>
       <c r="Q285" t="inlineStr">
@@ -12448,7 +12448,7 @@
       <c r="D286" t="inlineStr"/>
       <c r="E286" t="inlineStr">
         <is>
-          <t>Dynamax Beldum during Max Monday</t>
+          <t>Steel-type PokéStop Showcases</t>
         </is>
       </c>
       <c r="F286" t="inlineStr">
@@ -12467,7 +12467,7 @@
       <c r="O286" t="inlineStr"/>
       <c r="P286" t="inlineStr">
         <is>
-          <t>Max Mondays Dynamax Beldum during Max Monday Mon, Sep 29, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>PokéStop Showcase Steel-type PokéStop Showcases Mon, Sep 29, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q286" t="inlineStr">
@@ -12487,7 +12487,7 @@
       <c r="D287" t="inlineStr"/>
       <c r="E287" t="inlineStr">
         <is>
-          <t>Dynamax Beldum during Max Monday</t>
+          <t>Steel-type PokéStop Showcases</t>
         </is>
       </c>
       <c r="F287" t="inlineStr">
@@ -12506,7 +12506,7 @@
       <c r="O287" t="inlineStr"/>
       <c r="P287" t="inlineStr">
         <is>
-          <t>Dynamax Beldum during Max Monday Mon, Sep 29, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Steel-type PokéStop Showcases Mon, Sep 29, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q287" t="inlineStr">
@@ -12526,7 +12526,7 @@
       <c r="D288" t="inlineStr"/>
       <c r="E288" t="inlineStr">
         <is>
-          <t>Dynamax Beldum during Max Monday</t>
+          <t>Steel-type PokéStop Showcases</t>
         </is>
       </c>
       <c r="F288" t="inlineStr">
@@ -12545,7 +12545,7 @@
       <c r="O288" t="inlineStr"/>
       <c r="P288" t="inlineStr">
         <is>
-          <t>Dynamax Beldum during Max Monday Mon, Sep 29, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Steel-type PokéStop Showcases Mon, Sep 29, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q288" t="inlineStr">
@@ -12565,7 +12565,7 @@
       <c r="D289" t="inlineStr"/>
       <c r="E289" t="inlineStr">
         <is>
-          <t>Dynamax Beldum during Max Monday</t>
+          <t>Steel-type PokéStop Showcases</t>
         </is>
       </c>
       <c r="F289" t="inlineStr">
@@ -12584,7 +12584,7 @@
       <c r="O289" t="inlineStr"/>
       <c r="P289" t="inlineStr">
         <is>
-          <t>Dynamax Beldum during Max Monday Mon, Sep 29, at 6:00 PM Local Time</t>
+          <t>Steel-type PokéStop Showcases Mon, Sep 29, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q289" t="inlineStr">
@@ -12604,12 +12604,12 @@
       <c r="D290" t="inlineStr"/>
       <c r="E290" t="inlineStr">
         <is>
-          <t>Mega Steelix, Scizor, and Lucario in Mega Raids</t>
+          <t>Dynamax Beldum during Max Monday</t>
         </is>
       </c>
       <c r="F290" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G290" t="inlineStr"/>
@@ -12623,7 +12623,7 @@
       <c r="O290" t="inlineStr"/>
       <c r="P290" t="inlineStr">
         <is>
-          <t>Raid Battles Mega Steelix, Scizor, and Lucario in Mega Raids Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Max Mondays Dynamax Beldum during Max Monday Mon, Sep 29, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q290" t="inlineStr">
@@ -12643,12 +12643,12 @@
       <c r="D291" t="inlineStr"/>
       <c r="E291" t="inlineStr">
         <is>
-          <t>Mega Steelix, Scizor, and Lucario in Mega Raids</t>
+          <t>Dynamax Beldum during Max Monday</t>
         </is>
       </c>
       <c r="F291" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G291" t="inlineStr"/>
@@ -12662,7 +12662,7 @@
       <c r="O291" t="inlineStr"/>
       <c r="P291" t="inlineStr">
         <is>
-          <t>Mega Steelix, Scizor, and Lucario in Mega Raids Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Dynamax Beldum during Max Monday Mon, Sep 29, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q291" t="inlineStr">
@@ -12682,12 +12682,12 @@
       <c r="D292" t="inlineStr"/>
       <c r="E292" t="inlineStr">
         <is>
-          <t>Mega Steelix, Scizor, and Lucario in Mega Raids</t>
+          <t>Dynamax Beldum during Max Monday</t>
         </is>
       </c>
       <c r="F292" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G292" t="inlineStr"/>
@@ -12701,7 +12701,7 @@
       <c r="O292" t="inlineStr"/>
       <c r="P292" t="inlineStr">
         <is>
-          <t>Mega Steelix, Scizor, and Lucario in Mega Raids Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Dynamax Beldum during Max Monday Mon, Sep 29, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q292" t="inlineStr">
@@ -12721,12 +12721,12 @@
       <c r="D293" t="inlineStr"/>
       <c r="E293" t="inlineStr">
         <is>
-          <t>Mega Steelix, Scizor, and Lucario in Mega Raids</t>
+          <t>Dynamax Beldum during Max Monday</t>
         </is>
       </c>
       <c r="F293" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G293" t="inlineStr"/>
@@ -12740,7 +12740,7 @@
       <c r="O293" t="inlineStr"/>
       <c r="P293" t="inlineStr">
         <is>
-          <t>Mega Steelix, Scizor, and Lucario in Mega Raids Tue, Sep 30, at 10:00 AM Local Time</t>
+          <t>Dynamax Beldum during Max Monday Mon, Sep 29, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q293" t="inlineStr">
@@ -12760,12 +12760,12 @@
       <c r="D294" t="inlineStr"/>
       <c r="E294" t="inlineStr">
         <is>
-          <t>Steel Skyline</t>
+          <t>Mega Steelix, Scizor, and Lucario in Mega Raids</t>
         </is>
       </c>
       <c r="F294" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G294" t="inlineStr"/>
@@ -12779,7 +12779,7 @@
       <c r="O294" t="inlineStr"/>
       <c r="P294" t="inlineStr">
         <is>
-          <t>Event Steel Skyline Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Raid Battles Mega Steelix, Scizor, and Lucario in Mega Raids Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q294" t="inlineStr">
@@ -12799,12 +12799,12 @@
       <c r="D295" t="inlineStr"/>
       <c r="E295" t="inlineStr">
         <is>
-          <t>Steel Skyline</t>
+          <t>Mega Steelix, Scizor, and Lucario in Mega Raids</t>
         </is>
       </c>
       <c r="F295" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G295" t="inlineStr"/>
@@ -12818,7 +12818,7 @@
       <c r="O295" t="inlineStr"/>
       <c r="P295" t="inlineStr">
         <is>
-          <t>Steel Skyline Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Mega Steelix, Scizor, and Lucario in Mega Raids Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q295" t="inlineStr">
@@ -12838,12 +12838,12 @@
       <c r="D296" t="inlineStr"/>
       <c r="E296" t="inlineStr">
         <is>
-          <t>Steel Skyline</t>
+          <t>Mega Steelix, Scizor, and Lucario in Mega Raids</t>
         </is>
       </c>
       <c r="F296" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G296" t="inlineStr"/>
@@ -12857,7 +12857,7 @@
       <c r="O296" t="inlineStr"/>
       <c r="P296" t="inlineStr">
         <is>
-          <t>Steel Skyline Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Mega Steelix, Scizor, and Lucario in Mega Raids Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q296" t="inlineStr">
@@ -12877,12 +12877,12 @@
       <c r="D297" t="inlineStr"/>
       <c r="E297" t="inlineStr">
         <is>
-          <t>Steel Skyline</t>
+          <t>Mega Steelix, Scizor, and Lucario in Mega Raids</t>
         </is>
       </c>
       <c r="F297" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G297" t="inlineStr"/>
@@ -12896,7 +12896,7 @@
       <c r="O297" t="inlineStr"/>
       <c r="P297" t="inlineStr">
         <is>
-          <t>Steel Skyline Tue, Sep 30, at 10:00 AM Local Time</t>
+          <t>Mega Steelix, Scizor, and Lucario in Mega Raids Tue, Sep 30, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q297" t="inlineStr">
@@ -12916,7 +12916,7 @@
       <c r="D298" t="inlineStr"/>
       <c r="E298" t="inlineStr">
         <is>
-          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation</t>
+          <t>Steel Skyline</t>
         </is>
       </c>
       <c r="F298" t="inlineStr">
@@ -12935,7 +12935,7 @@
       <c r="O298" t="inlineStr"/>
       <c r="P298" t="inlineStr">
         <is>
-          <t>GO Battle League Great League and Fantasy Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Event Steel Skyline Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q298" t="inlineStr">
@@ -12955,7 +12955,7 @@
       <c r="D299" t="inlineStr"/>
       <c r="E299" t="inlineStr">
         <is>
-          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation</t>
+          <t>Steel Skyline</t>
         </is>
       </c>
       <c r="F299" t="inlineStr">
@@ -12974,7 +12974,7 @@
       <c r="O299" t="inlineStr"/>
       <c r="P299" t="inlineStr">
         <is>
-          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Steel Skyline Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q299" t="inlineStr">
@@ -12994,7 +12994,7 @@
       <c r="D300" t="inlineStr"/>
       <c r="E300" t="inlineStr">
         <is>
-          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation</t>
+          <t>Steel Skyline</t>
         </is>
       </c>
       <c r="F300" t="inlineStr">
@@ -13013,7 +13013,7 @@
       <c r="O300" t="inlineStr"/>
       <c r="P300" t="inlineStr">
         <is>
-          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Steel Skyline Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q300" t="inlineStr">
@@ -13033,7 +13033,7 @@
       <c r="D301" t="inlineStr"/>
       <c r="E301" t="inlineStr">
         <is>
-          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation</t>
+          <t>Steel Skyline</t>
         </is>
       </c>
       <c r="F301" t="inlineStr">
@@ -13052,7 +13052,7 @@
       <c r="O301" t="inlineStr"/>
       <c r="P301" t="inlineStr">
         <is>
-          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation Calculating...</t>
+          <t>Steel Skyline Tue, Sep 30, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q301" t="inlineStr">
@@ -13072,12 +13072,12 @@
       <c r="D302" t="inlineStr"/>
       <c r="E302" t="inlineStr">
         <is>
-          <t>Aron Spotlight Hour</t>
+          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F302" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G302" t="inlineStr"/>
@@ -13091,7 +13091,7 @@
       <c r="O302" t="inlineStr"/>
       <c r="P302" t="inlineStr">
         <is>
-          <t>Pokémon Spotlight Hour Aron Spotlight Hour Tue, Sep 30, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>GO Battle League Great League and Fantasy Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q302" t="inlineStr">
@@ -13111,12 +13111,12 @@
       <c r="D303" t="inlineStr"/>
       <c r="E303" t="inlineStr">
         <is>
-          <t>Aron Spotlight Hour</t>
+          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F303" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G303" t="inlineStr"/>
@@ -13130,7 +13130,7 @@
       <c r="O303" t="inlineStr"/>
       <c r="P303" t="inlineStr">
         <is>
-          <t>Aron Spotlight Hour Tue, Sep 30, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q303" t="inlineStr">
@@ -13150,12 +13150,12 @@
       <c r="D304" t="inlineStr"/>
       <c r="E304" t="inlineStr">
         <is>
-          <t>Aron Spotlight Hour</t>
+          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F304" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G304" t="inlineStr"/>
@@ -13169,7 +13169,7 @@
       <c r="O304" t="inlineStr"/>
       <c r="P304" t="inlineStr">
         <is>
-          <t>Aron Spotlight Hour Tue, Sep 30, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q304" t="inlineStr">
@@ -13189,12 +13189,12 @@
       <c r="D305" t="inlineStr"/>
       <c r="E305" t="inlineStr">
         <is>
-          <t>Aron Spotlight Hour</t>
+          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F305" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G305" t="inlineStr"/>
@@ -13208,7 +13208,7 @@
       <c r="O305" t="inlineStr"/>
       <c r="P305" t="inlineStr">
         <is>
-          <t>Aron Spotlight Hour Tue, Sep 30, at 6:00 PM Local Time</t>
+          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q305" t="inlineStr">
@@ -13228,12 +13228,12 @@
       <c r="D306" t="inlineStr"/>
       <c r="E306" t="inlineStr">
         <is>
-          <t>Dialga (Origin Forme) Raid Hour</t>
+          <t>Aron Spotlight Hour</t>
         </is>
       </c>
       <c r="F306" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G306" t="inlineStr"/>
@@ -13247,7 +13247,7 @@
       <c r="O306" t="inlineStr"/>
       <c r="P306" t="inlineStr">
         <is>
-          <t>Raid Hour Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Pokémon Spotlight Hour Aron Spotlight Hour Tue, Sep 30, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q306" t="inlineStr">
@@ -13267,12 +13267,12 @@
       <c r="D307" t="inlineStr"/>
       <c r="E307" t="inlineStr">
         <is>
-          <t>Dialga (Origin Forme) Raid Hour</t>
+          <t>Aron Spotlight Hour</t>
         </is>
       </c>
       <c r="F307" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G307" t="inlineStr"/>
@@ -13286,7 +13286,7 @@
       <c r="O307" t="inlineStr"/>
       <c r="P307" t="inlineStr">
         <is>
-          <t>Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Aron Spotlight Hour Tue, Sep 30, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q307" t="inlineStr">
@@ -13306,12 +13306,12 @@
       <c r="D308" t="inlineStr"/>
       <c r="E308" t="inlineStr">
         <is>
-          <t>Dialga (Origin Forme) Raid Hour</t>
+          <t>Aron Spotlight Hour</t>
         </is>
       </c>
       <c r="F308" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G308" t="inlineStr"/>
@@ -13325,7 +13325,7 @@
       <c r="O308" t="inlineStr"/>
       <c r="P308" t="inlineStr">
         <is>
-          <t>Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Aron Spotlight Hour Tue, Sep 30, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q308" t="inlineStr">
@@ -13345,12 +13345,12 @@
       <c r="D309" t="inlineStr"/>
       <c r="E309" t="inlineStr">
         <is>
-          <t>Dialga (Origin Forme) Raid Hour</t>
+          <t>Aron Spotlight Hour</t>
         </is>
       </c>
       <c r="F309" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G309" t="inlineStr"/>
@@ -13364,7 +13364,7 @@
       <c r="O309" t="inlineStr"/>
       <c r="P309" t="inlineStr">
         <is>
-          <t>Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 6:00 PM Local Time</t>
+          <t>Aron Spotlight Hour Tue, Sep 30, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q309" t="inlineStr">
@@ -13384,7 +13384,7 @@
       <c r="D310" t="inlineStr"/>
       <c r="E310" t="inlineStr">
         <is>
-          <t>Mega Metagross Raid Day</t>
+          <t>Dialga (Origin Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F310" t="inlineStr">
@@ -13403,7 +13403,7 @@
       <c r="O310" t="inlineStr"/>
       <c r="P310" t="inlineStr">
         <is>
-          <t>Raid Day Mega Metagross Raid Day Sat, Oct 4, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Raid Hour Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q310" t="inlineStr">
@@ -13423,7 +13423,7 @@
       <c r="D311" t="inlineStr"/>
       <c r="E311" t="inlineStr">
         <is>
-          <t>Mega Metagross Raid Day</t>
+          <t>Dialga (Origin Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F311" t="inlineStr">
@@ -13442,7 +13442,7 @@
       <c r="O311" t="inlineStr"/>
       <c r="P311" t="inlineStr">
         <is>
-          <t>Mega Metagross Raid Day Sat, Oct 4, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q311" t="inlineStr">
@@ -13462,7 +13462,7 @@
       <c r="D312" t="inlineStr"/>
       <c r="E312" t="inlineStr">
         <is>
-          <t>Mega Metagross Raid Day</t>
+          <t>Dialga (Origin Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F312" t="inlineStr">
@@ -13481,7 +13481,7 @@
       <c r="O312" t="inlineStr"/>
       <c r="P312" t="inlineStr">
         <is>
-          <t>Mega Metagross Raid Day Sat, Oct 4, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q312" t="inlineStr">
@@ -13501,7 +13501,7 @@
       <c r="D313" t="inlineStr"/>
       <c r="E313" t="inlineStr">
         <is>
-          <t>Mega Metagross Raid Day</t>
+          <t>Dialga (Origin Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F313" t="inlineStr">
@@ -13520,7 +13520,7 @@
       <c r="O313" t="inlineStr"/>
       <c r="P313" t="inlineStr">
         <is>
-          <t>Mega Metagross Raid Day Sat, Oct 4, at 2:00 PM Local Time</t>
+          <t>Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q313" t="inlineStr">
@@ -13540,12 +13540,12 @@
       <c r="D314" t="inlineStr"/>
       <c r="E314" t="inlineStr">
         <is>
-          <t>Dynamax Drilbur during Max Monday</t>
+          <t>Mega Metagross Raid Day</t>
         </is>
       </c>
       <c r="F314" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G314" t="inlineStr"/>
@@ -13559,7 +13559,7 @@
       <c r="O314" t="inlineStr"/>
       <c r="P314" t="inlineStr">
         <is>
-          <t>Max Mondays Dynamax Drilbur during Max Monday Mon, Oct 6, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Raid Day Mega Metagross Raid Day Sat, Oct 4, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q314" t="inlineStr">
@@ -13579,12 +13579,12 @@
       <c r="D315" t="inlineStr"/>
       <c r="E315" t="inlineStr">
         <is>
-          <t>Dynamax Drilbur during Max Monday</t>
+          <t>Mega Metagross Raid Day</t>
         </is>
       </c>
       <c r="F315" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G315" t="inlineStr"/>
@@ -13598,7 +13598,7 @@
       <c r="O315" t="inlineStr"/>
       <c r="P315" t="inlineStr">
         <is>
-          <t>Dynamax Drilbur during Max Monday Mon, Oct 6, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Mega Metagross Raid Day Sat, Oct 4, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q315" t="inlineStr">
@@ -13618,12 +13618,12 @@
       <c r="D316" t="inlineStr"/>
       <c r="E316" t="inlineStr">
         <is>
-          <t>Dynamax Drilbur during Max Monday</t>
+          <t>Mega Metagross Raid Day</t>
         </is>
       </c>
       <c r="F316" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G316" t="inlineStr"/>
@@ -13637,7 +13637,7 @@
       <c r="O316" t="inlineStr"/>
       <c r="P316" t="inlineStr">
         <is>
-          <t>Dynamax Drilbur during Max Monday Mon, Oct 6, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Mega Metagross Raid Day Sat, Oct 4, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q316" t="inlineStr">
@@ -13657,12 +13657,12 @@
       <c r="D317" t="inlineStr"/>
       <c r="E317" t="inlineStr">
         <is>
-          <t>Dynamax Drilbur during Max Monday</t>
+          <t>Mega Metagross Raid Day</t>
         </is>
       </c>
       <c r="F317" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G317" t="inlineStr"/>
@@ -13676,7 +13676,7 @@
       <c r="O317" t="inlineStr"/>
       <c r="P317" t="inlineStr">
         <is>
-          <t>Dynamax Drilbur during Max Monday Mon, Oct 6, at 6:00 PM Local Time</t>
+          <t>Mega Metagross Raid Day Sat, Oct 4, at 2:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q317" t="inlineStr">
@@ -13696,12 +13696,12 @@
       <c r="D318" t="inlineStr"/>
       <c r="E318" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles</t>
+          <t>Dynamax Drilbur during Max Monday</t>
         </is>
       </c>
       <c r="F318" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G318" t="inlineStr"/>
@@ -13715,7 +13715,7 @@
       <c r="O318" t="inlineStr"/>
       <c r="P318" t="inlineStr">
         <is>
-          <t>Raid Battles Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Max Mondays Dynamax Drilbur during Max Monday Mon, Oct 6, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q318" t="inlineStr">
@@ -13735,12 +13735,12 @@
       <c r="D319" t="inlineStr"/>
       <c r="E319" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles</t>
+          <t>Dynamax Drilbur during Max Monday</t>
         </is>
       </c>
       <c r="F319" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G319" t="inlineStr"/>
@@ -13754,7 +13754,7 @@
       <c r="O319" t="inlineStr"/>
       <c r="P319" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Dynamax Drilbur during Max Monday Mon, Oct 6, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q319" t="inlineStr">
@@ -13774,12 +13774,12 @@
       <c r="D320" t="inlineStr"/>
       <c r="E320" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles</t>
+          <t>Dynamax Drilbur during Max Monday</t>
         </is>
       </c>
       <c r="F320" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G320" t="inlineStr"/>
@@ -13793,7 +13793,7 @@
       <c r="O320" t="inlineStr"/>
       <c r="P320" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Dynamax Drilbur during Max Monday Mon, Oct 6, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q320" t="inlineStr">
@@ -13813,12 +13813,12 @@
       <c r="D321" t="inlineStr"/>
       <c r="E321" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles</t>
+          <t>Dynamax Drilbur during Max Monday</t>
         </is>
       </c>
       <c r="F321" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G321" t="inlineStr"/>
@@ -13832,7 +13832,7 @@
       <c r="O321" t="inlineStr"/>
       <c r="P321" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time</t>
+          <t>Dynamax Drilbur during Max Monday Mon, Oct 6, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q321" t="inlineStr">
@@ -13852,7 +13852,7 @@
       <c r="D322" t="inlineStr"/>
       <c r="E322" t="inlineStr">
         <is>
-          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids</t>
+          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F322" t="inlineStr">
@@ -13871,7 +13871,7 @@
       <c r="O322" t="inlineStr"/>
       <c r="P322" t="inlineStr">
         <is>
-          <t>Raid Battles Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Raid Battles Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q322" t="inlineStr">
@@ -13891,7 +13891,7 @@
       <c r="D323" t="inlineStr"/>
       <c r="E323" t="inlineStr">
         <is>
-          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids</t>
+          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F323" t="inlineStr">
@@ -13910,7 +13910,7 @@
       <c r="O323" t="inlineStr"/>
       <c r="P323" t="inlineStr">
         <is>
-          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q323" t="inlineStr">
@@ -13930,7 +13930,7 @@
       <c r="D324" t="inlineStr"/>
       <c r="E324" t="inlineStr">
         <is>
-          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids</t>
+          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F324" t="inlineStr">
@@ -13949,7 +13949,7 @@
       <c r="O324" t="inlineStr"/>
       <c r="P324" t="inlineStr">
         <is>
-          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q324" t="inlineStr">
@@ -13969,7 +13969,7 @@
       <c r="D325" t="inlineStr"/>
       <c r="E325" t="inlineStr">
         <is>
-          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids</t>
+          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F325" t="inlineStr">
@@ -13988,7 +13988,7 @@
       <c r="O325" t="inlineStr"/>
       <c r="P325" t="inlineStr">
         <is>
-          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids Tue, Oct 7, at 10:00 AM Local Time</t>
+          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q325" t="inlineStr">
@@ -14008,12 +14008,12 @@
       <c r="D326" t="inlineStr"/>
       <c r="E326" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
+          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids</t>
         </is>
       </c>
       <c r="F326" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G326" t="inlineStr"/>
@@ -14027,7 +14027,7 @@
       <c r="O326" t="inlineStr"/>
       <c r="P326" t="inlineStr">
         <is>
-          <t>GO Battle League Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Raid Battles Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q326" t="inlineStr">
@@ -14047,12 +14047,12 @@
       <c r="D327" t="inlineStr"/>
       <c r="E327" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
+          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids</t>
         </is>
       </c>
       <c r="F327" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G327" t="inlineStr"/>
@@ -14066,7 +14066,7 @@
       <c r="O327" t="inlineStr"/>
       <c r="P327" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q327" t="inlineStr">
@@ -14086,12 +14086,12 @@
       <c r="D328" t="inlineStr"/>
       <c r="E328" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
+          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids</t>
         </is>
       </c>
       <c r="F328" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G328" t="inlineStr"/>
@@ -14105,7 +14105,7 @@
       <c r="O328" t="inlineStr"/>
       <c r="P328" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q328" t="inlineStr">
@@ -14125,12 +14125,12 @@
       <c r="D329" t="inlineStr"/>
       <c r="E329" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
+          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids</t>
         </is>
       </c>
       <c r="F329" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G329" t="inlineStr"/>
@@ -14144,7 +14144,7 @@
       <c r="O329" t="inlineStr"/>
       <c r="P329" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating...</t>
+          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids Tue, Oct 7, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q329" t="inlineStr">
@@ -14164,12 +14164,12 @@
       <c r="D330" t="inlineStr"/>
       <c r="E330" t="inlineStr">
         <is>
-          <t>Ferroseed Spotlight Hour</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F330" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G330" t="inlineStr"/>
@@ -14183,7 +14183,7 @@
       <c r="O330" t="inlineStr"/>
       <c r="P330" t="inlineStr">
         <is>
-          <t>Pokémon Spotlight Hour Ferroseed Spotlight Hour Tue, Oct 7, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>GO Battle League Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q330" t="inlineStr">
@@ -14203,12 +14203,12 @@
       <c r="D331" t="inlineStr"/>
       <c r="E331" t="inlineStr">
         <is>
-          <t>Ferroseed Spotlight Hour</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F331" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G331" t="inlineStr"/>
@@ -14222,7 +14222,7 @@
       <c r="O331" t="inlineStr"/>
       <c r="P331" t="inlineStr">
         <is>
-          <t>Ferroseed Spotlight Hour Tue, Oct 7, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q331" t="inlineStr">
@@ -14242,12 +14242,12 @@
       <c r="D332" t="inlineStr"/>
       <c r="E332" t="inlineStr">
         <is>
-          <t>Ferroseed Spotlight Hour</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F332" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G332" t="inlineStr"/>
@@ -14261,7 +14261,7 @@
       <c r="O332" t="inlineStr"/>
       <c r="P332" t="inlineStr">
         <is>
-          <t>Ferroseed Spotlight Hour Tue, Oct 7, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q332" t="inlineStr">
@@ -14281,12 +14281,12 @@
       <c r="D333" t="inlineStr"/>
       <c r="E333" t="inlineStr">
         <is>
-          <t>Ferroseed Spotlight Hour</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F333" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G333" t="inlineStr"/>
@@ -14300,7 +14300,7 @@
       <c r="O333" t="inlineStr"/>
       <c r="P333" t="inlineStr">
         <is>
-          <t>Ferroseed Spotlight Hour Tue, Oct 7, at 6:00 PM Local Time</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q333" t="inlineStr">
@@ -14320,12 +14320,12 @@
       <c r="D334" t="inlineStr"/>
       <c r="E334" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour</t>
+          <t>Ferroseed Spotlight Hour</t>
         </is>
       </c>
       <c r="F334" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G334" t="inlineStr"/>
@@ -14339,7 +14339,7 @@
       <c r="O334" t="inlineStr"/>
       <c r="P334" t="inlineStr">
         <is>
-          <t>Raid Hour Deoxys (Normal &amp; Defense Forme) Raid Hour Wed, Oct 8, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Pokémon Spotlight Hour Ferroseed Spotlight Hour Tue, Oct 7, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q334" t="inlineStr">
@@ -14359,12 +14359,12 @@
       <c r="D335" t="inlineStr"/>
       <c r="E335" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour</t>
+          <t>Ferroseed Spotlight Hour</t>
         </is>
       </c>
       <c r="F335" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G335" t="inlineStr"/>
@@ -14378,7 +14378,7 @@
       <c r="O335" t="inlineStr"/>
       <c r="P335" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour Wed, Oct 8, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Ferroseed Spotlight Hour Tue, Oct 7, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q335" t="inlineStr">
@@ -14398,12 +14398,12 @@
       <c r="D336" t="inlineStr"/>
       <c r="E336" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour</t>
+          <t>Ferroseed Spotlight Hour</t>
         </is>
       </c>
       <c r="F336" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G336" t="inlineStr"/>
@@ -14417,7 +14417,7 @@
       <c r="O336" t="inlineStr"/>
       <c r="P336" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour Wed, Oct 8, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Ferroseed Spotlight Hour Tue, Oct 7, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q336" t="inlineStr">
@@ -14437,12 +14437,12 @@
       <c r="D337" t="inlineStr"/>
       <c r="E337" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour</t>
+          <t>Ferroseed Spotlight Hour</t>
         </is>
       </c>
       <c r="F337" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G337" t="inlineStr"/>
@@ -14456,7 +14456,7 @@
       <c r="O337" t="inlineStr"/>
       <c r="P337" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour Wed, Oct 8, at 6:00 PM Local Time</t>
+          <t>Ferroseed Spotlight Hour Tue, Oct 7, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q337" t="inlineStr">
@@ -14476,12 +14476,12 @@
       <c r="D338" t="inlineStr"/>
       <c r="E338" t="inlineStr">
         <is>
-          <t>Harvest Festival</t>
+          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F338" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G338" t="inlineStr"/>
@@ -14495,7 +14495,7 @@
       <c r="O338" t="inlineStr"/>
       <c r="P338" t="inlineStr">
         <is>
-          <t>Event Harvest Festival Fri, Oct 10, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Raid Hour Deoxys (Normal &amp; Defense Forme) Raid Hour Wed, Oct 8, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q338" t="inlineStr">
@@ -14515,12 +14515,12 @@
       <c r="D339" t="inlineStr"/>
       <c r="E339" t="inlineStr">
         <is>
-          <t>Harvest Festival</t>
+          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F339" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G339" t="inlineStr"/>
@@ -14534,7 +14534,7 @@
       <c r="O339" t="inlineStr"/>
       <c r="P339" t="inlineStr">
         <is>
-          <t>Harvest Festival Fri, Oct 10, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour Wed, Oct 8, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q339" t="inlineStr">
@@ -14554,12 +14554,12 @@
       <c r="D340" t="inlineStr"/>
       <c r="E340" t="inlineStr">
         <is>
-          <t>Harvest Festival</t>
+          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F340" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G340" t="inlineStr"/>
@@ -14573,7 +14573,7 @@
       <c r="O340" t="inlineStr"/>
       <c r="P340" t="inlineStr">
         <is>
-          <t>Harvest Festival Fri, Oct 10, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour Wed, Oct 8, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q340" t="inlineStr">
@@ -14593,12 +14593,12 @@
       <c r="D341" t="inlineStr"/>
       <c r="E341" t="inlineStr">
         <is>
-          <t>Harvest Festival</t>
+          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F341" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G341" t="inlineStr"/>
@@ -14612,7 +14612,7 @@
       <c r="O341" t="inlineStr"/>
       <c r="P341" t="inlineStr">
         <is>
-          <t>Harvest Festival Fri, Oct 10, at 10:00 AM Local Time</t>
+          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour Wed, Oct 8, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q341" t="inlineStr">
@@ -14632,12 +14632,12 @@
       <c r="D342" t="inlineStr"/>
       <c r="E342" t="inlineStr">
         <is>
-          <t>Solosis Community Day</t>
+          <t>Harvest Festival</t>
         </is>
       </c>
       <c r="F342" t="inlineStr">
         <is>
-          <t>Community Day</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G342" t="inlineStr"/>
@@ -14651,7 +14651,7 @@
       <c r="O342" t="inlineStr"/>
       <c r="P342" t="inlineStr">
         <is>
-          <t>Community Day Solosis Community Day Sun, Oct 12, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Event Harvest Festival Fri, Oct 10, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q342" t="inlineStr">
@@ -14671,12 +14671,12 @@
       <c r="D343" t="inlineStr"/>
       <c r="E343" t="inlineStr">
         <is>
-          <t>Solosis Community Day</t>
+          <t>Harvest Festival</t>
         </is>
       </c>
       <c r="F343" t="inlineStr">
         <is>
-          <t>Community Day</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G343" t="inlineStr"/>
@@ -14690,7 +14690,7 @@
       <c r="O343" t="inlineStr"/>
       <c r="P343" t="inlineStr">
         <is>
-          <t>Solosis Community Day Sun, Oct 12, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Harvest Festival Fri, Oct 10, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q343" t="inlineStr">
@@ -14710,12 +14710,12 @@
       <c r="D344" t="inlineStr"/>
       <c r="E344" t="inlineStr">
         <is>
-          <t>Solosis Community Day</t>
+          <t>Harvest Festival</t>
         </is>
       </c>
       <c r="F344" t="inlineStr">
         <is>
-          <t>Community Day</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G344" t="inlineStr"/>
@@ -14729,7 +14729,7 @@
       <c r="O344" t="inlineStr"/>
       <c r="P344" t="inlineStr">
         <is>
-          <t>Solosis Community Day Sun, Oct 12, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Harvest Festival Fri, Oct 10, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q344" t="inlineStr">
@@ -14749,12 +14749,12 @@
       <c r="D345" t="inlineStr"/>
       <c r="E345" t="inlineStr">
         <is>
-          <t>Solosis Community Day</t>
+          <t>Harvest Festival</t>
         </is>
       </c>
       <c r="F345" t="inlineStr">
         <is>
-          <t>Community Day</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G345" t="inlineStr"/>
@@ -14768,7 +14768,7 @@
       <c r="O345" t="inlineStr"/>
       <c r="P345" t="inlineStr">
         <is>
-          <t>Solosis Community Day Sun, Oct 12, at 2:00 PM Local Time</t>
+          <t>Harvest Festival Fri, Oct 10, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q345" t="inlineStr">
@@ -14788,12 +14788,12 @@
       <c r="D346" t="inlineStr"/>
       <c r="E346" t="inlineStr">
         <is>
-          <t>Dynamax Bounsweet during Max Monday</t>
+          <t>Solosis Community Day</t>
         </is>
       </c>
       <c r="F346" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Community Day</t>
         </is>
       </c>
       <c r="G346" t="inlineStr"/>
@@ -14807,7 +14807,7 @@
       <c r="O346" t="inlineStr"/>
       <c r="P346" t="inlineStr">
         <is>
-          <t>Max Mondays Dynamax Bounsweet during Max Monday Mon, Oct 13, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Community Day Solosis Community Day Sun, Oct 12, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q346" t="inlineStr">
@@ -14827,12 +14827,12 @@
       <c r="D347" t="inlineStr"/>
       <c r="E347" t="inlineStr">
         <is>
-          <t>Dynamax Bounsweet during Max Monday</t>
+          <t>Solosis Community Day</t>
         </is>
       </c>
       <c r="F347" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Community Day</t>
         </is>
       </c>
       <c r="G347" t="inlineStr"/>
@@ -14846,7 +14846,7 @@
       <c r="O347" t="inlineStr"/>
       <c r="P347" t="inlineStr">
         <is>
-          <t>Dynamax Bounsweet during Max Monday Mon, Oct 13, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Solosis Community Day Sun, Oct 12, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q347" t="inlineStr">
@@ -14866,12 +14866,12 @@
       <c r="D348" t="inlineStr"/>
       <c r="E348" t="inlineStr">
         <is>
-          <t>Dynamax Bounsweet during Max Monday</t>
+          <t>Solosis Community Day</t>
         </is>
       </c>
       <c r="F348" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Community Day</t>
         </is>
       </c>
       <c r="G348" t="inlineStr"/>
@@ -14885,7 +14885,7 @@
       <c r="O348" t="inlineStr"/>
       <c r="P348" t="inlineStr">
         <is>
-          <t>Dynamax Bounsweet during Max Monday Mon, Oct 13, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Solosis Community Day Sun, Oct 12, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q348" t="inlineStr">
@@ -14905,12 +14905,12 @@
       <c r="D349" t="inlineStr"/>
       <c r="E349" t="inlineStr">
         <is>
-          <t>Dynamax Bounsweet during Max Monday</t>
+          <t>Solosis Community Day</t>
         </is>
       </c>
       <c r="F349" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Community Day</t>
         </is>
       </c>
       <c r="G349" t="inlineStr"/>
@@ -14924,7 +14924,7 @@
       <c r="O349" t="inlineStr"/>
       <c r="P349" t="inlineStr">
         <is>
-          <t>Dynamax Bounsweet during Max Monday Mon, Oct 13, at 6:00 PM Local Time</t>
+          <t>Solosis Community Day Sun, Oct 12, at 2:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q349" t="inlineStr">
@@ -14944,12 +14944,12 @@
       <c r="D350" t="inlineStr"/>
       <c r="E350" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles</t>
+          <t>Dynamax Bounsweet during Max Monday</t>
         </is>
       </c>
       <c r="F350" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G350" t="inlineStr"/>
@@ -14963,7 +14963,7 @@
       <c r="O350" t="inlineStr"/>
       <c r="P350" t="inlineStr">
         <is>
-          <t>Raid Battles Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Max Mondays Dynamax Bounsweet during Max Monday Mon, Oct 13, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q350" t="inlineStr">
@@ -14983,12 +14983,12 @@
       <c r="D351" t="inlineStr"/>
       <c r="E351" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles</t>
+          <t>Dynamax Bounsweet during Max Monday</t>
         </is>
       </c>
       <c r="F351" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G351" t="inlineStr"/>
@@ -15002,7 +15002,7 @@
       <c r="O351" t="inlineStr"/>
       <c r="P351" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Dynamax Bounsweet during Max Monday Mon, Oct 13, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q351" t="inlineStr">
@@ -15022,12 +15022,12 @@
       <c r="D352" t="inlineStr"/>
       <c r="E352" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles</t>
+          <t>Dynamax Bounsweet during Max Monday</t>
         </is>
       </c>
       <c r="F352" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G352" t="inlineStr"/>
@@ -15041,7 +15041,7 @@
       <c r="O352" t="inlineStr"/>
       <c r="P352" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Dynamax Bounsweet during Max Monday Mon, Oct 13, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q352" t="inlineStr">
@@ -15061,12 +15061,12 @@
       <c r="D353" t="inlineStr"/>
       <c r="E353" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles</t>
+          <t>Dynamax Bounsweet during Max Monday</t>
         </is>
       </c>
       <c r="F353" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G353" t="inlineStr"/>
@@ -15080,7 +15080,7 @@
       <c r="O353" t="inlineStr"/>
       <c r="P353" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles Tue, Oct 14, at 10:00 AM Local Time</t>
+          <t>Dynamax Bounsweet during Max Monday Mon, Oct 13, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q353" t="inlineStr">
@@ -15100,7 +15100,7 @@
       <c r="D354" t="inlineStr"/>
       <c r="E354" t="inlineStr">
         <is>
-          <t>Mega Mawile and Mega Salamence in Mega Raids</t>
+          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F354" t="inlineStr">
@@ -15119,7 +15119,7 @@
       <c r="O354" t="inlineStr"/>
       <c r="P354" t="inlineStr">
         <is>
-          <t>Raid Battles Mega Mawile and Mega Salamence in Mega Raids Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Raid Battles Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q354" t="inlineStr">
@@ -15139,7 +15139,7 @@
       <c r="D355" t="inlineStr"/>
       <c r="E355" t="inlineStr">
         <is>
-          <t>Mega Mawile and Mega Salamence in Mega Raids</t>
+          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F355" t="inlineStr">
@@ -15158,7 +15158,7 @@
       <c r="O355" t="inlineStr"/>
       <c r="P355" t="inlineStr">
         <is>
-          <t>Mega Mawile and Mega Salamence in Mega Raids Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q355" t="inlineStr">
@@ -15178,7 +15178,7 @@
       <c r="D356" t="inlineStr"/>
       <c r="E356" t="inlineStr">
         <is>
-          <t>Mega Mawile and Mega Salamence in Mega Raids</t>
+          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F356" t="inlineStr">
@@ -15197,7 +15197,7 @@
       <c r="O356" t="inlineStr"/>
       <c r="P356" t="inlineStr">
         <is>
-          <t>Mega Mawile and Mega Salamence in Mega Raids Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q356" t="inlineStr">
@@ -15217,7 +15217,7 @@
       <c r="D357" t="inlineStr"/>
       <c r="E357" t="inlineStr">
         <is>
-          <t>Mega Mawile and Mega Salamence in Mega Raids</t>
+          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F357" t="inlineStr">
@@ -15236,7 +15236,7 @@
       <c r="O357" t="inlineStr"/>
       <c r="P357" t="inlineStr">
         <is>
-          <t>Mega Mawile and Mega Salamence in Mega Raids Tue, Oct 14, at 10:00 AM Local Time</t>
+          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles Tue, Oct 14, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q357" t="inlineStr">
@@ -15256,12 +15256,12 @@
       <c r="D358" t="inlineStr"/>
       <c r="E358" t="inlineStr">
         <is>
-          <t>Master Premier and Great League Remix | Tales of Transformation</t>
+          <t>Mega Mawile and Mega Salamence in Mega Raids</t>
         </is>
       </c>
       <c r="F358" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G358" t="inlineStr"/>
@@ -15275,7 +15275,7 @@
       <c r="O358" t="inlineStr"/>
       <c r="P358" t="inlineStr">
         <is>
-          <t>GO Battle League Master Premier and Great League Remix | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Raid Battles Mega Mawile and Mega Salamence in Mega Raids Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q358" t="inlineStr">
@@ -15295,12 +15295,12 @@
       <c r="D359" t="inlineStr"/>
       <c r="E359" t="inlineStr">
         <is>
-          <t>Master Premier and Great League Remix | Tales of Transformation</t>
+          <t>Mega Mawile and Mega Salamence in Mega Raids</t>
         </is>
       </c>
       <c r="F359" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G359" t="inlineStr"/>
@@ -15314,7 +15314,7 @@
       <c r="O359" t="inlineStr"/>
       <c r="P359" t="inlineStr">
         <is>
-          <t>Master Premier and Great League Remix | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Mega Mawile and Mega Salamence in Mega Raids Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q359" t="inlineStr">
@@ -15334,12 +15334,12 @@
       <c r="D360" t="inlineStr"/>
       <c r="E360" t="inlineStr">
         <is>
-          <t>Master Premier and Great League Remix | Tales of Transformation</t>
+          <t>Mega Mawile and Mega Salamence in Mega Raids</t>
         </is>
       </c>
       <c r="F360" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G360" t="inlineStr"/>
@@ -15353,7 +15353,7 @@
       <c r="O360" t="inlineStr"/>
       <c r="P360" t="inlineStr">
         <is>
-          <t>Master Premier and Great League Remix | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Mega Mawile and Mega Salamence in Mega Raids Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q360" t="inlineStr">
@@ -15373,12 +15373,12 @@
       <c r="D361" t="inlineStr"/>
       <c r="E361" t="inlineStr">
         <is>
-          <t>Master Premier and Great League Remix | Tales of Transformation</t>
+          <t>Mega Mawile and Mega Salamence in Mega Raids</t>
         </is>
       </c>
       <c r="F361" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G361" t="inlineStr"/>
@@ -15392,7 +15392,7 @@
       <c r="O361" t="inlineStr"/>
       <c r="P361" t="inlineStr">
         <is>
-          <t>Master Premier and Great League Remix | Tales of Transformation Calculating...</t>
+          <t>Mega Mawile and Mega Salamence in Mega Raids Tue, Oct 14, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q361" t="inlineStr">
@@ -15412,12 +15412,12 @@
       <c r="D362" t="inlineStr"/>
       <c r="E362" t="inlineStr">
         <is>
-          <t>Petilil Spotlight Hour</t>
+          <t>Master Premier and Great League Remix | Tales of Transformation</t>
         </is>
       </c>
       <c r="F362" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G362" t="inlineStr"/>
@@ -15431,7 +15431,7 @@
       <c r="O362" t="inlineStr"/>
       <c r="P362" t="inlineStr">
         <is>
-          <t>Pokémon Spotlight Hour Petilil Spotlight Hour Tue, Oct 14, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>GO Battle League Master Premier and Great League Remix | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q362" t="inlineStr">
@@ -15451,12 +15451,12 @@
       <c r="D363" t="inlineStr"/>
       <c r="E363" t="inlineStr">
         <is>
-          <t>Petilil Spotlight Hour</t>
+          <t>Master Premier and Great League Remix | Tales of Transformation</t>
         </is>
       </c>
       <c r="F363" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G363" t="inlineStr"/>
@@ -15470,7 +15470,7 @@
       <c r="O363" t="inlineStr"/>
       <c r="P363" t="inlineStr">
         <is>
-          <t>Petilil Spotlight Hour Tue, Oct 14, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Master Premier and Great League Remix | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q363" t="inlineStr">
@@ -15490,12 +15490,12 @@
       <c r="D364" t="inlineStr"/>
       <c r="E364" t="inlineStr">
         <is>
-          <t>Petilil Spotlight Hour</t>
+          <t>Master Premier and Great League Remix | Tales of Transformation</t>
         </is>
       </c>
       <c r="F364" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G364" t="inlineStr"/>
@@ -15509,7 +15509,7 @@
       <c r="O364" t="inlineStr"/>
       <c r="P364" t="inlineStr">
         <is>
-          <t>Petilil Spotlight Hour Tue, Oct 14, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Master Premier and Great League Remix | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q364" t="inlineStr">
@@ -15529,12 +15529,12 @@
       <c r="D365" t="inlineStr"/>
       <c r="E365" t="inlineStr">
         <is>
-          <t>Petilil Spotlight Hour</t>
+          <t>Master Premier and Great League Remix | Tales of Transformation</t>
         </is>
       </c>
       <c r="F365" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G365" t="inlineStr"/>
@@ -15548,7 +15548,7 @@
       <c r="O365" t="inlineStr"/>
       <c r="P365" t="inlineStr">
         <is>
-          <t>Petilil Spotlight Hour Tue, Oct 14, at 6:00 PM Local Time</t>
+          <t>Master Premier and Great League Remix | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q365" t="inlineStr">
@@ -15568,12 +15568,12 @@
       <c r="D366" t="inlineStr"/>
       <c r="E366" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour</t>
+          <t>Petilil Spotlight Hour</t>
         </is>
       </c>
       <c r="F366" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G366" t="inlineStr"/>
@@ -15587,7 +15587,7 @@
       <c r="O366" t="inlineStr"/>
       <c r="P366" t="inlineStr">
         <is>
-          <t>Raid Hour Deoxys (Attack &amp; Speed Forme) Raid Hour Wed, Oct 15, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Pokémon Spotlight Hour Petilil Spotlight Hour Tue, Oct 14, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q366" t="inlineStr">
@@ -15607,12 +15607,12 @@
       <c r="D367" t="inlineStr"/>
       <c r="E367" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour</t>
+          <t>Petilil Spotlight Hour</t>
         </is>
       </c>
       <c r="F367" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G367" t="inlineStr"/>
@@ -15626,7 +15626,7 @@
       <c r="O367" t="inlineStr"/>
       <c r="P367" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour Wed, Oct 15, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Petilil Spotlight Hour Tue, Oct 14, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q367" t="inlineStr">
@@ -15646,12 +15646,12 @@
       <c r="D368" t="inlineStr"/>
       <c r="E368" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour</t>
+          <t>Petilil Spotlight Hour</t>
         </is>
       </c>
       <c r="F368" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G368" t="inlineStr"/>
@@ -15665,7 +15665,7 @@
       <c r="O368" t="inlineStr"/>
       <c r="P368" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour Wed, Oct 15, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Petilil Spotlight Hour Tue, Oct 14, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q368" t="inlineStr">
@@ -15685,12 +15685,12 @@
       <c r="D369" t="inlineStr"/>
       <c r="E369" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour</t>
+          <t>Petilil Spotlight Hour</t>
         </is>
       </c>
       <c r="F369" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G369" t="inlineStr"/>
@@ -15704,7 +15704,7 @@
       <c r="O369" t="inlineStr"/>
       <c r="P369" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour Wed, Oct 15, at 6:00 PM Local Time</t>
+          <t>Petilil Spotlight Hour Tue, Oct 14, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q369" t="inlineStr">
@@ -15724,12 +15724,12 @@
       <c r="D370" t="inlineStr"/>
       <c r="E370" t="inlineStr">
         <is>
-          <t>Pokémon Legends: Z-A Celebration Event</t>
+          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F370" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G370" t="inlineStr"/>
@@ -15743,7 +15743,7 @@
       <c r="O370" t="inlineStr"/>
       <c r="P370" t="inlineStr">
         <is>
-          <t>Event Pokémon Legends: Z-A Celebration Event Thu, Oct 16, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Raid Hour Deoxys (Attack &amp; Speed Forme) Raid Hour Wed, Oct 15, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q370" t="inlineStr">
@@ -15763,12 +15763,12 @@
       <c r="D371" t="inlineStr"/>
       <c r="E371" t="inlineStr">
         <is>
-          <t>Pokémon Legends: Z-A Celebration Event</t>
+          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F371" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G371" t="inlineStr"/>
@@ -15782,7 +15782,7 @@
       <c r="O371" t="inlineStr"/>
       <c r="P371" t="inlineStr">
         <is>
-          <t>Pokémon Legends: Z-A Celebration Event Thu, Oct 16, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour Wed, Oct 15, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q371" t="inlineStr">
@@ -15802,12 +15802,12 @@
       <c r="D372" t="inlineStr"/>
       <c r="E372" t="inlineStr">
         <is>
-          <t>Pokémon Legends: Z-A Celebration Event</t>
+          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F372" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G372" t="inlineStr"/>
@@ -15821,7 +15821,7 @@
       <c r="O372" t="inlineStr"/>
       <c r="P372" t="inlineStr">
         <is>
-          <t>Pokémon Legends: Z-A Celebration Event Thu, Oct 16, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour Wed, Oct 15, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q372" t="inlineStr">
@@ -15841,12 +15841,12 @@
       <c r="D373" t="inlineStr"/>
       <c r="E373" t="inlineStr">
         <is>
-          <t>Pokémon Legends: Z-A Celebration Event</t>
+          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F373" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G373" t="inlineStr"/>
@@ -15860,7 +15860,7 @@
       <c r="O373" t="inlineStr"/>
       <c r="P373" t="inlineStr">
         <is>
-          <t>Pokémon Legends: Z-A Celebration Event Thu, Oct 16, at 10:00 AM Local Time</t>
+          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour Wed, Oct 15, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q373" t="inlineStr">
@@ -15880,12 +15880,12 @@
       <c r="D374" t="inlineStr"/>
       <c r="E374" t="inlineStr">
         <is>
-          <t>Mega Rayquaza Raid Day</t>
+          <t>Pokémon Legends: Z-A Celebration Event</t>
         </is>
       </c>
       <c r="F374" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G374" t="inlineStr"/>
@@ -15899,7 +15899,7 @@
       <c r="O374" t="inlineStr"/>
       <c r="P374" t="inlineStr">
         <is>
-          <t>Raid Day Mega Rayquaza Raid Day Sat, Oct 18, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Event Pokémon Legends: Z-A Celebration Event Thu, Oct 16, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q374" t="inlineStr">
@@ -15919,12 +15919,12 @@
       <c r="D375" t="inlineStr"/>
       <c r="E375" t="inlineStr">
         <is>
-          <t>Mega Rayquaza Raid Day</t>
+          <t>Pokémon Legends: Z-A Celebration Event</t>
         </is>
       </c>
       <c r="F375" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G375" t="inlineStr"/>
@@ -15938,7 +15938,7 @@
       <c r="O375" t="inlineStr"/>
       <c r="P375" t="inlineStr">
         <is>
-          <t>Mega Rayquaza Raid Day Sat, Oct 18, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Pokémon Legends: Z-A Celebration Event Thu, Oct 16, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q375" t="inlineStr">
@@ -15958,12 +15958,12 @@
       <c r="D376" t="inlineStr"/>
       <c r="E376" t="inlineStr">
         <is>
-          <t>Mega Rayquaza Raid Day</t>
+          <t>Pokémon Legends: Z-A Celebration Event</t>
         </is>
       </c>
       <c r="F376" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G376" t="inlineStr"/>
@@ -15977,7 +15977,7 @@
       <c r="O376" t="inlineStr"/>
       <c r="P376" t="inlineStr">
         <is>
-          <t>Mega Rayquaza Raid Day Sat, Oct 18, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Pokémon Legends: Z-A Celebration Event Thu, Oct 16, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q376" t="inlineStr">
@@ -15997,12 +15997,12 @@
       <c r="D377" t="inlineStr"/>
       <c r="E377" t="inlineStr">
         <is>
-          <t>Mega Rayquaza Raid Day</t>
+          <t>Pokémon Legends: Z-A Celebration Event</t>
         </is>
       </c>
       <c r="F377" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G377" t="inlineStr"/>
@@ -16016,7 +16016,7 @@
       <c r="O377" t="inlineStr"/>
       <c r="P377" t="inlineStr">
         <is>
-          <t>Mega Rayquaza Raid Day Sat, Oct 18, at 2:00 PM Local Time</t>
+          <t>Pokémon Legends: Z-A Celebration Event Thu, Oct 16, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q377" t="inlineStr">
@@ -16036,12 +16036,12 @@
       <c r="D378" t="inlineStr"/>
       <c r="E378" t="inlineStr">
         <is>
-          <t>Dynamax Gastly during Max Monday</t>
+          <t>Mega Rayquaza Raid Day</t>
         </is>
       </c>
       <c r="F378" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G378" t="inlineStr"/>
@@ -16055,7 +16055,7 @@
       <c r="O378" t="inlineStr"/>
       <c r="P378" t="inlineStr">
         <is>
-          <t>Max Mondays Dynamax Gastly during Max Monday Mon, Oct 20, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Raid Day Mega Rayquaza Raid Day Sat, Oct 18, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q378" t="inlineStr">
@@ -16075,12 +16075,12 @@
       <c r="D379" t="inlineStr"/>
       <c r="E379" t="inlineStr">
         <is>
-          <t>Dynamax Gastly during Max Monday</t>
+          <t>Mega Rayquaza Raid Day</t>
         </is>
       </c>
       <c r="F379" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G379" t="inlineStr"/>
@@ -16094,7 +16094,7 @@
       <c r="O379" t="inlineStr"/>
       <c r="P379" t="inlineStr">
         <is>
-          <t>Dynamax Gastly during Max Monday Mon, Oct 20, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Mega Rayquaza Raid Day Sat, Oct 18, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q379" t="inlineStr">
@@ -16114,12 +16114,12 @@
       <c r="D380" t="inlineStr"/>
       <c r="E380" t="inlineStr">
         <is>
-          <t>Dynamax Gastly during Max Monday</t>
+          <t>Mega Rayquaza Raid Day</t>
         </is>
       </c>
       <c r="F380" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G380" t="inlineStr"/>
@@ -16133,7 +16133,7 @@
       <c r="O380" t="inlineStr"/>
       <c r="P380" t="inlineStr">
         <is>
-          <t>Dynamax Gastly during Max Monday Mon, Oct 20, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Mega Rayquaza Raid Day Sat, Oct 18, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q380" t="inlineStr">
@@ -16153,12 +16153,12 @@
       <c r="D381" t="inlineStr"/>
       <c r="E381" t="inlineStr">
         <is>
-          <t>Dynamax Gastly during Max Monday</t>
+          <t>Mega Rayquaza Raid Day</t>
         </is>
       </c>
       <c r="F381" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G381" t="inlineStr"/>
@@ -16172,7 +16172,7 @@
       <c r="O381" t="inlineStr"/>
       <c r="P381" t="inlineStr">
         <is>
-          <t>Dynamax Gastly during Max Monday Mon, Oct 20, at 6:00 PM Local Time</t>
+          <t>Mega Rayquaza Raid Day Sat, Oct 18, at 2:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q381" t="inlineStr">
@@ -16192,7 +16192,7 @@
       <c r="D382" t="inlineStr"/>
       <c r="E382" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part I</t>
+          <t>Dynamax Gastly during Max Monday</t>
         </is>
       </c>
       <c r="F382" t="inlineStr">
@@ -16211,7 +16211,7 @@
       <c r="O382" t="inlineStr"/>
       <c r="P382" t="inlineStr">
         <is>
-          <t>Event Halloween 2025 Part I Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Max Mondays Dynamax Gastly during Max Monday Mon, Oct 20, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q382" t="inlineStr">
@@ -16231,7 +16231,7 @@
       <c r="D383" t="inlineStr"/>
       <c r="E383" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part I</t>
+          <t>Dynamax Gastly during Max Monday</t>
         </is>
       </c>
       <c r="F383" t="inlineStr">
@@ -16250,7 +16250,7 @@
       <c r="O383" t="inlineStr"/>
       <c r="P383" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part I Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Dynamax Gastly during Max Monday Mon, Oct 20, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q383" t="inlineStr">
@@ -16270,7 +16270,7 @@
       <c r="D384" t="inlineStr"/>
       <c r="E384" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part I</t>
+          <t>Dynamax Gastly during Max Monday</t>
         </is>
       </c>
       <c r="F384" t="inlineStr">
@@ -16289,7 +16289,7 @@
       <c r="O384" t="inlineStr"/>
       <c r="P384" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part I Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Dynamax Gastly during Max Monday Mon, Oct 20, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q384" t="inlineStr">
@@ -16309,7 +16309,7 @@
       <c r="D385" t="inlineStr"/>
       <c r="E385" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part I</t>
+          <t>Dynamax Gastly during Max Monday</t>
         </is>
       </c>
       <c r="F385" t="inlineStr">
@@ -16328,7 +16328,7 @@
       <c r="O385" t="inlineStr"/>
       <c r="P385" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part I Tue, Oct 21, at 10:00 AM Local Time</t>
+          <t>Dynamax Gastly during Max Monday Mon, Oct 20, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q385" t="inlineStr">
@@ -16348,12 +16348,12 @@
       <c r="D386" t="inlineStr"/>
       <c r="E386" t="inlineStr">
         <is>
-          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles</t>
+          <t>Halloween 2025 Part I</t>
         </is>
       </c>
       <c r="F386" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G386" t="inlineStr"/>
@@ -16367,7 +16367,7 @@
       <c r="O386" t="inlineStr"/>
       <c r="P386" t="inlineStr">
         <is>
-          <t>Raid Battles Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Event Halloween 2025 Part I Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q386" t="inlineStr">
@@ -16387,12 +16387,12 @@
       <c r="D387" t="inlineStr"/>
       <c r="E387" t="inlineStr">
         <is>
-          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles</t>
+          <t>Halloween 2025 Part I</t>
         </is>
       </c>
       <c r="F387" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G387" t="inlineStr"/>
@@ -16406,7 +16406,7 @@
       <c r="O387" t="inlineStr"/>
       <c r="P387" t="inlineStr">
         <is>
-          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Halloween 2025 Part I Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q387" t="inlineStr">
@@ -16426,12 +16426,12 @@
       <c r="D388" t="inlineStr"/>
       <c r="E388" t="inlineStr">
         <is>
-          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles</t>
+          <t>Halloween 2025 Part I</t>
         </is>
       </c>
       <c r="F388" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G388" t="inlineStr"/>
@@ -16445,7 +16445,7 @@
       <c r="O388" t="inlineStr"/>
       <c r="P388" t="inlineStr">
         <is>
-          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Halloween 2025 Part I Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q388" t="inlineStr">
@@ -16465,12 +16465,12 @@
       <c r="D389" t="inlineStr"/>
       <c r="E389" t="inlineStr">
         <is>
-          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles</t>
+          <t>Halloween 2025 Part I</t>
         </is>
       </c>
       <c r="F389" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G389" t="inlineStr"/>
@@ -16484,7 +16484,7 @@
       <c r="O389" t="inlineStr"/>
       <c r="P389" t="inlineStr">
         <is>
-          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles Tue, Oct 21, at 10:00 AM Local Time</t>
+          <t>Halloween 2025 Part I Tue, Oct 21, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q389" t="inlineStr">
@@ -16504,7 +16504,7 @@
       <c r="D390" t="inlineStr"/>
       <c r="E390" t="inlineStr">
         <is>
-          <t>Mega Houndoom and Mega Absol in Mega Raids</t>
+          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F390" t="inlineStr">
@@ -16523,7 +16523,7 @@
       <c r="O390" t="inlineStr"/>
       <c r="P390" t="inlineStr">
         <is>
-          <t>Raid Battles Mega Houndoom and Mega Absol in Mega Raids Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Raid Battles Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q390" t="inlineStr">
@@ -16543,7 +16543,7 @@
       <c r="D391" t="inlineStr"/>
       <c r="E391" t="inlineStr">
         <is>
-          <t>Mega Houndoom and Mega Absol in Mega Raids</t>
+          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F391" t="inlineStr">
@@ -16562,7 +16562,7 @@
       <c r="O391" t="inlineStr"/>
       <c r="P391" t="inlineStr">
         <is>
-          <t>Mega Houndoom and Mega Absol in Mega Raids Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q391" t="inlineStr">
@@ -16582,7 +16582,7 @@
       <c r="D392" t="inlineStr"/>
       <c r="E392" t="inlineStr">
         <is>
-          <t>Mega Houndoom and Mega Absol in Mega Raids</t>
+          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F392" t="inlineStr">
@@ -16601,7 +16601,7 @@
       <c r="O392" t="inlineStr"/>
       <c r="P392" t="inlineStr">
         <is>
-          <t>Mega Houndoom and Mega Absol in Mega Raids Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q392" t="inlineStr">
@@ -16621,7 +16621,7 @@
       <c r="D393" t="inlineStr"/>
       <c r="E393" t="inlineStr">
         <is>
-          <t>Mega Houndoom and Mega Absol in Mega Raids</t>
+          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F393" t="inlineStr">
@@ -16640,7 +16640,7 @@
       <c r="O393" t="inlineStr"/>
       <c r="P393" t="inlineStr">
         <is>
-          <t>Mega Houndoom and Mega Absol in Mega Raids Tue, Oct 21, at 10:00 AM Local Time</t>
+          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles Tue, Oct 21, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q393" t="inlineStr">
@@ -16660,12 +16660,12 @@
       <c r="D394" t="inlineStr"/>
       <c r="E394" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Mega Houndoom and Mega Absol in Mega Raids</t>
         </is>
       </c>
       <c r="F394" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G394" t="inlineStr"/>
@@ -16679,7 +16679,7 @@
       <c r="O394" t="inlineStr"/>
       <c r="P394" t="inlineStr">
         <is>
-          <t>GO Battle League Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Raid Battles Mega Houndoom and Mega Absol in Mega Raids Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q394" t="inlineStr">
@@ -16699,12 +16699,12 @@
       <c r="D395" t="inlineStr"/>
       <c r="E395" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Mega Houndoom and Mega Absol in Mega Raids</t>
         </is>
       </c>
       <c r="F395" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G395" t="inlineStr"/>
@@ -16718,7 +16718,7 @@
       <c r="O395" t="inlineStr"/>
       <c r="P395" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Mega Houndoom and Mega Absol in Mega Raids Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q395" t="inlineStr">
@@ -16738,12 +16738,12 @@
       <c r="D396" t="inlineStr"/>
       <c r="E396" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Mega Houndoom and Mega Absol in Mega Raids</t>
         </is>
       </c>
       <c r="F396" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G396" t="inlineStr"/>
@@ -16757,7 +16757,7 @@
       <c r="O396" t="inlineStr"/>
       <c r="P396" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Mega Houndoom and Mega Absol in Mega Raids Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q396" t="inlineStr">
@@ -16777,12 +16777,12 @@
       <c r="D397" t="inlineStr"/>
       <c r="E397" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Mega Houndoom and Mega Absol in Mega Raids</t>
         </is>
       </c>
       <c r="F397" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G397" t="inlineStr"/>
@@ -16796,7 +16796,7 @@
       <c r="O397" t="inlineStr"/>
       <c r="P397" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating...</t>
+          <t>Mega Houndoom and Mega Absol in Mega Raids Tue, Oct 21, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q397" t="inlineStr">
@@ -16816,12 +16816,12 @@
       <c r="D398" t="inlineStr"/>
       <c r="E398" t="inlineStr">
         <is>
-          <t>Gastly Spotlight Hour</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F398" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G398" t="inlineStr"/>
@@ -16835,7 +16835,7 @@
       <c r="O398" t="inlineStr"/>
       <c r="P398" t="inlineStr">
         <is>
-          <t>Pokémon Spotlight Hour Gastly Spotlight Hour Tue, Oct 21, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>GO Battle League Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q398" t="inlineStr">
@@ -16855,12 +16855,12 @@
       <c r="D399" t="inlineStr"/>
       <c r="E399" t="inlineStr">
         <is>
-          <t>Gastly Spotlight Hour</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F399" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G399" t="inlineStr"/>
@@ -16874,7 +16874,7 @@
       <c r="O399" t="inlineStr"/>
       <c r="P399" t="inlineStr">
         <is>
-          <t>Gastly Spotlight Hour Tue, Oct 21, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q399" t="inlineStr">
@@ -16894,12 +16894,12 @@
       <c r="D400" t="inlineStr"/>
       <c r="E400" t="inlineStr">
         <is>
-          <t>Gastly Spotlight Hour</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F400" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G400" t="inlineStr"/>
@@ -16913,7 +16913,7 @@
       <c r="O400" t="inlineStr"/>
       <c r="P400" t="inlineStr">
         <is>
-          <t>Gastly Spotlight Hour Tue, Oct 21, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q400" t="inlineStr">
@@ -16933,12 +16933,12 @@
       <c r="D401" t="inlineStr"/>
       <c r="E401" t="inlineStr">
         <is>
-          <t>Gastly Spotlight Hour</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F401" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G401" t="inlineStr"/>
@@ -16952,7 +16952,7 @@
       <c r="O401" t="inlineStr"/>
       <c r="P401" t="inlineStr">
         <is>
-          <t>Gastly Spotlight Hour Tue, Oct 21, at 6:00 PM Local Time</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q401" t="inlineStr">
@@ -16972,12 +16972,12 @@
       <c r="D402" t="inlineStr"/>
       <c r="E402" t="inlineStr">
         <is>
-          <t>Genesect Raid Hour</t>
+          <t>Gastly Spotlight Hour</t>
         </is>
       </c>
       <c r="F402" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G402" t="inlineStr"/>
@@ -16991,7 +16991,7 @@
       <c r="O402" t="inlineStr"/>
       <c r="P402" t="inlineStr">
         <is>
-          <t>Raid Hour Genesect Raid Hour Wed, Oct 22, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Pokémon Spotlight Hour Gastly Spotlight Hour Tue, Oct 21, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q402" t="inlineStr">
@@ -17011,12 +17011,12 @@
       <c r="D403" t="inlineStr"/>
       <c r="E403" t="inlineStr">
         <is>
-          <t>Genesect Raid Hour</t>
+          <t>Gastly Spotlight Hour</t>
         </is>
       </c>
       <c r="F403" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G403" t="inlineStr"/>
@@ -17030,7 +17030,7 @@
       <c r="O403" t="inlineStr"/>
       <c r="P403" t="inlineStr">
         <is>
-          <t>Genesect Raid Hour Wed, Oct 22, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Gastly Spotlight Hour Tue, Oct 21, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q403" t="inlineStr">
@@ -17050,12 +17050,12 @@
       <c r="D404" t="inlineStr"/>
       <c r="E404" t="inlineStr">
         <is>
-          <t>Genesect Raid Hour</t>
+          <t>Gastly Spotlight Hour</t>
         </is>
       </c>
       <c r="F404" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G404" t="inlineStr"/>
@@ -17069,7 +17069,7 @@
       <c r="O404" t="inlineStr"/>
       <c r="P404" t="inlineStr">
         <is>
-          <t>Genesect Raid Hour Wed, Oct 22, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Gastly Spotlight Hour Tue, Oct 21, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q404" t="inlineStr">
@@ -17089,12 +17089,12 @@
       <c r="D405" t="inlineStr"/>
       <c r="E405" t="inlineStr">
         <is>
-          <t>Genesect Raid Hour</t>
+          <t>Gastly Spotlight Hour</t>
         </is>
       </c>
       <c r="F405" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G405" t="inlineStr"/>
@@ -17108,7 +17108,7 @@
       <c r="O405" t="inlineStr"/>
       <c r="P405" t="inlineStr">
         <is>
-          <t>Genesect Raid Hour Wed, Oct 22, at 6:00 PM Local Time</t>
+          <t>Gastly Spotlight Hour Tue, Oct 21, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q405" t="inlineStr">
@@ -17128,12 +17128,12 @@
       <c r="D406" t="inlineStr"/>
       <c r="E406" t="inlineStr">
         <is>
-          <t>GO Battle Weekend: Tales of Transformation</t>
+          <t>Genesect Raid Hour</t>
         </is>
       </c>
       <c r="F406" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G406" t="inlineStr"/>
@@ -17147,7 +17147,7 @@
       <c r="O406" t="inlineStr"/>
       <c r="P406" t="inlineStr">
         <is>
-          <t>Event GO Battle Weekend: Tales of Transformation Sat, Oct 25, at 12:00 AM Local Time Starts: Calculating...</t>
+          <t>Raid Hour Genesect Raid Hour Wed, Oct 22, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q406" t="inlineStr">
@@ -17167,12 +17167,12 @@
       <c r="D407" t="inlineStr"/>
       <c r="E407" t="inlineStr">
         <is>
-          <t>GO Battle Weekend: Tales of Transformation</t>
+          <t>Genesect Raid Hour</t>
         </is>
       </c>
       <c r="F407" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G407" t="inlineStr"/>
@@ -17186,7 +17186,7 @@
       <c r="O407" t="inlineStr"/>
       <c r="P407" t="inlineStr">
         <is>
-          <t>GO Battle Weekend: Tales of Transformation Sat, Oct 25, at 12:00 AM Local Time Starts: Calculating...</t>
+          <t>Genesect Raid Hour Wed, Oct 22, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q407" t="inlineStr">
@@ -17206,12 +17206,12 @@
       <c r="D408" t="inlineStr"/>
       <c r="E408" t="inlineStr">
         <is>
-          <t>GO Battle Weekend: Tales of Transformation</t>
+          <t>Genesect Raid Hour</t>
         </is>
       </c>
       <c r="F408" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G408" t="inlineStr"/>
@@ -17225,7 +17225,7 @@
       <c r="O408" t="inlineStr"/>
       <c r="P408" t="inlineStr">
         <is>
-          <t>GO Battle Weekend: Tales of Transformation Sat, Oct 25, at 12:00 AM Local Time Starts: Calculating...</t>
+          <t>Genesect Raid Hour Wed, Oct 22, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q408" t="inlineStr">
@@ -17245,12 +17245,12 @@
       <c r="D409" t="inlineStr"/>
       <c r="E409" t="inlineStr">
         <is>
-          <t>GO Battle Weekend: Tales of Transformation</t>
+          <t>Genesect Raid Hour</t>
         </is>
       </c>
       <c r="F409" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G409" t="inlineStr"/>
@@ -17264,7 +17264,7 @@
       <c r="O409" t="inlineStr"/>
       <c r="P409" t="inlineStr">
         <is>
-          <t>GO Battle Weekend: Tales of Transformation Sat, Oct 25, at 12:00 AM Local Time</t>
+          <t>Genesect Raid Hour Wed, Oct 22, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q409" t="inlineStr">
@@ -17284,7 +17284,7 @@
       <c r="D410" t="inlineStr"/>
       <c r="E410" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part II</t>
+          <t>GO Battle Weekend: Tales of Transformation</t>
         </is>
       </c>
       <c r="F410" t="inlineStr">
@@ -17303,7 +17303,7 @@
       <c r="O410" t="inlineStr"/>
       <c r="P410" t="inlineStr">
         <is>
-          <t>Event Halloween 2025 Part II Mon, Oct 27, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Event GO Battle Weekend: Tales of Transformation Sat, Oct 25, at 12:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q410" t="inlineStr">
@@ -17323,7 +17323,7 @@
       <c r="D411" t="inlineStr"/>
       <c r="E411" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part II</t>
+          <t>GO Battle Weekend: Tales of Transformation</t>
         </is>
       </c>
       <c r="F411" t="inlineStr">
@@ -17342,7 +17342,7 @@
       <c r="O411" t="inlineStr"/>
       <c r="P411" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part II Mon, Oct 27, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>GO Battle Weekend: Tales of Transformation Sat, Oct 25, at 12:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q411" t="inlineStr">
@@ -17362,7 +17362,7 @@
       <c r="D412" t="inlineStr"/>
       <c r="E412" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part II</t>
+          <t>GO Battle Weekend: Tales of Transformation</t>
         </is>
       </c>
       <c r="F412" t="inlineStr">
@@ -17381,7 +17381,7 @@
       <c r="O412" t="inlineStr"/>
       <c r="P412" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part II Mon, Oct 27, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>GO Battle Weekend: Tales of Transformation Sat, Oct 25, at 12:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q412" t="inlineStr">
@@ -17401,7 +17401,7 @@
       <c r="D413" t="inlineStr"/>
       <c r="E413" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part II</t>
+          <t>GO Battle Weekend: Tales of Transformation</t>
         </is>
       </c>
       <c r="F413" t="inlineStr">
@@ -17420,7 +17420,7 @@
       <c r="O413" t="inlineStr"/>
       <c r="P413" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part II Mon, Oct 27, at 10:00 AM Local Time</t>
+          <t>GO Battle Weekend: Tales of Transformation Sat, Oct 25, at 12:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q413" t="inlineStr">
@@ -17440,7 +17440,7 @@
       <c r="D414" t="inlineStr"/>
       <c r="E414" t="inlineStr">
         <is>
-          <t>Dynamax Woobat during Max Monday</t>
+          <t>Halloween 2025 Part II</t>
         </is>
       </c>
       <c r="F414" t="inlineStr">
@@ -17459,7 +17459,7 @@
       <c r="O414" t="inlineStr"/>
       <c r="P414" t="inlineStr">
         <is>
-          <t>Max Mondays Dynamax Woobat during Max Monday Mon, Oct 27, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Event Halloween 2025 Part II Mon, Oct 27, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q414" t="inlineStr">
@@ -17479,7 +17479,7 @@
       <c r="D415" t="inlineStr"/>
       <c r="E415" t="inlineStr">
         <is>
-          <t>Dynamax Woobat during Max Monday</t>
+          <t>Halloween 2025 Part II</t>
         </is>
       </c>
       <c r="F415" t="inlineStr">
@@ -17498,7 +17498,7 @@
       <c r="O415" t="inlineStr"/>
       <c r="P415" t="inlineStr">
         <is>
-          <t>Dynamax Woobat during Max Monday Mon, Oct 27, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Halloween 2025 Part II Mon, Oct 27, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q415" t="inlineStr">
@@ -17518,7 +17518,7 @@
       <c r="D416" t="inlineStr"/>
       <c r="E416" t="inlineStr">
         <is>
-          <t>Dynamax Woobat during Max Monday</t>
+          <t>Halloween 2025 Part II</t>
         </is>
       </c>
       <c r="F416" t="inlineStr">
@@ -17537,7 +17537,7 @@
       <c r="O416" t="inlineStr"/>
       <c r="P416" t="inlineStr">
         <is>
-          <t>Dynamax Woobat during Max Monday Mon, Oct 27, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Halloween 2025 Part II Mon, Oct 27, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q416" t="inlineStr">
@@ -17557,7 +17557,7 @@
       <c r="D417" t="inlineStr"/>
       <c r="E417" t="inlineStr">
         <is>
-          <t>Dynamax Woobat during Max Monday</t>
+          <t>Halloween 2025 Part II</t>
         </is>
       </c>
       <c r="F417" t="inlineStr">
@@ -17576,7 +17576,7 @@
       <c r="O417" t="inlineStr"/>
       <c r="P417" t="inlineStr">
         <is>
-          <t>Dynamax Woobat during Max Monday Mon, Oct 27, at 6:00 PM Local Time</t>
+          <t>Halloween 2025 Part II Mon, Oct 27, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q417" t="inlineStr">
@@ -17596,12 +17596,12 @@
       <c r="D418" t="inlineStr"/>
       <c r="E418" t="inlineStr">
         <is>
-          <t>Giratina (Altered Forme) in 5-star Raid Battles</t>
+          <t>Dynamax Woobat during Max Monday</t>
         </is>
       </c>
       <c r="F418" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G418" t="inlineStr"/>
@@ -17615,7 +17615,7 @@
       <c r="O418" t="inlineStr"/>
       <c r="P418" t="inlineStr">
         <is>
-          <t>Raid Battles Giratina (Altered Forme) in 5-star Raid Battles Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Max Mondays Dynamax Woobat during Max Monday Mon, Oct 27, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q418" t="inlineStr">
@@ -17635,12 +17635,12 @@
       <c r="D419" t="inlineStr"/>
       <c r="E419" t="inlineStr">
         <is>
-          <t>Giratina (Altered Forme) in 5-star Raid Battles</t>
+          <t>Dynamax Woobat during Max Monday</t>
         </is>
       </c>
       <c r="F419" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G419" t="inlineStr"/>
@@ -17654,7 +17654,7 @@
       <c r="O419" t="inlineStr"/>
       <c r="P419" t="inlineStr">
         <is>
-          <t>Giratina (Altered Forme) in 5-star Raid Battles Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Dynamax Woobat during Max Monday Mon, Oct 27, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q419" t="inlineStr">
@@ -17674,12 +17674,12 @@
       <c r="D420" t="inlineStr"/>
       <c r="E420" t="inlineStr">
         <is>
-          <t>Giratina (Altered Forme) in 5-star Raid Battles</t>
+          <t>Dynamax Woobat during Max Monday</t>
         </is>
       </c>
       <c r="F420" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G420" t="inlineStr"/>
@@ -17693,7 +17693,7 @@
       <c r="O420" t="inlineStr"/>
       <c r="P420" t="inlineStr">
         <is>
-          <t>Giratina (Altered Forme) in 5-star Raid Battles Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Dynamax Woobat during Max Monday Mon, Oct 27, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q420" t="inlineStr">
@@ -17713,12 +17713,12 @@
       <c r="D421" t="inlineStr"/>
       <c r="E421" t="inlineStr">
         <is>
-          <t>Giratina (Altered Forme) in 5-star Raid Battles</t>
+          <t>Dynamax Woobat during Max Monday</t>
         </is>
       </c>
       <c r="F421" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G421" t="inlineStr"/>
@@ -17732,7 +17732,7 @@
       <c r="O421" t="inlineStr"/>
       <c r="P421" t="inlineStr">
         <is>
-          <t>Giratina (Altered Forme) in 5-star Raid Battles Tue, Oct 28, at 10:00 AM Local Time</t>
+          <t>Dynamax Woobat during Max Monday Mon, Oct 27, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q421" t="inlineStr">
@@ -17752,7 +17752,7 @@
       <c r="D422" t="inlineStr"/>
       <c r="E422" t="inlineStr">
         <is>
-          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids</t>
+          <t>Giratina (Altered Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F422" t="inlineStr">
@@ -17771,7 +17771,7 @@
       <c r="O422" t="inlineStr"/>
       <c r="P422" t="inlineStr">
         <is>
-          <t>Raid Battles Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Raid Battles Giratina (Altered Forme) in 5-star Raid Battles Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q422" t="inlineStr">
@@ -17791,7 +17791,7 @@
       <c r="D423" t="inlineStr"/>
       <c r="E423" t="inlineStr">
         <is>
-          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids</t>
+          <t>Giratina (Altered Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F423" t="inlineStr">
@@ -17810,7 +17810,7 @@
       <c r="O423" t="inlineStr"/>
       <c r="P423" t="inlineStr">
         <is>
-          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Giratina (Altered Forme) in 5-star Raid Battles Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q423" t="inlineStr">
@@ -17830,7 +17830,7 @@
       <c r="D424" t="inlineStr"/>
       <c r="E424" t="inlineStr">
         <is>
-          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids</t>
+          <t>Giratina (Altered Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F424" t="inlineStr">
@@ -17849,7 +17849,7 @@
       <c r="O424" t="inlineStr"/>
       <c r="P424" t="inlineStr">
         <is>
-          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Giratina (Altered Forme) in 5-star Raid Battles Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q424" t="inlineStr">
@@ -17869,7 +17869,7 @@
       <c r="D425" t="inlineStr"/>
       <c r="E425" t="inlineStr">
         <is>
-          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids</t>
+          <t>Giratina (Altered Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F425" t="inlineStr">
@@ -17888,7 +17888,7 @@
       <c r="O425" t="inlineStr"/>
       <c r="P425" t="inlineStr">
         <is>
-          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids Tue, Oct 28, at 10:00 AM Local Time</t>
+          <t>Giratina (Altered Forme) in 5-star Raid Battles Tue, Oct 28, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q425" t="inlineStr">
@@ -17908,12 +17908,12 @@
       <c r="D426" t="inlineStr"/>
       <c r="E426" t="inlineStr">
         <is>
-          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation</t>
+          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids</t>
         </is>
       </c>
       <c r="F426" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G426" t="inlineStr"/>
@@ -17927,7 +17927,7 @@
       <c r="O426" t="inlineStr"/>
       <c r="P426" t="inlineStr">
         <is>
-          <t>GO Battle League Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Raid Battles Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q426" t="inlineStr">
@@ -17947,12 +17947,12 @@
       <c r="D427" t="inlineStr"/>
       <c r="E427" t="inlineStr">
         <is>
-          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation</t>
+          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids</t>
         </is>
       </c>
       <c r="F427" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G427" t="inlineStr"/>
@@ -17966,7 +17966,7 @@
       <c r="O427" t="inlineStr"/>
       <c r="P427" t="inlineStr">
         <is>
-          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q427" t="inlineStr">
@@ -17986,12 +17986,12 @@
       <c r="D428" t="inlineStr"/>
       <c r="E428" t="inlineStr">
         <is>
-          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation</t>
+          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids</t>
         </is>
       </c>
       <c r="F428" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G428" t="inlineStr"/>
@@ -18005,7 +18005,7 @@
       <c r="O428" t="inlineStr"/>
       <c r="P428" t="inlineStr">
         <is>
-          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q428" t="inlineStr">
@@ -18025,12 +18025,12 @@
       <c r="D429" t="inlineStr"/>
       <c r="E429" t="inlineStr">
         <is>
-          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation</t>
+          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids</t>
         </is>
       </c>
       <c r="F429" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G429" t="inlineStr"/>
@@ -18044,7 +18044,7 @@
       <c r="O429" t="inlineStr"/>
       <c r="P429" t="inlineStr">
         <is>
-          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating...</t>
+          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids Tue, Oct 28, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q429" t="inlineStr">
@@ -18064,12 +18064,12 @@
       <c r="D430" t="inlineStr"/>
       <c r="E430" t="inlineStr">
         <is>
-          <t>Sinistea Spotlight Hour</t>
+          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F430" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G430" t="inlineStr"/>
@@ -18083,7 +18083,7 @@
       <c r="O430" t="inlineStr"/>
       <c r="P430" t="inlineStr">
         <is>
-          <t>Pokémon Spotlight Hour Sinistea Spotlight Hour Tue, Oct 28, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>GO Battle League Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q430" t="inlineStr">
@@ -18103,12 +18103,12 @@
       <c r="D431" t="inlineStr"/>
       <c r="E431" t="inlineStr">
         <is>
-          <t>Sinistea Spotlight Hour</t>
+          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F431" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G431" t="inlineStr"/>
@@ -18122,7 +18122,7 @@
       <c r="O431" t="inlineStr"/>
       <c r="P431" t="inlineStr">
         <is>
-          <t>Sinistea Spotlight Hour Tue, Oct 28, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q431" t="inlineStr">
@@ -18142,12 +18142,12 @@
       <c r="D432" t="inlineStr"/>
       <c r="E432" t="inlineStr">
         <is>
-          <t>Sinistea Spotlight Hour</t>
+          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F432" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G432" t="inlineStr"/>
@@ -18161,7 +18161,7 @@
       <c r="O432" t="inlineStr"/>
       <c r="P432" t="inlineStr">
         <is>
-          <t>Sinistea Spotlight Hour Tue, Oct 28, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q432" t="inlineStr">
@@ -18181,12 +18181,12 @@
       <c r="D433" t="inlineStr"/>
       <c r="E433" t="inlineStr">
         <is>
-          <t>Sinistea Spotlight Hour</t>
+          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F433" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G433" t="inlineStr"/>
@@ -18200,7 +18200,7 @@
       <c r="O433" t="inlineStr"/>
       <c r="P433" t="inlineStr">
         <is>
-          <t>Sinistea Spotlight Hour Tue, Oct 28, at 6:00 PM Local Time</t>
+          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q433" t="inlineStr">
@@ -18220,12 +18220,12 @@
       <c r="D434" t="inlineStr"/>
       <c r="E434" t="inlineStr">
         <is>
-          <t>Giratina (Origin Forme) Raid Hour</t>
+          <t>Sinistea Spotlight Hour</t>
         </is>
       </c>
       <c r="F434" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G434" t="inlineStr"/>
@@ -18239,7 +18239,7 @@
       <c r="O434" t="inlineStr"/>
       <c r="P434" t="inlineStr">
         <is>
-          <t>Raid Hour Giratina (Origin Forme) Raid Hour Wed, Oct 29, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Pokémon Spotlight Hour Sinistea Spotlight Hour Tue, Oct 28, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q434" t="inlineStr">
@@ -18259,12 +18259,12 @@
       <c r="D435" t="inlineStr"/>
       <c r="E435" t="inlineStr">
         <is>
-          <t>Giratina (Origin Forme) Raid Hour</t>
+          <t>Sinistea Spotlight Hour</t>
         </is>
       </c>
       <c r="F435" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G435" t="inlineStr"/>
@@ -18278,7 +18278,7 @@
       <c r="O435" t="inlineStr"/>
       <c r="P435" t="inlineStr">
         <is>
-          <t>Giratina (Origin Forme) Raid Hour Wed, Oct 29, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Sinistea Spotlight Hour Tue, Oct 28, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q435" t="inlineStr">
@@ -18298,12 +18298,12 @@
       <c r="D436" t="inlineStr"/>
       <c r="E436" t="inlineStr">
         <is>
-          <t>Giratina (Origin Forme) Raid Hour</t>
+          <t>Sinistea Spotlight Hour</t>
         </is>
       </c>
       <c r="F436" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G436" t="inlineStr"/>
@@ -18317,7 +18317,7 @@
       <c r="O436" t="inlineStr"/>
       <c r="P436" t="inlineStr">
         <is>
-          <t>Giratina (Origin Forme) Raid Hour Wed, Oct 29, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Sinistea Spotlight Hour Tue, Oct 28, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q436" t="inlineStr">
@@ -18337,12 +18337,12 @@
       <c r="D437" t="inlineStr"/>
       <c r="E437" t="inlineStr">
         <is>
-          <t>Giratina (Origin Forme) Raid Hour</t>
+          <t>Sinistea Spotlight Hour</t>
         </is>
       </c>
       <c r="F437" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G437" t="inlineStr"/>
@@ -18356,7 +18356,7 @@
       <c r="O437" t="inlineStr"/>
       <c r="P437" t="inlineStr">
         <is>
-          <t>Giratina (Origin Forme) Raid Hour Wed, Oct 29, at 6:00 PM Local Time</t>
+          <t>Sinistea Spotlight Hour Tue, Oct 28, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q437" t="inlineStr">
@@ -18376,12 +18376,12 @@
       <c r="D438" t="inlineStr"/>
       <c r="E438" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
+          <t>Giratina (Origin Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F438" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G438" t="inlineStr"/>
@@ -18395,7 +18395,7 @@
       <c r="O438" t="inlineStr"/>
       <c r="P438" t="inlineStr">
         <is>
-          <t>GO Battle League Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Raid Hour Giratina (Origin Forme) Raid Hour Wed, Oct 29, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q438" t="inlineStr">
@@ -18415,12 +18415,12 @@
       <c r="D439" t="inlineStr"/>
       <c r="E439" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
+          <t>Giratina (Origin Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F439" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G439" t="inlineStr"/>
@@ -18434,7 +18434,7 @@
       <c r="O439" t="inlineStr"/>
       <c r="P439" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Giratina (Origin Forme) Raid Hour Wed, Oct 29, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q439" t="inlineStr">
@@ -18454,12 +18454,12 @@
       <c r="D440" t="inlineStr"/>
       <c r="E440" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
+          <t>Giratina (Origin Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F440" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G440" t="inlineStr"/>
@@ -18473,7 +18473,7 @@
       <c r="O440" t="inlineStr"/>
       <c r="P440" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Giratina (Origin Forme) Raid Hour Wed, Oct 29, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q440" t="inlineStr">
@@ -18493,12 +18493,12 @@
       <c r="D441" t="inlineStr"/>
       <c r="E441" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
+          <t>Giratina (Origin Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F441" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G441" t="inlineStr"/>
@@ -18512,7 +18512,7 @@
       <c r="O441" t="inlineStr"/>
       <c r="P441" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating...</t>
+          <t>Giratina (Origin Forme) Raid Hour Wed, Oct 29, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q441" t="inlineStr">
@@ -18532,7 +18532,7 @@
       <c r="D442" t="inlineStr"/>
       <c r="E442" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Nagasaki</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F442" t="inlineStr">
@@ -18551,7 +18551,7 @@
       <c r="O442" t="inlineStr"/>
       <c r="P442" t="inlineStr">
         <is>
-          <t>Wild Area Pokémon GO Wild Area: Nagasaki Calculating... Starts: Calculating...</t>
+          <t>GO Battle League Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q442" t="inlineStr">
@@ -18571,7 +18571,7 @@
       <c r="D443" t="inlineStr"/>
       <c r="E443" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Nagasaki</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F443" t="inlineStr">
@@ -18590,7 +18590,7 @@
       <c r="O443" t="inlineStr"/>
       <c r="P443" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Nagasaki Calculating... Starts: Calculating...</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q443" t="inlineStr">
@@ -18610,7 +18610,7 @@
       <c r="D444" t="inlineStr"/>
       <c r="E444" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Nagasaki</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F444" t="inlineStr">
@@ -18629,7 +18629,7 @@
       <c r="O444" t="inlineStr"/>
       <c r="P444" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Nagasaki Calculating... Starts: Calculating...</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q444" t="inlineStr">
@@ -18649,7 +18649,7 @@
       <c r="D445" t="inlineStr"/>
       <c r="E445" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Nagasaki</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F445" t="inlineStr">
@@ -18668,7 +18668,7 @@
       <c r="O445" t="inlineStr"/>
       <c r="P445" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Nagasaki Calculating...</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q445" t="inlineStr">
@@ -18688,7 +18688,7 @@
       <c r="D446" t="inlineStr"/>
       <c r="E446" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Pokémon GO Wild Area: Nagasaki</t>
         </is>
       </c>
       <c r="F446" t="inlineStr">
@@ -18707,7 +18707,7 @@
       <c r="O446" t="inlineStr"/>
       <c r="P446" t="inlineStr">
         <is>
-          <t>GO Battle League Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Wild Area Pokémon GO Wild Area: Nagasaki Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q446" t="inlineStr">
@@ -18727,7 +18727,7 @@
       <c r="D447" t="inlineStr"/>
       <c r="E447" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Pokémon GO Wild Area: Nagasaki</t>
         </is>
       </c>
       <c r="F447" t="inlineStr">
@@ -18746,7 +18746,7 @@
       <c r="O447" t="inlineStr"/>
       <c r="P447" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Pokémon GO Wild Area: Nagasaki Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q447" t="inlineStr">
@@ -18766,7 +18766,7 @@
       <c r="D448" t="inlineStr"/>
       <c r="E448" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Pokémon GO Wild Area: Nagasaki</t>
         </is>
       </c>
       <c r="F448" t="inlineStr">
@@ -18785,7 +18785,7 @@
       <c r="O448" t="inlineStr"/>
       <c r="P448" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Pokémon GO Wild Area: Nagasaki Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q448" t="inlineStr">
@@ -18805,7 +18805,7 @@
       <c r="D449" t="inlineStr"/>
       <c r="E449" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Pokémon GO Wild Area: Nagasaki</t>
         </is>
       </c>
       <c r="F449" t="inlineStr">
@@ -18824,7 +18824,7 @@
       <c r="O449" t="inlineStr"/>
       <c r="P449" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating...</t>
+          <t>Pokémon GO Wild Area: Nagasaki Calculating...</t>
         </is>
       </c>
       <c r="Q449" t="inlineStr">
@@ -18844,7 +18844,7 @@
       <c r="D450" t="inlineStr"/>
       <c r="E450" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Global</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F450" t="inlineStr">
@@ -18863,7 +18863,7 @@
       <c r="O450" t="inlineStr"/>
       <c r="P450" t="inlineStr">
         <is>
-          <t>Wild Area Pokémon GO Wild Area: Global Sat, Nov 15, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>GO Battle League Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q450" t="inlineStr">
@@ -18883,7 +18883,7 @@
       <c r="D451" t="inlineStr"/>
       <c r="E451" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Global</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F451" t="inlineStr">
@@ -18902,7 +18902,7 @@
       <c r="O451" t="inlineStr"/>
       <c r="P451" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Global Sat, Nov 15, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q451" t="inlineStr">
@@ -18922,7 +18922,7 @@
       <c r="D452" t="inlineStr"/>
       <c r="E452" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Global</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F452" t="inlineStr">
@@ -18941,7 +18941,7 @@
       <c r="O452" t="inlineStr"/>
       <c r="P452" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Global Sat, Nov 15, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q452" t="inlineStr">
@@ -18961,7 +18961,7 @@
       <c r="D453" t="inlineStr"/>
       <c r="E453" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Global</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F453" t="inlineStr">
@@ -18980,7 +18980,7 @@
       <c r="O453" t="inlineStr"/>
       <c r="P453" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Global Sat, Nov 15, at 10:00 AM Local Time</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q453" t="inlineStr">
@@ -19000,12 +19000,12 @@
       <c r="D454" t="inlineStr"/>
       <c r="E454" t="inlineStr">
         <is>
-          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation</t>
+          <t>Pokémon GO Wild Area: Global</t>
         </is>
       </c>
       <c r="F454" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G454" t="inlineStr"/>
@@ -19019,7 +19019,7 @@
       <c r="O454" t="inlineStr"/>
       <c r="P454" t="inlineStr">
         <is>
-          <t>GO Battle League 2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Wild Area Pokémon GO Wild Area: Global Sat, Nov 15, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q454" t="inlineStr">
@@ -19039,12 +19039,12 @@
       <c r="D455" t="inlineStr"/>
       <c r="E455" t="inlineStr">
         <is>
-          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation</t>
+          <t>Pokémon GO Wild Area: Global</t>
         </is>
       </c>
       <c r="F455" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G455" t="inlineStr"/>
@@ -19058,7 +19058,7 @@
       <c r="O455" t="inlineStr"/>
       <c r="P455" t="inlineStr">
         <is>
-          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Pokémon GO Wild Area: Global Sat, Nov 15, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q455" t="inlineStr">
@@ -19078,12 +19078,12 @@
       <c r="D456" t="inlineStr"/>
       <c r="E456" t="inlineStr">
         <is>
-          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation</t>
+          <t>Pokémon GO Wild Area: Global</t>
         </is>
       </c>
       <c r="F456" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G456" t="inlineStr"/>
@@ -19097,7 +19097,7 @@
       <c r="O456" t="inlineStr"/>
       <c r="P456" t="inlineStr">
         <is>
-          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Pokémon GO Wild Area: Global Sat, Nov 15, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q456" t="inlineStr">
@@ -19117,12 +19117,12 @@
       <c r="D457" t="inlineStr"/>
       <c r="E457" t="inlineStr">
         <is>
-          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation</t>
+          <t>Pokémon GO Wild Area: Global</t>
         </is>
       </c>
       <c r="F457" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G457" t="inlineStr"/>
@@ -19136,7 +19136,7 @@
       <c r="O457" t="inlineStr"/>
       <c r="P457" t="inlineStr">
         <is>
-          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating...</t>
+          <t>Pokémon GO Wild Area: Global Sat, Nov 15, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q457" t="inlineStr">
@@ -19156,12 +19156,12 @@
       <c r="D458" t="inlineStr"/>
       <c r="E458" t="inlineStr">
         <is>
-          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation</t>
+          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F458" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G458" t="inlineStr"/>
@@ -19175,7 +19175,7 @@
       <c r="O458" t="inlineStr"/>
       <c r="P458" t="inlineStr">
         <is>
-          <t>GO Battle League Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>GO Battle League 2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q458" t="inlineStr">
@@ -19195,12 +19195,12 @@
       <c r="D459" t="inlineStr"/>
       <c r="E459" t="inlineStr">
         <is>
-          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation</t>
+          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F459" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G459" t="inlineStr"/>
@@ -19214,7 +19214,7 @@
       <c r="O459" t="inlineStr"/>
       <c r="P459" t="inlineStr">
         <is>
-          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q459" t="inlineStr">
@@ -19234,12 +19234,12 @@
       <c r="D460" t="inlineStr"/>
       <c r="E460" t="inlineStr">
         <is>
-          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation</t>
+          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F460" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G460" t="inlineStr"/>
@@ -19253,7 +19253,7 @@
       <c r="O460" t="inlineStr"/>
       <c r="P460" t="inlineStr">
         <is>
-          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q460" t="inlineStr">
@@ -19273,12 +19273,12 @@
       <c r="D461" t="inlineStr"/>
       <c r="E461" t="inlineStr">
         <is>
-          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation</t>
+          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F461" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G461" t="inlineStr"/>
@@ -19292,7 +19292,7 @@
       <c r="O461" t="inlineStr"/>
       <c r="P461" t="inlineStr">
         <is>
-          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating...</t>
+          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q461" t="inlineStr">
@@ -19312,12 +19312,12 @@
       <c r="D462" t="inlineStr"/>
       <c r="E462" t="inlineStr">
         <is>
-          <t>November Community Day</t>
+          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F462" t="inlineStr">
         <is>
-          <t>Community Day</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G462" t="inlineStr"/>
@@ -19331,7 +19331,7 @@
       <c r="O462" t="inlineStr"/>
       <c r="P462" t="inlineStr">
         <is>
-          <t>Community Day November Community Day Sun, Nov 30, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>GO Battle League Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q462" t="inlineStr">
@@ -19351,12 +19351,12 @@
       <c r="D463" t="inlineStr"/>
       <c r="E463" t="inlineStr">
         <is>
-          <t>November Community Day</t>
+          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F463" t="inlineStr">
         <is>
-          <t>Community Day</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G463" t="inlineStr"/>
@@ -19370,7 +19370,7 @@
       <c r="O463" t="inlineStr"/>
       <c r="P463" t="inlineStr">
         <is>
-          <t>November Community Day Sun, Nov 30, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q463" t="inlineStr">
@@ -19390,12 +19390,12 @@
       <c r="D464" t="inlineStr"/>
       <c r="E464" t="inlineStr">
         <is>
-          <t>November Community Day</t>
+          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F464" t="inlineStr">
         <is>
-          <t>Community Day</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G464" t="inlineStr"/>
@@ -19409,7 +19409,7 @@
       <c r="O464" t="inlineStr"/>
       <c r="P464" t="inlineStr">
         <is>
-          <t>November Community Day Sun, Nov 30, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q464" t="inlineStr">
@@ -19429,12 +19429,12 @@
       <c r="D465" t="inlineStr"/>
       <c r="E465" t="inlineStr">
         <is>
-          <t>November Community Day</t>
+          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F465" t="inlineStr">
         <is>
-          <t>Community Day</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G465" t="inlineStr"/>
@@ -19448,7 +19448,7 @@
       <c r="O465" t="inlineStr"/>
       <c r="P465" t="inlineStr">
         <is>
-          <t>November Community Day Sun, Nov 30, at 2:00 PM Local Time</t>
+          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q465" t="inlineStr">
@@ -19468,12 +19468,12 @@
       <c r="D466" t="inlineStr"/>
       <c r="E466" t="inlineStr">
         <is>
-          <t>Raid NOW</t>
+          <t>November Community Day</t>
         </is>
       </c>
       <c r="F466" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Community Day</t>
         </is>
       </c>
       <c r="G466" t="inlineStr"/>
@@ -19487,12 +19487,12 @@
       <c r="O466" t="inlineStr"/>
       <c r="P466" t="inlineStr">
         <is>
-          <t>Raid NOW From Leek Duck | Powered by GO FRIEND General Information It has been reported that the registration information (Trainer Name, Trainer Level, Trainer Code) is incorrect. Please check again. HOST HOST Auto join Raids you are joining (Latest 2) MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rpl_maxuser'] }} {{ val1['cnt'] }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} No.{{ val1['rpl_id'] }} No.{{ val1['rpl_id'] }} TL{{ val1['rpl_level'] }} {{ val1['rpl_glevel'] }} {{ ((val1['rpl_gescore'] == -1)?0:val1['rpl_gescore']) }} {{ aryPokemon[value]['raidbbs_short_name_en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} FULL Host TL 5 30 35 40 45 Host Rating - 0 {{ i }} MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['ti</t>
+          <t>Community Day November Community Day Sun, Nov 30, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q466" t="inlineStr">
         <is>
-          <t>2024-06-01_raid-now.html</t>
+          <t>2024-06-01_events.html</t>
         </is>
       </c>
     </row>
@@ -19507,12 +19507,12 @@
       <c r="D467" t="inlineStr"/>
       <c r="E467" t="inlineStr">
         <is>
-          <t>Raids you are joining (Latest 2)</t>
+          <t>November Community Day</t>
         </is>
       </c>
       <c r="F467" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Community Day</t>
         </is>
       </c>
       <c r="G467" t="inlineStr"/>
@@ -19526,12 +19526,12 @@
       <c r="O467" t="inlineStr"/>
       <c r="P467" t="inlineStr">
         <is>
-          <t>General Information It has been reported that the registration information (Trainer Name, Trainer Level, Trainer Code) is incorrect. Please check again. HOST HOST Auto join Raids you are joining (Latest 2) MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rpl_maxuser'] }} {{ val1['cnt'] }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} No.{{ val1['rpl_id'] }} No.{{ val1['rpl_id'] }} TL{{ val1['rpl_level'] }} {{ val1['rpl_glevel'] }} {{ ((val1['rpl_gescore'] == -1)?0:val1['rpl_gescore']) }} {{ aryPokemon[value]['raidbbs_short_name_en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} FULL Host TL 5 30 35 40 45 Host Rating - 0 {{ i }} MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rp</t>
+          <t>November Community Day Sun, Nov 30, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q467" t="inlineStr">
         <is>
-          <t>2024-06-01_raid-now.html</t>
+          <t>2024-06-01_events.html</t>
         </is>
       </c>
     </row>
@@ -19546,12 +19546,12 @@
       <c r="D468" t="inlineStr"/>
       <c r="E468" t="inlineStr">
         <is>
-          <t>Raids you are joining (Latest 2)</t>
+          <t>November Community Day</t>
         </is>
       </c>
       <c r="F468" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Community Day</t>
         </is>
       </c>
       <c r="G468" t="inlineStr"/>
@@ -19565,12 +19565,12 @@
       <c r="O468" t="inlineStr"/>
       <c r="P468" t="inlineStr">
         <is>
-          <t>Raids you are joining (Latest 2) MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rpl_maxuser'] }} {{ val1['cnt'] }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} No.{{ val1['rpl_id'] }} No.{{ val1['rpl_id'] }} TL{{ val1['rpl_level'] }} {{ val1['rpl_glevel'] }} {{ ((val1['rpl_gescore'] == -1)?0:val1['rpl_gescore']) }}</t>
+          <t>November Community Day Sun, Nov 30, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q468" t="inlineStr">
         <is>
-          <t>2024-06-01_raid-now.html</t>
+          <t>2024-06-01_events.html</t>
         </is>
       </c>
     </row>
@@ -19585,12 +19585,12 @@
       <c r="D469" t="inlineStr"/>
       <c r="E469" t="inlineStr">
         <is>
-          <t>まとめて評価</t>
+          <t>November Community Day</t>
         </is>
       </c>
       <c r="F469" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Community Day</t>
         </is>
       </c>
       <c r="G469" t="inlineStr"/>
@@ -19604,12 +19604,12 @@
       <c r="O469" t="inlineStr"/>
       <c r="P469" t="inlineStr">
         <is>
-          <t>まとめて評価 Can't rate</t>
+          <t>November Community Day Sun, Nov 30, at 2:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q469" t="inlineStr">
         <is>
-          <t>2024-06-01_raid-now.html</t>
+          <t>2024-06-01_events.html</t>
         </is>
       </c>
     </row>
@@ -19624,12 +19624,12 @@
       <c r="D470" t="inlineStr"/>
       <c r="E470" t="inlineStr">
         <is>
-          <t>Bonuses</t>
+          <t>Raid NOW</t>
         </is>
       </c>
       <c r="F470" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G470" t="inlineStr"/>
@@ -19643,12 +19643,12 @@
       <c r="O470" t="inlineStr"/>
       <c r="P470" t="inlineStr">
         <is>
-          <t>Bonuses 4× Stardust from win rewards. (This does not include end-of-set rewards.) The maximum number of sets you can play per day will increase from five to 20—for a total of 100 battles—from 12:00 a.m. to 11:59 p.m. local time. Free battle-themed Timed Research will be available. Rewards include glasses for your avatar inspired by Clemont. Pokémon encountered via GO Battle League rewards will have a wider variance of Attack, Defense, and HP. Active Leagues The following leagues will be active. Great League Ultra League Master League</t>
+          <t>Raid NOW From Leek Duck | Powered by GO FRIEND General Information It has been reported that the registration information (Trainer Name, Trainer Level, Trainer Code) is incorrect. Please check again. HOST HOST Auto join Raids you are joining (Latest 2) MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rpl_maxuser'] }} {{ val1['cnt'] }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} No.{{ val1['rpl_id'] }} No.{{ val1['rpl_id'] }} TL{{ val1['rpl_level'] }} {{ val1['rpl_glevel'] }} {{ ((val1['rpl_gescore'] == -1)?0:val1['rpl_gescore']) }} {{ aryPokemon[value]['raidbbs_short_name_en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} FULL Host TL 5 30 35 40 45 Host Rating - 0 {{ i }} MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['ti</t>
         </is>
       </c>
       <c r="Q470" t="inlineStr">
         <is>
-          <t>2024-06-01_event-go-battle-weekend-tales-of-transformation-sun-oct-26-at-1159-pm-local-time-ends-calculating.html</t>
+          <t>2024-06-01_raid-now.html</t>
         </is>
       </c>
     </row>
@@ -19663,12 +19663,12 @@
       <c r="D471" t="inlineStr"/>
       <c r="E471" t="inlineStr">
         <is>
-          <t>For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area?</t>
+          <t>Raids you are joining (Latest 2)</t>
         </is>
       </c>
       <c r="F471" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G471" t="inlineStr"/>
@@ -19682,12 +19682,12 @@
       <c r="O471" t="inlineStr"/>
       <c r="P471" t="inlineStr">
         <is>
-          <t xml:space="preserve">For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area? In this next chapter of Pokémon GO Wild Area, get ready to test your skills once again as you encounter Dark- and Fairy-type Pokémon, including Grimmsnarl, the Bulk Up Pokémon! Plus, exceptionally powerful Pokémon known as mighty Pokémon are appearing in the wild—use GO Wild Area–exclusive GO Safari Balls to improve your odds of catching these rare Pokémon. All event gameplay is exclusive to ticket holders. Tickets for Pokémon GO Wild Area: Nagasaki are now available on the Niantic events portal . Live Event Ticket - ¥3,600 (including applicable taxes and fees) Location: A citywide experience across Nagasaki City, Japan Dates: November 7, 8, or 9, 2025 Time: 9:00 a.m. – 5:00 p.m. JST Tickets for Pokémon GO Wild Area: Nagasaki include one day of event gameplay, and attendees may purchase add-ons that extend the gameplay for an additional day. One-day tickets are ¥3,600 (or the equivalent pricing tier in your local currency, including applicable taxes and fees). Event gameplay will be available only at the date, time, and location specified on your ticket. Note: Tickets to this event are </t>
+          <t>General Information It has been reported that the registration information (Trainer Name, Trainer Level, Trainer Code) is incorrect. Please check again. HOST HOST Auto join Raids you are joining (Latest 2) MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rpl_maxuser'] }} {{ val1['cnt'] }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} No.{{ val1['rpl_id'] }} No.{{ val1['rpl_id'] }} TL{{ val1['rpl_level'] }} {{ val1['rpl_glevel'] }} {{ ((val1['rpl_gescore'] == -1)?0:val1['rpl_gescore']) }} {{ aryPokemon[value]['raidbbs_short_name_en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} FULL Host TL 5 30 35 40 45 Host Rating - 0 {{ i }} MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rp</t>
         </is>
       </c>
       <c r="Q471" t="inlineStr">
         <is>
-          <t>2024-06-01_wild-area-pokmon-go-wild-area-nagasaki-calculating-ends-calculating.html</t>
+          <t>2024-06-01_raid-now.html</t>
         </is>
       </c>
     </row>
@@ -19702,12 +19702,12 @@
       <c r="D472" t="inlineStr"/>
       <c r="E472" t="inlineStr">
         <is>
-          <t>For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area?</t>
+          <t>Raids you are joining (Latest 2)</t>
         </is>
       </c>
       <c r="F472" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G472" t="inlineStr"/>
@@ -19721,10 +19721,166 @@
       <c r="O472" t="inlineStr"/>
       <c r="P472" t="inlineStr">
         <is>
+          <t>Raids you are joining (Latest 2) MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rpl_maxuser'] }} {{ val1['cnt'] }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} No.{{ val1['rpl_id'] }} No.{{ val1['rpl_id'] }} TL{{ val1['rpl_level'] }} {{ val1['rpl_glevel'] }} {{ ((val1['rpl_gescore'] == -1)?0:val1['rpl_gescore']) }}</t>
+        </is>
+      </c>
+      <c r="Q472" t="inlineStr">
+        <is>
+          <t>2024-06-01_raid-now.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>Leek Duck</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr"/>
+      <c r="C473" t="inlineStr"/>
+      <c r="D473" t="inlineStr"/>
+      <c r="E473" t="inlineStr">
+        <is>
+          <t>まとめて評価</t>
+        </is>
+      </c>
+      <c r="F473" t="inlineStr">
+        <is>
+          <t>Event/News</t>
+        </is>
+      </c>
+      <c r="G473" t="inlineStr"/>
+      <c r="H473" t="inlineStr"/>
+      <c r="I473" t="inlineStr"/>
+      <c r="J473" t="inlineStr"/>
+      <c r="K473" t="inlineStr"/>
+      <c r="L473" t="inlineStr"/>
+      <c r="M473" t="inlineStr"/>
+      <c r="N473" t="inlineStr"/>
+      <c r="O473" t="inlineStr"/>
+      <c r="P473" t="inlineStr">
+        <is>
+          <t>まとめて評価 Can't rate</t>
+        </is>
+      </c>
+      <c r="Q473" t="inlineStr">
+        <is>
+          <t>2024-06-01_raid-now.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>Leek Duck</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr"/>
+      <c r="C474" t="inlineStr"/>
+      <c r="D474" t="inlineStr"/>
+      <c r="E474" t="inlineStr">
+        <is>
+          <t>Bonuses</t>
+        </is>
+      </c>
+      <c r="F474" t="inlineStr">
+        <is>
+          <t>Event/News</t>
+        </is>
+      </c>
+      <c r="G474" t="inlineStr"/>
+      <c r="H474" t="inlineStr"/>
+      <c r="I474" t="inlineStr"/>
+      <c r="J474" t="inlineStr"/>
+      <c r="K474" t="inlineStr"/>
+      <c r="L474" t="inlineStr"/>
+      <c r="M474" t="inlineStr"/>
+      <c r="N474" t="inlineStr"/>
+      <c r="O474" t="inlineStr"/>
+      <c r="P474" t="inlineStr">
+        <is>
+          <t>Bonuses 4× Stardust from win rewards. (This does not include end-of-set rewards.) The maximum number of sets you can play per day will increase from five to 20—for a total of 100 battles—from 12:00 a.m. to 11:59 p.m. local time. Free battle-themed Timed Research will be available. Rewards include glasses for your avatar inspired by Clemont. Pokémon encountered via GO Battle League rewards will have a wider variance of Attack, Defense, and HP. Active Leagues The following leagues will be active. Great League Ultra League Master League</t>
+        </is>
+      </c>
+      <c r="Q474" t="inlineStr">
+        <is>
+          <t>2024-06-01_event-go-battle-weekend-tales-of-transformation-sun-oct-26-at-1159-pm-local-time-ends-calculating.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>Leek Duck</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr"/>
+      <c r="C475" t="inlineStr"/>
+      <c r="D475" t="inlineStr"/>
+      <c r="E475" t="inlineStr">
+        <is>
+          <t>For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area?</t>
+        </is>
+      </c>
+      <c r="F475" t="inlineStr">
+        <is>
+          <t>Event/News</t>
+        </is>
+      </c>
+      <c r="G475" t="inlineStr"/>
+      <c r="H475" t="inlineStr"/>
+      <c r="I475" t="inlineStr"/>
+      <c r="J475" t="inlineStr"/>
+      <c r="K475" t="inlineStr"/>
+      <c r="L475" t="inlineStr"/>
+      <c r="M475" t="inlineStr"/>
+      <c r="N475" t="inlineStr"/>
+      <c r="O475" t="inlineStr"/>
+      <c r="P475" t="inlineStr">
+        <is>
+          <t xml:space="preserve">For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area? In this next chapter of Pokémon GO Wild Area, get ready to test your skills once again as you encounter Dark- and Fairy-type Pokémon, including Grimmsnarl, the Bulk Up Pokémon! Plus, exceptionally powerful Pokémon known as mighty Pokémon are appearing in the wild—use GO Wild Area–exclusive GO Safari Balls to improve your odds of catching these rare Pokémon. All event gameplay is exclusive to ticket holders. Tickets for Pokémon GO Wild Area: Nagasaki are now available on the Niantic events portal . Live Event Ticket - ¥3,600 (including applicable taxes and fees) Location: A citywide experience across Nagasaki City, Japan Dates: November 7, 8, or 9, 2025 Time: 9:00 a.m. – 5:00 p.m. JST Tickets for Pokémon GO Wild Area: Nagasaki include one day of event gameplay, and attendees may purchase add-ons that extend the gameplay for an additional day. One-day tickets are ¥3,600 (or the equivalent pricing tier in your local currency, including applicable taxes and fees). Event gameplay will be available only at the date, time, and location specified on your ticket. Note: Tickets to this event are </t>
+        </is>
+      </c>
+      <c r="Q475" t="inlineStr">
+        <is>
+          <t>2024-06-01_wild-area-pokmon-go-wild-area-nagasaki-calculating-ends-calculating.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>Leek Duck</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr"/>
+      <c r="C476" t="inlineStr"/>
+      <c r="D476" t="inlineStr"/>
+      <c r="E476" t="inlineStr">
+        <is>
+          <t>For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area?</t>
+        </is>
+      </c>
+      <c r="F476" t="inlineStr">
+        <is>
+          <t>Event/News</t>
+        </is>
+      </c>
+      <c r="G476" t="inlineStr"/>
+      <c r="H476" t="inlineStr"/>
+      <c r="I476" t="inlineStr"/>
+      <c r="J476" t="inlineStr"/>
+      <c r="K476" t="inlineStr"/>
+      <c r="L476" t="inlineStr"/>
+      <c r="M476" t="inlineStr"/>
+      <c r="N476" t="inlineStr"/>
+      <c r="O476" t="inlineStr"/>
+      <c r="P476" t="inlineStr">
+        <is>
           <t>For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area? Trainers around the world can gear up for a worldwide adventure during Pokémon GO Wild Area: Global, available in-game for two days only! Looking to enhance your GO Wild Area weekend with exclusive Special Research, additional bonuses, and an increased chance of encountering Shiny Pokémon? Purchase a global event ticket from the Pokémon GO Web Store! Event Tickets Tickets for Pokémon GO Wild Area: Global are available now in the in-game Shop and Pokémon Go Web Store for $11.99 USD . Purchase your ticket on the Pokémon GO Web Store for a new avatar item! Trainers who purchase their Pokémon GO Wild Area: Global ticket on the Pokémon GO Web Store will receive a special avatar item—the Flower Crown! You can purchase your ticket on the web store until the last day of the event to receive this avatar item. Pokémon GO Wild Area: Nagasaki For details on the in-person event in Nagasaki, Japan, click here .</t>
         </is>
       </c>
-      <c r="Q472" t="inlineStr">
+      <c r="Q476" t="inlineStr">
         <is>
           <t>2024-06-01_wild-area-pokmon-go-wild-area-global-sun-nov-16-at-600-pm-local-time-ends-calculating.html</t>
         </is>

</xml_diff>

<commit_message>
Update latest digest: 2024-06-01 → 2025-09-30
</commit_message>
<xml_diff>
--- a/outputs/latest/POGO_Digest.xlsx
+++ b/outputs/latest/POGO_Digest.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q472"/>
+  <dimension ref="A1:Q468"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1328,7 +1328,7 @@
       <c r="O17" t="inlineStr"/>
       <c r="P17" t="inlineStr">
         <is>
-          <t>Steel Skyline Event Starts: Tuesday, September 30, 2025, at 10:00 AM Local Time Ends: Tuesday, October 7, 2025, at  8:00 PM Local Time Dynamax Duraludon makes its Pokémon GO debut during Steel Skyline! Complete Global Challenges, encounter Steel-type Pokémon, and participate in Max Battles. Features Spawns Raids Research Shiny Sales Features Dynamax Debut The following Pokémon will make its Pokémon GO debut in four-star Max Battles! Duraludon Global Challenges Global Challenges will take place throughout the Steel Skyline event! Work with Trainers around the world to complete Field Research tasks and complete throwing-based challenges to unlock bonuses for all to enjoy! Once a challenge is completed, special bonuses will be unlocked for the remainder of the event and the next Global Challenge will begin. How far can you get? Level 1 Reward Additional Candy for successfully catching Pokémon with Nice, Great, and Excellent Throws Increased chance for Trainers level 31 and up to receive Candy XL for catching Pokémon with Nice, Great, and Excellent Throws Level 2 Rewards Additional 5,000 XP from winning raids Level 3 Rewards One guaranteed Rare Candy XL from winning in-person Max Battl</t>
+          <t>Steel Skyline Event Starts: Tuesday, September 30, 2025, at 10:00 AM Local Time Ends: Tuesday, October 7, 2025, at  8:00 PM Local Time Dynamax Duraludon makes its Pokémon GO debut during Steel Skyline! Complete Global Challenges, encounter Steel-type Pokémon, and participate in Max Battles. Features Spawns Raids Research Shiny Sales Graphic Features Dynamax Debut The following Pokémon will make its Pokémon GO debut in four-star Max Battles! Duraludon Global Challenges Global Challenges will take place throughout the Steel Skyline event! Work with Trainers around the world to complete Field Research tasks and complete throwing-based challenges to unlock bonuses for all to enjoy! Once a challenge is completed, special bonuses will be unlocked for the remainder of the event and the next Global Challenge will begin. How far can you get? Level 1 Reward Additional Candy for successfully catching Pokémon with Nice, Great, and Excellent Throws Increased chance for Trainers level 31 and up to receive Candy XL for catching Pokémon with Nice, Great, and Excellent Throws Level 2 Rewards Additional 5,000 XP from winning raids Level 3 Rewards One guaranteed Rare Candy XL from winning in-person M</t>
         </is>
       </c>
       <c r="Q17" t="inlineStr">
@@ -12409,12 +12409,12 @@
       <c r="D285" t="inlineStr"/>
       <c r="E285" t="inlineStr">
         <is>
-          <t>Dynamax Beldum during Max Monday</t>
+          <t>Mega Steelix, Scizor, and Lucario in Mega Raids</t>
         </is>
       </c>
       <c r="F285" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G285" t="inlineStr"/>
@@ -12428,7 +12428,7 @@
       <c r="O285" t="inlineStr"/>
       <c r="P285" t="inlineStr">
         <is>
-          <t>Max Mondays Dynamax Beldum during Max Monday Mon, Sep 29, at 6:00 PM Local Time Starts: Calculating... Raid Battles Mega Steelix, Scizor, and Lucario in Mega Raids Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating... Event Steel Skyline Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating... GO Battle League Great League and Fantasy Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating... Pokémon Spotlight Hour Aron Spotlight Hour Tue, Sep 30, at 6:00 PM Local Time Starts: Calculating... Raid Hour Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 6:00 PM Local Time Starts: Calculating... Raid Day Mega Metagross Raid Day Sat, Oct 4, at 2:00 PM Local Time Starts: Calculating... Max Mondays Dynamax Drilbur during Max Monday Mon, Oct 6, at 6:00 PM Local Time Starts: Calculating... Raid Battles Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating... Raid Battles Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating... GO Battle League Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts</t>
+          <t>Raid Battles Mega Steelix, Scizor, and Lucario in Mega Raids Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating... Event Steel Skyline Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating... GO Battle League Great League and Fantasy Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating... Pokémon Spotlight Hour Aron Spotlight Hour Tue, Sep 30, at 6:00 PM Local Time Starts: Calculating... Raid Hour Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 6:00 PM Local Time Starts: Calculating... Raid Day Mega Metagross Raid Day Sat, Oct 4, at 2:00 PM Local Time Starts: Calculating... Max Mondays Dynamax Drilbur during Max Monday Mon, Oct 6, at 6:00 PM Local Time Starts: Calculating... Raid Battles Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating... Raid Battles Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating... GO Battle League Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating... Pokémon Spotlight Hour Ferroseed Spotlight Hour Tue, Oct 7, at 6:00 PM Local Time Star</t>
         </is>
       </c>
       <c r="Q285" t="inlineStr">
@@ -12448,12 +12448,12 @@
       <c r="D286" t="inlineStr"/>
       <c r="E286" t="inlineStr">
         <is>
-          <t>Dynamax Beldum during Max Monday</t>
+          <t>Mega Steelix, Scizor, and Lucario in Mega Raids</t>
         </is>
       </c>
       <c r="F286" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G286" t="inlineStr"/>
@@ -12467,7 +12467,7 @@
       <c r="O286" t="inlineStr"/>
       <c r="P286" t="inlineStr">
         <is>
-          <t>Max Mondays Dynamax Beldum during Max Monday Mon, Sep 29, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Raid Battles Mega Steelix, Scizor, and Lucario in Mega Raids Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q286" t="inlineStr">
@@ -12487,12 +12487,12 @@
       <c r="D287" t="inlineStr"/>
       <c r="E287" t="inlineStr">
         <is>
-          <t>Dynamax Beldum during Max Monday</t>
+          <t>Mega Steelix, Scizor, and Lucario in Mega Raids</t>
         </is>
       </c>
       <c r="F287" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G287" t="inlineStr"/>
@@ -12506,7 +12506,7 @@
       <c r="O287" t="inlineStr"/>
       <c r="P287" t="inlineStr">
         <is>
-          <t>Dynamax Beldum during Max Monday Mon, Sep 29, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Mega Steelix, Scizor, and Lucario in Mega Raids Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q287" t="inlineStr">
@@ -12526,12 +12526,12 @@
       <c r="D288" t="inlineStr"/>
       <c r="E288" t="inlineStr">
         <is>
-          <t>Dynamax Beldum during Max Monday</t>
+          <t>Mega Steelix, Scizor, and Lucario in Mega Raids</t>
         </is>
       </c>
       <c r="F288" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G288" t="inlineStr"/>
@@ -12545,7 +12545,7 @@
       <c r="O288" t="inlineStr"/>
       <c r="P288" t="inlineStr">
         <is>
-          <t>Dynamax Beldum during Max Monday Mon, Sep 29, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Mega Steelix, Scizor, and Lucario in Mega Raids Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q288" t="inlineStr">
@@ -12565,12 +12565,12 @@
       <c r="D289" t="inlineStr"/>
       <c r="E289" t="inlineStr">
         <is>
-          <t>Dynamax Beldum during Max Monday</t>
+          <t>Mega Steelix, Scizor, and Lucario in Mega Raids</t>
         </is>
       </c>
       <c r="F289" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G289" t="inlineStr"/>
@@ -12584,7 +12584,7 @@
       <c r="O289" t="inlineStr"/>
       <c r="P289" t="inlineStr">
         <is>
-          <t>Dynamax Beldum during Max Monday Mon, Sep 29, at 6:00 PM Local Time</t>
+          <t>Mega Steelix, Scizor, and Lucario in Mega Raids Tue, Sep 30, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q289" t="inlineStr">
@@ -12604,12 +12604,12 @@
       <c r="D290" t="inlineStr"/>
       <c r="E290" t="inlineStr">
         <is>
-          <t>Mega Steelix, Scizor, and Lucario in Mega Raids</t>
+          <t>Steel Skyline</t>
         </is>
       </c>
       <c r="F290" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G290" t="inlineStr"/>
@@ -12623,7 +12623,7 @@
       <c r="O290" t="inlineStr"/>
       <c r="P290" t="inlineStr">
         <is>
-          <t>Raid Battles Mega Steelix, Scizor, and Lucario in Mega Raids Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Event Steel Skyline Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q290" t="inlineStr">
@@ -12643,12 +12643,12 @@
       <c r="D291" t="inlineStr"/>
       <c r="E291" t="inlineStr">
         <is>
-          <t>Mega Steelix, Scizor, and Lucario in Mega Raids</t>
+          <t>Steel Skyline</t>
         </is>
       </c>
       <c r="F291" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G291" t="inlineStr"/>
@@ -12662,7 +12662,7 @@
       <c r="O291" t="inlineStr"/>
       <c r="P291" t="inlineStr">
         <is>
-          <t>Mega Steelix, Scizor, and Lucario in Mega Raids Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Steel Skyline Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q291" t="inlineStr">
@@ -12682,12 +12682,12 @@
       <c r="D292" t="inlineStr"/>
       <c r="E292" t="inlineStr">
         <is>
-          <t>Mega Steelix, Scizor, and Lucario in Mega Raids</t>
+          <t>Steel Skyline</t>
         </is>
       </c>
       <c r="F292" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G292" t="inlineStr"/>
@@ -12701,7 +12701,7 @@
       <c r="O292" t="inlineStr"/>
       <c r="P292" t="inlineStr">
         <is>
-          <t>Mega Steelix, Scizor, and Lucario in Mega Raids Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Steel Skyline Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q292" t="inlineStr">
@@ -12721,12 +12721,12 @@
       <c r="D293" t="inlineStr"/>
       <c r="E293" t="inlineStr">
         <is>
-          <t>Mega Steelix, Scizor, and Lucario in Mega Raids</t>
+          <t>Steel Skyline</t>
         </is>
       </c>
       <c r="F293" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G293" t="inlineStr"/>
@@ -12740,7 +12740,7 @@
       <c r="O293" t="inlineStr"/>
       <c r="P293" t="inlineStr">
         <is>
-          <t>Mega Steelix, Scizor, and Lucario in Mega Raids Tue, Sep 30, at 10:00 AM Local Time</t>
+          <t>Steel Skyline Tue, Sep 30, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q293" t="inlineStr">
@@ -12760,7 +12760,7 @@
       <c r="D294" t="inlineStr"/>
       <c r="E294" t="inlineStr">
         <is>
-          <t>Steel Skyline</t>
+          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F294" t="inlineStr">
@@ -12779,7 +12779,7 @@
       <c r="O294" t="inlineStr"/>
       <c r="P294" t="inlineStr">
         <is>
-          <t>Event Steel Skyline Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>GO Battle League Great League and Fantasy Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q294" t="inlineStr">
@@ -12799,7 +12799,7 @@
       <c r="D295" t="inlineStr"/>
       <c r="E295" t="inlineStr">
         <is>
-          <t>Steel Skyline</t>
+          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F295" t="inlineStr">
@@ -12818,7 +12818,7 @@
       <c r="O295" t="inlineStr"/>
       <c r="P295" t="inlineStr">
         <is>
-          <t>Steel Skyline Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q295" t="inlineStr">
@@ -12838,7 +12838,7 @@
       <c r="D296" t="inlineStr"/>
       <c r="E296" t="inlineStr">
         <is>
-          <t>Steel Skyline</t>
+          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F296" t="inlineStr">
@@ -12857,7 +12857,7 @@
       <c r="O296" t="inlineStr"/>
       <c r="P296" t="inlineStr">
         <is>
-          <t>Steel Skyline Tue, Sep 30, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q296" t="inlineStr">
@@ -12877,7 +12877,7 @@
       <c r="D297" t="inlineStr"/>
       <c r="E297" t="inlineStr">
         <is>
-          <t>Steel Skyline</t>
+          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F297" t="inlineStr">
@@ -12896,7 +12896,7 @@
       <c r="O297" t="inlineStr"/>
       <c r="P297" t="inlineStr">
         <is>
-          <t>Steel Skyline Tue, Sep 30, at 10:00 AM Local Time</t>
+          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q297" t="inlineStr">
@@ -12916,12 +12916,12 @@
       <c r="D298" t="inlineStr"/>
       <c r="E298" t="inlineStr">
         <is>
-          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation</t>
+          <t>Aron Spotlight Hour</t>
         </is>
       </c>
       <c r="F298" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G298" t="inlineStr"/>
@@ -12935,7 +12935,7 @@
       <c r="O298" t="inlineStr"/>
       <c r="P298" t="inlineStr">
         <is>
-          <t>GO Battle League Great League and Fantasy Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Pokémon Spotlight Hour Aron Spotlight Hour Tue, Sep 30, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q298" t="inlineStr">
@@ -12955,12 +12955,12 @@
       <c r="D299" t="inlineStr"/>
       <c r="E299" t="inlineStr">
         <is>
-          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation</t>
+          <t>Aron Spotlight Hour</t>
         </is>
       </c>
       <c r="F299" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G299" t="inlineStr"/>
@@ -12974,7 +12974,7 @@
       <c r="O299" t="inlineStr"/>
       <c r="P299" t="inlineStr">
         <is>
-          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Aron Spotlight Hour Tue, Sep 30, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q299" t="inlineStr">
@@ -12994,12 +12994,12 @@
       <c r="D300" t="inlineStr"/>
       <c r="E300" t="inlineStr">
         <is>
-          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation</t>
+          <t>Aron Spotlight Hour</t>
         </is>
       </c>
       <c r="F300" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G300" t="inlineStr"/>
@@ -13013,7 +13013,7 @@
       <c r="O300" t="inlineStr"/>
       <c r="P300" t="inlineStr">
         <is>
-          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Aron Spotlight Hour Tue, Sep 30, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q300" t="inlineStr">
@@ -13033,12 +13033,12 @@
       <c r="D301" t="inlineStr"/>
       <c r="E301" t="inlineStr">
         <is>
-          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation</t>
+          <t>Aron Spotlight Hour</t>
         </is>
       </c>
       <c r="F301" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G301" t="inlineStr"/>
@@ -13052,7 +13052,7 @@
       <c r="O301" t="inlineStr"/>
       <c r="P301" t="inlineStr">
         <is>
-          <t>Great League and Fantasy Cup: Great League Edition | Tales of Transformation Calculating...</t>
+          <t>Aron Spotlight Hour Tue, Sep 30, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q301" t="inlineStr">
@@ -13072,12 +13072,12 @@
       <c r="D302" t="inlineStr"/>
       <c r="E302" t="inlineStr">
         <is>
-          <t>Aron Spotlight Hour</t>
+          <t>Dialga (Origin Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F302" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G302" t="inlineStr"/>
@@ -13091,7 +13091,7 @@
       <c r="O302" t="inlineStr"/>
       <c r="P302" t="inlineStr">
         <is>
-          <t>Pokémon Spotlight Hour Aron Spotlight Hour Tue, Sep 30, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Raid Hour Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q302" t="inlineStr">
@@ -13111,12 +13111,12 @@
       <c r="D303" t="inlineStr"/>
       <c r="E303" t="inlineStr">
         <is>
-          <t>Aron Spotlight Hour</t>
+          <t>Dialga (Origin Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F303" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G303" t="inlineStr"/>
@@ -13130,7 +13130,7 @@
       <c r="O303" t="inlineStr"/>
       <c r="P303" t="inlineStr">
         <is>
-          <t>Aron Spotlight Hour Tue, Sep 30, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q303" t="inlineStr">
@@ -13150,12 +13150,12 @@
       <c r="D304" t="inlineStr"/>
       <c r="E304" t="inlineStr">
         <is>
-          <t>Aron Spotlight Hour</t>
+          <t>Dialga (Origin Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F304" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G304" t="inlineStr"/>
@@ -13169,7 +13169,7 @@
       <c r="O304" t="inlineStr"/>
       <c r="P304" t="inlineStr">
         <is>
-          <t>Aron Spotlight Hour Tue, Sep 30, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q304" t="inlineStr">
@@ -13189,12 +13189,12 @@
       <c r="D305" t="inlineStr"/>
       <c r="E305" t="inlineStr">
         <is>
-          <t>Aron Spotlight Hour</t>
+          <t>Dialga (Origin Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F305" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G305" t="inlineStr"/>
@@ -13208,7 +13208,7 @@
       <c r="O305" t="inlineStr"/>
       <c r="P305" t="inlineStr">
         <is>
-          <t>Aron Spotlight Hour Tue, Sep 30, at 6:00 PM Local Time</t>
+          <t>Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q305" t="inlineStr">
@@ -13228,7 +13228,7 @@
       <c r="D306" t="inlineStr"/>
       <c r="E306" t="inlineStr">
         <is>
-          <t>Dialga (Origin Forme) Raid Hour</t>
+          <t>Mega Metagross Raid Day</t>
         </is>
       </c>
       <c r="F306" t="inlineStr">
@@ -13247,7 +13247,7 @@
       <c r="O306" t="inlineStr"/>
       <c r="P306" t="inlineStr">
         <is>
-          <t>Raid Hour Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Raid Day Mega Metagross Raid Day Sat, Oct 4, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q306" t="inlineStr">
@@ -13267,7 +13267,7 @@
       <c r="D307" t="inlineStr"/>
       <c r="E307" t="inlineStr">
         <is>
-          <t>Dialga (Origin Forme) Raid Hour</t>
+          <t>Mega Metagross Raid Day</t>
         </is>
       </c>
       <c r="F307" t="inlineStr">
@@ -13286,7 +13286,7 @@
       <c r="O307" t="inlineStr"/>
       <c r="P307" t="inlineStr">
         <is>
-          <t>Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Mega Metagross Raid Day Sat, Oct 4, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q307" t="inlineStr">
@@ -13306,7 +13306,7 @@
       <c r="D308" t="inlineStr"/>
       <c r="E308" t="inlineStr">
         <is>
-          <t>Dialga (Origin Forme) Raid Hour</t>
+          <t>Mega Metagross Raid Day</t>
         </is>
       </c>
       <c r="F308" t="inlineStr">
@@ -13325,7 +13325,7 @@
       <c r="O308" t="inlineStr"/>
       <c r="P308" t="inlineStr">
         <is>
-          <t>Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Mega Metagross Raid Day Sat, Oct 4, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q308" t="inlineStr">
@@ -13345,7 +13345,7 @@
       <c r="D309" t="inlineStr"/>
       <c r="E309" t="inlineStr">
         <is>
-          <t>Dialga (Origin Forme) Raid Hour</t>
+          <t>Mega Metagross Raid Day</t>
         </is>
       </c>
       <c r="F309" t="inlineStr">
@@ -13364,7 +13364,7 @@
       <c r="O309" t="inlineStr"/>
       <c r="P309" t="inlineStr">
         <is>
-          <t>Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 6:00 PM Local Time</t>
+          <t>Mega Metagross Raid Day Sat, Oct 4, at 2:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q309" t="inlineStr">
@@ -13384,12 +13384,12 @@
       <c r="D310" t="inlineStr"/>
       <c r="E310" t="inlineStr">
         <is>
-          <t>Mega Metagross Raid Day</t>
+          <t>Dynamax Drilbur during Max Monday</t>
         </is>
       </c>
       <c r="F310" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G310" t="inlineStr"/>
@@ -13403,7 +13403,7 @@
       <c r="O310" t="inlineStr"/>
       <c r="P310" t="inlineStr">
         <is>
-          <t>Raid Day Mega Metagross Raid Day Sat, Oct 4, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Max Mondays Dynamax Drilbur during Max Monday Mon, Oct 6, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q310" t="inlineStr">
@@ -13423,12 +13423,12 @@
       <c r="D311" t="inlineStr"/>
       <c r="E311" t="inlineStr">
         <is>
-          <t>Mega Metagross Raid Day</t>
+          <t>Dynamax Drilbur during Max Monday</t>
         </is>
       </c>
       <c r="F311" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G311" t="inlineStr"/>
@@ -13442,7 +13442,7 @@
       <c r="O311" t="inlineStr"/>
       <c r="P311" t="inlineStr">
         <is>
-          <t>Mega Metagross Raid Day Sat, Oct 4, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Dynamax Drilbur during Max Monday Mon, Oct 6, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q311" t="inlineStr">
@@ -13462,12 +13462,12 @@
       <c r="D312" t="inlineStr"/>
       <c r="E312" t="inlineStr">
         <is>
-          <t>Mega Metagross Raid Day</t>
+          <t>Dynamax Drilbur during Max Monday</t>
         </is>
       </c>
       <c r="F312" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G312" t="inlineStr"/>
@@ -13481,7 +13481,7 @@
       <c r="O312" t="inlineStr"/>
       <c r="P312" t="inlineStr">
         <is>
-          <t>Mega Metagross Raid Day Sat, Oct 4, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Dynamax Drilbur during Max Monday Mon, Oct 6, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q312" t="inlineStr">
@@ -13501,12 +13501,12 @@
       <c r="D313" t="inlineStr"/>
       <c r="E313" t="inlineStr">
         <is>
-          <t>Mega Metagross Raid Day</t>
+          <t>Dynamax Drilbur during Max Monday</t>
         </is>
       </c>
       <c r="F313" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G313" t="inlineStr"/>
@@ -13520,7 +13520,7 @@
       <c r="O313" t="inlineStr"/>
       <c r="P313" t="inlineStr">
         <is>
-          <t>Mega Metagross Raid Day Sat, Oct 4, at 2:00 PM Local Time</t>
+          <t>Dynamax Drilbur during Max Monday Mon, Oct 6, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q313" t="inlineStr">
@@ -13540,12 +13540,12 @@
       <c r="D314" t="inlineStr"/>
       <c r="E314" t="inlineStr">
         <is>
-          <t>Dynamax Drilbur during Max Monday</t>
+          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F314" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G314" t="inlineStr"/>
@@ -13559,7 +13559,7 @@
       <c r="O314" t="inlineStr"/>
       <c r="P314" t="inlineStr">
         <is>
-          <t>Max Mondays Dynamax Drilbur during Max Monday Mon, Oct 6, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Raid Battles Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q314" t="inlineStr">
@@ -13579,12 +13579,12 @@
       <c r="D315" t="inlineStr"/>
       <c r="E315" t="inlineStr">
         <is>
-          <t>Dynamax Drilbur during Max Monday</t>
+          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F315" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G315" t="inlineStr"/>
@@ -13598,7 +13598,7 @@
       <c r="O315" t="inlineStr"/>
       <c r="P315" t="inlineStr">
         <is>
-          <t>Dynamax Drilbur during Max Monday Mon, Oct 6, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q315" t="inlineStr">
@@ -13618,12 +13618,12 @@
       <c r="D316" t="inlineStr"/>
       <c r="E316" t="inlineStr">
         <is>
-          <t>Dynamax Drilbur during Max Monday</t>
+          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F316" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G316" t="inlineStr"/>
@@ -13637,7 +13637,7 @@
       <c r="O316" t="inlineStr"/>
       <c r="P316" t="inlineStr">
         <is>
-          <t>Dynamax Drilbur during Max Monday Mon, Oct 6, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q316" t="inlineStr">
@@ -13657,12 +13657,12 @@
       <c r="D317" t="inlineStr"/>
       <c r="E317" t="inlineStr">
         <is>
-          <t>Dynamax Drilbur during Max Monday</t>
+          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F317" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G317" t="inlineStr"/>
@@ -13676,7 +13676,7 @@
       <c r="O317" t="inlineStr"/>
       <c r="P317" t="inlineStr">
         <is>
-          <t>Dynamax Drilbur during Max Monday Mon, Oct 6, at 6:00 PM Local Time</t>
+          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q317" t="inlineStr">
@@ -13696,7 +13696,7 @@
       <c r="D318" t="inlineStr"/>
       <c r="E318" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles</t>
+          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids</t>
         </is>
       </c>
       <c r="F318" t="inlineStr">
@@ -13715,7 +13715,7 @@
       <c r="O318" t="inlineStr"/>
       <c r="P318" t="inlineStr">
         <is>
-          <t>Raid Battles Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Raid Battles Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q318" t="inlineStr">
@@ -13735,7 +13735,7 @@
       <c r="D319" t="inlineStr"/>
       <c r="E319" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles</t>
+          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids</t>
         </is>
       </c>
       <c r="F319" t="inlineStr">
@@ -13754,7 +13754,7 @@
       <c r="O319" t="inlineStr"/>
       <c r="P319" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q319" t="inlineStr">
@@ -13774,7 +13774,7 @@
       <c r="D320" t="inlineStr"/>
       <c r="E320" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles</t>
+          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids</t>
         </is>
       </c>
       <c r="F320" t="inlineStr">
@@ -13793,7 +13793,7 @@
       <c r="O320" t="inlineStr"/>
       <c r="P320" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q320" t="inlineStr">
@@ -13813,7 +13813,7 @@
       <c r="D321" t="inlineStr"/>
       <c r="E321" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles</t>
+          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids</t>
         </is>
       </c>
       <c r="F321" t="inlineStr">
@@ -13832,7 +13832,7 @@
       <c r="O321" t="inlineStr"/>
       <c r="P321" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time</t>
+          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids Tue, Oct 7, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q321" t="inlineStr">
@@ -13852,12 +13852,12 @@
       <c r="D322" t="inlineStr"/>
       <c r="E322" t="inlineStr">
         <is>
-          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F322" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G322" t="inlineStr"/>
@@ -13871,7 +13871,7 @@
       <c r="O322" t="inlineStr"/>
       <c r="P322" t="inlineStr">
         <is>
-          <t>Raid Battles Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>GO Battle League Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q322" t="inlineStr">
@@ -13891,12 +13891,12 @@
       <c r="D323" t="inlineStr"/>
       <c r="E323" t="inlineStr">
         <is>
-          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F323" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G323" t="inlineStr"/>
@@ -13910,7 +13910,7 @@
       <c r="O323" t="inlineStr"/>
       <c r="P323" t="inlineStr">
         <is>
-          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q323" t="inlineStr">
@@ -13930,12 +13930,12 @@
       <c r="D324" t="inlineStr"/>
       <c r="E324" t="inlineStr">
         <is>
-          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F324" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G324" t="inlineStr"/>
@@ -13949,7 +13949,7 @@
       <c r="O324" t="inlineStr"/>
       <c r="P324" t="inlineStr">
         <is>
-          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q324" t="inlineStr">
@@ -13969,12 +13969,12 @@
       <c r="D325" t="inlineStr"/>
       <c r="E325" t="inlineStr">
         <is>
-          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F325" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G325" t="inlineStr"/>
@@ -13988,7 +13988,7 @@
       <c r="O325" t="inlineStr"/>
       <c r="P325" t="inlineStr">
         <is>
-          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids Tue, Oct 7, at 10:00 AM Local Time</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q325" t="inlineStr">
@@ -14008,12 +14008,12 @@
       <c r="D326" t="inlineStr"/>
       <c r="E326" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
+          <t>Ferroseed Spotlight Hour</t>
         </is>
       </c>
       <c r="F326" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G326" t="inlineStr"/>
@@ -14027,7 +14027,7 @@
       <c r="O326" t="inlineStr"/>
       <c r="P326" t="inlineStr">
         <is>
-          <t>GO Battle League Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Pokémon Spotlight Hour Ferroseed Spotlight Hour Tue, Oct 7, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q326" t="inlineStr">
@@ -14047,12 +14047,12 @@
       <c r="D327" t="inlineStr"/>
       <c r="E327" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
+          <t>Ferroseed Spotlight Hour</t>
         </is>
       </c>
       <c r="F327" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G327" t="inlineStr"/>
@@ -14066,7 +14066,7 @@
       <c r="O327" t="inlineStr"/>
       <c r="P327" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Ferroseed Spotlight Hour Tue, Oct 7, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q327" t="inlineStr">
@@ -14086,12 +14086,12 @@
       <c r="D328" t="inlineStr"/>
       <c r="E328" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
+          <t>Ferroseed Spotlight Hour</t>
         </is>
       </c>
       <c r="F328" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G328" t="inlineStr"/>
@@ -14105,7 +14105,7 @@
       <c r="O328" t="inlineStr"/>
       <c r="P328" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Ferroseed Spotlight Hour Tue, Oct 7, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q328" t="inlineStr">
@@ -14125,12 +14125,12 @@
       <c r="D329" t="inlineStr"/>
       <c r="E329" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
+          <t>Ferroseed Spotlight Hour</t>
         </is>
       </c>
       <c r="F329" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G329" t="inlineStr"/>
@@ -14144,7 +14144,7 @@
       <c r="O329" t="inlineStr"/>
       <c r="P329" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating...</t>
+          <t>Ferroseed Spotlight Hour Tue, Oct 7, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q329" t="inlineStr">
@@ -14164,12 +14164,12 @@
       <c r="D330" t="inlineStr"/>
       <c r="E330" t="inlineStr">
         <is>
-          <t>Ferroseed Spotlight Hour</t>
+          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F330" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G330" t="inlineStr"/>
@@ -14183,7 +14183,7 @@
       <c r="O330" t="inlineStr"/>
       <c r="P330" t="inlineStr">
         <is>
-          <t>Pokémon Spotlight Hour Ferroseed Spotlight Hour Tue, Oct 7, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Raid Hour Deoxys (Normal &amp; Defense Forme) Raid Hour Wed, Oct 8, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q330" t="inlineStr">
@@ -14203,12 +14203,12 @@
       <c r="D331" t="inlineStr"/>
       <c r="E331" t="inlineStr">
         <is>
-          <t>Ferroseed Spotlight Hour</t>
+          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F331" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G331" t="inlineStr"/>
@@ -14222,7 +14222,7 @@
       <c r="O331" t="inlineStr"/>
       <c r="P331" t="inlineStr">
         <is>
-          <t>Ferroseed Spotlight Hour Tue, Oct 7, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour Wed, Oct 8, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q331" t="inlineStr">
@@ -14242,12 +14242,12 @@
       <c r="D332" t="inlineStr"/>
       <c r="E332" t="inlineStr">
         <is>
-          <t>Ferroseed Spotlight Hour</t>
+          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F332" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G332" t="inlineStr"/>
@@ -14261,7 +14261,7 @@
       <c r="O332" t="inlineStr"/>
       <c r="P332" t="inlineStr">
         <is>
-          <t>Ferroseed Spotlight Hour Tue, Oct 7, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour Wed, Oct 8, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q332" t="inlineStr">
@@ -14281,12 +14281,12 @@
       <c r="D333" t="inlineStr"/>
       <c r="E333" t="inlineStr">
         <is>
-          <t>Ferroseed Spotlight Hour</t>
+          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F333" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G333" t="inlineStr"/>
@@ -14300,7 +14300,7 @@
       <c r="O333" t="inlineStr"/>
       <c r="P333" t="inlineStr">
         <is>
-          <t>Ferroseed Spotlight Hour Tue, Oct 7, at 6:00 PM Local Time</t>
+          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour Wed, Oct 8, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q333" t="inlineStr">
@@ -14320,12 +14320,12 @@
       <c r="D334" t="inlineStr"/>
       <c r="E334" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour</t>
+          <t>Harvest Festival</t>
         </is>
       </c>
       <c r="F334" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G334" t="inlineStr"/>
@@ -14339,7 +14339,7 @@
       <c r="O334" t="inlineStr"/>
       <c r="P334" t="inlineStr">
         <is>
-          <t>Raid Hour Deoxys (Normal &amp; Defense Forme) Raid Hour Wed, Oct 8, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Event Harvest Festival Fri, Oct 10, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q334" t="inlineStr">
@@ -14359,12 +14359,12 @@
       <c r="D335" t="inlineStr"/>
       <c r="E335" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour</t>
+          <t>Harvest Festival</t>
         </is>
       </c>
       <c r="F335" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G335" t="inlineStr"/>
@@ -14378,7 +14378,7 @@
       <c r="O335" t="inlineStr"/>
       <c r="P335" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour Wed, Oct 8, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Harvest Festival Fri, Oct 10, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q335" t="inlineStr">
@@ -14398,12 +14398,12 @@
       <c r="D336" t="inlineStr"/>
       <c r="E336" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour</t>
+          <t>Harvest Festival</t>
         </is>
       </c>
       <c r="F336" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G336" t="inlineStr"/>
@@ -14417,7 +14417,7 @@
       <c r="O336" t="inlineStr"/>
       <c r="P336" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour Wed, Oct 8, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Harvest Festival Fri, Oct 10, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q336" t="inlineStr">
@@ -14437,12 +14437,12 @@
       <c r="D337" t="inlineStr"/>
       <c r="E337" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour</t>
+          <t>Harvest Festival</t>
         </is>
       </c>
       <c r="F337" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G337" t="inlineStr"/>
@@ -14456,7 +14456,7 @@
       <c r="O337" t="inlineStr"/>
       <c r="P337" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour Wed, Oct 8, at 6:00 PM Local Time</t>
+          <t>Harvest Festival Fri, Oct 10, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q337" t="inlineStr">
@@ -14476,12 +14476,12 @@
       <c r="D338" t="inlineStr"/>
       <c r="E338" t="inlineStr">
         <is>
-          <t>Harvest Festival</t>
+          <t>Solosis Community Day</t>
         </is>
       </c>
       <c r="F338" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Community Day</t>
         </is>
       </c>
       <c r="G338" t="inlineStr"/>
@@ -14495,7 +14495,7 @@
       <c r="O338" t="inlineStr"/>
       <c r="P338" t="inlineStr">
         <is>
-          <t>Event Harvest Festival Fri, Oct 10, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Community Day Solosis Community Day Sun, Oct 12, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q338" t="inlineStr">
@@ -14515,12 +14515,12 @@
       <c r="D339" t="inlineStr"/>
       <c r="E339" t="inlineStr">
         <is>
-          <t>Harvest Festival</t>
+          <t>Solosis Community Day</t>
         </is>
       </c>
       <c r="F339" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Community Day</t>
         </is>
       </c>
       <c r="G339" t="inlineStr"/>
@@ -14534,7 +14534,7 @@
       <c r="O339" t="inlineStr"/>
       <c r="P339" t="inlineStr">
         <is>
-          <t>Harvest Festival Fri, Oct 10, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Solosis Community Day Sun, Oct 12, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q339" t="inlineStr">
@@ -14554,12 +14554,12 @@
       <c r="D340" t="inlineStr"/>
       <c r="E340" t="inlineStr">
         <is>
-          <t>Harvest Festival</t>
+          <t>Solosis Community Day</t>
         </is>
       </c>
       <c r="F340" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Community Day</t>
         </is>
       </c>
       <c r="G340" t="inlineStr"/>
@@ -14573,7 +14573,7 @@
       <c r="O340" t="inlineStr"/>
       <c r="P340" t="inlineStr">
         <is>
-          <t>Harvest Festival Fri, Oct 10, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Solosis Community Day Sun, Oct 12, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q340" t="inlineStr">
@@ -14593,12 +14593,12 @@
       <c r="D341" t="inlineStr"/>
       <c r="E341" t="inlineStr">
         <is>
-          <t>Harvest Festival</t>
+          <t>Solosis Community Day</t>
         </is>
       </c>
       <c r="F341" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Community Day</t>
         </is>
       </c>
       <c r="G341" t="inlineStr"/>
@@ -14612,7 +14612,7 @@
       <c r="O341" t="inlineStr"/>
       <c r="P341" t="inlineStr">
         <is>
-          <t>Harvest Festival Fri, Oct 10, at 10:00 AM Local Time</t>
+          <t>Solosis Community Day Sun, Oct 12, at 2:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q341" t="inlineStr">
@@ -14632,12 +14632,12 @@
       <c r="D342" t="inlineStr"/>
       <c r="E342" t="inlineStr">
         <is>
-          <t>Solosis Community Day</t>
+          <t>Dynamax Bounsweet during Max Monday</t>
         </is>
       </c>
       <c r="F342" t="inlineStr">
         <is>
-          <t>Community Day</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G342" t="inlineStr"/>
@@ -14651,7 +14651,7 @@
       <c r="O342" t="inlineStr"/>
       <c r="P342" t="inlineStr">
         <is>
-          <t>Community Day Solosis Community Day Sun, Oct 12, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Max Mondays Dynamax Bounsweet during Max Monday Mon, Oct 13, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q342" t="inlineStr">
@@ -14671,12 +14671,12 @@
       <c r="D343" t="inlineStr"/>
       <c r="E343" t="inlineStr">
         <is>
-          <t>Solosis Community Day</t>
+          <t>Dynamax Bounsweet during Max Monday</t>
         </is>
       </c>
       <c r="F343" t="inlineStr">
         <is>
-          <t>Community Day</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G343" t="inlineStr"/>
@@ -14690,7 +14690,7 @@
       <c r="O343" t="inlineStr"/>
       <c r="P343" t="inlineStr">
         <is>
-          <t>Solosis Community Day Sun, Oct 12, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Dynamax Bounsweet during Max Monday Mon, Oct 13, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q343" t="inlineStr">
@@ -14710,12 +14710,12 @@
       <c r="D344" t="inlineStr"/>
       <c r="E344" t="inlineStr">
         <is>
-          <t>Solosis Community Day</t>
+          <t>Dynamax Bounsweet during Max Monday</t>
         </is>
       </c>
       <c r="F344" t="inlineStr">
         <is>
-          <t>Community Day</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G344" t="inlineStr"/>
@@ -14729,7 +14729,7 @@
       <c r="O344" t="inlineStr"/>
       <c r="P344" t="inlineStr">
         <is>
-          <t>Solosis Community Day Sun, Oct 12, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Dynamax Bounsweet during Max Monday Mon, Oct 13, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q344" t="inlineStr">
@@ -14749,12 +14749,12 @@
       <c r="D345" t="inlineStr"/>
       <c r="E345" t="inlineStr">
         <is>
-          <t>Solosis Community Day</t>
+          <t>Dynamax Bounsweet during Max Monday</t>
         </is>
       </c>
       <c r="F345" t="inlineStr">
         <is>
-          <t>Community Day</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G345" t="inlineStr"/>
@@ -14768,7 +14768,7 @@
       <c r="O345" t="inlineStr"/>
       <c r="P345" t="inlineStr">
         <is>
-          <t>Solosis Community Day Sun, Oct 12, at 2:00 PM Local Time</t>
+          <t>Dynamax Bounsweet during Max Monday Mon, Oct 13, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q345" t="inlineStr">
@@ -14788,12 +14788,12 @@
       <c r="D346" t="inlineStr"/>
       <c r="E346" t="inlineStr">
         <is>
-          <t>Dynamax Bounsweet during Max Monday</t>
+          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F346" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G346" t="inlineStr"/>
@@ -14807,7 +14807,7 @@
       <c r="O346" t="inlineStr"/>
       <c r="P346" t="inlineStr">
         <is>
-          <t>Max Mondays Dynamax Bounsweet during Max Monday Mon, Oct 13, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Raid Battles Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q346" t="inlineStr">
@@ -14827,12 +14827,12 @@
       <c r="D347" t="inlineStr"/>
       <c r="E347" t="inlineStr">
         <is>
-          <t>Dynamax Bounsweet during Max Monday</t>
+          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F347" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G347" t="inlineStr"/>
@@ -14846,7 +14846,7 @@
       <c r="O347" t="inlineStr"/>
       <c r="P347" t="inlineStr">
         <is>
-          <t>Dynamax Bounsweet during Max Monday Mon, Oct 13, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q347" t="inlineStr">
@@ -14866,12 +14866,12 @@
       <c r="D348" t="inlineStr"/>
       <c r="E348" t="inlineStr">
         <is>
-          <t>Dynamax Bounsweet during Max Monday</t>
+          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F348" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G348" t="inlineStr"/>
@@ -14885,7 +14885,7 @@
       <c r="O348" t="inlineStr"/>
       <c r="P348" t="inlineStr">
         <is>
-          <t>Dynamax Bounsweet during Max Monday Mon, Oct 13, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q348" t="inlineStr">
@@ -14905,12 +14905,12 @@
       <c r="D349" t="inlineStr"/>
       <c r="E349" t="inlineStr">
         <is>
-          <t>Dynamax Bounsweet during Max Monday</t>
+          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F349" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G349" t="inlineStr"/>
@@ -14924,7 +14924,7 @@
       <c r="O349" t="inlineStr"/>
       <c r="P349" t="inlineStr">
         <is>
-          <t>Dynamax Bounsweet during Max Monday Mon, Oct 13, at 6:00 PM Local Time</t>
+          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles Tue, Oct 14, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q349" t="inlineStr">
@@ -14944,7 +14944,7 @@
       <c r="D350" t="inlineStr"/>
       <c r="E350" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles</t>
+          <t>Mega Mawile and Mega Salamence in Mega Raids</t>
         </is>
       </c>
       <c r="F350" t="inlineStr">
@@ -14963,7 +14963,7 @@
       <c r="O350" t="inlineStr"/>
       <c r="P350" t="inlineStr">
         <is>
-          <t>Raid Battles Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Raid Battles Mega Mawile and Mega Salamence in Mega Raids Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q350" t="inlineStr">
@@ -14983,7 +14983,7 @@
       <c r="D351" t="inlineStr"/>
       <c r="E351" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles</t>
+          <t>Mega Mawile and Mega Salamence in Mega Raids</t>
         </is>
       </c>
       <c r="F351" t="inlineStr">
@@ -15002,7 +15002,7 @@
       <c r="O351" t="inlineStr"/>
       <c r="P351" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Mega Mawile and Mega Salamence in Mega Raids Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q351" t="inlineStr">
@@ -15022,7 +15022,7 @@
       <c r="D352" t="inlineStr"/>
       <c r="E352" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles</t>
+          <t>Mega Mawile and Mega Salamence in Mega Raids</t>
         </is>
       </c>
       <c r="F352" t="inlineStr">
@@ -15041,7 +15041,7 @@
       <c r="O352" t="inlineStr"/>
       <c r="P352" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Mega Mawile and Mega Salamence in Mega Raids Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q352" t="inlineStr">
@@ -15061,7 +15061,7 @@
       <c r="D353" t="inlineStr"/>
       <c r="E353" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles</t>
+          <t>Mega Mawile and Mega Salamence in Mega Raids</t>
         </is>
       </c>
       <c r="F353" t="inlineStr">
@@ -15080,7 +15080,7 @@
       <c r="O353" t="inlineStr"/>
       <c r="P353" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles Tue, Oct 14, at 10:00 AM Local Time</t>
+          <t>Mega Mawile and Mega Salamence in Mega Raids Tue, Oct 14, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q353" t="inlineStr">
@@ -15100,12 +15100,12 @@
       <c r="D354" t="inlineStr"/>
       <c r="E354" t="inlineStr">
         <is>
-          <t>Mega Mawile and Mega Salamence in Mega Raids</t>
+          <t>Master Premier and Great League Remix | Tales of Transformation</t>
         </is>
       </c>
       <c r="F354" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G354" t="inlineStr"/>
@@ -15119,7 +15119,7 @@
       <c r="O354" t="inlineStr"/>
       <c r="P354" t="inlineStr">
         <is>
-          <t>Raid Battles Mega Mawile and Mega Salamence in Mega Raids Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>GO Battle League Master Premier and Great League Remix | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q354" t="inlineStr">
@@ -15139,12 +15139,12 @@
       <c r="D355" t="inlineStr"/>
       <c r="E355" t="inlineStr">
         <is>
-          <t>Mega Mawile and Mega Salamence in Mega Raids</t>
+          <t>Master Premier and Great League Remix | Tales of Transformation</t>
         </is>
       </c>
       <c r="F355" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G355" t="inlineStr"/>
@@ -15158,7 +15158,7 @@
       <c r="O355" t="inlineStr"/>
       <c r="P355" t="inlineStr">
         <is>
-          <t>Mega Mawile and Mega Salamence in Mega Raids Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Master Premier and Great League Remix | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q355" t="inlineStr">
@@ -15178,12 +15178,12 @@
       <c r="D356" t="inlineStr"/>
       <c r="E356" t="inlineStr">
         <is>
-          <t>Mega Mawile and Mega Salamence in Mega Raids</t>
+          <t>Master Premier and Great League Remix | Tales of Transformation</t>
         </is>
       </c>
       <c r="F356" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G356" t="inlineStr"/>
@@ -15197,7 +15197,7 @@
       <c r="O356" t="inlineStr"/>
       <c r="P356" t="inlineStr">
         <is>
-          <t>Mega Mawile and Mega Salamence in Mega Raids Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Master Premier and Great League Remix | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q356" t="inlineStr">
@@ -15217,12 +15217,12 @@
       <c r="D357" t="inlineStr"/>
       <c r="E357" t="inlineStr">
         <is>
-          <t>Mega Mawile and Mega Salamence in Mega Raids</t>
+          <t>Master Premier and Great League Remix | Tales of Transformation</t>
         </is>
       </c>
       <c r="F357" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G357" t="inlineStr"/>
@@ -15236,7 +15236,7 @@
       <c r="O357" t="inlineStr"/>
       <c r="P357" t="inlineStr">
         <is>
-          <t>Mega Mawile and Mega Salamence in Mega Raids Tue, Oct 14, at 10:00 AM Local Time</t>
+          <t>Master Premier and Great League Remix | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q357" t="inlineStr">
@@ -15256,12 +15256,12 @@
       <c r="D358" t="inlineStr"/>
       <c r="E358" t="inlineStr">
         <is>
-          <t>Master Premier and Great League Remix | Tales of Transformation</t>
+          <t>Petilil Spotlight Hour</t>
         </is>
       </c>
       <c r="F358" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G358" t="inlineStr"/>
@@ -15275,7 +15275,7 @@
       <c r="O358" t="inlineStr"/>
       <c r="P358" t="inlineStr">
         <is>
-          <t>GO Battle League Master Premier and Great League Remix | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Pokémon Spotlight Hour Petilil Spotlight Hour Tue, Oct 14, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q358" t="inlineStr">
@@ -15295,12 +15295,12 @@
       <c r="D359" t="inlineStr"/>
       <c r="E359" t="inlineStr">
         <is>
-          <t>Master Premier and Great League Remix | Tales of Transformation</t>
+          <t>Petilil Spotlight Hour</t>
         </is>
       </c>
       <c r="F359" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G359" t="inlineStr"/>
@@ -15314,7 +15314,7 @@
       <c r="O359" t="inlineStr"/>
       <c r="P359" t="inlineStr">
         <is>
-          <t>Master Premier and Great League Remix | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Petilil Spotlight Hour Tue, Oct 14, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q359" t="inlineStr">
@@ -15334,12 +15334,12 @@
       <c r="D360" t="inlineStr"/>
       <c r="E360" t="inlineStr">
         <is>
-          <t>Master Premier and Great League Remix | Tales of Transformation</t>
+          <t>Petilil Spotlight Hour</t>
         </is>
       </c>
       <c r="F360" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G360" t="inlineStr"/>
@@ -15353,7 +15353,7 @@
       <c r="O360" t="inlineStr"/>
       <c r="P360" t="inlineStr">
         <is>
-          <t>Master Premier and Great League Remix | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Petilil Spotlight Hour Tue, Oct 14, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q360" t="inlineStr">
@@ -15373,12 +15373,12 @@
       <c r="D361" t="inlineStr"/>
       <c r="E361" t="inlineStr">
         <is>
-          <t>Master Premier and Great League Remix | Tales of Transformation</t>
+          <t>Petilil Spotlight Hour</t>
         </is>
       </c>
       <c r="F361" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G361" t="inlineStr"/>
@@ -15392,7 +15392,7 @@
       <c r="O361" t="inlineStr"/>
       <c r="P361" t="inlineStr">
         <is>
-          <t>Master Premier and Great League Remix | Tales of Transformation Calculating...</t>
+          <t>Petilil Spotlight Hour Tue, Oct 14, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q361" t="inlineStr">
@@ -15412,12 +15412,12 @@
       <c r="D362" t="inlineStr"/>
       <c r="E362" t="inlineStr">
         <is>
-          <t>Petilil Spotlight Hour</t>
+          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F362" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G362" t="inlineStr"/>
@@ -15431,7 +15431,7 @@
       <c r="O362" t="inlineStr"/>
       <c r="P362" t="inlineStr">
         <is>
-          <t>Pokémon Spotlight Hour Petilil Spotlight Hour Tue, Oct 14, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Raid Hour Deoxys (Attack &amp; Speed Forme) Raid Hour Wed, Oct 15, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q362" t="inlineStr">
@@ -15451,12 +15451,12 @@
       <c r="D363" t="inlineStr"/>
       <c r="E363" t="inlineStr">
         <is>
-          <t>Petilil Spotlight Hour</t>
+          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F363" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G363" t="inlineStr"/>
@@ -15470,7 +15470,7 @@
       <c r="O363" t="inlineStr"/>
       <c r="P363" t="inlineStr">
         <is>
-          <t>Petilil Spotlight Hour Tue, Oct 14, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour Wed, Oct 15, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q363" t="inlineStr">
@@ -15490,12 +15490,12 @@
       <c r="D364" t="inlineStr"/>
       <c r="E364" t="inlineStr">
         <is>
-          <t>Petilil Spotlight Hour</t>
+          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F364" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G364" t="inlineStr"/>
@@ -15509,7 +15509,7 @@
       <c r="O364" t="inlineStr"/>
       <c r="P364" t="inlineStr">
         <is>
-          <t>Petilil Spotlight Hour Tue, Oct 14, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour Wed, Oct 15, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q364" t="inlineStr">
@@ -15529,12 +15529,12 @@
       <c r="D365" t="inlineStr"/>
       <c r="E365" t="inlineStr">
         <is>
-          <t>Petilil Spotlight Hour</t>
+          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F365" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G365" t="inlineStr"/>
@@ -15548,7 +15548,7 @@
       <c r="O365" t="inlineStr"/>
       <c r="P365" t="inlineStr">
         <is>
-          <t>Petilil Spotlight Hour Tue, Oct 14, at 6:00 PM Local Time</t>
+          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour Wed, Oct 15, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q365" t="inlineStr">
@@ -15568,12 +15568,12 @@
       <c r="D366" t="inlineStr"/>
       <c r="E366" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour</t>
+          <t>Pokémon Legends: Z-A Celebration Event</t>
         </is>
       </c>
       <c r="F366" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G366" t="inlineStr"/>
@@ -15587,7 +15587,7 @@
       <c r="O366" t="inlineStr"/>
       <c r="P366" t="inlineStr">
         <is>
-          <t>Raid Hour Deoxys (Attack &amp; Speed Forme) Raid Hour Wed, Oct 15, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Event Pokémon Legends: Z-A Celebration Event Thu, Oct 16, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q366" t="inlineStr">
@@ -15607,12 +15607,12 @@
       <c r="D367" t="inlineStr"/>
       <c r="E367" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour</t>
+          <t>Pokémon Legends: Z-A Celebration Event</t>
         </is>
       </c>
       <c r="F367" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G367" t="inlineStr"/>
@@ -15626,7 +15626,7 @@
       <c r="O367" t="inlineStr"/>
       <c r="P367" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour Wed, Oct 15, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Pokémon Legends: Z-A Celebration Event Thu, Oct 16, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q367" t="inlineStr">
@@ -15646,12 +15646,12 @@
       <c r="D368" t="inlineStr"/>
       <c r="E368" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour</t>
+          <t>Pokémon Legends: Z-A Celebration Event</t>
         </is>
       </c>
       <c r="F368" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G368" t="inlineStr"/>
@@ -15665,7 +15665,7 @@
       <c r="O368" t="inlineStr"/>
       <c r="P368" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour Wed, Oct 15, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Pokémon Legends: Z-A Celebration Event Thu, Oct 16, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q368" t="inlineStr">
@@ -15685,12 +15685,12 @@
       <c r="D369" t="inlineStr"/>
       <c r="E369" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour</t>
+          <t>Pokémon Legends: Z-A Celebration Event</t>
         </is>
       </c>
       <c r="F369" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G369" t="inlineStr"/>
@@ -15704,7 +15704,7 @@
       <c r="O369" t="inlineStr"/>
       <c r="P369" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour Wed, Oct 15, at 6:00 PM Local Time</t>
+          <t>Pokémon Legends: Z-A Celebration Event Thu, Oct 16, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q369" t="inlineStr">
@@ -15724,12 +15724,12 @@
       <c r="D370" t="inlineStr"/>
       <c r="E370" t="inlineStr">
         <is>
-          <t>Pokémon Legends: Z-A Celebration Event</t>
+          <t>Mega Rayquaza Raid Day</t>
         </is>
       </c>
       <c r="F370" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G370" t="inlineStr"/>
@@ -15743,7 +15743,7 @@
       <c r="O370" t="inlineStr"/>
       <c r="P370" t="inlineStr">
         <is>
-          <t>Event Pokémon Legends: Z-A Celebration Event Thu, Oct 16, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Raid Day Mega Rayquaza Raid Day Sat, Oct 18, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q370" t="inlineStr">
@@ -15763,12 +15763,12 @@
       <c r="D371" t="inlineStr"/>
       <c r="E371" t="inlineStr">
         <is>
-          <t>Pokémon Legends: Z-A Celebration Event</t>
+          <t>Mega Rayquaza Raid Day</t>
         </is>
       </c>
       <c r="F371" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G371" t="inlineStr"/>
@@ -15782,7 +15782,7 @@
       <c r="O371" t="inlineStr"/>
       <c r="P371" t="inlineStr">
         <is>
-          <t>Pokémon Legends: Z-A Celebration Event Thu, Oct 16, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Mega Rayquaza Raid Day Sat, Oct 18, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q371" t="inlineStr">
@@ -15802,12 +15802,12 @@
       <c r="D372" t="inlineStr"/>
       <c r="E372" t="inlineStr">
         <is>
-          <t>Pokémon Legends: Z-A Celebration Event</t>
+          <t>Mega Rayquaza Raid Day</t>
         </is>
       </c>
       <c r="F372" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G372" t="inlineStr"/>
@@ -15821,7 +15821,7 @@
       <c r="O372" t="inlineStr"/>
       <c r="P372" t="inlineStr">
         <is>
-          <t>Pokémon Legends: Z-A Celebration Event Thu, Oct 16, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Mega Rayquaza Raid Day Sat, Oct 18, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q372" t="inlineStr">
@@ -15841,12 +15841,12 @@
       <c r="D373" t="inlineStr"/>
       <c r="E373" t="inlineStr">
         <is>
-          <t>Pokémon Legends: Z-A Celebration Event</t>
+          <t>Mega Rayquaza Raid Day</t>
         </is>
       </c>
       <c r="F373" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G373" t="inlineStr"/>
@@ -15860,7 +15860,7 @@
       <c r="O373" t="inlineStr"/>
       <c r="P373" t="inlineStr">
         <is>
-          <t>Pokémon Legends: Z-A Celebration Event Thu, Oct 16, at 10:00 AM Local Time</t>
+          <t>Mega Rayquaza Raid Day Sat, Oct 18, at 2:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q373" t="inlineStr">
@@ -15880,12 +15880,12 @@
       <c r="D374" t="inlineStr"/>
       <c r="E374" t="inlineStr">
         <is>
-          <t>Mega Rayquaza Raid Day</t>
+          <t>Dynamax Gastly during Max Monday</t>
         </is>
       </c>
       <c r="F374" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G374" t="inlineStr"/>
@@ -15899,7 +15899,7 @@
       <c r="O374" t="inlineStr"/>
       <c r="P374" t="inlineStr">
         <is>
-          <t>Raid Day Mega Rayquaza Raid Day Sat, Oct 18, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Max Mondays Dynamax Gastly during Max Monday Mon, Oct 20, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q374" t="inlineStr">
@@ -15919,12 +15919,12 @@
       <c r="D375" t="inlineStr"/>
       <c r="E375" t="inlineStr">
         <is>
-          <t>Mega Rayquaza Raid Day</t>
+          <t>Dynamax Gastly during Max Monday</t>
         </is>
       </c>
       <c r="F375" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G375" t="inlineStr"/>
@@ -15938,7 +15938,7 @@
       <c r="O375" t="inlineStr"/>
       <c r="P375" t="inlineStr">
         <is>
-          <t>Mega Rayquaza Raid Day Sat, Oct 18, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Dynamax Gastly during Max Monday Mon, Oct 20, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q375" t="inlineStr">
@@ -15958,12 +15958,12 @@
       <c r="D376" t="inlineStr"/>
       <c r="E376" t="inlineStr">
         <is>
-          <t>Mega Rayquaza Raid Day</t>
+          <t>Dynamax Gastly during Max Monday</t>
         </is>
       </c>
       <c r="F376" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G376" t="inlineStr"/>
@@ -15977,7 +15977,7 @@
       <c r="O376" t="inlineStr"/>
       <c r="P376" t="inlineStr">
         <is>
-          <t>Mega Rayquaza Raid Day Sat, Oct 18, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Dynamax Gastly during Max Monday Mon, Oct 20, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q376" t="inlineStr">
@@ -15997,12 +15997,12 @@
       <c r="D377" t="inlineStr"/>
       <c r="E377" t="inlineStr">
         <is>
-          <t>Mega Rayquaza Raid Day</t>
+          <t>Dynamax Gastly during Max Monday</t>
         </is>
       </c>
       <c r="F377" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G377" t="inlineStr"/>
@@ -16016,7 +16016,7 @@
       <c r="O377" t="inlineStr"/>
       <c r="P377" t="inlineStr">
         <is>
-          <t>Mega Rayquaza Raid Day Sat, Oct 18, at 2:00 PM Local Time</t>
+          <t>Dynamax Gastly during Max Monday Mon, Oct 20, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q377" t="inlineStr">
@@ -16036,7 +16036,7 @@
       <c r="D378" t="inlineStr"/>
       <c r="E378" t="inlineStr">
         <is>
-          <t>Dynamax Gastly during Max Monday</t>
+          <t>Halloween 2025 Part I</t>
         </is>
       </c>
       <c r="F378" t="inlineStr">
@@ -16055,7 +16055,7 @@
       <c r="O378" t="inlineStr"/>
       <c r="P378" t="inlineStr">
         <is>
-          <t>Max Mondays Dynamax Gastly during Max Monday Mon, Oct 20, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Event Halloween 2025 Part I Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q378" t="inlineStr">
@@ -16075,7 +16075,7 @@
       <c r="D379" t="inlineStr"/>
       <c r="E379" t="inlineStr">
         <is>
-          <t>Dynamax Gastly during Max Monday</t>
+          <t>Halloween 2025 Part I</t>
         </is>
       </c>
       <c r="F379" t="inlineStr">
@@ -16094,7 +16094,7 @@
       <c r="O379" t="inlineStr"/>
       <c r="P379" t="inlineStr">
         <is>
-          <t>Dynamax Gastly during Max Monday Mon, Oct 20, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Halloween 2025 Part I Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q379" t="inlineStr">
@@ -16114,7 +16114,7 @@
       <c r="D380" t="inlineStr"/>
       <c r="E380" t="inlineStr">
         <is>
-          <t>Dynamax Gastly during Max Monday</t>
+          <t>Halloween 2025 Part I</t>
         </is>
       </c>
       <c r="F380" t="inlineStr">
@@ -16133,7 +16133,7 @@
       <c r="O380" t="inlineStr"/>
       <c r="P380" t="inlineStr">
         <is>
-          <t>Dynamax Gastly during Max Monday Mon, Oct 20, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Halloween 2025 Part I Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q380" t="inlineStr">
@@ -16153,7 +16153,7 @@
       <c r="D381" t="inlineStr"/>
       <c r="E381" t="inlineStr">
         <is>
-          <t>Dynamax Gastly during Max Monday</t>
+          <t>Halloween 2025 Part I</t>
         </is>
       </c>
       <c r="F381" t="inlineStr">
@@ -16172,7 +16172,7 @@
       <c r="O381" t="inlineStr"/>
       <c r="P381" t="inlineStr">
         <is>
-          <t>Dynamax Gastly during Max Monday Mon, Oct 20, at 6:00 PM Local Time</t>
+          <t>Halloween 2025 Part I Tue, Oct 21, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q381" t="inlineStr">
@@ -16192,12 +16192,12 @@
       <c r="D382" t="inlineStr"/>
       <c r="E382" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part I</t>
+          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F382" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G382" t="inlineStr"/>
@@ -16211,7 +16211,7 @@
       <c r="O382" t="inlineStr"/>
       <c r="P382" t="inlineStr">
         <is>
-          <t>Event Halloween 2025 Part I Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Raid Battles Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q382" t="inlineStr">
@@ -16231,12 +16231,12 @@
       <c r="D383" t="inlineStr"/>
       <c r="E383" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part I</t>
+          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F383" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G383" t="inlineStr"/>
@@ -16250,7 +16250,7 @@
       <c r="O383" t="inlineStr"/>
       <c r="P383" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part I Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q383" t="inlineStr">
@@ -16270,12 +16270,12 @@
       <c r="D384" t="inlineStr"/>
       <c r="E384" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part I</t>
+          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F384" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G384" t="inlineStr"/>
@@ -16289,7 +16289,7 @@
       <c r="O384" t="inlineStr"/>
       <c r="P384" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part I Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q384" t="inlineStr">
@@ -16309,12 +16309,12 @@
       <c r="D385" t="inlineStr"/>
       <c r="E385" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part I</t>
+          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F385" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G385" t="inlineStr"/>
@@ -16328,7 +16328,7 @@
       <c r="O385" t="inlineStr"/>
       <c r="P385" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part I Tue, Oct 21, at 10:00 AM Local Time</t>
+          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles Tue, Oct 21, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q385" t="inlineStr">
@@ -16348,7 +16348,7 @@
       <c r="D386" t="inlineStr"/>
       <c r="E386" t="inlineStr">
         <is>
-          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles</t>
+          <t>Mega Houndoom and Mega Absol in Mega Raids</t>
         </is>
       </c>
       <c r="F386" t="inlineStr">
@@ -16367,7 +16367,7 @@
       <c r="O386" t="inlineStr"/>
       <c r="P386" t="inlineStr">
         <is>
-          <t>Raid Battles Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Raid Battles Mega Houndoom and Mega Absol in Mega Raids Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q386" t="inlineStr">
@@ -16387,7 +16387,7 @@
       <c r="D387" t="inlineStr"/>
       <c r="E387" t="inlineStr">
         <is>
-          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles</t>
+          <t>Mega Houndoom and Mega Absol in Mega Raids</t>
         </is>
       </c>
       <c r="F387" t="inlineStr">
@@ -16406,7 +16406,7 @@
       <c r="O387" t="inlineStr"/>
       <c r="P387" t="inlineStr">
         <is>
-          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Mega Houndoom and Mega Absol in Mega Raids Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q387" t="inlineStr">
@@ -16426,7 +16426,7 @@
       <c r="D388" t="inlineStr"/>
       <c r="E388" t="inlineStr">
         <is>
-          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles</t>
+          <t>Mega Houndoom and Mega Absol in Mega Raids</t>
         </is>
       </c>
       <c r="F388" t="inlineStr">
@@ -16445,7 +16445,7 @@
       <c r="O388" t="inlineStr"/>
       <c r="P388" t="inlineStr">
         <is>
-          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Mega Houndoom and Mega Absol in Mega Raids Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q388" t="inlineStr">
@@ -16465,7 +16465,7 @@
       <c r="D389" t="inlineStr"/>
       <c r="E389" t="inlineStr">
         <is>
-          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles</t>
+          <t>Mega Houndoom and Mega Absol in Mega Raids</t>
         </is>
       </c>
       <c r="F389" t="inlineStr">
@@ -16484,7 +16484,7 @@
       <c r="O389" t="inlineStr"/>
       <c r="P389" t="inlineStr">
         <is>
-          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles Tue, Oct 21, at 10:00 AM Local Time</t>
+          <t>Mega Houndoom and Mega Absol in Mega Raids Tue, Oct 21, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q389" t="inlineStr">
@@ -16504,12 +16504,12 @@
       <c r="D390" t="inlineStr"/>
       <c r="E390" t="inlineStr">
         <is>
-          <t>Mega Houndoom and Mega Absol in Mega Raids</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F390" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G390" t="inlineStr"/>
@@ -16523,7 +16523,7 @@
       <c r="O390" t="inlineStr"/>
       <c r="P390" t="inlineStr">
         <is>
-          <t>Raid Battles Mega Houndoom and Mega Absol in Mega Raids Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>GO Battle League Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q390" t="inlineStr">
@@ -16543,12 +16543,12 @@
       <c r="D391" t="inlineStr"/>
       <c r="E391" t="inlineStr">
         <is>
-          <t>Mega Houndoom and Mega Absol in Mega Raids</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F391" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G391" t="inlineStr"/>
@@ -16562,7 +16562,7 @@
       <c r="O391" t="inlineStr"/>
       <c r="P391" t="inlineStr">
         <is>
-          <t>Mega Houndoom and Mega Absol in Mega Raids Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q391" t="inlineStr">
@@ -16582,12 +16582,12 @@
       <c r="D392" t="inlineStr"/>
       <c r="E392" t="inlineStr">
         <is>
-          <t>Mega Houndoom and Mega Absol in Mega Raids</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F392" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G392" t="inlineStr"/>
@@ -16601,7 +16601,7 @@
       <c r="O392" t="inlineStr"/>
       <c r="P392" t="inlineStr">
         <is>
-          <t>Mega Houndoom and Mega Absol in Mega Raids Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q392" t="inlineStr">
@@ -16621,12 +16621,12 @@
       <c r="D393" t="inlineStr"/>
       <c r="E393" t="inlineStr">
         <is>
-          <t>Mega Houndoom and Mega Absol in Mega Raids</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F393" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G393" t="inlineStr"/>
@@ -16640,7 +16640,7 @@
       <c r="O393" t="inlineStr"/>
       <c r="P393" t="inlineStr">
         <is>
-          <t>Mega Houndoom and Mega Absol in Mega Raids Tue, Oct 21, at 10:00 AM Local Time</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q393" t="inlineStr">
@@ -16660,12 +16660,12 @@
       <c r="D394" t="inlineStr"/>
       <c r="E394" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Gastly Spotlight Hour</t>
         </is>
       </c>
       <c r="F394" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G394" t="inlineStr"/>
@@ -16679,7 +16679,7 @@
       <c r="O394" t="inlineStr"/>
       <c r="P394" t="inlineStr">
         <is>
-          <t>GO Battle League Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Pokémon Spotlight Hour Gastly Spotlight Hour Tue, Oct 21, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q394" t="inlineStr">
@@ -16699,12 +16699,12 @@
       <c r="D395" t="inlineStr"/>
       <c r="E395" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Gastly Spotlight Hour</t>
         </is>
       </c>
       <c r="F395" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G395" t="inlineStr"/>
@@ -16718,7 +16718,7 @@
       <c r="O395" t="inlineStr"/>
       <c r="P395" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Gastly Spotlight Hour Tue, Oct 21, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q395" t="inlineStr">
@@ -16738,12 +16738,12 @@
       <c r="D396" t="inlineStr"/>
       <c r="E396" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Gastly Spotlight Hour</t>
         </is>
       </c>
       <c r="F396" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G396" t="inlineStr"/>
@@ -16757,7 +16757,7 @@
       <c r="O396" t="inlineStr"/>
       <c r="P396" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Gastly Spotlight Hour Tue, Oct 21, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q396" t="inlineStr">
@@ -16777,12 +16777,12 @@
       <c r="D397" t="inlineStr"/>
       <c r="E397" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Gastly Spotlight Hour</t>
         </is>
       </c>
       <c r="F397" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G397" t="inlineStr"/>
@@ -16796,7 +16796,7 @@
       <c r="O397" t="inlineStr"/>
       <c r="P397" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating...</t>
+          <t>Gastly Spotlight Hour Tue, Oct 21, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q397" t="inlineStr">
@@ -16816,12 +16816,12 @@
       <c r="D398" t="inlineStr"/>
       <c r="E398" t="inlineStr">
         <is>
-          <t>Gastly Spotlight Hour</t>
+          <t>Genesect Raid Hour</t>
         </is>
       </c>
       <c r="F398" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G398" t="inlineStr"/>
@@ -16835,7 +16835,7 @@
       <c r="O398" t="inlineStr"/>
       <c r="P398" t="inlineStr">
         <is>
-          <t>Pokémon Spotlight Hour Gastly Spotlight Hour Tue, Oct 21, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Raid Hour Genesect Raid Hour Wed, Oct 22, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q398" t="inlineStr">
@@ -16855,12 +16855,12 @@
       <c r="D399" t="inlineStr"/>
       <c r="E399" t="inlineStr">
         <is>
-          <t>Gastly Spotlight Hour</t>
+          <t>Genesect Raid Hour</t>
         </is>
       </c>
       <c r="F399" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G399" t="inlineStr"/>
@@ -16874,7 +16874,7 @@
       <c r="O399" t="inlineStr"/>
       <c r="P399" t="inlineStr">
         <is>
-          <t>Gastly Spotlight Hour Tue, Oct 21, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Genesect Raid Hour Wed, Oct 22, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q399" t="inlineStr">
@@ -16894,12 +16894,12 @@
       <c r="D400" t="inlineStr"/>
       <c r="E400" t="inlineStr">
         <is>
-          <t>Gastly Spotlight Hour</t>
+          <t>Genesect Raid Hour</t>
         </is>
       </c>
       <c r="F400" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G400" t="inlineStr"/>
@@ -16913,7 +16913,7 @@
       <c r="O400" t="inlineStr"/>
       <c r="P400" t="inlineStr">
         <is>
-          <t>Gastly Spotlight Hour Tue, Oct 21, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Genesect Raid Hour Wed, Oct 22, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q400" t="inlineStr">
@@ -16933,12 +16933,12 @@
       <c r="D401" t="inlineStr"/>
       <c r="E401" t="inlineStr">
         <is>
-          <t>Gastly Spotlight Hour</t>
+          <t>Genesect Raid Hour</t>
         </is>
       </c>
       <c r="F401" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G401" t="inlineStr"/>
@@ -16952,7 +16952,7 @@
       <c r="O401" t="inlineStr"/>
       <c r="P401" t="inlineStr">
         <is>
-          <t>Gastly Spotlight Hour Tue, Oct 21, at 6:00 PM Local Time</t>
+          <t>Genesect Raid Hour Wed, Oct 22, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q401" t="inlineStr">
@@ -16972,12 +16972,12 @@
       <c r="D402" t="inlineStr"/>
       <c r="E402" t="inlineStr">
         <is>
-          <t>Genesect Raid Hour</t>
+          <t>GO Battle Weekend: Tales of Transformation</t>
         </is>
       </c>
       <c r="F402" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G402" t="inlineStr"/>
@@ -16991,7 +16991,7 @@
       <c r="O402" t="inlineStr"/>
       <c r="P402" t="inlineStr">
         <is>
-          <t>Raid Hour Genesect Raid Hour Wed, Oct 22, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Event GO Battle Weekend: Tales of Transformation Sat, Oct 25, at 12:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q402" t="inlineStr">
@@ -17011,12 +17011,12 @@
       <c r="D403" t="inlineStr"/>
       <c r="E403" t="inlineStr">
         <is>
-          <t>Genesect Raid Hour</t>
+          <t>GO Battle Weekend: Tales of Transformation</t>
         </is>
       </c>
       <c r="F403" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G403" t="inlineStr"/>
@@ -17030,7 +17030,7 @@
       <c r="O403" t="inlineStr"/>
       <c r="P403" t="inlineStr">
         <is>
-          <t>Genesect Raid Hour Wed, Oct 22, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>GO Battle Weekend: Tales of Transformation Sat, Oct 25, at 12:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q403" t="inlineStr">
@@ -17050,12 +17050,12 @@
       <c r="D404" t="inlineStr"/>
       <c r="E404" t="inlineStr">
         <is>
-          <t>Genesect Raid Hour</t>
+          <t>GO Battle Weekend: Tales of Transformation</t>
         </is>
       </c>
       <c r="F404" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G404" t="inlineStr"/>
@@ -17069,7 +17069,7 @@
       <c r="O404" t="inlineStr"/>
       <c r="P404" t="inlineStr">
         <is>
-          <t>Genesect Raid Hour Wed, Oct 22, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>GO Battle Weekend: Tales of Transformation Sat, Oct 25, at 12:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q404" t="inlineStr">
@@ -17089,12 +17089,12 @@
       <c r="D405" t="inlineStr"/>
       <c r="E405" t="inlineStr">
         <is>
-          <t>Genesect Raid Hour</t>
+          <t>GO Battle Weekend: Tales of Transformation</t>
         </is>
       </c>
       <c r="F405" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G405" t="inlineStr"/>
@@ -17108,7 +17108,7 @@
       <c r="O405" t="inlineStr"/>
       <c r="P405" t="inlineStr">
         <is>
-          <t>Genesect Raid Hour Wed, Oct 22, at 6:00 PM Local Time</t>
+          <t>GO Battle Weekend: Tales of Transformation Sat, Oct 25, at 12:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q405" t="inlineStr">
@@ -17128,7 +17128,7 @@
       <c r="D406" t="inlineStr"/>
       <c r="E406" t="inlineStr">
         <is>
-          <t>GO Battle Weekend: Tales of Transformation</t>
+          <t>Halloween 2025 Part II</t>
         </is>
       </c>
       <c r="F406" t="inlineStr">
@@ -17147,7 +17147,7 @@
       <c r="O406" t="inlineStr"/>
       <c r="P406" t="inlineStr">
         <is>
-          <t>Event GO Battle Weekend: Tales of Transformation Sat, Oct 25, at 12:00 AM Local Time Starts: Calculating...</t>
+          <t>Event Halloween 2025 Part II Mon, Oct 27, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q406" t="inlineStr">
@@ -17167,7 +17167,7 @@
       <c r="D407" t="inlineStr"/>
       <c r="E407" t="inlineStr">
         <is>
-          <t>GO Battle Weekend: Tales of Transformation</t>
+          <t>Halloween 2025 Part II</t>
         </is>
       </c>
       <c r="F407" t="inlineStr">
@@ -17186,7 +17186,7 @@
       <c r="O407" t="inlineStr"/>
       <c r="P407" t="inlineStr">
         <is>
-          <t>GO Battle Weekend: Tales of Transformation Sat, Oct 25, at 12:00 AM Local Time Starts: Calculating...</t>
+          <t>Halloween 2025 Part II Mon, Oct 27, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q407" t="inlineStr">
@@ -17206,7 +17206,7 @@
       <c r="D408" t="inlineStr"/>
       <c r="E408" t="inlineStr">
         <is>
-          <t>GO Battle Weekend: Tales of Transformation</t>
+          <t>Halloween 2025 Part II</t>
         </is>
       </c>
       <c r="F408" t="inlineStr">
@@ -17225,7 +17225,7 @@
       <c r="O408" t="inlineStr"/>
       <c r="P408" t="inlineStr">
         <is>
-          <t>GO Battle Weekend: Tales of Transformation Sat, Oct 25, at 12:00 AM Local Time Starts: Calculating...</t>
+          <t>Halloween 2025 Part II Mon, Oct 27, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q408" t="inlineStr">
@@ -17245,7 +17245,7 @@
       <c r="D409" t="inlineStr"/>
       <c r="E409" t="inlineStr">
         <is>
-          <t>GO Battle Weekend: Tales of Transformation</t>
+          <t>Halloween 2025 Part II</t>
         </is>
       </c>
       <c r="F409" t="inlineStr">
@@ -17264,7 +17264,7 @@
       <c r="O409" t="inlineStr"/>
       <c r="P409" t="inlineStr">
         <is>
-          <t>GO Battle Weekend: Tales of Transformation Sat, Oct 25, at 12:00 AM Local Time</t>
+          <t>Halloween 2025 Part II Mon, Oct 27, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q409" t="inlineStr">
@@ -17284,7 +17284,7 @@
       <c r="D410" t="inlineStr"/>
       <c r="E410" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part II</t>
+          <t>Dynamax Woobat during Max Monday</t>
         </is>
       </c>
       <c r="F410" t="inlineStr">
@@ -17303,7 +17303,7 @@
       <c r="O410" t="inlineStr"/>
       <c r="P410" t="inlineStr">
         <is>
-          <t>Event Halloween 2025 Part II Mon, Oct 27, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Max Mondays Dynamax Woobat during Max Monday Mon, Oct 27, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q410" t="inlineStr">
@@ -17323,7 +17323,7 @@
       <c r="D411" t="inlineStr"/>
       <c r="E411" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part II</t>
+          <t>Dynamax Woobat during Max Monday</t>
         </is>
       </c>
       <c r="F411" t="inlineStr">
@@ -17342,7 +17342,7 @@
       <c r="O411" t="inlineStr"/>
       <c r="P411" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part II Mon, Oct 27, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Dynamax Woobat during Max Monday Mon, Oct 27, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q411" t="inlineStr">
@@ -17362,7 +17362,7 @@
       <c r="D412" t="inlineStr"/>
       <c r="E412" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part II</t>
+          <t>Dynamax Woobat during Max Monday</t>
         </is>
       </c>
       <c r="F412" t="inlineStr">
@@ -17381,7 +17381,7 @@
       <c r="O412" t="inlineStr"/>
       <c r="P412" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part II Mon, Oct 27, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Dynamax Woobat during Max Monday Mon, Oct 27, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q412" t="inlineStr">
@@ -17401,7 +17401,7 @@
       <c r="D413" t="inlineStr"/>
       <c r="E413" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part II</t>
+          <t>Dynamax Woobat during Max Monday</t>
         </is>
       </c>
       <c r="F413" t="inlineStr">
@@ -17420,7 +17420,7 @@
       <c r="O413" t="inlineStr"/>
       <c r="P413" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part II Mon, Oct 27, at 10:00 AM Local Time</t>
+          <t>Dynamax Woobat during Max Monday Mon, Oct 27, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q413" t="inlineStr">
@@ -17440,12 +17440,12 @@
       <c r="D414" t="inlineStr"/>
       <c r="E414" t="inlineStr">
         <is>
-          <t>Dynamax Woobat during Max Monday</t>
+          <t>Giratina (Altered Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F414" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G414" t="inlineStr"/>
@@ -17459,7 +17459,7 @@
       <c r="O414" t="inlineStr"/>
       <c r="P414" t="inlineStr">
         <is>
-          <t>Max Mondays Dynamax Woobat during Max Monday Mon, Oct 27, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Raid Battles Giratina (Altered Forme) in 5-star Raid Battles Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q414" t="inlineStr">
@@ -17479,12 +17479,12 @@
       <c r="D415" t="inlineStr"/>
       <c r="E415" t="inlineStr">
         <is>
-          <t>Dynamax Woobat during Max Monday</t>
+          <t>Giratina (Altered Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F415" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G415" t="inlineStr"/>
@@ -17498,7 +17498,7 @@
       <c r="O415" t="inlineStr"/>
       <c r="P415" t="inlineStr">
         <is>
-          <t>Dynamax Woobat during Max Monday Mon, Oct 27, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Giratina (Altered Forme) in 5-star Raid Battles Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q415" t="inlineStr">
@@ -17518,12 +17518,12 @@
       <c r="D416" t="inlineStr"/>
       <c r="E416" t="inlineStr">
         <is>
-          <t>Dynamax Woobat during Max Monday</t>
+          <t>Giratina (Altered Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F416" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G416" t="inlineStr"/>
@@ -17537,7 +17537,7 @@
       <c r="O416" t="inlineStr"/>
       <c r="P416" t="inlineStr">
         <is>
-          <t>Dynamax Woobat during Max Monday Mon, Oct 27, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Giratina (Altered Forme) in 5-star Raid Battles Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q416" t="inlineStr">
@@ -17557,12 +17557,12 @@
       <c r="D417" t="inlineStr"/>
       <c r="E417" t="inlineStr">
         <is>
-          <t>Dynamax Woobat during Max Monday</t>
+          <t>Giratina (Altered Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F417" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G417" t="inlineStr"/>
@@ -17576,7 +17576,7 @@
       <c r="O417" t="inlineStr"/>
       <c r="P417" t="inlineStr">
         <is>
-          <t>Dynamax Woobat during Max Monday Mon, Oct 27, at 6:00 PM Local Time</t>
+          <t>Giratina (Altered Forme) in 5-star Raid Battles Tue, Oct 28, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q417" t="inlineStr">
@@ -17596,7 +17596,7 @@
       <c r="D418" t="inlineStr"/>
       <c r="E418" t="inlineStr">
         <is>
-          <t>Giratina (Altered Forme) in 5-star Raid Battles</t>
+          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids</t>
         </is>
       </c>
       <c r="F418" t="inlineStr">
@@ -17615,7 +17615,7 @@
       <c r="O418" t="inlineStr"/>
       <c r="P418" t="inlineStr">
         <is>
-          <t>Raid Battles Giratina (Altered Forme) in 5-star Raid Battles Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Raid Battles Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q418" t="inlineStr">
@@ -17635,7 +17635,7 @@
       <c r="D419" t="inlineStr"/>
       <c r="E419" t="inlineStr">
         <is>
-          <t>Giratina (Altered Forme) in 5-star Raid Battles</t>
+          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids</t>
         </is>
       </c>
       <c r="F419" t="inlineStr">
@@ -17654,7 +17654,7 @@
       <c r="O419" t="inlineStr"/>
       <c r="P419" t="inlineStr">
         <is>
-          <t>Giratina (Altered Forme) in 5-star Raid Battles Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q419" t="inlineStr">
@@ -17674,7 +17674,7 @@
       <c r="D420" t="inlineStr"/>
       <c r="E420" t="inlineStr">
         <is>
-          <t>Giratina (Altered Forme) in 5-star Raid Battles</t>
+          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids</t>
         </is>
       </c>
       <c r="F420" t="inlineStr">
@@ -17693,7 +17693,7 @@
       <c r="O420" t="inlineStr"/>
       <c r="P420" t="inlineStr">
         <is>
-          <t>Giratina (Altered Forme) in 5-star Raid Battles Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q420" t="inlineStr">
@@ -17713,7 +17713,7 @@
       <c r="D421" t="inlineStr"/>
       <c r="E421" t="inlineStr">
         <is>
-          <t>Giratina (Altered Forme) in 5-star Raid Battles</t>
+          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids</t>
         </is>
       </c>
       <c r="F421" t="inlineStr">
@@ -17732,7 +17732,7 @@
       <c r="O421" t="inlineStr"/>
       <c r="P421" t="inlineStr">
         <is>
-          <t>Giratina (Altered Forme) in 5-star Raid Battles Tue, Oct 28, at 10:00 AM Local Time</t>
+          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids Tue, Oct 28, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q421" t="inlineStr">
@@ -17752,12 +17752,12 @@
       <c r="D422" t="inlineStr"/>
       <c r="E422" t="inlineStr">
         <is>
-          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids</t>
+          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F422" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G422" t="inlineStr"/>
@@ -17771,7 +17771,7 @@
       <c r="O422" t="inlineStr"/>
       <c r="P422" t="inlineStr">
         <is>
-          <t>Raid Battles Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>GO Battle League Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q422" t="inlineStr">
@@ -17791,12 +17791,12 @@
       <c r="D423" t="inlineStr"/>
       <c r="E423" t="inlineStr">
         <is>
-          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids</t>
+          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F423" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G423" t="inlineStr"/>
@@ -17810,7 +17810,7 @@
       <c r="O423" t="inlineStr"/>
       <c r="P423" t="inlineStr">
         <is>
-          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q423" t="inlineStr">
@@ -17830,12 +17830,12 @@
       <c r="D424" t="inlineStr"/>
       <c r="E424" t="inlineStr">
         <is>
-          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids</t>
+          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F424" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G424" t="inlineStr"/>
@@ -17849,7 +17849,7 @@
       <c r="O424" t="inlineStr"/>
       <c r="P424" t="inlineStr">
         <is>
-          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q424" t="inlineStr">
@@ -17869,12 +17869,12 @@
       <c r="D425" t="inlineStr"/>
       <c r="E425" t="inlineStr">
         <is>
-          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids</t>
+          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F425" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G425" t="inlineStr"/>
@@ -17888,7 +17888,7 @@
       <c r="O425" t="inlineStr"/>
       <c r="P425" t="inlineStr">
         <is>
-          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids Tue, Oct 28, at 10:00 AM Local Time</t>
+          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q425" t="inlineStr">
@@ -17908,12 +17908,12 @@
       <c r="D426" t="inlineStr"/>
       <c r="E426" t="inlineStr">
         <is>
-          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation</t>
+          <t>Sinistea Spotlight Hour</t>
         </is>
       </c>
       <c r="F426" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G426" t="inlineStr"/>
@@ -17927,7 +17927,7 @@
       <c r="O426" t="inlineStr"/>
       <c r="P426" t="inlineStr">
         <is>
-          <t>GO Battle League Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Pokémon Spotlight Hour Sinistea Spotlight Hour Tue, Oct 28, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q426" t="inlineStr">
@@ -17947,12 +17947,12 @@
       <c r="D427" t="inlineStr"/>
       <c r="E427" t="inlineStr">
         <is>
-          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation</t>
+          <t>Sinistea Spotlight Hour</t>
         </is>
       </c>
       <c r="F427" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G427" t="inlineStr"/>
@@ -17966,7 +17966,7 @@
       <c r="O427" t="inlineStr"/>
       <c r="P427" t="inlineStr">
         <is>
-          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Sinistea Spotlight Hour Tue, Oct 28, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q427" t="inlineStr">
@@ -17986,12 +17986,12 @@
       <c r="D428" t="inlineStr"/>
       <c r="E428" t="inlineStr">
         <is>
-          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation</t>
+          <t>Sinistea Spotlight Hour</t>
         </is>
       </c>
       <c r="F428" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G428" t="inlineStr"/>
@@ -18005,7 +18005,7 @@
       <c r="O428" t="inlineStr"/>
       <c r="P428" t="inlineStr">
         <is>
-          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Sinistea Spotlight Hour Tue, Oct 28, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q428" t="inlineStr">
@@ -18025,12 +18025,12 @@
       <c r="D429" t="inlineStr"/>
       <c r="E429" t="inlineStr">
         <is>
-          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation</t>
+          <t>Sinistea Spotlight Hour</t>
         </is>
       </c>
       <c r="F429" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G429" t="inlineStr"/>
@@ -18044,7 +18044,7 @@
       <c r="O429" t="inlineStr"/>
       <c r="P429" t="inlineStr">
         <is>
-          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating...</t>
+          <t>Sinistea Spotlight Hour Tue, Oct 28, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q429" t="inlineStr">
@@ -18064,12 +18064,12 @@
       <c r="D430" t="inlineStr"/>
       <c r="E430" t="inlineStr">
         <is>
-          <t>Sinistea Spotlight Hour</t>
+          <t>Giratina (Origin Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F430" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G430" t="inlineStr"/>
@@ -18083,7 +18083,7 @@
       <c r="O430" t="inlineStr"/>
       <c r="P430" t="inlineStr">
         <is>
-          <t>Pokémon Spotlight Hour Sinistea Spotlight Hour Tue, Oct 28, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Raid Hour Giratina (Origin Forme) Raid Hour Wed, Oct 29, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q430" t="inlineStr">
@@ -18103,12 +18103,12 @@
       <c r="D431" t="inlineStr"/>
       <c r="E431" t="inlineStr">
         <is>
-          <t>Sinistea Spotlight Hour</t>
+          <t>Giratina (Origin Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F431" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G431" t="inlineStr"/>
@@ -18122,7 +18122,7 @@
       <c r="O431" t="inlineStr"/>
       <c r="P431" t="inlineStr">
         <is>
-          <t>Sinistea Spotlight Hour Tue, Oct 28, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Giratina (Origin Forme) Raid Hour Wed, Oct 29, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q431" t="inlineStr">
@@ -18142,12 +18142,12 @@
       <c r="D432" t="inlineStr"/>
       <c r="E432" t="inlineStr">
         <is>
-          <t>Sinistea Spotlight Hour</t>
+          <t>Giratina (Origin Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F432" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G432" t="inlineStr"/>
@@ -18161,7 +18161,7 @@
       <c r="O432" t="inlineStr"/>
       <c r="P432" t="inlineStr">
         <is>
-          <t>Sinistea Spotlight Hour Tue, Oct 28, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Giratina (Origin Forme) Raid Hour Wed, Oct 29, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q432" t="inlineStr">
@@ -18181,12 +18181,12 @@
       <c r="D433" t="inlineStr"/>
       <c r="E433" t="inlineStr">
         <is>
-          <t>Sinistea Spotlight Hour</t>
+          <t>Giratina (Origin Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F433" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G433" t="inlineStr"/>
@@ -18200,7 +18200,7 @@
       <c r="O433" t="inlineStr"/>
       <c r="P433" t="inlineStr">
         <is>
-          <t>Sinistea Spotlight Hour Tue, Oct 28, at 6:00 PM Local Time</t>
+          <t>Giratina (Origin Forme) Raid Hour Wed, Oct 29, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q433" t="inlineStr">
@@ -18220,12 +18220,12 @@
       <c r="D434" t="inlineStr"/>
       <c r="E434" t="inlineStr">
         <is>
-          <t>Giratina (Origin Forme) Raid Hour</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F434" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G434" t="inlineStr"/>
@@ -18239,7 +18239,7 @@
       <c r="O434" t="inlineStr"/>
       <c r="P434" t="inlineStr">
         <is>
-          <t>Raid Hour Giratina (Origin Forme) Raid Hour Wed, Oct 29, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>GO Battle League Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q434" t="inlineStr">
@@ -18259,12 +18259,12 @@
       <c r="D435" t="inlineStr"/>
       <c r="E435" t="inlineStr">
         <is>
-          <t>Giratina (Origin Forme) Raid Hour</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F435" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G435" t="inlineStr"/>
@@ -18278,7 +18278,7 @@
       <c r="O435" t="inlineStr"/>
       <c r="P435" t="inlineStr">
         <is>
-          <t>Giratina (Origin Forme) Raid Hour Wed, Oct 29, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q435" t="inlineStr">
@@ -18298,12 +18298,12 @@
       <c r="D436" t="inlineStr"/>
       <c r="E436" t="inlineStr">
         <is>
-          <t>Giratina (Origin Forme) Raid Hour</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F436" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G436" t="inlineStr"/>
@@ -18317,7 +18317,7 @@
       <c r="O436" t="inlineStr"/>
       <c r="P436" t="inlineStr">
         <is>
-          <t>Giratina (Origin Forme) Raid Hour Wed, Oct 29, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q436" t="inlineStr">
@@ -18337,12 +18337,12 @@
       <c r="D437" t="inlineStr"/>
       <c r="E437" t="inlineStr">
         <is>
-          <t>Giratina (Origin Forme) Raid Hour</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F437" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G437" t="inlineStr"/>
@@ -18356,7 +18356,7 @@
       <c r="O437" t="inlineStr"/>
       <c r="P437" t="inlineStr">
         <is>
-          <t>Giratina (Origin Forme) Raid Hour Wed, Oct 29, at 6:00 PM Local Time</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q437" t="inlineStr">
@@ -18376,7 +18376,7 @@
       <c r="D438" t="inlineStr"/>
       <c r="E438" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
+          <t>Pokémon GO Wild Area: Nagasaki</t>
         </is>
       </c>
       <c r="F438" t="inlineStr">
@@ -18395,7 +18395,7 @@
       <c r="O438" t="inlineStr"/>
       <c r="P438" t="inlineStr">
         <is>
-          <t>GO Battle League Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Wild Area Pokémon GO Wild Area: Nagasaki Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q438" t="inlineStr">
@@ -18415,7 +18415,7 @@
       <c r="D439" t="inlineStr"/>
       <c r="E439" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
+          <t>Pokémon GO Wild Area: Nagasaki</t>
         </is>
       </c>
       <c r="F439" t="inlineStr">
@@ -18434,7 +18434,7 @@
       <c r="O439" t="inlineStr"/>
       <c r="P439" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Pokémon GO Wild Area: Nagasaki Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q439" t="inlineStr">
@@ -18454,7 +18454,7 @@
       <c r="D440" t="inlineStr"/>
       <c r="E440" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
+          <t>Pokémon GO Wild Area: Nagasaki</t>
         </is>
       </c>
       <c r="F440" t="inlineStr">
@@ -18473,7 +18473,7 @@
       <c r="O440" t="inlineStr"/>
       <c r="P440" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Pokémon GO Wild Area: Nagasaki Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q440" t="inlineStr">
@@ -18493,7 +18493,7 @@
       <c r="D441" t="inlineStr"/>
       <c r="E441" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
+          <t>Pokémon GO Wild Area: Nagasaki</t>
         </is>
       </c>
       <c r="F441" t="inlineStr">
@@ -18512,7 +18512,7 @@
       <c r="O441" t="inlineStr"/>
       <c r="P441" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating...</t>
+          <t>Pokémon GO Wild Area: Nagasaki Calculating...</t>
         </is>
       </c>
       <c r="Q441" t="inlineStr">
@@ -18532,7 +18532,7 @@
       <c r="D442" t="inlineStr"/>
       <c r="E442" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Nagasaki</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F442" t="inlineStr">
@@ -18551,7 +18551,7 @@
       <c r="O442" t="inlineStr"/>
       <c r="P442" t="inlineStr">
         <is>
-          <t>Wild Area Pokémon GO Wild Area: Nagasaki Calculating... Starts: Calculating...</t>
+          <t>GO Battle League Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q442" t="inlineStr">
@@ -18571,7 +18571,7 @@
       <c r="D443" t="inlineStr"/>
       <c r="E443" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Nagasaki</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F443" t="inlineStr">
@@ -18590,7 +18590,7 @@
       <c r="O443" t="inlineStr"/>
       <c r="P443" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Nagasaki Calculating... Starts: Calculating...</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q443" t="inlineStr">
@@ -18610,7 +18610,7 @@
       <c r="D444" t="inlineStr"/>
       <c r="E444" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Nagasaki</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F444" t="inlineStr">
@@ -18629,7 +18629,7 @@
       <c r="O444" t="inlineStr"/>
       <c r="P444" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Nagasaki Calculating... Starts: Calculating...</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q444" t="inlineStr">
@@ -18649,7 +18649,7 @@
       <c r="D445" t="inlineStr"/>
       <c r="E445" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Nagasaki</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F445" t="inlineStr">
@@ -18668,7 +18668,7 @@
       <c r="O445" t="inlineStr"/>
       <c r="P445" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Nagasaki Calculating...</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q445" t="inlineStr">
@@ -18688,7 +18688,7 @@
       <c r="D446" t="inlineStr"/>
       <c r="E446" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Pokémon GO Wild Area: Global</t>
         </is>
       </c>
       <c r="F446" t="inlineStr">
@@ -18707,7 +18707,7 @@
       <c r="O446" t="inlineStr"/>
       <c r="P446" t="inlineStr">
         <is>
-          <t>GO Battle League Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Wild Area Pokémon GO Wild Area: Global Sat, Nov 15, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q446" t="inlineStr">
@@ -18727,7 +18727,7 @@
       <c r="D447" t="inlineStr"/>
       <c r="E447" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Pokémon GO Wild Area: Global</t>
         </is>
       </c>
       <c r="F447" t="inlineStr">
@@ -18746,7 +18746,7 @@
       <c r="O447" t="inlineStr"/>
       <c r="P447" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Pokémon GO Wild Area: Global Sat, Nov 15, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q447" t="inlineStr">
@@ -18766,7 +18766,7 @@
       <c r="D448" t="inlineStr"/>
       <c r="E448" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Pokémon GO Wild Area: Global</t>
         </is>
       </c>
       <c r="F448" t="inlineStr">
@@ -18785,7 +18785,7 @@
       <c r="O448" t="inlineStr"/>
       <c r="P448" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Pokémon GO Wild Area: Global Sat, Nov 15, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q448" t="inlineStr">
@@ -18805,7 +18805,7 @@
       <c r="D449" t="inlineStr"/>
       <c r="E449" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Pokémon GO Wild Area: Global</t>
         </is>
       </c>
       <c r="F449" t="inlineStr">
@@ -18824,7 +18824,7 @@
       <c r="O449" t="inlineStr"/>
       <c r="P449" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating...</t>
+          <t>Pokémon GO Wild Area: Global Sat, Nov 15, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q449" t="inlineStr">
@@ -18844,12 +18844,12 @@
       <c r="D450" t="inlineStr"/>
       <c r="E450" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Global</t>
+          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F450" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G450" t="inlineStr"/>
@@ -18863,7 +18863,7 @@
       <c r="O450" t="inlineStr"/>
       <c r="P450" t="inlineStr">
         <is>
-          <t>Wild Area Pokémon GO Wild Area: Global Sat, Nov 15, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>GO Battle League 2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q450" t="inlineStr">
@@ -18883,12 +18883,12 @@
       <c r="D451" t="inlineStr"/>
       <c r="E451" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Global</t>
+          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F451" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G451" t="inlineStr"/>
@@ -18902,7 +18902,7 @@
       <c r="O451" t="inlineStr"/>
       <c r="P451" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Global Sat, Nov 15, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q451" t="inlineStr">
@@ -18922,12 +18922,12 @@
       <c r="D452" t="inlineStr"/>
       <c r="E452" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Global</t>
+          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F452" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G452" t="inlineStr"/>
@@ -18941,7 +18941,7 @@
       <c r="O452" t="inlineStr"/>
       <c r="P452" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Global Sat, Nov 15, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q452" t="inlineStr">
@@ -18961,12 +18961,12 @@
       <c r="D453" t="inlineStr"/>
       <c r="E453" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Global</t>
+          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F453" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G453" t="inlineStr"/>
@@ -18980,7 +18980,7 @@
       <c r="O453" t="inlineStr"/>
       <c r="P453" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Global Sat, Nov 15, at 10:00 AM Local Time</t>
+          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q453" t="inlineStr">
@@ -19000,12 +19000,12 @@
       <c r="D454" t="inlineStr"/>
       <c r="E454" t="inlineStr">
         <is>
-          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation</t>
+          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F454" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G454" t="inlineStr"/>
@@ -19019,7 +19019,7 @@
       <c r="O454" t="inlineStr"/>
       <c r="P454" t="inlineStr">
         <is>
-          <t>GO Battle League 2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>GO Battle League Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q454" t="inlineStr">
@@ -19039,12 +19039,12 @@
       <c r="D455" t="inlineStr"/>
       <c r="E455" t="inlineStr">
         <is>
-          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation</t>
+          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F455" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G455" t="inlineStr"/>
@@ -19058,7 +19058,7 @@
       <c r="O455" t="inlineStr"/>
       <c r="P455" t="inlineStr">
         <is>
-          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q455" t="inlineStr">
@@ -19078,12 +19078,12 @@
       <c r="D456" t="inlineStr"/>
       <c r="E456" t="inlineStr">
         <is>
-          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation</t>
+          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F456" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G456" t="inlineStr"/>
@@ -19097,7 +19097,7 @@
       <c r="O456" t="inlineStr"/>
       <c r="P456" t="inlineStr">
         <is>
-          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q456" t="inlineStr">
@@ -19117,12 +19117,12 @@
       <c r="D457" t="inlineStr"/>
       <c r="E457" t="inlineStr">
         <is>
-          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation</t>
+          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F457" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G457" t="inlineStr"/>
@@ -19136,7 +19136,7 @@
       <c r="O457" t="inlineStr"/>
       <c r="P457" t="inlineStr">
         <is>
-          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating...</t>
+          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q457" t="inlineStr">
@@ -19156,12 +19156,12 @@
       <c r="D458" t="inlineStr"/>
       <c r="E458" t="inlineStr">
         <is>
-          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation</t>
+          <t>November Community Day</t>
         </is>
       </c>
       <c r="F458" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Community Day</t>
         </is>
       </c>
       <c r="G458" t="inlineStr"/>
@@ -19175,7 +19175,7 @@
       <c r="O458" t="inlineStr"/>
       <c r="P458" t="inlineStr">
         <is>
-          <t>GO Battle League Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Community Day November Community Day Sun, Nov 30, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q458" t="inlineStr">
@@ -19195,12 +19195,12 @@
       <c r="D459" t="inlineStr"/>
       <c r="E459" t="inlineStr">
         <is>
-          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation</t>
+          <t>November Community Day</t>
         </is>
       </c>
       <c r="F459" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Community Day</t>
         </is>
       </c>
       <c r="G459" t="inlineStr"/>
@@ -19214,7 +19214,7 @@
       <c r="O459" t="inlineStr"/>
       <c r="P459" t="inlineStr">
         <is>
-          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>November Community Day Sun, Nov 30, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q459" t="inlineStr">
@@ -19234,12 +19234,12 @@
       <c r="D460" t="inlineStr"/>
       <c r="E460" t="inlineStr">
         <is>
-          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation</t>
+          <t>November Community Day</t>
         </is>
       </c>
       <c r="F460" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Community Day</t>
         </is>
       </c>
       <c r="G460" t="inlineStr"/>
@@ -19253,7 +19253,7 @@
       <c r="O460" t="inlineStr"/>
       <c r="P460" t="inlineStr">
         <is>
-          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>November Community Day Sun, Nov 30, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q460" t="inlineStr">
@@ -19273,12 +19273,12 @@
       <c r="D461" t="inlineStr"/>
       <c r="E461" t="inlineStr">
         <is>
-          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation</t>
+          <t>November Community Day</t>
         </is>
       </c>
       <c r="F461" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Community Day</t>
         </is>
       </c>
       <c r="G461" t="inlineStr"/>
@@ -19292,7 +19292,7 @@
       <c r="O461" t="inlineStr"/>
       <c r="P461" t="inlineStr">
         <is>
-          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating...</t>
+          <t>November Community Day Sun, Nov 30, at 2:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q461" t="inlineStr">
@@ -19312,12 +19312,12 @@
       <c r="D462" t="inlineStr"/>
       <c r="E462" t="inlineStr">
         <is>
-          <t>November Community Day</t>
+          <t>Raid NOW</t>
         </is>
       </c>
       <c r="F462" t="inlineStr">
         <is>
-          <t>Community Day</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G462" t="inlineStr"/>
@@ -19331,12 +19331,12 @@
       <c r="O462" t="inlineStr"/>
       <c r="P462" t="inlineStr">
         <is>
-          <t>Community Day November Community Day Sun, Nov 30, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Raid NOW From Leek Duck | Powered by GO FRIEND General Information It has been reported that the registration information (Trainer Name, Trainer Level, Trainer Code) is incorrect. Please check again. HOST HOST Auto join Raids you are joining (Latest 2) MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rpl_maxuser'] }} {{ val1['cnt'] }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} No.{{ val1['rpl_id'] }} No.{{ val1['rpl_id'] }} TL{{ val1['rpl_level'] }} {{ val1['rpl_glevel'] }} {{ ((val1['rpl_gescore'] == -1)?0:val1['rpl_gescore']) }} {{ aryPokemon[value]['raidbbs_short_name_en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} FULL Host TL 5 30 35 40 45 Host Rating - 0 {{ i }} MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['ti</t>
         </is>
       </c>
       <c r="Q462" t="inlineStr">
         <is>
-          <t>2024-06-01_events.html</t>
+          <t>2024-06-01_raid-now.html</t>
         </is>
       </c>
     </row>
@@ -19351,12 +19351,12 @@
       <c r="D463" t="inlineStr"/>
       <c r="E463" t="inlineStr">
         <is>
-          <t>November Community Day</t>
+          <t>Raids you are joining (Latest 2)</t>
         </is>
       </c>
       <c r="F463" t="inlineStr">
         <is>
-          <t>Community Day</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G463" t="inlineStr"/>
@@ -19370,12 +19370,12 @@
       <c r="O463" t="inlineStr"/>
       <c r="P463" t="inlineStr">
         <is>
-          <t>November Community Day Sun, Nov 30, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>General Information It has been reported that the registration information (Trainer Name, Trainer Level, Trainer Code) is incorrect. Please check again. HOST HOST Auto join Raids you are joining (Latest 2) MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rpl_maxuser'] }} {{ val1['cnt'] }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} No.{{ val1['rpl_id'] }} No.{{ val1['rpl_id'] }} TL{{ val1['rpl_level'] }} {{ val1['rpl_glevel'] }} {{ ((val1['rpl_gescore'] == -1)?0:val1['rpl_gescore']) }} {{ aryPokemon[value]['raidbbs_short_name_en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} FULL Host TL 5 30 35 40 45 Host Rating - 0 {{ i }} MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rp</t>
         </is>
       </c>
       <c r="Q463" t="inlineStr">
         <is>
-          <t>2024-06-01_events.html</t>
+          <t>2024-06-01_raid-now.html</t>
         </is>
       </c>
     </row>
@@ -19390,12 +19390,12 @@
       <c r="D464" t="inlineStr"/>
       <c r="E464" t="inlineStr">
         <is>
-          <t>November Community Day</t>
+          <t>Raids you are joining (Latest 2)</t>
         </is>
       </c>
       <c r="F464" t="inlineStr">
         <is>
-          <t>Community Day</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G464" t="inlineStr"/>
@@ -19409,12 +19409,12 @@
       <c r="O464" t="inlineStr"/>
       <c r="P464" t="inlineStr">
         <is>
-          <t>November Community Day Sun, Nov 30, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Raids you are joining (Latest 2) MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rpl_maxuser'] }} {{ val1['cnt'] }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} No.{{ val1['rpl_id'] }} No.{{ val1['rpl_id'] }} TL{{ val1['rpl_level'] }} {{ val1['rpl_glevel'] }} {{ ((val1['rpl_gescore'] == -1)?0:val1['rpl_gescore']) }}</t>
         </is>
       </c>
       <c r="Q464" t="inlineStr">
         <is>
-          <t>2024-06-01_events.html</t>
+          <t>2024-06-01_raid-now.html</t>
         </is>
       </c>
     </row>
@@ -19429,12 +19429,12 @@
       <c r="D465" t="inlineStr"/>
       <c r="E465" t="inlineStr">
         <is>
-          <t>November Community Day</t>
+          <t>まとめて評価</t>
         </is>
       </c>
       <c r="F465" t="inlineStr">
         <is>
-          <t>Community Day</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G465" t="inlineStr"/>
@@ -19448,12 +19448,12 @@
       <c r="O465" t="inlineStr"/>
       <c r="P465" t="inlineStr">
         <is>
-          <t>November Community Day Sun, Nov 30, at 2:00 PM Local Time</t>
+          <t>まとめて評価 Can't rate</t>
         </is>
       </c>
       <c r="Q465" t="inlineStr">
         <is>
-          <t>2024-06-01_events.html</t>
+          <t>2024-06-01_raid-now.html</t>
         </is>
       </c>
     </row>
@@ -19468,12 +19468,12 @@
       <c r="D466" t="inlineStr"/>
       <c r="E466" t="inlineStr">
         <is>
-          <t>Raid NOW</t>
+          <t>Bonuses</t>
         </is>
       </c>
       <c r="F466" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G466" t="inlineStr"/>
@@ -19487,12 +19487,12 @@
       <c r="O466" t="inlineStr"/>
       <c r="P466" t="inlineStr">
         <is>
-          <t>Raid NOW From Leek Duck | Powered by GO FRIEND General Information It has been reported that the registration information (Trainer Name, Trainer Level, Trainer Code) is incorrect. Please check again. HOST HOST Auto join Raids you are joining (Latest 2) MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rpl_maxuser'] }} {{ val1['cnt'] }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} No.{{ val1['rpl_id'] }} No.{{ val1['rpl_id'] }} TL{{ val1['rpl_level'] }} {{ val1['rpl_glevel'] }} {{ ((val1['rpl_gescore'] == -1)?0:val1['rpl_gescore']) }} {{ aryPokemon[value]['raidbbs_short_name_en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} FULL Host TL 5 30 35 40 45 Host Rating - 0 {{ i }} MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['ti</t>
+          <t>Bonuses 4× Stardust from win rewards. (This does not include end-of-set rewards.) The maximum number of sets you can play per day will increase from five to 20—for a total of 100 battles—from 12:00 a.m. to 11:59 p.m. local time. Free battle-themed Timed Research will be available. Rewards include glasses for your avatar inspired by Clemont. Pokémon encountered via GO Battle League rewards will have a wider variance of Attack, Defense, and HP. Active Leagues The following leagues will be active. Great League Ultra League Master League</t>
         </is>
       </c>
       <c r="Q466" t="inlineStr">
         <is>
-          <t>2024-06-01_raid-now.html</t>
+          <t>2024-06-01_event-go-battle-weekend-tales-of-transformation-sun-oct-26-at-1159-pm-local-time-ends-calculating.html</t>
         </is>
       </c>
     </row>
@@ -19507,12 +19507,12 @@
       <c r="D467" t="inlineStr"/>
       <c r="E467" t="inlineStr">
         <is>
-          <t>Raids you are joining (Latest 2)</t>
+          <t>For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area?</t>
         </is>
       </c>
       <c r="F467" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G467" t="inlineStr"/>
@@ -19526,12 +19526,12 @@
       <c r="O467" t="inlineStr"/>
       <c r="P467" t="inlineStr">
         <is>
-          <t>General Information It has been reported that the registration information (Trainer Name, Trainer Level, Trainer Code) is incorrect. Please check again. HOST HOST Auto join Raids you are joining (Latest 2) MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rpl_maxuser'] }} {{ val1['cnt'] }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} No.{{ val1['rpl_id'] }} No.{{ val1['rpl_id'] }} TL{{ val1['rpl_level'] }} {{ val1['rpl_glevel'] }} {{ ((val1['rpl_gescore'] == -1)?0:val1['rpl_gescore']) }} {{ aryPokemon[value]['raidbbs_short_name_en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} FULL Host TL 5 30 35 40 45 Host Rating - 0 {{ i }} MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rp</t>
+          <t xml:space="preserve">For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area? In this next chapter of Pokémon GO Wild Area, get ready to test your skills once again as you encounter Dark- and Fairy-type Pokémon, including Grimmsnarl, the Bulk Up Pokémon! Plus, exceptionally powerful Pokémon known as mighty Pokémon are appearing in the wild—use GO Wild Area–exclusive GO Safari Balls to improve your odds of catching these rare Pokémon. All event gameplay is exclusive to ticket holders. Tickets for Pokémon GO Wild Area: Nagasaki are now available on the Niantic events portal . Live Event Ticket - ¥3,600 (including applicable taxes and fees) Location: A citywide experience across Nagasaki City, Japan Dates: November 7, 8, or 9, 2025 Time: 9:00 a.m. – 5:00 p.m. JST Tickets for Pokémon GO Wild Area: Nagasaki include one day of event gameplay, and attendees may purchase add-ons that extend the gameplay for an additional day. One-day tickets are ¥3,600 (or the equivalent pricing tier in your local currency, including applicable taxes and fees). Event gameplay will be available only at the date, time, and location specified on your ticket. Note: Tickets to this event are </t>
         </is>
       </c>
       <c r="Q467" t="inlineStr">
         <is>
-          <t>2024-06-01_raid-now.html</t>
+          <t>2024-06-01_wild-area-pokmon-go-wild-area-nagasaki-calculating-ends-calculating.html</t>
         </is>
       </c>
     </row>
@@ -19546,12 +19546,12 @@
       <c r="D468" t="inlineStr"/>
       <c r="E468" t="inlineStr">
         <is>
-          <t>Raids you are joining (Latest 2)</t>
+          <t>For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area?</t>
         </is>
       </c>
       <c r="F468" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G468" t="inlineStr"/>
@@ -19565,166 +19565,10 @@
       <c r="O468" t="inlineStr"/>
       <c r="P468" t="inlineStr">
         <is>
-          <t>Raids you are joining (Latest 2) MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rpl_maxuser'] }} {{ val1['cnt'] }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} No.{{ val1['rpl_id'] }} No.{{ val1['rpl_id'] }} TL{{ val1['rpl_level'] }} {{ val1['rpl_glevel'] }} {{ ((val1['rpl_gescore'] == -1)?0:val1['rpl_gescore']) }}</t>
+          <t>For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area? Trainers around the world can gear up for a worldwide adventure during Pokémon GO Wild Area: Global, available in-game for two days only! Looking to enhance your GO Wild Area weekend with exclusive Special Research, additional bonuses, and an increased chance of encountering Shiny Pokémon? Purchase a global event ticket from the Pokémon GO Web Store! Event Tickets Tickets for Pokémon GO Wild Area: Global are available now in the in-game Shop and Pokémon Go Web Store for $11.99 USD . Purchase your ticket on the Pokémon GO Web Store for a new avatar item! Trainers who purchase their Pokémon GO Wild Area: Global ticket on the Pokémon GO Web Store will receive a special avatar item—the Flower Crown! You can purchase your ticket on the web store until the last day of the event to receive this avatar item. Pokémon GO Wild Area: Nagasaki For details on the in-person event in Nagasaki, Japan, click here .</t>
         </is>
       </c>
       <c r="Q468" t="inlineStr">
-        <is>
-          <t>2024-06-01_raid-now.html</t>
-        </is>
-      </c>
-    </row>
-    <row r="469">
-      <c r="A469" t="inlineStr">
-        <is>
-          <t>Leek Duck</t>
-        </is>
-      </c>
-      <c r="B469" t="inlineStr"/>
-      <c r="C469" t="inlineStr"/>
-      <c r="D469" t="inlineStr"/>
-      <c r="E469" t="inlineStr">
-        <is>
-          <t>まとめて評価</t>
-        </is>
-      </c>
-      <c r="F469" t="inlineStr">
-        <is>
-          <t>Event/News</t>
-        </is>
-      </c>
-      <c r="G469" t="inlineStr"/>
-      <c r="H469" t="inlineStr"/>
-      <c r="I469" t="inlineStr"/>
-      <c r="J469" t="inlineStr"/>
-      <c r="K469" t="inlineStr"/>
-      <c r="L469" t="inlineStr"/>
-      <c r="M469" t="inlineStr"/>
-      <c r="N469" t="inlineStr"/>
-      <c r="O469" t="inlineStr"/>
-      <c r="P469" t="inlineStr">
-        <is>
-          <t>まとめて評価 Can't rate</t>
-        </is>
-      </c>
-      <c r="Q469" t="inlineStr">
-        <is>
-          <t>2024-06-01_raid-now.html</t>
-        </is>
-      </c>
-    </row>
-    <row r="470">
-      <c r="A470" t="inlineStr">
-        <is>
-          <t>Leek Duck</t>
-        </is>
-      </c>
-      <c r="B470" t="inlineStr"/>
-      <c r="C470" t="inlineStr"/>
-      <c r="D470" t="inlineStr"/>
-      <c r="E470" t="inlineStr">
-        <is>
-          <t>Bonuses</t>
-        </is>
-      </c>
-      <c r="F470" t="inlineStr">
-        <is>
-          <t>Event/News</t>
-        </is>
-      </c>
-      <c r="G470" t="inlineStr"/>
-      <c r="H470" t="inlineStr"/>
-      <c r="I470" t="inlineStr"/>
-      <c r="J470" t="inlineStr"/>
-      <c r="K470" t="inlineStr"/>
-      <c r="L470" t="inlineStr"/>
-      <c r="M470" t="inlineStr"/>
-      <c r="N470" t="inlineStr"/>
-      <c r="O470" t="inlineStr"/>
-      <c r="P470" t="inlineStr">
-        <is>
-          <t>Bonuses 4× Stardust from win rewards. (This does not include end-of-set rewards.) The maximum number of sets you can play per day will increase from five to 20—for a total of 100 battles—from 12:00 a.m. to 11:59 p.m. local time. Free battle-themed Timed Research will be available. Rewards include glasses for your avatar inspired by Clemont. Pokémon encountered via GO Battle League rewards will have a wider variance of Attack, Defense, and HP. Active Leagues The following leagues will be active. Great League Ultra League Master League</t>
-        </is>
-      </c>
-      <c r="Q470" t="inlineStr">
-        <is>
-          <t>2024-06-01_event-go-battle-weekend-tales-of-transformation-sun-oct-26-at-1159-pm-local-time-ends-calculating.html</t>
-        </is>
-      </c>
-    </row>
-    <row r="471">
-      <c r="A471" t="inlineStr">
-        <is>
-          <t>Leek Duck</t>
-        </is>
-      </c>
-      <c r="B471" t="inlineStr"/>
-      <c r="C471" t="inlineStr"/>
-      <c r="D471" t="inlineStr"/>
-      <c r="E471" t="inlineStr">
-        <is>
-          <t>For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area?</t>
-        </is>
-      </c>
-      <c r="F471" t="inlineStr">
-        <is>
-          <t>Event/News</t>
-        </is>
-      </c>
-      <c r="G471" t="inlineStr"/>
-      <c r="H471" t="inlineStr"/>
-      <c r="I471" t="inlineStr"/>
-      <c r="J471" t="inlineStr"/>
-      <c r="K471" t="inlineStr"/>
-      <c r="L471" t="inlineStr"/>
-      <c r="M471" t="inlineStr"/>
-      <c r="N471" t="inlineStr"/>
-      <c r="O471" t="inlineStr"/>
-      <c r="P471" t="inlineStr">
-        <is>
-          <t xml:space="preserve">For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area? In this next chapter of Pokémon GO Wild Area, get ready to test your skills once again as you encounter Dark- and Fairy-type Pokémon, including Grimmsnarl, the Bulk Up Pokémon! Plus, exceptionally powerful Pokémon known as mighty Pokémon are appearing in the wild—use GO Wild Area–exclusive GO Safari Balls to improve your odds of catching these rare Pokémon. All event gameplay is exclusive to ticket holders. Tickets for Pokémon GO Wild Area: Nagasaki are now available on the Niantic events portal . Live Event Ticket - ¥3,600 (including applicable taxes and fees) Location: A citywide experience across Nagasaki City, Japan Dates: November 7, 8, or 9, 2025 Time: 9:00 a.m. – 5:00 p.m. JST Tickets for Pokémon GO Wild Area: Nagasaki include one day of event gameplay, and attendees may purchase add-ons that extend the gameplay for an additional day. One-day tickets are ¥3,600 (or the equivalent pricing tier in your local currency, including applicable taxes and fees). Event gameplay will be available only at the date, time, and location specified on your ticket. Note: Tickets to this event are </t>
-        </is>
-      </c>
-      <c r="Q471" t="inlineStr">
-        <is>
-          <t>2024-06-01_wild-area-pokmon-go-wild-area-nagasaki-calculating-ends-calculating.html</t>
-        </is>
-      </c>
-    </row>
-    <row r="472">
-      <c r="A472" t="inlineStr">
-        <is>
-          <t>Leek Duck</t>
-        </is>
-      </c>
-      <c r="B472" t="inlineStr"/>
-      <c r="C472" t="inlineStr"/>
-      <c r="D472" t="inlineStr"/>
-      <c r="E472" t="inlineStr">
-        <is>
-          <t>For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area?</t>
-        </is>
-      </c>
-      <c r="F472" t="inlineStr">
-        <is>
-          <t>Event/News</t>
-        </is>
-      </c>
-      <c r="G472" t="inlineStr"/>
-      <c r="H472" t="inlineStr"/>
-      <c r="I472" t="inlineStr"/>
-      <c r="J472" t="inlineStr"/>
-      <c r="K472" t="inlineStr"/>
-      <c r="L472" t="inlineStr"/>
-      <c r="M472" t="inlineStr"/>
-      <c r="N472" t="inlineStr"/>
-      <c r="O472" t="inlineStr"/>
-      <c r="P472" t="inlineStr">
-        <is>
-          <t>For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area? Trainers around the world can gear up for a worldwide adventure during Pokémon GO Wild Area: Global, available in-game for two days only! Looking to enhance your GO Wild Area weekend with exclusive Special Research, additional bonuses, and an increased chance of encountering Shiny Pokémon? Purchase a global event ticket from the Pokémon GO Web Store! Event Tickets Tickets for Pokémon GO Wild Area: Global are available now in the in-game Shop and Pokémon Go Web Store for $11.99 USD . Purchase your ticket on the Pokémon GO Web Store for a new avatar item! Trainers who purchase their Pokémon GO Wild Area: Global ticket on the Pokémon GO Web Store will receive a special avatar item—the Flower Crown! You can purchase your ticket on the web store until the last day of the event to receive this avatar item. Pokémon GO Wild Area: Nagasaki For details on the in-person event in Nagasaki, Japan, click here .</t>
-        </is>
-      </c>
-      <c r="Q472" t="inlineStr">
         <is>
           <t>2024-06-01_wild-area-pokmon-go-wild-area-global-sun-nov-16-at-600-pm-local-time-ends-calculating.html</t>
         </is>

</xml_diff>

<commit_message>
Update latest digest: 2024-06-01 → 2025-10-02
</commit_message>
<xml_diff>
--- a/outputs/latest/POGO_Digest.xlsx
+++ b/outputs/latest/POGO_Digest.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q445"/>
+  <dimension ref="A1:Q441"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11944,7 +11944,7 @@
       <c r="D274" t="inlineStr"/>
       <c r="E274" t="inlineStr">
         <is>
-          <t>Dialga (Origin Forme) Raid Hour</t>
+          <t>Mega Metagross Raid Day</t>
         </is>
       </c>
       <c r="F274" t="inlineStr">
@@ -11963,7 +11963,7 @@
       <c r="O274" t="inlineStr"/>
       <c r="P274" t="inlineStr">
         <is>
-          <t>Raid Hour Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 6:00 PM Local Time Starts: Calculating... Raid Day Mega Metagross Raid Day Sat, Oct 4, at 2:00 PM Local Time Starts: Calculating... Max Mondays Dynamax Drilbur during Max Monday Mon, Oct 6, at 6:00 PM Local Time Starts: Calculating... GO Pass GO Pass: October Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating... Raid Battles Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating... Raid Battles Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating... GO Battle League Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating... Pokémon Spotlight Hour Ferroseed Spotlight Hour Tue, Oct 7, at 6:00 PM Local Time Starts: Calculating... Raid Hour Deoxys (Normal &amp; Defense Forme) Raid Hour Wed, Oct 8, at 6:00 PM Local Time Starts: Calculating... Event Harvest Festival Fri, Oct 10, at 10:00 AM Local Time Starts: Calculating... Community Day Solosis Community Day Sun, Oct 12, at 2:00 PM Local Time Starts: Calculating... Max Mondays Dynamax Bounsweet during Max Mond</t>
+          <t>Raid Day Mega Metagross Raid Day Sat, Oct 4, at 2:00 PM Local Time Starts: Calculating... Max Mondays Dynamax Drilbur during Max Monday Mon, Oct 6, at 6:00 PM Local Time Starts: Calculating... GO Pass GO Pass: October Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating... Raid Battles Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating... Raid Battles Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating... GO Battle League Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating... Pokémon Spotlight Hour Ferroseed Spotlight Hour Tue, Oct 7, at 6:00 PM Local Time Starts: Calculating... Raid Hour Deoxys (Normal &amp; Defense Forme) Raid Hour Wed, Oct 8, at 6:00 PM Local Time Starts: Calculating... Event Harvest Festival Fri, Oct 10, at 10:00 AM Local Time Starts: Calculating... Community Day Solosis Community Day Sun, Oct 12, at 2:00 PM Local Time Starts: Calculating... Max Mondays Dynamax Bounsweet during Max Monday Mon, Oct 13, at 6:00 PM Local Time Starts: Calculating... Raid Battles Deoxys (Attack &amp; Speed Fo</t>
         </is>
       </c>
       <c r="Q274" t="inlineStr">
@@ -11983,7 +11983,7 @@
       <c r="D275" t="inlineStr"/>
       <c r="E275" t="inlineStr">
         <is>
-          <t>Dialga (Origin Forme) Raid Hour</t>
+          <t>Mega Metagross Raid Day</t>
         </is>
       </c>
       <c r="F275" t="inlineStr">
@@ -12002,7 +12002,7 @@
       <c r="O275" t="inlineStr"/>
       <c r="P275" t="inlineStr">
         <is>
-          <t>Raid Hour Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Raid Day Mega Metagross Raid Day Sat, Oct 4, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q275" t="inlineStr">
@@ -12022,7 +12022,7 @@
       <c r="D276" t="inlineStr"/>
       <c r="E276" t="inlineStr">
         <is>
-          <t>Dialga (Origin Forme) Raid Hour</t>
+          <t>Mega Metagross Raid Day</t>
         </is>
       </c>
       <c r="F276" t="inlineStr">
@@ -12041,7 +12041,7 @@
       <c r="O276" t="inlineStr"/>
       <c r="P276" t="inlineStr">
         <is>
-          <t>Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Mega Metagross Raid Day Sat, Oct 4, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q276" t="inlineStr">
@@ -12061,7 +12061,7 @@
       <c r="D277" t="inlineStr"/>
       <c r="E277" t="inlineStr">
         <is>
-          <t>Dialga (Origin Forme) Raid Hour</t>
+          <t>Mega Metagross Raid Day</t>
         </is>
       </c>
       <c r="F277" t="inlineStr">
@@ -12080,7 +12080,7 @@
       <c r="O277" t="inlineStr"/>
       <c r="P277" t="inlineStr">
         <is>
-          <t>Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Mega Metagross Raid Day Sat, Oct 4, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q277" t="inlineStr">
@@ -12100,7 +12100,7 @@
       <c r="D278" t="inlineStr"/>
       <c r="E278" t="inlineStr">
         <is>
-          <t>Dialga (Origin Forme) Raid Hour</t>
+          <t>Mega Metagross Raid Day</t>
         </is>
       </c>
       <c r="F278" t="inlineStr">
@@ -12119,7 +12119,7 @@
       <c r="O278" t="inlineStr"/>
       <c r="P278" t="inlineStr">
         <is>
-          <t>Dialga (Origin Forme) Raid Hour Wed, Oct 1, at 6:00 PM Local Time</t>
+          <t>Mega Metagross Raid Day Sat, Oct 4, at 2:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q278" t="inlineStr">
@@ -12139,12 +12139,12 @@
       <c r="D279" t="inlineStr"/>
       <c r="E279" t="inlineStr">
         <is>
-          <t>Mega Metagross Raid Day</t>
+          <t>Dynamax Drilbur during Max Monday</t>
         </is>
       </c>
       <c r="F279" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G279" t="inlineStr"/>
@@ -12158,7 +12158,7 @@
       <c r="O279" t="inlineStr"/>
       <c r="P279" t="inlineStr">
         <is>
-          <t>Raid Day Mega Metagross Raid Day Sat, Oct 4, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Max Mondays Dynamax Drilbur during Max Monday Mon, Oct 6, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q279" t="inlineStr">
@@ -12178,12 +12178,12 @@
       <c r="D280" t="inlineStr"/>
       <c r="E280" t="inlineStr">
         <is>
-          <t>Mega Metagross Raid Day</t>
+          <t>Dynamax Drilbur during Max Monday</t>
         </is>
       </c>
       <c r="F280" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G280" t="inlineStr"/>
@@ -12197,7 +12197,7 @@
       <c r="O280" t="inlineStr"/>
       <c r="P280" t="inlineStr">
         <is>
-          <t>Mega Metagross Raid Day Sat, Oct 4, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Dynamax Drilbur during Max Monday Mon, Oct 6, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q280" t="inlineStr">
@@ -12217,12 +12217,12 @@
       <c r="D281" t="inlineStr"/>
       <c r="E281" t="inlineStr">
         <is>
-          <t>Mega Metagross Raid Day</t>
+          <t>Dynamax Drilbur during Max Monday</t>
         </is>
       </c>
       <c r="F281" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G281" t="inlineStr"/>
@@ -12236,7 +12236,7 @@
       <c r="O281" t="inlineStr"/>
       <c r="P281" t="inlineStr">
         <is>
-          <t>Mega Metagross Raid Day Sat, Oct 4, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Dynamax Drilbur during Max Monday Mon, Oct 6, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q281" t="inlineStr">
@@ -12256,12 +12256,12 @@
       <c r="D282" t="inlineStr"/>
       <c r="E282" t="inlineStr">
         <is>
-          <t>Mega Metagross Raid Day</t>
+          <t>Dynamax Drilbur during Max Monday</t>
         </is>
       </c>
       <c r="F282" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G282" t="inlineStr"/>
@@ -12275,7 +12275,7 @@
       <c r="O282" t="inlineStr"/>
       <c r="P282" t="inlineStr">
         <is>
-          <t>Mega Metagross Raid Day Sat, Oct 4, at 2:00 PM Local Time</t>
+          <t>Dynamax Drilbur during Max Monday Mon, Oct 6, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q282" t="inlineStr">
@@ -12295,7 +12295,7 @@
       <c r="D283" t="inlineStr"/>
       <c r="E283" t="inlineStr">
         <is>
-          <t>Dynamax Drilbur during Max Monday</t>
+          <t>GO Pass: October</t>
         </is>
       </c>
       <c r="F283" t="inlineStr">
@@ -12314,7 +12314,7 @@
       <c r="O283" t="inlineStr"/>
       <c r="P283" t="inlineStr">
         <is>
-          <t>Max Mondays Dynamax Drilbur during Max Monday Mon, Oct 6, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>GO Pass GO Pass: October Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q283" t="inlineStr">
@@ -12334,7 +12334,7 @@
       <c r="D284" t="inlineStr"/>
       <c r="E284" t="inlineStr">
         <is>
-          <t>Dynamax Drilbur during Max Monday</t>
+          <t>GO Pass: October</t>
         </is>
       </c>
       <c r="F284" t="inlineStr">
@@ -12353,7 +12353,7 @@
       <c r="O284" t="inlineStr"/>
       <c r="P284" t="inlineStr">
         <is>
-          <t>Dynamax Drilbur during Max Monday Mon, Oct 6, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>GO Pass: October Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q284" t="inlineStr">
@@ -12373,7 +12373,7 @@
       <c r="D285" t="inlineStr"/>
       <c r="E285" t="inlineStr">
         <is>
-          <t>Dynamax Drilbur during Max Monday</t>
+          <t>GO Pass: October</t>
         </is>
       </c>
       <c r="F285" t="inlineStr">
@@ -12392,7 +12392,7 @@
       <c r="O285" t="inlineStr"/>
       <c r="P285" t="inlineStr">
         <is>
-          <t>Dynamax Drilbur during Max Monday Mon, Oct 6, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>GO Pass: October Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q285" t="inlineStr">
@@ -12412,7 +12412,7 @@
       <c r="D286" t="inlineStr"/>
       <c r="E286" t="inlineStr">
         <is>
-          <t>Dynamax Drilbur during Max Monday</t>
+          <t>GO Pass: October</t>
         </is>
       </c>
       <c r="F286" t="inlineStr">
@@ -12431,7 +12431,7 @@
       <c r="O286" t="inlineStr"/>
       <c r="P286" t="inlineStr">
         <is>
-          <t>Dynamax Drilbur during Max Monday Mon, Oct 6, at 6:00 PM Local Time</t>
+          <t>GO Pass: October Tue, Oct 7, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q286" t="inlineStr">
@@ -12451,12 +12451,12 @@
       <c r="D287" t="inlineStr"/>
       <c r="E287" t="inlineStr">
         <is>
-          <t>GO Pass: October</t>
+          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F287" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G287" t="inlineStr"/>
@@ -12470,7 +12470,7 @@
       <c r="O287" t="inlineStr"/>
       <c r="P287" t="inlineStr">
         <is>
-          <t>GO Pass GO Pass: October Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Raid Battles Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q287" t="inlineStr">
@@ -12490,12 +12490,12 @@
       <c r="D288" t="inlineStr"/>
       <c r="E288" t="inlineStr">
         <is>
-          <t>GO Pass: October</t>
+          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F288" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G288" t="inlineStr"/>
@@ -12509,7 +12509,7 @@
       <c r="O288" t="inlineStr"/>
       <c r="P288" t="inlineStr">
         <is>
-          <t>GO Pass: October Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q288" t="inlineStr">
@@ -12529,12 +12529,12 @@
       <c r="D289" t="inlineStr"/>
       <c r="E289" t="inlineStr">
         <is>
-          <t>GO Pass: October</t>
+          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F289" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G289" t="inlineStr"/>
@@ -12548,7 +12548,7 @@
       <c r="O289" t="inlineStr"/>
       <c r="P289" t="inlineStr">
         <is>
-          <t>GO Pass: October Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q289" t="inlineStr">
@@ -12568,12 +12568,12 @@
       <c r="D290" t="inlineStr"/>
       <c r="E290" t="inlineStr">
         <is>
-          <t>GO Pass: October</t>
+          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F290" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G290" t="inlineStr"/>
@@ -12587,7 +12587,7 @@
       <c r="O290" t="inlineStr"/>
       <c r="P290" t="inlineStr">
         <is>
-          <t>GO Pass: October Tue, Oct 7, at 10:00 AM Local Time</t>
+          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q290" t="inlineStr">
@@ -12607,7 +12607,7 @@
       <c r="D291" t="inlineStr"/>
       <c r="E291" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles</t>
+          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids</t>
         </is>
       </c>
       <c r="F291" t="inlineStr">
@@ -12626,7 +12626,7 @@
       <c r="O291" t="inlineStr"/>
       <c r="P291" t="inlineStr">
         <is>
-          <t>Raid Battles Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Raid Battles Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q291" t="inlineStr">
@@ -12646,7 +12646,7 @@
       <c r="D292" t="inlineStr"/>
       <c r="E292" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles</t>
+          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids</t>
         </is>
       </c>
       <c r="F292" t="inlineStr">
@@ -12665,7 +12665,7 @@
       <c r="O292" t="inlineStr"/>
       <c r="P292" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q292" t="inlineStr">
@@ -12685,7 +12685,7 @@
       <c r="D293" t="inlineStr"/>
       <c r="E293" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles</t>
+          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids</t>
         </is>
       </c>
       <c r="F293" t="inlineStr">
@@ -12704,7 +12704,7 @@
       <c r="O293" t="inlineStr"/>
       <c r="P293" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q293" t="inlineStr">
@@ -12724,7 +12724,7 @@
       <c r="D294" t="inlineStr"/>
       <c r="E294" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles</t>
+          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids</t>
         </is>
       </c>
       <c r="F294" t="inlineStr">
@@ -12743,7 +12743,7 @@
       <c r="O294" t="inlineStr"/>
       <c r="P294" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time</t>
+          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids Tue, Oct 7, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q294" t="inlineStr">
@@ -12763,12 +12763,12 @@
       <c r="D295" t="inlineStr"/>
       <c r="E295" t="inlineStr">
         <is>
-          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F295" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G295" t="inlineStr"/>
@@ -12782,7 +12782,7 @@
       <c r="O295" t="inlineStr"/>
       <c r="P295" t="inlineStr">
         <is>
-          <t>Raid Battles Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>GO Battle League Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q295" t="inlineStr">
@@ -12802,12 +12802,12 @@
       <c r="D296" t="inlineStr"/>
       <c r="E296" t="inlineStr">
         <is>
-          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F296" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G296" t="inlineStr"/>
@@ -12821,7 +12821,7 @@
       <c r="O296" t="inlineStr"/>
       <c r="P296" t="inlineStr">
         <is>
-          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q296" t="inlineStr">
@@ -12841,12 +12841,12 @@
       <c r="D297" t="inlineStr"/>
       <c r="E297" t="inlineStr">
         <is>
-          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F297" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G297" t="inlineStr"/>
@@ -12860,7 +12860,7 @@
       <c r="O297" t="inlineStr"/>
       <c r="P297" t="inlineStr">
         <is>
-          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q297" t="inlineStr">
@@ -12880,12 +12880,12 @@
       <c r="D298" t="inlineStr"/>
       <c r="E298" t="inlineStr">
         <is>
-          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F298" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G298" t="inlineStr"/>
@@ -12899,7 +12899,7 @@
       <c r="O298" t="inlineStr"/>
       <c r="P298" t="inlineStr">
         <is>
-          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids Tue, Oct 7, at 10:00 AM Local Time</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q298" t="inlineStr">
@@ -12919,12 +12919,12 @@
       <c r="D299" t="inlineStr"/>
       <c r="E299" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
+          <t>Ferroseed Spotlight Hour</t>
         </is>
       </c>
       <c r="F299" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G299" t="inlineStr"/>
@@ -12938,7 +12938,7 @@
       <c r="O299" t="inlineStr"/>
       <c r="P299" t="inlineStr">
         <is>
-          <t>GO Battle League Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Pokémon Spotlight Hour Ferroseed Spotlight Hour Tue, Oct 7, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q299" t="inlineStr">
@@ -12958,12 +12958,12 @@
       <c r="D300" t="inlineStr"/>
       <c r="E300" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
+          <t>Ferroseed Spotlight Hour</t>
         </is>
       </c>
       <c r="F300" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G300" t="inlineStr"/>
@@ -12977,7 +12977,7 @@
       <c r="O300" t="inlineStr"/>
       <c r="P300" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Ferroseed Spotlight Hour Tue, Oct 7, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q300" t="inlineStr">
@@ -12997,12 +12997,12 @@
       <c r="D301" t="inlineStr"/>
       <c r="E301" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
+          <t>Ferroseed Spotlight Hour</t>
         </is>
       </c>
       <c r="F301" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G301" t="inlineStr"/>
@@ -13016,7 +13016,7 @@
       <c r="O301" t="inlineStr"/>
       <c r="P301" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Ferroseed Spotlight Hour Tue, Oct 7, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q301" t="inlineStr">
@@ -13036,12 +13036,12 @@
       <c r="D302" t="inlineStr"/>
       <c r="E302" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
+          <t>Ferroseed Spotlight Hour</t>
         </is>
       </c>
       <c r="F302" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G302" t="inlineStr"/>
@@ -13055,7 +13055,7 @@
       <c r="O302" t="inlineStr"/>
       <c r="P302" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating...</t>
+          <t>Ferroseed Spotlight Hour Tue, Oct 7, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q302" t="inlineStr">
@@ -13075,12 +13075,12 @@
       <c r="D303" t="inlineStr"/>
       <c r="E303" t="inlineStr">
         <is>
-          <t>Ferroseed Spotlight Hour</t>
+          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F303" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G303" t="inlineStr"/>
@@ -13094,7 +13094,7 @@
       <c r="O303" t="inlineStr"/>
       <c r="P303" t="inlineStr">
         <is>
-          <t>Pokémon Spotlight Hour Ferroseed Spotlight Hour Tue, Oct 7, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Raid Hour Deoxys (Normal &amp; Defense Forme) Raid Hour Wed, Oct 8, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q303" t="inlineStr">
@@ -13114,12 +13114,12 @@
       <c r="D304" t="inlineStr"/>
       <c r="E304" t="inlineStr">
         <is>
-          <t>Ferroseed Spotlight Hour</t>
+          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F304" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G304" t="inlineStr"/>
@@ -13133,7 +13133,7 @@
       <c r="O304" t="inlineStr"/>
       <c r="P304" t="inlineStr">
         <is>
-          <t>Ferroseed Spotlight Hour Tue, Oct 7, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour Wed, Oct 8, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q304" t="inlineStr">
@@ -13153,12 +13153,12 @@
       <c r="D305" t="inlineStr"/>
       <c r="E305" t="inlineStr">
         <is>
-          <t>Ferroseed Spotlight Hour</t>
+          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F305" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G305" t="inlineStr"/>
@@ -13172,7 +13172,7 @@
       <c r="O305" t="inlineStr"/>
       <c r="P305" t="inlineStr">
         <is>
-          <t>Ferroseed Spotlight Hour Tue, Oct 7, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour Wed, Oct 8, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q305" t="inlineStr">
@@ -13192,12 +13192,12 @@
       <c r="D306" t="inlineStr"/>
       <c r="E306" t="inlineStr">
         <is>
-          <t>Ferroseed Spotlight Hour</t>
+          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F306" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G306" t="inlineStr"/>
@@ -13211,7 +13211,7 @@
       <c r="O306" t="inlineStr"/>
       <c r="P306" t="inlineStr">
         <is>
-          <t>Ferroseed Spotlight Hour Tue, Oct 7, at 6:00 PM Local Time</t>
+          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour Wed, Oct 8, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q306" t="inlineStr">
@@ -13231,12 +13231,12 @@
       <c r="D307" t="inlineStr"/>
       <c r="E307" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour</t>
+          <t>Harvest Festival</t>
         </is>
       </c>
       <c r="F307" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G307" t="inlineStr"/>
@@ -13250,7 +13250,7 @@
       <c r="O307" t="inlineStr"/>
       <c r="P307" t="inlineStr">
         <is>
-          <t>Raid Hour Deoxys (Normal &amp; Defense Forme) Raid Hour Wed, Oct 8, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Event Harvest Festival Fri, Oct 10, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q307" t="inlineStr">
@@ -13270,12 +13270,12 @@
       <c r="D308" t="inlineStr"/>
       <c r="E308" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour</t>
+          <t>Harvest Festival</t>
         </is>
       </c>
       <c r="F308" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G308" t="inlineStr"/>
@@ -13289,7 +13289,7 @@
       <c r="O308" t="inlineStr"/>
       <c r="P308" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour Wed, Oct 8, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Harvest Festival Fri, Oct 10, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q308" t="inlineStr">
@@ -13309,12 +13309,12 @@
       <c r="D309" t="inlineStr"/>
       <c r="E309" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour</t>
+          <t>Harvest Festival</t>
         </is>
       </c>
       <c r="F309" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G309" t="inlineStr"/>
@@ -13328,7 +13328,7 @@
       <c r="O309" t="inlineStr"/>
       <c r="P309" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour Wed, Oct 8, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Harvest Festival Fri, Oct 10, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q309" t="inlineStr">
@@ -13348,12 +13348,12 @@
       <c r="D310" t="inlineStr"/>
       <c r="E310" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour</t>
+          <t>Harvest Festival</t>
         </is>
       </c>
       <c r="F310" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G310" t="inlineStr"/>
@@ -13367,7 +13367,7 @@
       <c r="O310" t="inlineStr"/>
       <c r="P310" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour Wed, Oct 8, at 6:00 PM Local Time</t>
+          <t>Harvest Festival Fri, Oct 10, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q310" t="inlineStr">
@@ -13387,12 +13387,12 @@
       <c r="D311" t="inlineStr"/>
       <c r="E311" t="inlineStr">
         <is>
-          <t>Harvest Festival</t>
+          <t>Solosis Community Day</t>
         </is>
       </c>
       <c r="F311" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Community Day</t>
         </is>
       </c>
       <c r="G311" t="inlineStr"/>
@@ -13406,7 +13406,7 @@
       <c r="O311" t="inlineStr"/>
       <c r="P311" t="inlineStr">
         <is>
-          <t>Event Harvest Festival Fri, Oct 10, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Community Day Solosis Community Day Sun, Oct 12, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q311" t="inlineStr">
@@ -13426,12 +13426,12 @@
       <c r="D312" t="inlineStr"/>
       <c r="E312" t="inlineStr">
         <is>
-          <t>Harvest Festival</t>
+          <t>Solosis Community Day</t>
         </is>
       </c>
       <c r="F312" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Community Day</t>
         </is>
       </c>
       <c r="G312" t="inlineStr"/>
@@ -13445,7 +13445,7 @@
       <c r="O312" t="inlineStr"/>
       <c r="P312" t="inlineStr">
         <is>
-          <t>Harvest Festival Fri, Oct 10, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Solosis Community Day Sun, Oct 12, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q312" t="inlineStr">
@@ -13465,12 +13465,12 @@
       <c r="D313" t="inlineStr"/>
       <c r="E313" t="inlineStr">
         <is>
-          <t>Harvest Festival</t>
+          <t>Solosis Community Day</t>
         </is>
       </c>
       <c r="F313" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Community Day</t>
         </is>
       </c>
       <c r="G313" t="inlineStr"/>
@@ -13484,7 +13484,7 @@
       <c r="O313" t="inlineStr"/>
       <c r="P313" t="inlineStr">
         <is>
-          <t>Harvest Festival Fri, Oct 10, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Solosis Community Day Sun, Oct 12, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q313" t="inlineStr">
@@ -13504,12 +13504,12 @@
       <c r="D314" t="inlineStr"/>
       <c r="E314" t="inlineStr">
         <is>
-          <t>Harvest Festival</t>
+          <t>Solosis Community Day</t>
         </is>
       </c>
       <c r="F314" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Community Day</t>
         </is>
       </c>
       <c r="G314" t="inlineStr"/>
@@ -13523,7 +13523,7 @@
       <c r="O314" t="inlineStr"/>
       <c r="P314" t="inlineStr">
         <is>
-          <t>Harvest Festival Fri, Oct 10, at 10:00 AM Local Time</t>
+          <t>Solosis Community Day Sun, Oct 12, at 2:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q314" t="inlineStr">
@@ -13543,12 +13543,12 @@
       <c r="D315" t="inlineStr"/>
       <c r="E315" t="inlineStr">
         <is>
-          <t>Solosis Community Day</t>
+          <t>Dynamax Bounsweet during Max Monday</t>
         </is>
       </c>
       <c r="F315" t="inlineStr">
         <is>
-          <t>Community Day</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G315" t="inlineStr"/>
@@ -13562,7 +13562,7 @@
       <c r="O315" t="inlineStr"/>
       <c r="P315" t="inlineStr">
         <is>
-          <t>Community Day Solosis Community Day Sun, Oct 12, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Max Mondays Dynamax Bounsweet during Max Monday Mon, Oct 13, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q315" t="inlineStr">
@@ -13582,12 +13582,12 @@
       <c r="D316" t="inlineStr"/>
       <c r="E316" t="inlineStr">
         <is>
-          <t>Solosis Community Day</t>
+          <t>Dynamax Bounsweet during Max Monday</t>
         </is>
       </c>
       <c r="F316" t="inlineStr">
         <is>
-          <t>Community Day</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G316" t="inlineStr"/>
@@ -13601,7 +13601,7 @@
       <c r="O316" t="inlineStr"/>
       <c r="P316" t="inlineStr">
         <is>
-          <t>Solosis Community Day Sun, Oct 12, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Dynamax Bounsweet during Max Monday Mon, Oct 13, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q316" t="inlineStr">
@@ -13621,12 +13621,12 @@
       <c r="D317" t="inlineStr"/>
       <c r="E317" t="inlineStr">
         <is>
-          <t>Solosis Community Day</t>
+          <t>Dynamax Bounsweet during Max Monday</t>
         </is>
       </c>
       <c r="F317" t="inlineStr">
         <is>
-          <t>Community Day</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G317" t="inlineStr"/>
@@ -13640,7 +13640,7 @@
       <c r="O317" t="inlineStr"/>
       <c r="P317" t="inlineStr">
         <is>
-          <t>Solosis Community Day Sun, Oct 12, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Dynamax Bounsweet during Max Monday Mon, Oct 13, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q317" t="inlineStr">
@@ -13660,12 +13660,12 @@
       <c r="D318" t="inlineStr"/>
       <c r="E318" t="inlineStr">
         <is>
-          <t>Solosis Community Day</t>
+          <t>Dynamax Bounsweet during Max Monday</t>
         </is>
       </c>
       <c r="F318" t="inlineStr">
         <is>
-          <t>Community Day</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G318" t="inlineStr"/>
@@ -13679,7 +13679,7 @@
       <c r="O318" t="inlineStr"/>
       <c r="P318" t="inlineStr">
         <is>
-          <t>Solosis Community Day Sun, Oct 12, at 2:00 PM Local Time</t>
+          <t>Dynamax Bounsweet during Max Monday Mon, Oct 13, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q318" t="inlineStr">
@@ -13699,12 +13699,12 @@
       <c r="D319" t="inlineStr"/>
       <c r="E319" t="inlineStr">
         <is>
-          <t>Dynamax Bounsweet during Max Monday</t>
+          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F319" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G319" t="inlineStr"/>
@@ -13718,7 +13718,7 @@
       <c r="O319" t="inlineStr"/>
       <c r="P319" t="inlineStr">
         <is>
-          <t>Max Mondays Dynamax Bounsweet during Max Monday Mon, Oct 13, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Raid Battles Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q319" t="inlineStr">
@@ -13738,12 +13738,12 @@
       <c r="D320" t="inlineStr"/>
       <c r="E320" t="inlineStr">
         <is>
-          <t>Dynamax Bounsweet during Max Monday</t>
+          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F320" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G320" t="inlineStr"/>
@@ -13757,7 +13757,7 @@
       <c r="O320" t="inlineStr"/>
       <c r="P320" t="inlineStr">
         <is>
-          <t>Dynamax Bounsweet during Max Monday Mon, Oct 13, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q320" t="inlineStr">
@@ -13777,12 +13777,12 @@
       <c r="D321" t="inlineStr"/>
       <c r="E321" t="inlineStr">
         <is>
-          <t>Dynamax Bounsweet during Max Monday</t>
+          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F321" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G321" t="inlineStr"/>
@@ -13796,7 +13796,7 @@
       <c r="O321" t="inlineStr"/>
       <c r="P321" t="inlineStr">
         <is>
-          <t>Dynamax Bounsweet during Max Monday Mon, Oct 13, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q321" t="inlineStr">
@@ -13816,12 +13816,12 @@
       <c r="D322" t="inlineStr"/>
       <c r="E322" t="inlineStr">
         <is>
-          <t>Dynamax Bounsweet during Max Monday</t>
+          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F322" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G322" t="inlineStr"/>
@@ -13835,7 +13835,7 @@
       <c r="O322" t="inlineStr"/>
       <c r="P322" t="inlineStr">
         <is>
-          <t>Dynamax Bounsweet during Max Monday Mon, Oct 13, at 6:00 PM Local Time</t>
+          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles Tue, Oct 14, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q322" t="inlineStr">
@@ -13855,7 +13855,7 @@
       <c r="D323" t="inlineStr"/>
       <c r="E323" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles</t>
+          <t>Mega Mawile and Mega Salamence in Mega Raids</t>
         </is>
       </c>
       <c r="F323" t="inlineStr">
@@ -13874,7 +13874,7 @@
       <c r="O323" t="inlineStr"/>
       <c r="P323" t="inlineStr">
         <is>
-          <t>Raid Battles Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Raid Battles Mega Mawile and Mega Salamence in Mega Raids Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q323" t="inlineStr">
@@ -13894,7 +13894,7 @@
       <c r="D324" t="inlineStr"/>
       <c r="E324" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles</t>
+          <t>Mega Mawile and Mega Salamence in Mega Raids</t>
         </is>
       </c>
       <c r="F324" t="inlineStr">
@@ -13913,7 +13913,7 @@
       <c r="O324" t="inlineStr"/>
       <c r="P324" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Mega Mawile and Mega Salamence in Mega Raids Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q324" t="inlineStr">
@@ -13933,7 +13933,7 @@
       <c r="D325" t="inlineStr"/>
       <c r="E325" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles</t>
+          <t>Mega Mawile and Mega Salamence in Mega Raids</t>
         </is>
       </c>
       <c r="F325" t="inlineStr">
@@ -13952,7 +13952,7 @@
       <c r="O325" t="inlineStr"/>
       <c r="P325" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Mega Mawile and Mega Salamence in Mega Raids Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q325" t="inlineStr">
@@ -13972,7 +13972,7 @@
       <c r="D326" t="inlineStr"/>
       <c r="E326" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles</t>
+          <t>Mega Mawile and Mega Salamence in Mega Raids</t>
         </is>
       </c>
       <c r="F326" t="inlineStr">
@@ -13991,7 +13991,7 @@
       <c r="O326" t="inlineStr"/>
       <c r="P326" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles Tue, Oct 14, at 10:00 AM Local Time</t>
+          <t>Mega Mawile and Mega Salamence in Mega Raids Tue, Oct 14, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q326" t="inlineStr">
@@ -14011,12 +14011,12 @@
       <c r="D327" t="inlineStr"/>
       <c r="E327" t="inlineStr">
         <is>
-          <t>Mega Mawile and Mega Salamence in Mega Raids</t>
+          <t>Master Premier and Great League Remix | Tales of Transformation</t>
         </is>
       </c>
       <c r="F327" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G327" t="inlineStr"/>
@@ -14030,7 +14030,7 @@
       <c r="O327" t="inlineStr"/>
       <c r="P327" t="inlineStr">
         <is>
-          <t>Raid Battles Mega Mawile and Mega Salamence in Mega Raids Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>GO Battle League Master Premier and Great League Remix | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q327" t="inlineStr">
@@ -14050,12 +14050,12 @@
       <c r="D328" t="inlineStr"/>
       <c r="E328" t="inlineStr">
         <is>
-          <t>Mega Mawile and Mega Salamence in Mega Raids</t>
+          <t>Master Premier and Great League Remix | Tales of Transformation</t>
         </is>
       </c>
       <c r="F328" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G328" t="inlineStr"/>
@@ -14069,7 +14069,7 @@
       <c r="O328" t="inlineStr"/>
       <c r="P328" t="inlineStr">
         <is>
-          <t>Mega Mawile and Mega Salamence in Mega Raids Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Master Premier and Great League Remix | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q328" t="inlineStr">
@@ -14089,12 +14089,12 @@
       <c r="D329" t="inlineStr"/>
       <c r="E329" t="inlineStr">
         <is>
-          <t>Mega Mawile and Mega Salamence in Mega Raids</t>
+          <t>Master Premier and Great League Remix | Tales of Transformation</t>
         </is>
       </c>
       <c r="F329" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G329" t="inlineStr"/>
@@ -14108,7 +14108,7 @@
       <c r="O329" t="inlineStr"/>
       <c r="P329" t="inlineStr">
         <is>
-          <t>Mega Mawile and Mega Salamence in Mega Raids Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Master Premier and Great League Remix | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q329" t="inlineStr">
@@ -14128,12 +14128,12 @@
       <c r="D330" t="inlineStr"/>
       <c r="E330" t="inlineStr">
         <is>
-          <t>Mega Mawile and Mega Salamence in Mega Raids</t>
+          <t>Master Premier and Great League Remix | Tales of Transformation</t>
         </is>
       </c>
       <c r="F330" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G330" t="inlineStr"/>
@@ -14147,7 +14147,7 @@
       <c r="O330" t="inlineStr"/>
       <c r="P330" t="inlineStr">
         <is>
-          <t>Mega Mawile and Mega Salamence in Mega Raids Tue, Oct 14, at 10:00 AM Local Time</t>
+          <t>Master Premier and Great League Remix | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q330" t="inlineStr">
@@ -14167,12 +14167,12 @@
       <c r="D331" t="inlineStr"/>
       <c r="E331" t="inlineStr">
         <is>
-          <t>Master Premier and Great League Remix | Tales of Transformation</t>
+          <t>Petilil Spotlight Hour</t>
         </is>
       </c>
       <c r="F331" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G331" t="inlineStr"/>
@@ -14186,7 +14186,7 @@
       <c r="O331" t="inlineStr"/>
       <c r="P331" t="inlineStr">
         <is>
-          <t>GO Battle League Master Premier and Great League Remix | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Pokémon Spotlight Hour Petilil Spotlight Hour Tue, Oct 14, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q331" t="inlineStr">
@@ -14206,12 +14206,12 @@
       <c r="D332" t="inlineStr"/>
       <c r="E332" t="inlineStr">
         <is>
-          <t>Master Premier and Great League Remix | Tales of Transformation</t>
+          <t>Petilil Spotlight Hour</t>
         </is>
       </c>
       <c r="F332" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G332" t="inlineStr"/>
@@ -14225,7 +14225,7 @@
       <c r="O332" t="inlineStr"/>
       <c r="P332" t="inlineStr">
         <is>
-          <t>Master Premier and Great League Remix | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Petilil Spotlight Hour Tue, Oct 14, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q332" t="inlineStr">
@@ -14245,12 +14245,12 @@
       <c r="D333" t="inlineStr"/>
       <c r="E333" t="inlineStr">
         <is>
-          <t>Master Premier and Great League Remix | Tales of Transformation</t>
+          <t>Petilil Spotlight Hour</t>
         </is>
       </c>
       <c r="F333" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G333" t="inlineStr"/>
@@ -14264,7 +14264,7 @@
       <c r="O333" t="inlineStr"/>
       <c r="P333" t="inlineStr">
         <is>
-          <t>Master Premier and Great League Remix | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Petilil Spotlight Hour Tue, Oct 14, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q333" t="inlineStr">
@@ -14284,12 +14284,12 @@
       <c r="D334" t="inlineStr"/>
       <c r="E334" t="inlineStr">
         <is>
-          <t>Master Premier and Great League Remix | Tales of Transformation</t>
+          <t>Petilil Spotlight Hour</t>
         </is>
       </c>
       <c r="F334" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G334" t="inlineStr"/>
@@ -14303,7 +14303,7 @@
       <c r="O334" t="inlineStr"/>
       <c r="P334" t="inlineStr">
         <is>
-          <t>Master Premier and Great League Remix | Tales of Transformation Calculating...</t>
+          <t>Petilil Spotlight Hour Tue, Oct 14, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q334" t="inlineStr">
@@ -14323,12 +14323,12 @@
       <c r="D335" t="inlineStr"/>
       <c r="E335" t="inlineStr">
         <is>
-          <t>Petilil Spotlight Hour</t>
+          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F335" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G335" t="inlineStr"/>
@@ -14342,7 +14342,7 @@
       <c r="O335" t="inlineStr"/>
       <c r="P335" t="inlineStr">
         <is>
-          <t>Pokémon Spotlight Hour Petilil Spotlight Hour Tue, Oct 14, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Raid Hour Deoxys (Attack &amp; Speed Forme) Raid Hour Wed, Oct 15, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q335" t="inlineStr">
@@ -14362,12 +14362,12 @@
       <c r="D336" t="inlineStr"/>
       <c r="E336" t="inlineStr">
         <is>
-          <t>Petilil Spotlight Hour</t>
+          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F336" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G336" t="inlineStr"/>
@@ -14381,7 +14381,7 @@
       <c r="O336" t="inlineStr"/>
       <c r="P336" t="inlineStr">
         <is>
-          <t>Petilil Spotlight Hour Tue, Oct 14, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour Wed, Oct 15, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q336" t="inlineStr">
@@ -14401,12 +14401,12 @@
       <c r="D337" t="inlineStr"/>
       <c r="E337" t="inlineStr">
         <is>
-          <t>Petilil Spotlight Hour</t>
+          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F337" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G337" t="inlineStr"/>
@@ -14420,7 +14420,7 @@
       <c r="O337" t="inlineStr"/>
       <c r="P337" t="inlineStr">
         <is>
-          <t>Petilil Spotlight Hour Tue, Oct 14, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour Wed, Oct 15, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q337" t="inlineStr">
@@ -14440,12 +14440,12 @@
       <c r="D338" t="inlineStr"/>
       <c r="E338" t="inlineStr">
         <is>
-          <t>Petilil Spotlight Hour</t>
+          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F338" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G338" t="inlineStr"/>
@@ -14459,7 +14459,7 @@
       <c r="O338" t="inlineStr"/>
       <c r="P338" t="inlineStr">
         <is>
-          <t>Petilil Spotlight Hour Tue, Oct 14, at 6:00 PM Local Time</t>
+          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour Wed, Oct 15, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q338" t="inlineStr">
@@ -14479,12 +14479,12 @@
       <c r="D339" t="inlineStr"/>
       <c r="E339" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour</t>
+          <t>Pokémon Legends: Z-A Celebration Event</t>
         </is>
       </c>
       <c r="F339" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G339" t="inlineStr"/>
@@ -14498,7 +14498,7 @@
       <c r="O339" t="inlineStr"/>
       <c r="P339" t="inlineStr">
         <is>
-          <t>Raid Hour Deoxys (Attack &amp; Speed Forme) Raid Hour Wed, Oct 15, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Event Pokémon Legends: Z-A Celebration Event Thu, Oct 16, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q339" t="inlineStr">
@@ -14518,12 +14518,12 @@
       <c r="D340" t="inlineStr"/>
       <c r="E340" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour</t>
+          <t>Pokémon Legends: Z-A Celebration Event</t>
         </is>
       </c>
       <c r="F340" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G340" t="inlineStr"/>
@@ -14537,7 +14537,7 @@
       <c r="O340" t="inlineStr"/>
       <c r="P340" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour Wed, Oct 15, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Pokémon Legends: Z-A Celebration Event Thu, Oct 16, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q340" t="inlineStr">
@@ -14557,12 +14557,12 @@
       <c r="D341" t="inlineStr"/>
       <c r="E341" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour</t>
+          <t>Pokémon Legends: Z-A Celebration Event</t>
         </is>
       </c>
       <c r="F341" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G341" t="inlineStr"/>
@@ -14576,7 +14576,7 @@
       <c r="O341" t="inlineStr"/>
       <c r="P341" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour Wed, Oct 15, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Pokémon Legends: Z-A Celebration Event Thu, Oct 16, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q341" t="inlineStr">
@@ -14596,12 +14596,12 @@
       <c r="D342" t="inlineStr"/>
       <c r="E342" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour</t>
+          <t>Pokémon Legends: Z-A Celebration Event</t>
         </is>
       </c>
       <c r="F342" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G342" t="inlineStr"/>
@@ -14615,7 +14615,7 @@
       <c r="O342" t="inlineStr"/>
       <c r="P342" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour Wed, Oct 15, at 6:00 PM Local Time</t>
+          <t>Pokémon Legends: Z-A Celebration Event Thu, Oct 16, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q342" t="inlineStr">
@@ -14635,12 +14635,12 @@
       <c r="D343" t="inlineStr"/>
       <c r="E343" t="inlineStr">
         <is>
-          <t>Pokémon Legends: Z-A Celebration Event</t>
+          <t>Mega Rayquaza Raid Day</t>
         </is>
       </c>
       <c r="F343" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G343" t="inlineStr"/>
@@ -14654,7 +14654,7 @@
       <c r="O343" t="inlineStr"/>
       <c r="P343" t="inlineStr">
         <is>
-          <t>Event Pokémon Legends: Z-A Celebration Event Thu, Oct 16, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Raid Day Mega Rayquaza Raid Day Sat, Oct 18, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q343" t="inlineStr">
@@ -14674,12 +14674,12 @@
       <c r="D344" t="inlineStr"/>
       <c r="E344" t="inlineStr">
         <is>
-          <t>Pokémon Legends: Z-A Celebration Event</t>
+          <t>Mega Rayquaza Raid Day</t>
         </is>
       </c>
       <c r="F344" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G344" t="inlineStr"/>
@@ -14693,7 +14693,7 @@
       <c r="O344" t="inlineStr"/>
       <c r="P344" t="inlineStr">
         <is>
-          <t>Pokémon Legends: Z-A Celebration Event Thu, Oct 16, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Mega Rayquaza Raid Day Sat, Oct 18, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q344" t="inlineStr">
@@ -14713,12 +14713,12 @@
       <c r="D345" t="inlineStr"/>
       <c r="E345" t="inlineStr">
         <is>
-          <t>Pokémon Legends: Z-A Celebration Event</t>
+          <t>Mega Rayquaza Raid Day</t>
         </is>
       </c>
       <c r="F345" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G345" t="inlineStr"/>
@@ -14732,7 +14732,7 @@
       <c r="O345" t="inlineStr"/>
       <c r="P345" t="inlineStr">
         <is>
-          <t>Pokémon Legends: Z-A Celebration Event Thu, Oct 16, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Mega Rayquaza Raid Day Sat, Oct 18, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q345" t="inlineStr">
@@ -14752,12 +14752,12 @@
       <c r="D346" t="inlineStr"/>
       <c r="E346" t="inlineStr">
         <is>
-          <t>Pokémon Legends: Z-A Celebration Event</t>
+          <t>Mega Rayquaza Raid Day</t>
         </is>
       </c>
       <c r="F346" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G346" t="inlineStr"/>
@@ -14771,7 +14771,7 @@
       <c r="O346" t="inlineStr"/>
       <c r="P346" t="inlineStr">
         <is>
-          <t>Pokémon Legends: Z-A Celebration Event Thu, Oct 16, at 10:00 AM Local Time</t>
+          <t>Mega Rayquaza Raid Day Sat, Oct 18, at 2:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q346" t="inlineStr">
@@ -14791,12 +14791,12 @@
       <c r="D347" t="inlineStr"/>
       <c r="E347" t="inlineStr">
         <is>
-          <t>Mega Rayquaza Raid Day</t>
+          <t>Dynamax Gastly during Max Monday</t>
         </is>
       </c>
       <c r="F347" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G347" t="inlineStr"/>
@@ -14810,7 +14810,7 @@
       <c r="O347" t="inlineStr"/>
       <c r="P347" t="inlineStr">
         <is>
-          <t>Raid Day Mega Rayquaza Raid Day Sat, Oct 18, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Max Mondays Dynamax Gastly during Max Monday Mon, Oct 20, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q347" t="inlineStr">
@@ -14830,12 +14830,12 @@
       <c r="D348" t="inlineStr"/>
       <c r="E348" t="inlineStr">
         <is>
-          <t>Mega Rayquaza Raid Day</t>
+          <t>Dynamax Gastly during Max Monday</t>
         </is>
       </c>
       <c r="F348" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G348" t="inlineStr"/>
@@ -14849,7 +14849,7 @@
       <c r="O348" t="inlineStr"/>
       <c r="P348" t="inlineStr">
         <is>
-          <t>Mega Rayquaza Raid Day Sat, Oct 18, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Dynamax Gastly during Max Monday Mon, Oct 20, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q348" t="inlineStr">
@@ -14869,12 +14869,12 @@
       <c r="D349" t="inlineStr"/>
       <c r="E349" t="inlineStr">
         <is>
-          <t>Mega Rayquaza Raid Day</t>
+          <t>Dynamax Gastly during Max Monday</t>
         </is>
       </c>
       <c r="F349" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G349" t="inlineStr"/>
@@ -14888,7 +14888,7 @@
       <c r="O349" t="inlineStr"/>
       <c r="P349" t="inlineStr">
         <is>
-          <t>Mega Rayquaza Raid Day Sat, Oct 18, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Dynamax Gastly during Max Monday Mon, Oct 20, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q349" t="inlineStr">
@@ -14908,12 +14908,12 @@
       <c r="D350" t="inlineStr"/>
       <c r="E350" t="inlineStr">
         <is>
-          <t>Mega Rayquaza Raid Day</t>
+          <t>Dynamax Gastly during Max Monday</t>
         </is>
       </c>
       <c r="F350" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G350" t="inlineStr"/>
@@ -14927,7 +14927,7 @@
       <c r="O350" t="inlineStr"/>
       <c r="P350" t="inlineStr">
         <is>
-          <t>Mega Rayquaza Raid Day Sat, Oct 18, at 2:00 PM Local Time</t>
+          <t>Dynamax Gastly during Max Monday Mon, Oct 20, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q350" t="inlineStr">
@@ -14947,7 +14947,7 @@
       <c r="D351" t="inlineStr"/>
       <c r="E351" t="inlineStr">
         <is>
-          <t>Dynamax Gastly during Max Monday</t>
+          <t>Halloween 2025 Part I</t>
         </is>
       </c>
       <c r="F351" t="inlineStr">
@@ -14966,7 +14966,7 @@
       <c r="O351" t="inlineStr"/>
       <c r="P351" t="inlineStr">
         <is>
-          <t>Max Mondays Dynamax Gastly during Max Monday Mon, Oct 20, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Event Halloween 2025 Part I Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q351" t="inlineStr">
@@ -14986,7 +14986,7 @@
       <c r="D352" t="inlineStr"/>
       <c r="E352" t="inlineStr">
         <is>
-          <t>Dynamax Gastly during Max Monday</t>
+          <t>Halloween 2025 Part I</t>
         </is>
       </c>
       <c r="F352" t="inlineStr">
@@ -15005,7 +15005,7 @@
       <c r="O352" t="inlineStr"/>
       <c r="P352" t="inlineStr">
         <is>
-          <t>Dynamax Gastly during Max Monday Mon, Oct 20, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Halloween 2025 Part I Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q352" t="inlineStr">
@@ -15025,7 +15025,7 @@
       <c r="D353" t="inlineStr"/>
       <c r="E353" t="inlineStr">
         <is>
-          <t>Dynamax Gastly during Max Monday</t>
+          <t>Halloween 2025 Part I</t>
         </is>
       </c>
       <c r="F353" t="inlineStr">
@@ -15044,7 +15044,7 @@
       <c r="O353" t="inlineStr"/>
       <c r="P353" t="inlineStr">
         <is>
-          <t>Dynamax Gastly during Max Monday Mon, Oct 20, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Halloween 2025 Part I Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q353" t="inlineStr">
@@ -15064,7 +15064,7 @@
       <c r="D354" t="inlineStr"/>
       <c r="E354" t="inlineStr">
         <is>
-          <t>Dynamax Gastly during Max Monday</t>
+          <t>Halloween 2025 Part I</t>
         </is>
       </c>
       <c r="F354" t="inlineStr">
@@ -15083,7 +15083,7 @@
       <c r="O354" t="inlineStr"/>
       <c r="P354" t="inlineStr">
         <is>
-          <t>Dynamax Gastly during Max Monday Mon, Oct 20, at 6:00 PM Local Time</t>
+          <t>Halloween 2025 Part I Tue, Oct 21, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q354" t="inlineStr">
@@ -15103,12 +15103,12 @@
       <c r="D355" t="inlineStr"/>
       <c r="E355" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part I</t>
+          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F355" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G355" t="inlineStr"/>
@@ -15122,7 +15122,7 @@
       <c r="O355" t="inlineStr"/>
       <c r="P355" t="inlineStr">
         <is>
-          <t>Event Halloween 2025 Part I Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Raid Battles Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q355" t="inlineStr">
@@ -15142,12 +15142,12 @@
       <c r="D356" t="inlineStr"/>
       <c r="E356" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part I</t>
+          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F356" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G356" t="inlineStr"/>
@@ -15161,7 +15161,7 @@
       <c r="O356" t="inlineStr"/>
       <c r="P356" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part I Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q356" t="inlineStr">
@@ -15181,12 +15181,12 @@
       <c r="D357" t="inlineStr"/>
       <c r="E357" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part I</t>
+          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F357" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G357" t="inlineStr"/>
@@ -15200,7 +15200,7 @@
       <c r="O357" t="inlineStr"/>
       <c r="P357" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part I Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q357" t="inlineStr">
@@ -15220,12 +15220,12 @@
       <c r="D358" t="inlineStr"/>
       <c r="E358" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part I</t>
+          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F358" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G358" t="inlineStr"/>
@@ -15239,7 +15239,7 @@
       <c r="O358" t="inlineStr"/>
       <c r="P358" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part I Tue, Oct 21, at 10:00 AM Local Time</t>
+          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles Tue, Oct 21, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q358" t="inlineStr">
@@ -15259,7 +15259,7 @@
       <c r="D359" t="inlineStr"/>
       <c r="E359" t="inlineStr">
         <is>
-          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles</t>
+          <t>Mega Houndoom and Mega Absol in Mega Raids</t>
         </is>
       </c>
       <c r="F359" t="inlineStr">
@@ -15278,7 +15278,7 @@
       <c r="O359" t="inlineStr"/>
       <c r="P359" t="inlineStr">
         <is>
-          <t>Raid Battles Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Raid Battles Mega Houndoom and Mega Absol in Mega Raids Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q359" t="inlineStr">
@@ -15298,7 +15298,7 @@
       <c r="D360" t="inlineStr"/>
       <c r="E360" t="inlineStr">
         <is>
-          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles</t>
+          <t>Mega Houndoom and Mega Absol in Mega Raids</t>
         </is>
       </c>
       <c r="F360" t="inlineStr">
@@ -15317,7 +15317,7 @@
       <c r="O360" t="inlineStr"/>
       <c r="P360" t="inlineStr">
         <is>
-          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Mega Houndoom and Mega Absol in Mega Raids Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q360" t="inlineStr">
@@ -15337,7 +15337,7 @@
       <c r="D361" t="inlineStr"/>
       <c r="E361" t="inlineStr">
         <is>
-          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles</t>
+          <t>Mega Houndoom and Mega Absol in Mega Raids</t>
         </is>
       </c>
       <c r="F361" t="inlineStr">
@@ -15356,7 +15356,7 @@
       <c r="O361" t="inlineStr"/>
       <c r="P361" t="inlineStr">
         <is>
-          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Mega Houndoom and Mega Absol in Mega Raids Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q361" t="inlineStr">
@@ -15376,7 +15376,7 @@
       <c r="D362" t="inlineStr"/>
       <c r="E362" t="inlineStr">
         <is>
-          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles</t>
+          <t>Mega Houndoom and Mega Absol in Mega Raids</t>
         </is>
       </c>
       <c r="F362" t="inlineStr">
@@ -15395,7 +15395,7 @@
       <c r="O362" t="inlineStr"/>
       <c r="P362" t="inlineStr">
         <is>
-          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles Tue, Oct 21, at 10:00 AM Local Time</t>
+          <t>Mega Houndoom and Mega Absol in Mega Raids Tue, Oct 21, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q362" t="inlineStr">
@@ -15415,12 +15415,12 @@
       <c r="D363" t="inlineStr"/>
       <c r="E363" t="inlineStr">
         <is>
-          <t>Mega Houndoom and Mega Absol in Mega Raids</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F363" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G363" t="inlineStr"/>
@@ -15434,7 +15434,7 @@
       <c r="O363" t="inlineStr"/>
       <c r="P363" t="inlineStr">
         <is>
-          <t>Raid Battles Mega Houndoom and Mega Absol in Mega Raids Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>GO Battle League Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q363" t="inlineStr">
@@ -15454,12 +15454,12 @@
       <c r="D364" t="inlineStr"/>
       <c r="E364" t="inlineStr">
         <is>
-          <t>Mega Houndoom and Mega Absol in Mega Raids</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F364" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G364" t="inlineStr"/>
@@ -15473,7 +15473,7 @@
       <c r="O364" t="inlineStr"/>
       <c r="P364" t="inlineStr">
         <is>
-          <t>Mega Houndoom and Mega Absol in Mega Raids Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q364" t="inlineStr">
@@ -15493,12 +15493,12 @@
       <c r="D365" t="inlineStr"/>
       <c r="E365" t="inlineStr">
         <is>
-          <t>Mega Houndoom and Mega Absol in Mega Raids</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F365" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G365" t="inlineStr"/>
@@ -15512,7 +15512,7 @@
       <c r="O365" t="inlineStr"/>
       <c r="P365" t="inlineStr">
         <is>
-          <t>Mega Houndoom and Mega Absol in Mega Raids Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q365" t="inlineStr">
@@ -15532,12 +15532,12 @@
       <c r="D366" t="inlineStr"/>
       <c r="E366" t="inlineStr">
         <is>
-          <t>Mega Houndoom and Mega Absol in Mega Raids</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F366" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G366" t="inlineStr"/>
@@ -15551,7 +15551,7 @@
       <c r="O366" t="inlineStr"/>
       <c r="P366" t="inlineStr">
         <is>
-          <t>Mega Houndoom and Mega Absol in Mega Raids Tue, Oct 21, at 10:00 AM Local Time</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q366" t="inlineStr">
@@ -15571,12 +15571,12 @@
       <c r="D367" t="inlineStr"/>
       <c r="E367" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Gastly Spotlight Hour</t>
         </is>
       </c>
       <c r="F367" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G367" t="inlineStr"/>
@@ -15590,7 +15590,7 @@
       <c r="O367" t="inlineStr"/>
       <c r="P367" t="inlineStr">
         <is>
-          <t>GO Battle League Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Pokémon Spotlight Hour Gastly Spotlight Hour Tue, Oct 21, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q367" t="inlineStr">
@@ -15610,12 +15610,12 @@
       <c r="D368" t="inlineStr"/>
       <c r="E368" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Gastly Spotlight Hour</t>
         </is>
       </c>
       <c r="F368" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G368" t="inlineStr"/>
@@ -15629,7 +15629,7 @@
       <c r="O368" t="inlineStr"/>
       <c r="P368" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Gastly Spotlight Hour Tue, Oct 21, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q368" t="inlineStr">
@@ -15649,12 +15649,12 @@
       <c r="D369" t="inlineStr"/>
       <c r="E369" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Gastly Spotlight Hour</t>
         </is>
       </c>
       <c r="F369" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G369" t="inlineStr"/>
@@ -15668,7 +15668,7 @@
       <c r="O369" t="inlineStr"/>
       <c r="P369" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Gastly Spotlight Hour Tue, Oct 21, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q369" t="inlineStr">
@@ -15688,12 +15688,12 @@
       <c r="D370" t="inlineStr"/>
       <c r="E370" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Gastly Spotlight Hour</t>
         </is>
       </c>
       <c r="F370" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G370" t="inlineStr"/>
@@ -15707,7 +15707,7 @@
       <c r="O370" t="inlineStr"/>
       <c r="P370" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating...</t>
+          <t>Gastly Spotlight Hour Tue, Oct 21, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q370" t="inlineStr">
@@ -15727,12 +15727,12 @@
       <c r="D371" t="inlineStr"/>
       <c r="E371" t="inlineStr">
         <is>
-          <t>Gastly Spotlight Hour</t>
+          <t>Genesect Raid Hour</t>
         </is>
       </c>
       <c r="F371" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G371" t="inlineStr"/>
@@ -15746,7 +15746,7 @@
       <c r="O371" t="inlineStr"/>
       <c r="P371" t="inlineStr">
         <is>
-          <t>Pokémon Spotlight Hour Gastly Spotlight Hour Tue, Oct 21, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Raid Hour Genesect Raid Hour Wed, Oct 22, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q371" t="inlineStr">
@@ -15766,12 +15766,12 @@
       <c r="D372" t="inlineStr"/>
       <c r="E372" t="inlineStr">
         <is>
-          <t>Gastly Spotlight Hour</t>
+          <t>Genesect Raid Hour</t>
         </is>
       </c>
       <c r="F372" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G372" t="inlineStr"/>
@@ -15785,7 +15785,7 @@
       <c r="O372" t="inlineStr"/>
       <c r="P372" t="inlineStr">
         <is>
-          <t>Gastly Spotlight Hour Tue, Oct 21, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Genesect Raid Hour Wed, Oct 22, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q372" t="inlineStr">
@@ -15805,12 +15805,12 @@
       <c r="D373" t="inlineStr"/>
       <c r="E373" t="inlineStr">
         <is>
-          <t>Gastly Spotlight Hour</t>
+          <t>Genesect Raid Hour</t>
         </is>
       </c>
       <c r="F373" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G373" t="inlineStr"/>
@@ -15824,7 +15824,7 @@
       <c r="O373" t="inlineStr"/>
       <c r="P373" t="inlineStr">
         <is>
-          <t>Gastly Spotlight Hour Tue, Oct 21, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Genesect Raid Hour Wed, Oct 22, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q373" t="inlineStr">
@@ -15844,12 +15844,12 @@
       <c r="D374" t="inlineStr"/>
       <c r="E374" t="inlineStr">
         <is>
-          <t>Gastly Spotlight Hour</t>
+          <t>Genesect Raid Hour</t>
         </is>
       </c>
       <c r="F374" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G374" t="inlineStr"/>
@@ -15863,7 +15863,7 @@
       <c r="O374" t="inlineStr"/>
       <c r="P374" t="inlineStr">
         <is>
-          <t>Gastly Spotlight Hour Tue, Oct 21, at 6:00 PM Local Time</t>
+          <t>Genesect Raid Hour Wed, Oct 22, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q374" t="inlineStr">
@@ -15883,12 +15883,12 @@
       <c r="D375" t="inlineStr"/>
       <c r="E375" t="inlineStr">
         <is>
-          <t>Genesect Raid Hour</t>
+          <t>GO Battle Weekend: Tales of Transformation</t>
         </is>
       </c>
       <c r="F375" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G375" t="inlineStr"/>
@@ -15902,7 +15902,7 @@
       <c r="O375" t="inlineStr"/>
       <c r="P375" t="inlineStr">
         <is>
-          <t>Raid Hour Genesect Raid Hour Wed, Oct 22, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Event GO Battle Weekend: Tales of Transformation Sat, Oct 25, at 12:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q375" t="inlineStr">
@@ -15922,12 +15922,12 @@
       <c r="D376" t="inlineStr"/>
       <c r="E376" t="inlineStr">
         <is>
-          <t>Genesect Raid Hour</t>
+          <t>GO Battle Weekend: Tales of Transformation</t>
         </is>
       </c>
       <c r="F376" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G376" t="inlineStr"/>
@@ -15941,7 +15941,7 @@
       <c r="O376" t="inlineStr"/>
       <c r="P376" t="inlineStr">
         <is>
-          <t>Genesect Raid Hour Wed, Oct 22, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>GO Battle Weekend: Tales of Transformation Sat, Oct 25, at 12:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q376" t="inlineStr">
@@ -15961,12 +15961,12 @@
       <c r="D377" t="inlineStr"/>
       <c r="E377" t="inlineStr">
         <is>
-          <t>Genesect Raid Hour</t>
+          <t>GO Battle Weekend: Tales of Transformation</t>
         </is>
       </c>
       <c r="F377" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G377" t="inlineStr"/>
@@ -15980,7 +15980,7 @@
       <c r="O377" t="inlineStr"/>
       <c r="P377" t="inlineStr">
         <is>
-          <t>Genesect Raid Hour Wed, Oct 22, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>GO Battle Weekend: Tales of Transformation Sat, Oct 25, at 12:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q377" t="inlineStr">
@@ -16000,12 +16000,12 @@
       <c r="D378" t="inlineStr"/>
       <c r="E378" t="inlineStr">
         <is>
-          <t>Genesect Raid Hour</t>
+          <t>GO Battle Weekend: Tales of Transformation</t>
         </is>
       </c>
       <c r="F378" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G378" t="inlineStr"/>
@@ -16019,7 +16019,7 @@
       <c r="O378" t="inlineStr"/>
       <c r="P378" t="inlineStr">
         <is>
-          <t>Genesect Raid Hour Wed, Oct 22, at 6:00 PM Local Time</t>
+          <t>GO Battle Weekend: Tales of Transformation Sat, Oct 25, at 12:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q378" t="inlineStr">
@@ -16039,7 +16039,7 @@
       <c r="D379" t="inlineStr"/>
       <c r="E379" t="inlineStr">
         <is>
-          <t>GO Battle Weekend: Tales of Transformation</t>
+          <t>Halloween 2025 Part II</t>
         </is>
       </c>
       <c r="F379" t="inlineStr">
@@ -16058,7 +16058,7 @@
       <c r="O379" t="inlineStr"/>
       <c r="P379" t="inlineStr">
         <is>
-          <t>Event GO Battle Weekend: Tales of Transformation Sat, Oct 25, at 12:00 AM Local Time Starts: Calculating...</t>
+          <t>Event Halloween 2025 Part II Mon, Oct 27, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q379" t="inlineStr">
@@ -16078,7 +16078,7 @@
       <c r="D380" t="inlineStr"/>
       <c r="E380" t="inlineStr">
         <is>
-          <t>GO Battle Weekend: Tales of Transformation</t>
+          <t>Halloween 2025 Part II</t>
         </is>
       </c>
       <c r="F380" t="inlineStr">
@@ -16097,7 +16097,7 @@
       <c r="O380" t="inlineStr"/>
       <c r="P380" t="inlineStr">
         <is>
-          <t>GO Battle Weekend: Tales of Transformation Sat, Oct 25, at 12:00 AM Local Time Starts: Calculating...</t>
+          <t>Halloween 2025 Part II Mon, Oct 27, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q380" t="inlineStr">
@@ -16117,7 +16117,7 @@
       <c r="D381" t="inlineStr"/>
       <c r="E381" t="inlineStr">
         <is>
-          <t>GO Battle Weekend: Tales of Transformation</t>
+          <t>Halloween 2025 Part II</t>
         </is>
       </c>
       <c r="F381" t="inlineStr">
@@ -16136,7 +16136,7 @@
       <c r="O381" t="inlineStr"/>
       <c r="P381" t="inlineStr">
         <is>
-          <t>GO Battle Weekend: Tales of Transformation Sat, Oct 25, at 12:00 AM Local Time Starts: Calculating...</t>
+          <t>Halloween 2025 Part II Mon, Oct 27, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q381" t="inlineStr">
@@ -16156,7 +16156,7 @@
       <c r="D382" t="inlineStr"/>
       <c r="E382" t="inlineStr">
         <is>
-          <t>GO Battle Weekend: Tales of Transformation</t>
+          <t>Halloween 2025 Part II</t>
         </is>
       </c>
       <c r="F382" t="inlineStr">
@@ -16175,7 +16175,7 @@
       <c r="O382" t="inlineStr"/>
       <c r="P382" t="inlineStr">
         <is>
-          <t>GO Battle Weekend: Tales of Transformation Sat, Oct 25, at 12:00 AM Local Time</t>
+          <t>Halloween 2025 Part II Mon, Oct 27, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q382" t="inlineStr">
@@ -16195,7 +16195,7 @@
       <c r="D383" t="inlineStr"/>
       <c r="E383" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part II</t>
+          <t>Dynamax Woobat during Max Monday</t>
         </is>
       </c>
       <c r="F383" t="inlineStr">
@@ -16214,7 +16214,7 @@
       <c r="O383" t="inlineStr"/>
       <c r="P383" t="inlineStr">
         <is>
-          <t>Event Halloween 2025 Part II Mon, Oct 27, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Max Mondays Dynamax Woobat during Max Monday Mon, Oct 27, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q383" t="inlineStr">
@@ -16234,7 +16234,7 @@
       <c r="D384" t="inlineStr"/>
       <c r="E384" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part II</t>
+          <t>Dynamax Woobat during Max Monday</t>
         </is>
       </c>
       <c r="F384" t="inlineStr">
@@ -16253,7 +16253,7 @@
       <c r="O384" t="inlineStr"/>
       <c r="P384" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part II Mon, Oct 27, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Dynamax Woobat during Max Monday Mon, Oct 27, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q384" t="inlineStr">
@@ -16273,7 +16273,7 @@
       <c r="D385" t="inlineStr"/>
       <c r="E385" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part II</t>
+          <t>Dynamax Woobat during Max Monday</t>
         </is>
       </c>
       <c r="F385" t="inlineStr">
@@ -16292,7 +16292,7 @@
       <c r="O385" t="inlineStr"/>
       <c r="P385" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part II Mon, Oct 27, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Dynamax Woobat during Max Monday Mon, Oct 27, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q385" t="inlineStr">
@@ -16312,7 +16312,7 @@
       <c r="D386" t="inlineStr"/>
       <c r="E386" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part II</t>
+          <t>Dynamax Woobat during Max Monday</t>
         </is>
       </c>
       <c r="F386" t="inlineStr">
@@ -16331,7 +16331,7 @@
       <c r="O386" t="inlineStr"/>
       <c r="P386" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part II Mon, Oct 27, at 10:00 AM Local Time</t>
+          <t>Dynamax Woobat during Max Monday Mon, Oct 27, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q386" t="inlineStr">
@@ -16351,12 +16351,12 @@
       <c r="D387" t="inlineStr"/>
       <c r="E387" t="inlineStr">
         <is>
-          <t>Dynamax Woobat during Max Monday</t>
+          <t>Giratina (Altered Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F387" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G387" t="inlineStr"/>
@@ -16370,7 +16370,7 @@
       <c r="O387" t="inlineStr"/>
       <c r="P387" t="inlineStr">
         <is>
-          <t>Max Mondays Dynamax Woobat during Max Monday Mon, Oct 27, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Raid Battles Giratina (Altered Forme) in 5-star Raid Battles Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q387" t="inlineStr">
@@ -16390,12 +16390,12 @@
       <c r="D388" t="inlineStr"/>
       <c r="E388" t="inlineStr">
         <is>
-          <t>Dynamax Woobat during Max Monday</t>
+          <t>Giratina (Altered Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F388" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G388" t="inlineStr"/>
@@ -16409,7 +16409,7 @@
       <c r="O388" t="inlineStr"/>
       <c r="P388" t="inlineStr">
         <is>
-          <t>Dynamax Woobat during Max Monday Mon, Oct 27, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Giratina (Altered Forme) in 5-star Raid Battles Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q388" t="inlineStr">
@@ -16429,12 +16429,12 @@
       <c r="D389" t="inlineStr"/>
       <c r="E389" t="inlineStr">
         <is>
-          <t>Dynamax Woobat during Max Monday</t>
+          <t>Giratina (Altered Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F389" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G389" t="inlineStr"/>
@@ -16448,7 +16448,7 @@
       <c r="O389" t="inlineStr"/>
       <c r="P389" t="inlineStr">
         <is>
-          <t>Dynamax Woobat during Max Monday Mon, Oct 27, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Giratina (Altered Forme) in 5-star Raid Battles Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q389" t="inlineStr">
@@ -16468,12 +16468,12 @@
       <c r="D390" t="inlineStr"/>
       <c r="E390" t="inlineStr">
         <is>
-          <t>Dynamax Woobat during Max Monday</t>
+          <t>Giratina (Altered Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F390" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G390" t="inlineStr"/>
@@ -16487,7 +16487,7 @@
       <c r="O390" t="inlineStr"/>
       <c r="P390" t="inlineStr">
         <is>
-          <t>Dynamax Woobat during Max Monday Mon, Oct 27, at 6:00 PM Local Time</t>
+          <t>Giratina (Altered Forme) in 5-star Raid Battles Tue, Oct 28, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q390" t="inlineStr">
@@ -16507,7 +16507,7 @@
       <c r="D391" t="inlineStr"/>
       <c r="E391" t="inlineStr">
         <is>
-          <t>Giratina (Altered Forme) in 5-star Raid Battles</t>
+          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids</t>
         </is>
       </c>
       <c r="F391" t="inlineStr">
@@ -16526,7 +16526,7 @@
       <c r="O391" t="inlineStr"/>
       <c r="P391" t="inlineStr">
         <is>
-          <t>Raid Battles Giratina (Altered Forme) in 5-star Raid Battles Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Raid Battles Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q391" t="inlineStr">
@@ -16546,7 +16546,7 @@
       <c r="D392" t="inlineStr"/>
       <c r="E392" t="inlineStr">
         <is>
-          <t>Giratina (Altered Forme) in 5-star Raid Battles</t>
+          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids</t>
         </is>
       </c>
       <c r="F392" t="inlineStr">
@@ -16565,7 +16565,7 @@
       <c r="O392" t="inlineStr"/>
       <c r="P392" t="inlineStr">
         <is>
-          <t>Giratina (Altered Forme) in 5-star Raid Battles Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q392" t="inlineStr">
@@ -16585,7 +16585,7 @@
       <c r="D393" t="inlineStr"/>
       <c r="E393" t="inlineStr">
         <is>
-          <t>Giratina (Altered Forme) in 5-star Raid Battles</t>
+          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids</t>
         </is>
       </c>
       <c r="F393" t="inlineStr">
@@ -16604,7 +16604,7 @@
       <c r="O393" t="inlineStr"/>
       <c r="P393" t="inlineStr">
         <is>
-          <t>Giratina (Altered Forme) in 5-star Raid Battles Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q393" t="inlineStr">
@@ -16624,7 +16624,7 @@
       <c r="D394" t="inlineStr"/>
       <c r="E394" t="inlineStr">
         <is>
-          <t>Giratina (Altered Forme) in 5-star Raid Battles</t>
+          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids</t>
         </is>
       </c>
       <c r="F394" t="inlineStr">
@@ -16643,7 +16643,7 @@
       <c r="O394" t="inlineStr"/>
       <c r="P394" t="inlineStr">
         <is>
-          <t>Giratina (Altered Forme) in 5-star Raid Battles Tue, Oct 28, at 10:00 AM Local Time</t>
+          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids Tue, Oct 28, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q394" t="inlineStr">
@@ -16663,12 +16663,12 @@
       <c r="D395" t="inlineStr"/>
       <c r="E395" t="inlineStr">
         <is>
-          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids</t>
+          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F395" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G395" t="inlineStr"/>
@@ -16682,7 +16682,7 @@
       <c r="O395" t="inlineStr"/>
       <c r="P395" t="inlineStr">
         <is>
-          <t>Raid Battles Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>GO Battle League Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q395" t="inlineStr">
@@ -16702,12 +16702,12 @@
       <c r="D396" t="inlineStr"/>
       <c r="E396" t="inlineStr">
         <is>
-          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids</t>
+          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F396" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G396" t="inlineStr"/>
@@ -16721,7 +16721,7 @@
       <c r="O396" t="inlineStr"/>
       <c r="P396" t="inlineStr">
         <is>
-          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q396" t="inlineStr">
@@ -16741,12 +16741,12 @@
       <c r="D397" t="inlineStr"/>
       <c r="E397" t="inlineStr">
         <is>
-          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids</t>
+          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F397" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G397" t="inlineStr"/>
@@ -16760,7 +16760,7 @@
       <c r="O397" t="inlineStr"/>
       <c r="P397" t="inlineStr">
         <is>
-          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q397" t="inlineStr">
@@ -16780,12 +16780,12 @@
       <c r="D398" t="inlineStr"/>
       <c r="E398" t="inlineStr">
         <is>
-          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids</t>
+          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F398" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G398" t="inlineStr"/>
@@ -16799,7 +16799,7 @@
       <c r="O398" t="inlineStr"/>
       <c r="P398" t="inlineStr">
         <is>
-          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids Tue, Oct 28, at 10:00 AM Local Time</t>
+          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q398" t="inlineStr">
@@ -16819,12 +16819,12 @@
       <c r="D399" t="inlineStr"/>
       <c r="E399" t="inlineStr">
         <is>
-          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation</t>
+          <t>Sinistea Spotlight Hour</t>
         </is>
       </c>
       <c r="F399" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G399" t="inlineStr"/>
@@ -16838,7 +16838,7 @@
       <c r="O399" t="inlineStr"/>
       <c r="P399" t="inlineStr">
         <is>
-          <t>GO Battle League Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Pokémon Spotlight Hour Sinistea Spotlight Hour Tue, Oct 28, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q399" t="inlineStr">
@@ -16858,12 +16858,12 @@
       <c r="D400" t="inlineStr"/>
       <c r="E400" t="inlineStr">
         <is>
-          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation</t>
+          <t>Sinistea Spotlight Hour</t>
         </is>
       </c>
       <c r="F400" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G400" t="inlineStr"/>
@@ -16877,7 +16877,7 @@
       <c r="O400" t="inlineStr"/>
       <c r="P400" t="inlineStr">
         <is>
-          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Sinistea Spotlight Hour Tue, Oct 28, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q400" t="inlineStr">
@@ -16897,12 +16897,12 @@
       <c r="D401" t="inlineStr"/>
       <c r="E401" t="inlineStr">
         <is>
-          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation</t>
+          <t>Sinistea Spotlight Hour</t>
         </is>
       </c>
       <c r="F401" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G401" t="inlineStr"/>
@@ -16916,7 +16916,7 @@
       <c r="O401" t="inlineStr"/>
       <c r="P401" t="inlineStr">
         <is>
-          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Sinistea Spotlight Hour Tue, Oct 28, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q401" t="inlineStr">
@@ -16936,12 +16936,12 @@
       <c r="D402" t="inlineStr"/>
       <c r="E402" t="inlineStr">
         <is>
-          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation</t>
+          <t>Sinistea Spotlight Hour</t>
         </is>
       </c>
       <c r="F402" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G402" t="inlineStr"/>
@@ -16955,7 +16955,7 @@
       <c r="O402" t="inlineStr"/>
       <c r="P402" t="inlineStr">
         <is>
-          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating...</t>
+          <t>Sinistea Spotlight Hour Tue, Oct 28, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q402" t="inlineStr">
@@ -16975,12 +16975,12 @@
       <c r="D403" t="inlineStr"/>
       <c r="E403" t="inlineStr">
         <is>
-          <t>Sinistea Spotlight Hour</t>
+          <t>Giratina (Origin Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F403" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G403" t="inlineStr"/>
@@ -16994,7 +16994,7 @@
       <c r="O403" t="inlineStr"/>
       <c r="P403" t="inlineStr">
         <is>
-          <t>Pokémon Spotlight Hour Sinistea Spotlight Hour Tue, Oct 28, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Raid Hour Giratina (Origin Forme) Raid Hour Wed, Oct 29, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q403" t="inlineStr">
@@ -17014,12 +17014,12 @@
       <c r="D404" t="inlineStr"/>
       <c r="E404" t="inlineStr">
         <is>
-          <t>Sinistea Spotlight Hour</t>
+          <t>Giratina (Origin Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F404" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G404" t="inlineStr"/>
@@ -17033,7 +17033,7 @@
       <c r="O404" t="inlineStr"/>
       <c r="P404" t="inlineStr">
         <is>
-          <t>Sinistea Spotlight Hour Tue, Oct 28, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Giratina (Origin Forme) Raid Hour Wed, Oct 29, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q404" t="inlineStr">
@@ -17053,12 +17053,12 @@
       <c r="D405" t="inlineStr"/>
       <c r="E405" t="inlineStr">
         <is>
-          <t>Sinistea Spotlight Hour</t>
+          <t>Giratina (Origin Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F405" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G405" t="inlineStr"/>
@@ -17072,7 +17072,7 @@
       <c r="O405" t="inlineStr"/>
       <c r="P405" t="inlineStr">
         <is>
-          <t>Sinistea Spotlight Hour Tue, Oct 28, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Giratina (Origin Forme) Raid Hour Wed, Oct 29, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q405" t="inlineStr">
@@ -17092,12 +17092,12 @@
       <c r="D406" t="inlineStr"/>
       <c r="E406" t="inlineStr">
         <is>
-          <t>Sinistea Spotlight Hour</t>
+          <t>Giratina (Origin Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F406" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G406" t="inlineStr"/>
@@ -17111,7 +17111,7 @@
       <c r="O406" t="inlineStr"/>
       <c r="P406" t="inlineStr">
         <is>
-          <t>Sinistea Spotlight Hour Tue, Oct 28, at 6:00 PM Local Time</t>
+          <t>Giratina (Origin Forme) Raid Hour Wed, Oct 29, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q406" t="inlineStr">
@@ -17131,12 +17131,12 @@
       <c r="D407" t="inlineStr"/>
       <c r="E407" t="inlineStr">
         <is>
-          <t>Giratina (Origin Forme) Raid Hour</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F407" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G407" t="inlineStr"/>
@@ -17150,7 +17150,7 @@
       <c r="O407" t="inlineStr"/>
       <c r="P407" t="inlineStr">
         <is>
-          <t>Raid Hour Giratina (Origin Forme) Raid Hour Wed, Oct 29, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>GO Battle League Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q407" t="inlineStr">
@@ -17170,12 +17170,12 @@
       <c r="D408" t="inlineStr"/>
       <c r="E408" t="inlineStr">
         <is>
-          <t>Giratina (Origin Forme) Raid Hour</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F408" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G408" t="inlineStr"/>
@@ -17189,7 +17189,7 @@
       <c r="O408" t="inlineStr"/>
       <c r="P408" t="inlineStr">
         <is>
-          <t>Giratina (Origin Forme) Raid Hour Wed, Oct 29, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q408" t="inlineStr">
@@ -17209,12 +17209,12 @@
       <c r="D409" t="inlineStr"/>
       <c r="E409" t="inlineStr">
         <is>
-          <t>Giratina (Origin Forme) Raid Hour</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F409" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G409" t="inlineStr"/>
@@ -17228,7 +17228,7 @@
       <c r="O409" t="inlineStr"/>
       <c r="P409" t="inlineStr">
         <is>
-          <t>Giratina (Origin Forme) Raid Hour Wed, Oct 29, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q409" t="inlineStr">
@@ -17248,12 +17248,12 @@
       <c r="D410" t="inlineStr"/>
       <c r="E410" t="inlineStr">
         <is>
-          <t>Giratina (Origin Forme) Raid Hour</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F410" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G410" t="inlineStr"/>
@@ -17267,7 +17267,7 @@
       <c r="O410" t="inlineStr"/>
       <c r="P410" t="inlineStr">
         <is>
-          <t>Giratina (Origin Forme) Raid Hour Wed, Oct 29, at 6:00 PM Local Time</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q410" t="inlineStr">
@@ -17287,7 +17287,7 @@
       <c r="D411" t="inlineStr"/>
       <c r="E411" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
+          <t>Pokémon GO Wild Area: Nagasaki</t>
         </is>
       </c>
       <c r="F411" t="inlineStr">
@@ -17306,7 +17306,7 @@
       <c r="O411" t="inlineStr"/>
       <c r="P411" t="inlineStr">
         <is>
-          <t>GO Battle League Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Wild Area Pokémon GO Wild Area: Nagasaki Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q411" t="inlineStr">
@@ -17326,7 +17326,7 @@
       <c r="D412" t="inlineStr"/>
       <c r="E412" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
+          <t>Pokémon GO Wild Area: Nagasaki</t>
         </is>
       </c>
       <c r="F412" t="inlineStr">
@@ -17345,7 +17345,7 @@
       <c r="O412" t="inlineStr"/>
       <c r="P412" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Pokémon GO Wild Area: Nagasaki Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q412" t="inlineStr">
@@ -17365,7 +17365,7 @@
       <c r="D413" t="inlineStr"/>
       <c r="E413" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
+          <t>Pokémon GO Wild Area: Nagasaki</t>
         </is>
       </c>
       <c r="F413" t="inlineStr">
@@ -17384,7 +17384,7 @@
       <c r="O413" t="inlineStr"/>
       <c r="P413" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Pokémon GO Wild Area: Nagasaki Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q413" t="inlineStr">
@@ -17404,7 +17404,7 @@
       <c r="D414" t="inlineStr"/>
       <c r="E414" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
+          <t>Pokémon GO Wild Area: Nagasaki</t>
         </is>
       </c>
       <c r="F414" t="inlineStr">
@@ -17423,7 +17423,7 @@
       <c r="O414" t="inlineStr"/>
       <c r="P414" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating...</t>
+          <t>Pokémon GO Wild Area: Nagasaki Calculating...</t>
         </is>
       </c>
       <c r="Q414" t="inlineStr">
@@ -17443,7 +17443,7 @@
       <c r="D415" t="inlineStr"/>
       <c r="E415" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Nagasaki</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F415" t="inlineStr">
@@ -17462,7 +17462,7 @@
       <c r="O415" t="inlineStr"/>
       <c r="P415" t="inlineStr">
         <is>
-          <t>Wild Area Pokémon GO Wild Area: Nagasaki Calculating... Starts: Calculating...</t>
+          <t>GO Battle League Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q415" t="inlineStr">
@@ -17482,7 +17482,7 @@
       <c r="D416" t="inlineStr"/>
       <c r="E416" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Nagasaki</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F416" t="inlineStr">
@@ -17501,7 +17501,7 @@
       <c r="O416" t="inlineStr"/>
       <c r="P416" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Nagasaki Calculating... Starts: Calculating...</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q416" t="inlineStr">
@@ -17521,7 +17521,7 @@
       <c r="D417" t="inlineStr"/>
       <c r="E417" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Nagasaki</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F417" t="inlineStr">
@@ -17540,7 +17540,7 @@
       <c r="O417" t="inlineStr"/>
       <c r="P417" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Nagasaki Calculating... Starts: Calculating...</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q417" t="inlineStr">
@@ -17560,7 +17560,7 @@
       <c r="D418" t="inlineStr"/>
       <c r="E418" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Nagasaki</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F418" t="inlineStr">
@@ -17579,7 +17579,7 @@
       <c r="O418" t="inlineStr"/>
       <c r="P418" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Nagasaki Calculating...</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q418" t="inlineStr">
@@ -17599,7 +17599,7 @@
       <c r="D419" t="inlineStr"/>
       <c r="E419" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Pokémon GO Wild Area: Global</t>
         </is>
       </c>
       <c r="F419" t="inlineStr">
@@ -17618,7 +17618,7 @@
       <c r="O419" t="inlineStr"/>
       <c r="P419" t="inlineStr">
         <is>
-          <t>GO Battle League Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Wild Area Pokémon GO Wild Area: Global Sat, Nov 15, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q419" t="inlineStr">
@@ -17638,7 +17638,7 @@
       <c r="D420" t="inlineStr"/>
       <c r="E420" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Pokémon GO Wild Area: Global</t>
         </is>
       </c>
       <c r="F420" t="inlineStr">
@@ -17657,7 +17657,7 @@
       <c r="O420" t="inlineStr"/>
       <c r="P420" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Pokémon GO Wild Area: Global Sat, Nov 15, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q420" t="inlineStr">
@@ -17677,7 +17677,7 @@
       <c r="D421" t="inlineStr"/>
       <c r="E421" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Pokémon GO Wild Area: Global</t>
         </is>
       </c>
       <c r="F421" t="inlineStr">
@@ -17696,7 +17696,7 @@
       <c r="O421" t="inlineStr"/>
       <c r="P421" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Pokémon GO Wild Area: Global Sat, Nov 15, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q421" t="inlineStr">
@@ -17716,7 +17716,7 @@
       <c r="D422" t="inlineStr"/>
       <c r="E422" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Pokémon GO Wild Area: Global</t>
         </is>
       </c>
       <c r="F422" t="inlineStr">
@@ -17735,7 +17735,7 @@
       <c r="O422" t="inlineStr"/>
       <c r="P422" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating...</t>
+          <t>Pokémon GO Wild Area: Global Sat, Nov 15, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q422" t="inlineStr">
@@ -17755,12 +17755,12 @@
       <c r="D423" t="inlineStr"/>
       <c r="E423" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Global</t>
+          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F423" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G423" t="inlineStr"/>
@@ -17774,7 +17774,7 @@
       <c r="O423" t="inlineStr"/>
       <c r="P423" t="inlineStr">
         <is>
-          <t>Wild Area Pokémon GO Wild Area: Global Sat, Nov 15, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>GO Battle League 2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q423" t="inlineStr">
@@ -17794,12 +17794,12 @@
       <c r="D424" t="inlineStr"/>
       <c r="E424" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Global</t>
+          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F424" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G424" t="inlineStr"/>
@@ -17813,7 +17813,7 @@
       <c r="O424" t="inlineStr"/>
       <c r="P424" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Global Sat, Nov 15, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q424" t="inlineStr">
@@ -17833,12 +17833,12 @@
       <c r="D425" t="inlineStr"/>
       <c r="E425" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Global</t>
+          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F425" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G425" t="inlineStr"/>
@@ -17852,7 +17852,7 @@
       <c r="O425" t="inlineStr"/>
       <c r="P425" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Global Sat, Nov 15, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q425" t="inlineStr">
@@ -17872,12 +17872,12 @@
       <c r="D426" t="inlineStr"/>
       <c r="E426" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Global</t>
+          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F426" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G426" t="inlineStr"/>
@@ -17891,7 +17891,7 @@
       <c r="O426" t="inlineStr"/>
       <c r="P426" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Global Sat, Nov 15, at 10:00 AM Local Time</t>
+          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q426" t="inlineStr">
@@ -17911,12 +17911,12 @@
       <c r="D427" t="inlineStr"/>
       <c r="E427" t="inlineStr">
         <is>
-          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation</t>
+          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F427" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G427" t="inlineStr"/>
@@ -17930,7 +17930,7 @@
       <c r="O427" t="inlineStr"/>
       <c r="P427" t="inlineStr">
         <is>
-          <t>GO Battle League 2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>GO Battle League Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q427" t="inlineStr">
@@ -17950,12 +17950,12 @@
       <c r="D428" t="inlineStr"/>
       <c r="E428" t="inlineStr">
         <is>
-          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation</t>
+          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F428" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G428" t="inlineStr"/>
@@ -17969,7 +17969,7 @@
       <c r="O428" t="inlineStr"/>
       <c r="P428" t="inlineStr">
         <is>
-          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q428" t="inlineStr">
@@ -17989,12 +17989,12 @@
       <c r="D429" t="inlineStr"/>
       <c r="E429" t="inlineStr">
         <is>
-          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation</t>
+          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F429" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G429" t="inlineStr"/>
@@ -18008,7 +18008,7 @@
       <c r="O429" t="inlineStr"/>
       <c r="P429" t="inlineStr">
         <is>
-          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q429" t="inlineStr">
@@ -18028,12 +18028,12 @@
       <c r="D430" t="inlineStr"/>
       <c r="E430" t="inlineStr">
         <is>
-          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation</t>
+          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F430" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G430" t="inlineStr"/>
@@ -18047,7 +18047,7 @@
       <c r="O430" t="inlineStr"/>
       <c r="P430" t="inlineStr">
         <is>
-          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating...</t>
+          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q430" t="inlineStr">
@@ -18067,12 +18067,12 @@
       <c r="D431" t="inlineStr"/>
       <c r="E431" t="inlineStr">
         <is>
-          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation</t>
+          <t>November Community Day</t>
         </is>
       </c>
       <c r="F431" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Community Day</t>
         </is>
       </c>
       <c r="G431" t="inlineStr"/>
@@ -18086,7 +18086,7 @@
       <c r="O431" t="inlineStr"/>
       <c r="P431" t="inlineStr">
         <is>
-          <t>GO Battle League Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Community Day November Community Day Sun, Nov 30, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q431" t="inlineStr">
@@ -18106,12 +18106,12 @@
       <c r="D432" t="inlineStr"/>
       <c r="E432" t="inlineStr">
         <is>
-          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation</t>
+          <t>November Community Day</t>
         </is>
       </c>
       <c r="F432" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Community Day</t>
         </is>
       </c>
       <c r="G432" t="inlineStr"/>
@@ -18125,7 +18125,7 @@
       <c r="O432" t="inlineStr"/>
       <c r="P432" t="inlineStr">
         <is>
-          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>November Community Day Sun, Nov 30, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q432" t="inlineStr">
@@ -18145,12 +18145,12 @@
       <c r="D433" t="inlineStr"/>
       <c r="E433" t="inlineStr">
         <is>
-          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation</t>
+          <t>November Community Day</t>
         </is>
       </c>
       <c r="F433" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Community Day</t>
         </is>
       </c>
       <c r="G433" t="inlineStr"/>
@@ -18164,7 +18164,7 @@
       <c r="O433" t="inlineStr"/>
       <c r="P433" t="inlineStr">
         <is>
-          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>November Community Day Sun, Nov 30, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q433" t="inlineStr">
@@ -18184,12 +18184,12 @@
       <c r="D434" t="inlineStr"/>
       <c r="E434" t="inlineStr">
         <is>
-          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation</t>
+          <t>November Community Day</t>
         </is>
       </c>
       <c r="F434" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Community Day</t>
         </is>
       </c>
       <c r="G434" t="inlineStr"/>
@@ -18203,7 +18203,7 @@
       <c r="O434" t="inlineStr"/>
       <c r="P434" t="inlineStr">
         <is>
-          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating...</t>
+          <t>November Community Day Sun, Nov 30, at 2:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q434" t="inlineStr">
@@ -18223,12 +18223,12 @@
       <c r="D435" t="inlineStr"/>
       <c r="E435" t="inlineStr">
         <is>
-          <t>November Community Day</t>
+          <t>Raid NOW</t>
         </is>
       </c>
       <c r="F435" t="inlineStr">
         <is>
-          <t>Community Day</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G435" t="inlineStr"/>
@@ -18242,12 +18242,12 @@
       <c r="O435" t="inlineStr"/>
       <c r="P435" t="inlineStr">
         <is>
-          <t>Community Day November Community Day Sun, Nov 30, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Raid NOW From Leek Duck | Powered by GO FRIEND General Information It has been reported that the registration information (Trainer Name, Trainer Level, Trainer Code) is incorrect. Please check again. HOST HOST Auto join Raids you are joining (Latest 2) MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rpl_maxuser'] }} {{ val1['cnt'] }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} No.{{ val1['rpl_id'] }} No.{{ val1['rpl_id'] }} TL{{ val1['rpl_level'] }} {{ val1['rpl_glevel'] }} {{ ((val1['rpl_gescore'] == -1)?0:val1['rpl_gescore']) }} {{ aryPokemon[value]['raidbbs_short_name_en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} FULL Host TL 5 30 35 40 45 Host Rating - 0 {{ i }} MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['ti</t>
         </is>
       </c>
       <c r="Q435" t="inlineStr">
         <is>
-          <t>2024-06-01_events.html</t>
+          <t>2024-06-01_raid-now.html</t>
         </is>
       </c>
     </row>
@@ -18262,12 +18262,12 @@
       <c r="D436" t="inlineStr"/>
       <c r="E436" t="inlineStr">
         <is>
-          <t>November Community Day</t>
+          <t>Raids you are joining (Latest 2)</t>
         </is>
       </c>
       <c r="F436" t="inlineStr">
         <is>
-          <t>Community Day</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G436" t="inlineStr"/>
@@ -18281,12 +18281,12 @@
       <c r="O436" t="inlineStr"/>
       <c r="P436" t="inlineStr">
         <is>
-          <t>November Community Day Sun, Nov 30, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>General Information It has been reported that the registration information (Trainer Name, Trainer Level, Trainer Code) is incorrect. Please check again. HOST HOST Auto join Raids you are joining (Latest 2) MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rpl_maxuser'] }} {{ val1['cnt'] }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} No.{{ val1['rpl_id'] }} No.{{ val1['rpl_id'] }} TL{{ val1['rpl_level'] }} {{ val1['rpl_glevel'] }} {{ ((val1['rpl_gescore'] == -1)?0:val1['rpl_gescore']) }} {{ aryPokemon[value]['raidbbs_short_name_en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} FULL Host TL 5 30 35 40 45 Host Rating - 0 {{ i }} MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rp</t>
         </is>
       </c>
       <c r="Q436" t="inlineStr">
         <is>
-          <t>2024-06-01_events.html</t>
+          <t>2024-06-01_raid-now.html</t>
         </is>
       </c>
     </row>
@@ -18301,12 +18301,12 @@
       <c r="D437" t="inlineStr"/>
       <c r="E437" t="inlineStr">
         <is>
-          <t>November Community Day</t>
+          <t>Raids you are joining (Latest 2)</t>
         </is>
       </c>
       <c r="F437" t="inlineStr">
         <is>
-          <t>Community Day</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G437" t="inlineStr"/>
@@ -18320,12 +18320,12 @@
       <c r="O437" t="inlineStr"/>
       <c r="P437" t="inlineStr">
         <is>
-          <t>November Community Day Sun, Nov 30, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Raids you are joining (Latest 2) MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rpl_maxuser'] }} {{ val1['cnt'] }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} No.{{ val1['rpl_id'] }} No.{{ val1['rpl_id'] }} TL{{ val1['rpl_level'] }} {{ val1['rpl_glevel'] }} {{ ((val1['rpl_gescore'] == -1)?0:val1['rpl_gescore']) }}</t>
         </is>
       </c>
       <c r="Q437" t="inlineStr">
         <is>
-          <t>2024-06-01_events.html</t>
+          <t>2024-06-01_raid-now.html</t>
         </is>
       </c>
     </row>
@@ -18340,12 +18340,12 @@
       <c r="D438" t="inlineStr"/>
       <c r="E438" t="inlineStr">
         <is>
-          <t>November Community Day</t>
+          <t>まとめて評価</t>
         </is>
       </c>
       <c r="F438" t="inlineStr">
         <is>
-          <t>Community Day</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G438" t="inlineStr"/>
@@ -18359,12 +18359,12 @@
       <c r="O438" t="inlineStr"/>
       <c r="P438" t="inlineStr">
         <is>
-          <t>November Community Day Sun, Nov 30, at 2:00 PM Local Time</t>
+          <t>まとめて評価 Can't rate</t>
         </is>
       </c>
       <c r="Q438" t="inlineStr">
         <is>
-          <t>2024-06-01_events.html</t>
+          <t>2024-06-01_raid-now.html</t>
         </is>
       </c>
     </row>
@@ -18379,12 +18379,12 @@
       <c r="D439" t="inlineStr"/>
       <c r="E439" t="inlineStr">
         <is>
-          <t>Raid NOW</t>
+          <t>Bonuses</t>
         </is>
       </c>
       <c r="F439" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G439" t="inlineStr"/>
@@ -18398,12 +18398,12 @@
       <c r="O439" t="inlineStr"/>
       <c r="P439" t="inlineStr">
         <is>
-          <t>Raid NOW From Leek Duck | Powered by GO FRIEND General Information It has been reported that the registration information (Trainer Name, Trainer Level, Trainer Code) is incorrect. Please check again. HOST HOST Auto join Raids you are joining (Latest 2) MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rpl_maxuser'] }} {{ val1['cnt'] }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} No.{{ val1['rpl_id'] }} No.{{ val1['rpl_id'] }} TL{{ val1['rpl_level'] }} {{ val1['rpl_glevel'] }} {{ ((val1['rpl_gescore'] == -1)?0:val1['rpl_gescore']) }} {{ aryPokemon[value]['raidbbs_short_name_en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} FULL Host TL 5 30 35 40 45 Host Rating - 0 {{ i }} MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['ti</t>
+          <t>Bonuses 4× Stardust from win rewards. (This does not include end-of-set rewards.) The maximum number of sets you can play per day will increase from five to 20—for a total of 100 battles—from 12:00 a.m. to 11:59 p.m. local time. Free battle-themed Timed Research will be available. Rewards include glasses for your avatar inspired by Clemont. Pokémon encountered via GO Battle League rewards will have a wider variance of Attack, Defense, and HP. Active Leagues The following leagues will be active. Great League Ultra League Master League</t>
         </is>
       </c>
       <c r="Q439" t="inlineStr">
         <is>
-          <t>2024-06-01_raid-now.html</t>
+          <t>2024-06-01_event-go-battle-weekend-tales-of-transformation-sun-oct-26-at-1159-pm-local-time-ends-calculating.html</t>
         </is>
       </c>
     </row>
@@ -18418,12 +18418,12 @@
       <c r="D440" t="inlineStr"/>
       <c r="E440" t="inlineStr">
         <is>
-          <t>Raids you are joining (Latest 2)</t>
+          <t>For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area?</t>
         </is>
       </c>
       <c r="F440" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G440" t="inlineStr"/>
@@ -18437,12 +18437,12 @@
       <c r="O440" t="inlineStr"/>
       <c r="P440" t="inlineStr">
         <is>
-          <t>General Information It has been reported that the registration information (Trainer Name, Trainer Level, Trainer Code) is incorrect. Please check again. HOST HOST Auto join Raids you are joining (Latest 2) MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rpl_maxuser'] }} {{ val1['cnt'] }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} No.{{ val1['rpl_id'] }} No.{{ val1['rpl_id'] }} TL{{ val1['rpl_level'] }} {{ val1['rpl_glevel'] }} {{ ((val1['rpl_gescore'] == -1)?0:val1['rpl_gescore']) }} {{ aryPokemon[value]['raidbbs_short_name_en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} FULL Host TL 5 30 35 40 45 Host Rating - 0 {{ i }} MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rp</t>
+          <t xml:space="preserve">For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area? In this next chapter of Pokémon GO Wild Area, get ready to test your skills once again as you encounter Dark- and Fairy-type Pokémon, including Grimmsnarl, the Bulk Up Pokémon! Plus, exceptionally powerful Pokémon known as mighty Pokémon are appearing in the wild—use GO Wild Area–exclusive GO Safari Balls to improve your odds of catching these rare Pokémon. All event gameplay is exclusive to ticket holders. Tickets for Pokémon GO Wild Area: Nagasaki are now available on the Niantic events portal . Live Event Ticket - ¥3,600 (including applicable taxes and fees) Location: A citywide experience across Nagasaki City, Japan Dates: November 7, 8, or 9, 2025 Time: 9:00 a.m. – 5:00 p.m. JST Tickets for Pokémon GO Wild Area: Nagasaki include one day of event gameplay, and attendees may purchase add-ons that extend the gameplay for an additional day. One-day tickets are ¥3,600 (or the equivalent pricing tier in your local currency, including applicable taxes and fees). Event gameplay will be available only at the date, time, and location specified on your ticket. Note: Tickets to this event are </t>
         </is>
       </c>
       <c r="Q440" t="inlineStr">
         <is>
-          <t>2024-06-01_raid-now.html</t>
+          <t>2024-06-01_wild-area-pokmon-go-wild-area-nagasaki-calculating-ends-calculating.html</t>
         </is>
       </c>
     </row>
@@ -18457,12 +18457,12 @@
       <c r="D441" t="inlineStr"/>
       <c r="E441" t="inlineStr">
         <is>
-          <t>Raids you are joining (Latest 2)</t>
+          <t>For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area?</t>
         </is>
       </c>
       <c r="F441" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G441" t="inlineStr"/>
@@ -18476,166 +18476,10 @@
       <c r="O441" t="inlineStr"/>
       <c r="P441" t="inlineStr">
         <is>
-          <t>Raids you are joining (Latest 2) MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rpl_maxuser'] }} {{ val1['cnt'] }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} No.{{ val1['rpl_id'] }} No.{{ val1['rpl_id'] }} TL{{ val1['rpl_level'] }} {{ val1['rpl_glevel'] }} {{ ((val1['rpl_gescore'] == -1)?0:val1['rpl_gescore']) }}</t>
+          <t>For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area? Trainers around the world can gear up for a worldwide adventure during Pokémon GO Wild Area: Global, available in-game for two days only! Looking to enhance your GO Wild Area weekend with exclusive Special Research, additional bonuses, and an increased chance of encountering Shiny Pokémon? Purchase a global event ticket from the Pokémon GO Web Store! Event Tickets Tickets for Pokémon GO Wild Area: Global are available now in the in-game Shop and Pokémon Go Web Store for $11.99 USD . Purchase your ticket on the Pokémon GO Web Store for a new avatar item! Trainers who purchase their Pokémon GO Wild Area: Global ticket on the Pokémon GO Web Store will receive a special avatar item—the Flower Crown! You can purchase your ticket on the web store until the last day of the event to receive this avatar item. Pokémon GO Wild Area: Nagasaki For details on the in-person event in Nagasaki, Japan, click here .</t>
         </is>
       </c>
       <c r="Q441" t="inlineStr">
-        <is>
-          <t>2024-06-01_raid-now.html</t>
-        </is>
-      </c>
-    </row>
-    <row r="442">
-      <c r="A442" t="inlineStr">
-        <is>
-          <t>Leek Duck</t>
-        </is>
-      </c>
-      <c r="B442" t="inlineStr"/>
-      <c r="C442" t="inlineStr"/>
-      <c r="D442" t="inlineStr"/>
-      <c r="E442" t="inlineStr">
-        <is>
-          <t>まとめて評価</t>
-        </is>
-      </c>
-      <c r="F442" t="inlineStr">
-        <is>
-          <t>Event/News</t>
-        </is>
-      </c>
-      <c r="G442" t="inlineStr"/>
-      <c r="H442" t="inlineStr"/>
-      <c r="I442" t="inlineStr"/>
-      <c r="J442" t="inlineStr"/>
-      <c r="K442" t="inlineStr"/>
-      <c r="L442" t="inlineStr"/>
-      <c r="M442" t="inlineStr"/>
-      <c r="N442" t="inlineStr"/>
-      <c r="O442" t="inlineStr"/>
-      <c r="P442" t="inlineStr">
-        <is>
-          <t>まとめて評価 Can't rate</t>
-        </is>
-      </c>
-      <c r="Q442" t="inlineStr">
-        <is>
-          <t>2024-06-01_raid-now.html</t>
-        </is>
-      </c>
-    </row>
-    <row r="443">
-      <c r="A443" t="inlineStr">
-        <is>
-          <t>Leek Duck</t>
-        </is>
-      </c>
-      <c r="B443" t="inlineStr"/>
-      <c r="C443" t="inlineStr"/>
-      <c r="D443" t="inlineStr"/>
-      <c r="E443" t="inlineStr">
-        <is>
-          <t>Bonuses</t>
-        </is>
-      </c>
-      <c r="F443" t="inlineStr">
-        <is>
-          <t>Event/News</t>
-        </is>
-      </c>
-      <c r="G443" t="inlineStr"/>
-      <c r="H443" t="inlineStr"/>
-      <c r="I443" t="inlineStr"/>
-      <c r="J443" t="inlineStr"/>
-      <c r="K443" t="inlineStr"/>
-      <c r="L443" t="inlineStr"/>
-      <c r="M443" t="inlineStr"/>
-      <c r="N443" t="inlineStr"/>
-      <c r="O443" t="inlineStr"/>
-      <c r="P443" t="inlineStr">
-        <is>
-          <t>Bonuses 4× Stardust from win rewards. (This does not include end-of-set rewards.) The maximum number of sets you can play per day will increase from five to 20—for a total of 100 battles—from 12:00 a.m. to 11:59 p.m. local time. Free battle-themed Timed Research will be available. Rewards include glasses for your avatar inspired by Clemont. Pokémon encountered via GO Battle League rewards will have a wider variance of Attack, Defense, and HP. Active Leagues The following leagues will be active. Great League Ultra League Master League</t>
-        </is>
-      </c>
-      <c r="Q443" t="inlineStr">
-        <is>
-          <t>2024-06-01_event-go-battle-weekend-tales-of-transformation-sun-oct-26-at-1159-pm-local-time-ends-calculating.html</t>
-        </is>
-      </c>
-    </row>
-    <row r="444">
-      <c r="A444" t="inlineStr">
-        <is>
-          <t>Leek Duck</t>
-        </is>
-      </c>
-      <c r="B444" t="inlineStr"/>
-      <c r="C444" t="inlineStr"/>
-      <c r="D444" t="inlineStr"/>
-      <c r="E444" t="inlineStr">
-        <is>
-          <t>For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area?</t>
-        </is>
-      </c>
-      <c r="F444" t="inlineStr">
-        <is>
-          <t>Event/News</t>
-        </is>
-      </c>
-      <c r="G444" t="inlineStr"/>
-      <c r="H444" t="inlineStr"/>
-      <c r="I444" t="inlineStr"/>
-      <c r="J444" t="inlineStr"/>
-      <c r="K444" t="inlineStr"/>
-      <c r="L444" t="inlineStr"/>
-      <c r="M444" t="inlineStr"/>
-      <c r="N444" t="inlineStr"/>
-      <c r="O444" t="inlineStr"/>
-      <c r="P444" t="inlineStr">
-        <is>
-          <t xml:space="preserve">For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area? In this next chapter of Pokémon GO Wild Area, get ready to test your skills once again as you encounter Dark- and Fairy-type Pokémon, including Grimmsnarl, the Bulk Up Pokémon! Plus, exceptionally powerful Pokémon known as mighty Pokémon are appearing in the wild—use GO Wild Area–exclusive GO Safari Balls to improve your odds of catching these rare Pokémon. All event gameplay is exclusive to ticket holders. Tickets for Pokémon GO Wild Area: Nagasaki are now available on the Niantic events portal . Live Event Ticket - ¥3,600 (including applicable taxes and fees) Location: A citywide experience across Nagasaki City, Japan Dates: November 7, 8, or 9, 2025 Time: 9:00 a.m. – 5:00 p.m. JST Tickets for Pokémon GO Wild Area: Nagasaki include one day of event gameplay, and attendees may purchase add-ons that extend the gameplay for an additional day. One-day tickets are ¥3,600 (or the equivalent pricing tier in your local currency, including applicable taxes and fees). Event gameplay will be available only at the date, time, and location specified on your ticket. Note: Tickets to this event are </t>
-        </is>
-      </c>
-      <c r="Q444" t="inlineStr">
-        <is>
-          <t>2024-06-01_wild-area-pokmon-go-wild-area-nagasaki-calculating-ends-calculating.html</t>
-        </is>
-      </c>
-    </row>
-    <row r="445">
-      <c r="A445" t="inlineStr">
-        <is>
-          <t>Leek Duck</t>
-        </is>
-      </c>
-      <c r="B445" t="inlineStr"/>
-      <c r="C445" t="inlineStr"/>
-      <c r="D445" t="inlineStr"/>
-      <c r="E445" t="inlineStr">
-        <is>
-          <t>For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area?</t>
-        </is>
-      </c>
-      <c r="F445" t="inlineStr">
-        <is>
-          <t>Event/News</t>
-        </is>
-      </c>
-      <c r="G445" t="inlineStr"/>
-      <c r="H445" t="inlineStr"/>
-      <c r="I445" t="inlineStr"/>
-      <c r="J445" t="inlineStr"/>
-      <c r="K445" t="inlineStr"/>
-      <c r="L445" t="inlineStr"/>
-      <c r="M445" t="inlineStr"/>
-      <c r="N445" t="inlineStr"/>
-      <c r="O445" t="inlineStr"/>
-      <c r="P445" t="inlineStr">
-        <is>
-          <t>For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area? Trainers around the world can gear up for a worldwide adventure during Pokémon GO Wild Area: Global, available in-game for two days only! Looking to enhance your GO Wild Area weekend with exclusive Special Research, additional bonuses, and an increased chance of encountering Shiny Pokémon? Purchase a global event ticket from the Pokémon GO Web Store! Event Tickets Tickets for Pokémon GO Wild Area: Global are available now in the in-game Shop and Pokémon Go Web Store for $11.99 USD . Purchase your ticket on the Pokémon GO Web Store for a new avatar item! Trainers who purchase their Pokémon GO Wild Area: Global ticket on the Pokémon GO Web Store will receive a special avatar item—the Flower Crown! You can purchase your ticket on the web store until the last day of the event to receive this avatar item. Pokémon GO Wild Area: Nagasaki For details on the in-person event in Nagasaki, Japan, click here .</t>
-        </is>
-      </c>
-      <c r="Q445" t="inlineStr">
         <is>
           <t>2024-06-01_wild-area-pokmon-go-wild-area-global-sun-nov-16-at-600-pm-local-time-ends-calculating.html</t>
         </is>

</xml_diff>

<commit_message>
Update latest digest: 2024-06-01 → 2025-10-03
</commit_message>
<xml_diff>
--- a/outputs/latest/POGO_Digest.xlsx
+++ b/outputs/latest/POGO_Digest.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q426"/>
+  <dimension ref="A1:Q422"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17602,12 +17602,12 @@
       <c r="D420" t="inlineStr"/>
       <c r="E420" t="inlineStr">
         <is>
-          <t>Raid NOW</t>
+          <t>Bonuses</t>
         </is>
       </c>
       <c r="F420" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G420" t="inlineStr"/>
@@ -17621,12 +17621,12 @@
       <c r="O420" t="inlineStr"/>
       <c r="P420" t="inlineStr">
         <is>
-          <t>Raid NOW From Leek Duck | Powered by GO FRIEND General Information It has been reported that the registration information (Trainer Name, Trainer Level, Trainer Code) is incorrect. Please check again. HOST HOST Auto join Raids you are joining (Latest 2) MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rpl_maxuser'] }} {{ val1['cnt'] }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} No.{{ val1['rpl_id'] }} No.{{ val1['rpl_id'] }} TL{{ val1['rpl_level'] }} {{ val1['rpl_glevel'] }} {{ ((val1['rpl_gescore'] == -1)?0:val1['rpl_gescore']) }} {{ aryPokemon[value]['raidbbs_short_name_en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} FULL Host TL 5 30 35 40 45 Host Rating - 0 {{ i }} MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['ti</t>
+          <t>Bonuses 4× Stardust from win rewards. (This does not include end-of-set rewards.) The maximum number of sets you can play per day will increase from five to 20—for a total of 100 battles—from 12:00 a.m. to 11:59 p.m. local time. Free battle-themed Timed Research will be available. Rewards include glasses for your avatar inspired by Clemont. Pokémon encountered via GO Battle League rewards will have a wider variance of Attack, Defense, and HP. Active Leagues The following leagues will be active. Great League Ultra League Master League</t>
         </is>
       </c>
       <c r="Q420" t="inlineStr">
         <is>
-          <t>2024-06-01_raid-now.html</t>
+          <t>2024-06-01_event-go-battle-weekend-tales-of-transformation-sun-oct-26-at-1159-pm-local-time-ends-calculating.html</t>
         </is>
       </c>
     </row>
@@ -17641,12 +17641,12 @@
       <c r="D421" t="inlineStr"/>
       <c r="E421" t="inlineStr">
         <is>
-          <t>Raids you are joining (Latest 2)</t>
+          <t>For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area?</t>
         </is>
       </c>
       <c r="F421" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G421" t="inlineStr"/>
@@ -17660,12 +17660,12 @@
       <c r="O421" t="inlineStr"/>
       <c r="P421" t="inlineStr">
         <is>
-          <t>General Information It has been reported that the registration information (Trainer Name, Trainer Level, Trainer Code) is incorrect. Please check again. HOST HOST Auto join Raids you are joining (Latest 2) MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rpl_maxuser'] }} {{ val1['cnt'] }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} No.{{ val1['rpl_id'] }} No.{{ val1['rpl_id'] }} TL{{ val1['rpl_level'] }} {{ val1['rpl_glevel'] }} {{ ((val1['rpl_gescore'] == -1)?0:val1['rpl_gescore']) }} {{ aryPokemon[value]['raidbbs_short_name_en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} FULL Host TL 5 30 35 40 45 Host Rating - 0 {{ i }} MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rp</t>
+          <t xml:space="preserve">For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area? In this next chapter of Pokémon GO Wild Area, get ready to test your skills once again as you encounter Dark- and Fairy-type Pokémon, including Grimmsnarl, the Bulk Up Pokémon! Plus, exceptionally powerful Pokémon known as mighty Pokémon are appearing in the wild—use GO Wild Area–exclusive GO Safari Balls to improve your odds of catching these rare Pokémon. All event gameplay is exclusive to ticket holders. Tickets for Pokémon GO Wild Area: Nagasaki are now available on the Niantic events portal . Live Event Ticket - ¥3,600 (including applicable taxes and fees) Location: A citywide experience across Nagasaki City, Japan Dates: November 7, 8, or 9, 2025 Time: 9:00 a.m. – 5:00 p.m. JST Tickets for Pokémon GO Wild Area: Nagasaki include one day of event gameplay, and attendees may purchase add-ons that extend the gameplay for an additional day. One-day tickets are ¥3,600 (or the equivalent pricing tier in your local currency, including applicable taxes and fees). Event gameplay will be available only at the date, time, and location specified on your ticket. Note: Tickets to this event are </t>
         </is>
       </c>
       <c r="Q421" t="inlineStr">
         <is>
-          <t>2024-06-01_raid-now.html</t>
+          <t>2024-06-01_wild-area-pokmon-go-wild-area-nagasaki-calculating-ends-calculating.html</t>
         </is>
       </c>
     </row>
@@ -17680,12 +17680,12 @@
       <c r="D422" t="inlineStr"/>
       <c r="E422" t="inlineStr">
         <is>
-          <t>Raids you are joining (Latest 2)</t>
+          <t>For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area?</t>
         </is>
       </c>
       <c r="F422" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G422" t="inlineStr"/>
@@ -17699,166 +17699,10 @@
       <c r="O422" t="inlineStr"/>
       <c r="P422" t="inlineStr">
         <is>
-          <t>Raids you are joining (Latest 2) MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rpl_maxuser'] }} {{ val1['cnt'] }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} No.{{ val1['rpl_id'] }} No.{{ val1['rpl_id'] }} TL{{ val1['rpl_level'] }} {{ val1['rpl_glevel'] }} {{ ((val1['rpl_gescore'] == -1)?0:val1['rpl_gescore']) }}</t>
+          <t>For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area? Trainers around the world can gear up for a worldwide adventure during Pokémon GO Wild Area: Global, available in-game for two days only! Looking to enhance your GO Wild Area weekend with exclusive Special Research, additional bonuses, and an increased chance of encountering Shiny Pokémon? Purchase a global event ticket from the Pokémon GO Web Store! Event Tickets Tickets for Pokémon GO Wild Area: Global are available now in the in-game Shop and Pokémon Go Web Store for $11.99 USD . Purchase your ticket on the Pokémon GO Web Store for a new avatar item! Trainers who purchase their Pokémon GO Wild Area: Global ticket on the Pokémon GO Web Store will receive a special avatar item—the Flower Crown! You can purchase your ticket on the web store until the last day of the event to receive this avatar item. Pokémon GO Wild Area: Nagasaki For details on the in-person event in Nagasaki, Japan, click here .</t>
         </is>
       </c>
       <c r="Q422" t="inlineStr">
-        <is>
-          <t>2024-06-01_raid-now.html</t>
-        </is>
-      </c>
-    </row>
-    <row r="423">
-      <c r="A423" t="inlineStr">
-        <is>
-          <t>Leek Duck</t>
-        </is>
-      </c>
-      <c r="B423" t="inlineStr"/>
-      <c r="C423" t="inlineStr"/>
-      <c r="D423" t="inlineStr"/>
-      <c r="E423" t="inlineStr">
-        <is>
-          <t>まとめて評価</t>
-        </is>
-      </c>
-      <c r="F423" t="inlineStr">
-        <is>
-          <t>Event/News</t>
-        </is>
-      </c>
-      <c r="G423" t="inlineStr"/>
-      <c r="H423" t="inlineStr"/>
-      <c r="I423" t="inlineStr"/>
-      <c r="J423" t="inlineStr"/>
-      <c r="K423" t="inlineStr"/>
-      <c r="L423" t="inlineStr"/>
-      <c r="M423" t="inlineStr"/>
-      <c r="N423" t="inlineStr"/>
-      <c r="O423" t="inlineStr"/>
-      <c r="P423" t="inlineStr">
-        <is>
-          <t>まとめて評価 Can't rate</t>
-        </is>
-      </c>
-      <c r="Q423" t="inlineStr">
-        <is>
-          <t>2024-06-01_raid-now.html</t>
-        </is>
-      </c>
-    </row>
-    <row r="424">
-      <c r="A424" t="inlineStr">
-        <is>
-          <t>Leek Duck</t>
-        </is>
-      </c>
-      <c r="B424" t="inlineStr"/>
-      <c r="C424" t="inlineStr"/>
-      <c r="D424" t="inlineStr"/>
-      <c r="E424" t="inlineStr">
-        <is>
-          <t>Bonuses</t>
-        </is>
-      </c>
-      <c r="F424" t="inlineStr">
-        <is>
-          <t>Event/News</t>
-        </is>
-      </c>
-      <c r="G424" t="inlineStr"/>
-      <c r="H424" t="inlineStr"/>
-      <c r="I424" t="inlineStr"/>
-      <c r="J424" t="inlineStr"/>
-      <c r="K424" t="inlineStr"/>
-      <c r="L424" t="inlineStr"/>
-      <c r="M424" t="inlineStr"/>
-      <c r="N424" t="inlineStr"/>
-      <c r="O424" t="inlineStr"/>
-      <c r="P424" t="inlineStr">
-        <is>
-          <t>Bonuses 4× Stardust from win rewards. (This does not include end-of-set rewards.) The maximum number of sets you can play per day will increase from five to 20—for a total of 100 battles—from 12:00 a.m. to 11:59 p.m. local time. Free battle-themed Timed Research will be available. Rewards include glasses for your avatar inspired by Clemont. Pokémon encountered via GO Battle League rewards will have a wider variance of Attack, Defense, and HP. Active Leagues The following leagues will be active. Great League Ultra League Master League</t>
-        </is>
-      </c>
-      <c r="Q424" t="inlineStr">
-        <is>
-          <t>2024-06-01_event-go-battle-weekend-tales-of-transformation-sun-oct-26-at-1159-pm-local-time-ends-calculating.html</t>
-        </is>
-      </c>
-    </row>
-    <row r="425">
-      <c r="A425" t="inlineStr">
-        <is>
-          <t>Leek Duck</t>
-        </is>
-      </c>
-      <c r="B425" t="inlineStr"/>
-      <c r="C425" t="inlineStr"/>
-      <c r="D425" t="inlineStr"/>
-      <c r="E425" t="inlineStr">
-        <is>
-          <t>For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area?</t>
-        </is>
-      </c>
-      <c r="F425" t="inlineStr">
-        <is>
-          <t>Event/News</t>
-        </is>
-      </c>
-      <c r="G425" t="inlineStr"/>
-      <c r="H425" t="inlineStr"/>
-      <c r="I425" t="inlineStr"/>
-      <c r="J425" t="inlineStr"/>
-      <c r="K425" t="inlineStr"/>
-      <c r="L425" t="inlineStr"/>
-      <c r="M425" t="inlineStr"/>
-      <c r="N425" t="inlineStr"/>
-      <c r="O425" t="inlineStr"/>
-      <c r="P425" t="inlineStr">
-        <is>
-          <t xml:space="preserve">For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area? In this next chapter of Pokémon GO Wild Area, get ready to test your skills once again as you encounter Dark- and Fairy-type Pokémon, including Grimmsnarl, the Bulk Up Pokémon! Plus, exceptionally powerful Pokémon known as mighty Pokémon are appearing in the wild—use GO Wild Area–exclusive GO Safari Balls to improve your odds of catching these rare Pokémon. All event gameplay is exclusive to ticket holders. Tickets for Pokémon GO Wild Area: Nagasaki are now available on the Niantic events portal . Live Event Ticket - ¥3,600 (including applicable taxes and fees) Location: A citywide experience across Nagasaki City, Japan Dates: November 7, 8, or 9, 2025 Time: 9:00 a.m. – 5:00 p.m. JST Tickets for Pokémon GO Wild Area: Nagasaki include one day of event gameplay, and attendees may purchase add-ons that extend the gameplay for an additional day. One-day tickets are ¥3,600 (or the equivalent pricing tier in your local currency, including applicable taxes and fees). Event gameplay will be available only at the date, time, and location specified on your ticket. Note: Tickets to this event are </t>
-        </is>
-      </c>
-      <c r="Q425" t="inlineStr">
-        <is>
-          <t>2024-06-01_wild-area-pokmon-go-wild-area-nagasaki-calculating-ends-calculating.html</t>
-        </is>
-      </c>
-    </row>
-    <row r="426">
-      <c r="A426" t="inlineStr">
-        <is>
-          <t>Leek Duck</t>
-        </is>
-      </c>
-      <c r="B426" t="inlineStr"/>
-      <c r="C426" t="inlineStr"/>
-      <c r="D426" t="inlineStr"/>
-      <c r="E426" t="inlineStr">
-        <is>
-          <t>For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area?</t>
-        </is>
-      </c>
-      <c r="F426" t="inlineStr">
-        <is>
-          <t>Event/News</t>
-        </is>
-      </c>
-      <c r="G426" t="inlineStr"/>
-      <c r="H426" t="inlineStr"/>
-      <c r="I426" t="inlineStr"/>
-      <c r="J426" t="inlineStr"/>
-      <c r="K426" t="inlineStr"/>
-      <c r="L426" t="inlineStr"/>
-      <c r="M426" t="inlineStr"/>
-      <c r="N426" t="inlineStr"/>
-      <c r="O426" t="inlineStr"/>
-      <c r="P426" t="inlineStr">
-        <is>
-          <t>For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area? Trainers around the world can gear up for a worldwide adventure during Pokémon GO Wild Area: Global, available in-game for two days only! Looking to enhance your GO Wild Area weekend with exclusive Special Research, additional bonuses, and an increased chance of encountering Shiny Pokémon? Purchase a global event ticket from the Pokémon GO Web Store! Event Tickets Tickets for Pokémon GO Wild Area: Global are available now in the in-game Shop and Pokémon Go Web Store for $11.99 USD . Purchase your ticket on the Pokémon GO Web Store for a new avatar item! Trainers who purchase their Pokémon GO Wild Area: Global ticket on the Pokémon GO Web Store will receive a special avatar item—the Flower Crown! You can purchase your ticket on the web store until the last day of the event to receive this avatar item. Pokémon GO Wild Area: Nagasaki For details on the in-person event in Nagasaki, Japan, click here .</t>
-        </is>
-      </c>
-      <c r="Q426" t="inlineStr">
         <is>
           <t>2024-06-01_wild-area-pokmon-go-wild-area-global-sun-nov-16-at-600-pm-local-time-ends-calculating.html</t>
         </is>

</xml_diff>

<commit_message>
Update latest digest: 2024-06-01 → 2025-10-07
</commit_message>
<xml_diff>
--- a/outputs/latest/POGO_Digest.xlsx
+++ b/outputs/latest/POGO_Digest.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q431"/>
+  <dimension ref="A1:Q427"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11530,7 +11530,7 @@
       <c r="D264" t="inlineStr"/>
       <c r="E264" t="inlineStr">
         <is>
-          <t>Dynamax Drilbur during Max Monday</t>
+          <t>GO Pass: October</t>
         </is>
       </c>
       <c r="F264" t="inlineStr">
@@ -11549,7 +11549,7 @@
       <c r="O264" t="inlineStr"/>
       <c r="P264" t="inlineStr">
         <is>
-          <t>Max Mondays Dynamax Drilbur during Max Monday Mon, Oct 6, at 6:00 PM Local Time Starts: Calculating... GO Pass GO Pass: October Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating... Raid Battles Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating... Raid Battles Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating... GO Battle League Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating... Pokémon Spotlight Hour Ferroseed Spotlight Hour Tue, Oct 7, at 6:00 PM Local Time Starts: Calculating... Raid Hour Deoxys (Normal &amp; Defense Forme) Raid Hour Wed, Oct 8, at 6:00 PM Local Time Starts: Calculating... Event Harvest Festival Fri, Oct 10, at 10:00 AM Local Time Starts: Calculating... Community Day Solosis Community Day Sun, Oct 12, at 2:00 PM Local Time Starts: Calculating... Max Mondays Dynamax Bounsweet during Max Monday Mon, Oct 13, at 6:00 PM Local Time Starts: Calculating... Raid Battles Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating... Rai</t>
+          <t>GO Pass GO Pass: October Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating... Raid Battles Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating... Raid Battles Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating... GO Battle League Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating... Pokémon Spotlight Hour Ferroseed Spotlight Hour Tue, Oct 7, at 6:00 PM Local Time Starts: Calculating... Raid Hour Deoxys (Normal &amp; Defense Forme) Raid Hour Wed, Oct 8, at 6:00 PM Local Time Starts: Calculating... Event Harvest Festival Fri, Oct 10, at 10:00 AM Local Time Starts: Calculating... Community Day Solosis Community Day Sun, Oct 12, at 2:00 PM Local Time Starts: Calculating... Max Mondays Dynamax Bounsweet during Max Monday Mon, Oct 13, at 6:00 PM Local Time Starts: Calculating... Raid Battles Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating... Raid Battles Mega Mawile and Mega Salamence in Mega Raids Tue, Oct 14, at 10:00 AM Local Time Starts: Calc</t>
         </is>
       </c>
       <c r="Q264" t="inlineStr">
@@ -11569,7 +11569,7 @@
       <c r="D265" t="inlineStr"/>
       <c r="E265" t="inlineStr">
         <is>
-          <t>Dynamax Drilbur during Max Monday</t>
+          <t>GO Pass: October</t>
         </is>
       </c>
       <c r="F265" t="inlineStr">
@@ -11588,7 +11588,7 @@
       <c r="O265" t="inlineStr"/>
       <c r="P265" t="inlineStr">
         <is>
-          <t>Max Mondays Dynamax Drilbur during Max Monday Mon, Oct 6, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>GO Pass GO Pass: October Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q265" t="inlineStr">
@@ -11608,7 +11608,7 @@
       <c r="D266" t="inlineStr"/>
       <c r="E266" t="inlineStr">
         <is>
-          <t>Dynamax Drilbur during Max Monday</t>
+          <t>GO Pass: October</t>
         </is>
       </c>
       <c r="F266" t="inlineStr">
@@ -11627,7 +11627,7 @@
       <c r="O266" t="inlineStr"/>
       <c r="P266" t="inlineStr">
         <is>
-          <t>Dynamax Drilbur during Max Monday Mon, Oct 6, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>GO Pass: October Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q266" t="inlineStr">
@@ -11647,7 +11647,7 @@
       <c r="D267" t="inlineStr"/>
       <c r="E267" t="inlineStr">
         <is>
-          <t>Dynamax Drilbur during Max Monday</t>
+          <t>GO Pass: October</t>
         </is>
       </c>
       <c r="F267" t="inlineStr">
@@ -11666,7 +11666,7 @@
       <c r="O267" t="inlineStr"/>
       <c r="P267" t="inlineStr">
         <is>
-          <t>Dynamax Drilbur during Max Monday Mon, Oct 6, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>GO Pass: October Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q267" t="inlineStr">
@@ -11686,7 +11686,7 @@
       <c r="D268" t="inlineStr"/>
       <c r="E268" t="inlineStr">
         <is>
-          <t>Dynamax Drilbur during Max Monday</t>
+          <t>GO Pass: October</t>
         </is>
       </c>
       <c r="F268" t="inlineStr">
@@ -11705,7 +11705,7 @@
       <c r="O268" t="inlineStr"/>
       <c r="P268" t="inlineStr">
         <is>
-          <t>Dynamax Drilbur during Max Monday Mon, Oct 6, at 6:00 PM Local Time</t>
+          <t>GO Pass: October Tue, Oct 7, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q268" t="inlineStr">
@@ -11725,12 +11725,12 @@
       <c r="D269" t="inlineStr"/>
       <c r="E269" t="inlineStr">
         <is>
-          <t>GO Pass: October</t>
+          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F269" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G269" t="inlineStr"/>
@@ -11744,7 +11744,7 @@
       <c r="O269" t="inlineStr"/>
       <c r="P269" t="inlineStr">
         <is>
-          <t>GO Pass GO Pass: October Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Raid Battles Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q269" t="inlineStr">
@@ -11764,12 +11764,12 @@
       <c r="D270" t="inlineStr"/>
       <c r="E270" t="inlineStr">
         <is>
-          <t>GO Pass: October</t>
+          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F270" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G270" t="inlineStr"/>
@@ -11783,7 +11783,7 @@
       <c r="O270" t="inlineStr"/>
       <c r="P270" t="inlineStr">
         <is>
-          <t>GO Pass: October Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q270" t="inlineStr">
@@ -11803,12 +11803,12 @@
       <c r="D271" t="inlineStr"/>
       <c r="E271" t="inlineStr">
         <is>
-          <t>GO Pass: October</t>
+          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F271" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G271" t="inlineStr"/>
@@ -11822,7 +11822,7 @@
       <c r="O271" t="inlineStr"/>
       <c r="P271" t="inlineStr">
         <is>
-          <t>GO Pass: October Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q271" t="inlineStr">
@@ -11842,12 +11842,12 @@
       <c r="D272" t="inlineStr"/>
       <c r="E272" t="inlineStr">
         <is>
-          <t>GO Pass: October</t>
+          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F272" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G272" t="inlineStr"/>
@@ -11861,7 +11861,7 @@
       <c r="O272" t="inlineStr"/>
       <c r="P272" t="inlineStr">
         <is>
-          <t>GO Pass: October Tue, Oct 7, at 10:00 AM Local Time</t>
+          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q272" t="inlineStr">
@@ -11881,7 +11881,7 @@
       <c r="D273" t="inlineStr"/>
       <c r="E273" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles</t>
+          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids</t>
         </is>
       </c>
       <c r="F273" t="inlineStr">
@@ -11900,7 +11900,7 @@
       <c r="O273" t="inlineStr"/>
       <c r="P273" t="inlineStr">
         <is>
-          <t>Raid Battles Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Raid Battles Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q273" t="inlineStr">
@@ -11920,7 +11920,7 @@
       <c r="D274" t="inlineStr"/>
       <c r="E274" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles</t>
+          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids</t>
         </is>
       </c>
       <c r="F274" t="inlineStr">
@@ -11939,7 +11939,7 @@
       <c r="O274" t="inlineStr"/>
       <c r="P274" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q274" t="inlineStr">
@@ -11959,7 +11959,7 @@
       <c r="D275" t="inlineStr"/>
       <c r="E275" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles</t>
+          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids</t>
         </is>
       </c>
       <c r="F275" t="inlineStr">
@@ -11978,7 +11978,7 @@
       <c r="O275" t="inlineStr"/>
       <c r="P275" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q275" t="inlineStr">
@@ -11998,7 +11998,7 @@
       <c r="D276" t="inlineStr"/>
       <c r="E276" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles</t>
+          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids</t>
         </is>
       </c>
       <c r="F276" t="inlineStr">
@@ -12017,7 +12017,7 @@
       <c r="O276" t="inlineStr"/>
       <c r="P276" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) in 5-star Raid Battles Tue, Oct 7, at 10:00 AM Local Time</t>
+          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids Tue, Oct 7, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q276" t="inlineStr">
@@ -12037,12 +12037,12 @@
       <c r="D277" t="inlineStr"/>
       <c r="E277" t="inlineStr">
         <is>
-          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F277" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G277" t="inlineStr"/>
@@ -12056,7 +12056,7 @@
       <c r="O277" t="inlineStr"/>
       <c r="P277" t="inlineStr">
         <is>
-          <t>Raid Battles Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>GO Battle League Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q277" t="inlineStr">
@@ -12076,12 +12076,12 @@
       <c r="D278" t="inlineStr"/>
       <c r="E278" t="inlineStr">
         <is>
-          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F278" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G278" t="inlineStr"/>
@@ -12095,7 +12095,7 @@
       <c r="O278" t="inlineStr"/>
       <c r="P278" t="inlineStr">
         <is>
-          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q278" t="inlineStr">
@@ -12115,12 +12115,12 @@
       <c r="D279" t="inlineStr"/>
       <c r="E279" t="inlineStr">
         <is>
-          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F279" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G279" t="inlineStr"/>
@@ -12134,7 +12134,7 @@
       <c r="O279" t="inlineStr"/>
       <c r="P279" t="inlineStr">
         <is>
-          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids Tue, Oct 7, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q279" t="inlineStr">
@@ -12154,12 +12154,12 @@
       <c r="D280" t="inlineStr"/>
       <c r="E280" t="inlineStr">
         <is>
-          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F280" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G280" t="inlineStr"/>
@@ -12173,7 +12173,7 @@
       <c r="O280" t="inlineStr"/>
       <c r="P280" t="inlineStr">
         <is>
-          <t>Mega Sceptile, Mega Blaziken, and Mega Swampert in Mega Raids Tue, Oct 7, at 10:00 AM Local Time</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q280" t="inlineStr">
@@ -12193,12 +12193,12 @@
       <c r="D281" t="inlineStr"/>
       <c r="E281" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
+          <t>Ferroseed Spotlight Hour</t>
         </is>
       </c>
       <c r="F281" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G281" t="inlineStr"/>
@@ -12212,7 +12212,7 @@
       <c r="O281" t="inlineStr"/>
       <c r="P281" t="inlineStr">
         <is>
-          <t>GO Battle League Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Pokémon Spotlight Hour Ferroseed Spotlight Hour Tue, Oct 7, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q281" t="inlineStr">
@@ -12232,12 +12232,12 @@
       <c r="D282" t="inlineStr"/>
       <c r="E282" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
+          <t>Ferroseed Spotlight Hour</t>
         </is>
       </c>
       <c r="F282" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G282" t="inlineStr"/>
@@ -12251,7 +12251,7 @@
       <c r="O282" t="inlineStr"/>
       <c r="P282" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Ferroseed Spotlight Hour Tue, Oct 7, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q282" t="inlineStr">
@@ -12271,12 +12271,12 @@
       <c r="D283" t="inlineStr"/>
       <c r="E283" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
+          <t>Ferroseed Spotlight Hour</t>
         </is>
       </c>
       <c r="F283" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G283" t="inlineStr"/>
@@ -12290,7 +12290,7 @@
       <c r="O283" t="inlineStr"/>
       <c r="P283" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Ferroseed Spotlight Hour Tue, Oct 7, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q283" t="inlineStr">
@@ -12310,12 +12310,12 @@
       <c r="D284" t="inlineStr"/>
       <c r="E284" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
+          <t>Ferroseed Spotlight Hour</t>
         </is>
       </c>
       <c r="F284" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G284" t="inlineStr"/>
@@ -12329,7 +12329,7 @@
       <c r="O284" t="inlineStr"/>
       <c r="P284" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating...</t>
+          <t>Ferroseed Spotlight Hour Tue, Oct 7, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q284" t="inlineStr">
@@ -12349,12 +12349,12 @@
       <c r="D285" t="inlineStr"/>
       <c r="E285" t="inlineStr">
         <is>
-          <t>Ferroseed Spotlight Hour</t>
+          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F285" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G285" t="inlineStr"/>
@@ -12368,7 +12368,7 @@
       <c r="O285" t="inlineStr"/>
       <c r="P285" t="inlineStr">
         <is>
-          <t>Pokémon Spotlight Hour Ferroseed Spotlight Hour Tue, Oct 7, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Raid Hour Deoxys (Normal &amp; Defense Forme) Raid Hour Wed, Oct 8, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q285" t="inlineStr">
@@ -12388,12 +12388,12 @@
       <c r="D286" t="inlineStr"/>
       <c r="E286" t="inlineStr">
         <is>
-          <t>Ferroseed Spotlight Hour</t>
+          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F286" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G286" t="inlineStr"/>
@@ -12407,7 +12407,7 @@
       <c r="O286" t="inlineStr"/>
       <c r="P286" t="inlineStr">
         <is>
-          <t>Ferroseed Spotlight Hour Tue, Oct 7, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour Wed, Oct 8, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q286" t="inlineStr">
@@ -12427,12 +12427,12 @@
       <c r="D287" t="inlineStr"/>
       <c r="E287" t="inlineStr">
         <is>
-          <t>Ferroseed Spotlight Hour</t>
+          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F287" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G287" t="inlineStr"/>
@@ -12446,7 +12446,7 @@
       <c r="O287" t="inlineStr"/>
       <c r="P287" t="inlineStr">
         <is>
-          <t>Ferroseed Spotlight Hour Tue, Oct 7, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour Wed, Oct 8, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q287" t="inlineStr">
@@ -12466,12 +12466,12 @@
       <c r="D288" t="inlineStr"/>
       <c r="E288" t="inlineStr">
         <is>
-          <t>Ferroseed Spotlight Hour</t>
+          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F288" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G288" t="inlineStr"/>
@@ -12485,7 +12485,7 @@
       <c r="O288" t="inlineStr"/>
       <c r="P288" t="inlineStr">
         <is>
-          <t>Ferroseed Spotlight Hour Tue, Oct 7, at 6:00 PM Local Time</t>
+          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour Wed, Oct 8, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q288" t="inlineStr">
@@ -12505,12 +12505,12 @@
       <c r="D289" t="inlineStr"/>
       <c r="E289" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour</t>
+          <t>Harvest Festival</t>
         </is>
       </c>
       <c r="F289" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G289" t="inlineStr"/>
@@ -12524,7 +12524,7 @@
       <c r="O289" t="inlineStr"/>
       <c r="P289" t="inlineStr">
         <is>
-          <t>Raid Hour Deoxys (Normal &amp; Defense Forme) Raid Hour Wed, Oct 8, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Event Harvest Festival Fri, Oct 10, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q289" t="inlineStr">
@@ -12544,12 +12544,12 @@
       <c r="D290" t="inlineStr"/>
       <c r="E290" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour</t>
+          <t>Harvest Festival</t>
         </is>
       </c>
       <c r="F290" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G290" t="inlineStr"/>
@@ -12563,7 +12563,7 @@
       <c r="O290" t="inlineStr"/>
       <c r="P290" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour Wed, Oct 8, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Harvest Festival Fri, Oct 10, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q290" t="inlineStr">
@@ -12583,12 +12583,12 @@
       <c r="D291" t="inlineStr"/>
       <c r="E291" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour</t>
+          <t>Harvest Festival</t>
         </is>
       </c>
       <c r="F291" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G291" t="inlineStr"/>
@@ -12602,7 +12602,7 @@
       <c r="O291" t="inlineStr"/>
       <c r="P291" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour Wed, Oct 8, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Harvest Festival Fri, Oct 10, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q291" t="inlineStr">
@@ -12622,12 +12622,12 @@
       <c r="D292" t="inlineStr"/>
       <c r="E292" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour</t>
+          <t>Harvest Festival</t>
         </is>
       </c>
       <c r="F292" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G292" t="inlineStr"/>
@@ -12641,7 +12641,7 @@
       <c r="O292" t="inlineStr"/>
       <c r="P292" t="inlineStr">
         <is>
-          <t>Deoxys (Normal &amp; Defense Forme) Raid Hour Wed, Oct 8, at 6:00 PM Local Time</t>
+          <t>Harvest Festival Fri, Oct 10, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q292" t="inlineStr">
@@ -12661,12 +12661,12 @@
       <c r="D293" t="inlineStr"/>
       <c r="E293" t="inlineStr">
         <is>
-          <t>Harvest Festival</t>
+          <t>Solosis Community Day</t>
         </is>
       </c>
       <c r="F293" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Community Day</t>
         </is>
       </c>
       <c r="G293" t="inlineStr"/>
@@ -12680,7 +12680,7 @@
       <c r="O293" t="inlineStr"/>
       <c r="P293" t="inlineStr">
         <is>
-          <t>Event Harvest Festival Fri, Oct 10, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Community Day Solosis Community Day Sun, Oct 12, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q293" t="inlineStr">
@@ -12700,12 +12700,12 @@
       <c r="D294" t="inlineStr"/>
       <c r="E294" t="inlineStr">
         <is>
-          <t>Harvest Festival</t>
+          <t>Solosis Community Day</t>
         </is>
       </c>
       <c r="F294" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Community Day</t>
         </is>
       </c>
       <c r="G294" t="inlineStr"/>
@@ -12719,7 +12719,7 @@
       <c r="O294" t="inlineStr"/>
       <c r="P294" t="inlineStr">
         <is>
-          <t>Harvest Festival Fri, Oct 10, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Solosis Community Day Sun, Oct 12, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q294" t="inlineStr">
@@ -12739,12 +12739,12 @@
       <c r="D295" t="inlineStr"/>
       <c r="E295" t="inlineStr">
         <is>
-          <t>Harvest Festival</t>
+          <t>Solosis Community Day</t>
         </is>
       </c>
       <c r="F295" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Community Day</t>
         </is>
       </c>
       <c r="G295" t="inlineStr"/>
@@ -12758,7 +12758,7 @@
       <c r="O295" t="inlineStr"/>
       <c r="P295" t="inlineStr">
         <is>
-          <t>Harvest Festival Fri, Oct 10, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Solosis Community Day Sun, Oct 12, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q295" t="inlineStr">
@@ -12778,12 +12778,12 @@
       <c r="D296" t="inlineStr"/>
       <c r="E296" t="inlineStr">
         <is>
-          <t>Harvest Festival</t>
+          <t>Solosis Community Day</t>
         </is>
       </c>
       <c r="F296" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Community Day</t>
         </is>
       </c>
       <c r="G296" t="inlineStr"/>
@@ -12797,7 +12797,7 @@
       <c r="O296" t="inlineStr"/>
       <c r="P296" t="inlineStr">
         <is>
-          <t>Harvest Festival Fri, Oct 10, at 10:00 AM Local Time</t>
+          <t>Solosis Community Day Sun, Oct 12, at 2:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q296" t="inlineStr">
@@ -12817,12 +12817,12 @@
       <c r="D297" t="inlineStr"/>
       <c r="E297" t="inlineStr">
         <is>
-          <t>Solosis Community Day</t>
+          <t>Dynamax Bounsweet during Max Monday</t>
         </is>
       </c>
       <c r="F297" t="inlineStr">
         <is>
-          <t>Community Day</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G297" t="inlineStr"/>
@@ -12836,7 +12836,7 @@
       <c r="O297" t="inlineStr"/>
       <c r="P297" t="inlineStr">
         <is>
-          <t>Community Day Solosis Community Day Sun, Oct 12, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Max Mondays Dynamax Bounsweet during Max Monday Mon, Oct 13, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q297" t="inlineStr">
@@ -12856,12 +12856,12 @@
       <c r="D298" t="inlineStr"/>
       <c r="E298" t="inlineStr">
         <is>
-          <t>Solosis Community Day</t>
+          <t>Dynamax Bounsweet during Max Monday</t>
         </is>
       </c>
       <c r="F298" t="inlineStr">
         <is>
-          <t>Community Day</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G298" t="inlineStr"/>
@@ -12875,7 +12875,7 @@
       <c r="O298" t="inlineStr"/>
       <c r="P298" t="inlineStr">
         <is>
-          <t>Solosis Community Day Sun, Oct 12, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Dynamax Bounsweet during Max Monday Mon, Oct 13, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q298" t="inlineStr">
@@ -12895,12 +12895,12 @@
       <c r="D299" t="inlineStr"/>
       <c r="E299" t="inlineStr">
         <is>
-          <t>Solosis Community Day</t>
+          <t>Dynamax Bounsweet during Max Monday</t>
         </is>
       </c>
       <c r="F299" t="inlineStr">
         <is>
-          <t>Community Day</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G299" t="inlineStr"/>
@@ -12914,7 +12914,7 @@
       <c r="O299" t="inlineStr"/>
       <c r="P299" t="inlineStr">
         <is>
-          <t>Solosis Community Day Sun, Oct 12, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Dynamax Bounsweet during Max Monday Mon, Oct 13, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q299" t="inlineStr">
@@ -12934,12 +12934,12 @@
       <c r="D300" t="inlineStr"/>
       <c r="E300" t="inlineStr">
         <is>
-          <t>Solosis Community Day</t>
+          <t>Dynamax Bounsweet during Max Monday</t>
         </is>
       </c>
       <c r="F300" t="inlineStr">
         <is>
-          <t>Community Day</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G300" t="inlineStr"/>
@@ -12953,7 +12953,7 @@
       <c r="O300" t="inlineStr"/>
       <c r="P300" t="inlineStr">
         <is>
-          <t>Solosis Community Day Sun, Oct 12, at 2:00 PM Local Time</t>
+          <t>Dynamax Bounsweet during Max Monday Mon, Oct 13, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q300" t="inlineStr">
@@ -12973,12 +12973,12 @@
       <c r="D301" t="inlineStr"/>
       <c r="E301" t="inlineStr">
         <is>
-          <t>Dynamax Bounsweet during Max Monday</t>
+          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F301" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G301" t="inlineStr"/>
@@ -12992,7 +12992,7 @@
       <c r="O301" t="inlineStr"/>
       <c r="P301" t="inlineStr">
         <is>
-          <t>Max Mondays Dynamax Bounsweet during Max Monday Mon, Oct 13, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Raid Battles Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q301" t="inlineStr">
@@ -13012,12 +13012,12 @@
       <c r="D302" t="inlineStr"/>
       <c r="E302" t="inlineStr">
         <is>
-          <t>Dynamax Bounsweet during Max Monday</t>
+          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F302" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G302" t="inlineStr"/>
@@ -13031,7 +13031,7 @@
       <c r="O302" t="inlineStr"/>
       <c r="P302" t="inlineStr">
         <is>
-          <t>Dynamax Bounsweet during Max Monday Mon, Oct 13, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q302" t="inlineStr">
@@ -13051,12 +13051,12 @@
       <c r="D303" t="inlineStr"/>
       <c r="E303" t="inlineStr">
         <is>
-          <t>Dynamax Bounsweet during Max Monday</t>
+          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F303" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G303" t="inlineStr"/>
@@ -13070,7 +13070,7 @@
       <c r="O303" t="inlineStr"/>
       <c r="P303" t="inlineStr">
         <is>
-          <t>Dynamax Bounsweet during Max Monday Mon, Oct 13, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q303" t="inlineStr">
@@ -13090,12 +13090,12 @@
       <c r="D304" t="inlineStr"/>
       <c r="E304" t="inlineStr">
         <is>
-          <t>Dynamax Bounsweet during Max Monday</t>
+          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F304" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G304" t="inlineStr"/>
@@ -13109,7 +13109,7 @@
       <c r="O304" t="inlineStr"/>
       <c r="P304" t="inlineStr">
         <is>
-          <t>Dynamax Bounsweet during Max Monday Mon, Oct 13, at 6:00 PM Local Time</t>
+          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles Tue, Oct 14, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q304" t="inlineStr">
@@ -13129,7 +13129,7 @@
       <c r="D305" t="inlineStr"/>
       <c r="E305" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles</t>
+          <t>Mega Mawile and Mega Salamence in Mega Raids</t>
         </is>
       </c>
       <c r="F305" t="inlineStr">
@@ -13148,7 +13148,7 @@
       <c r="O305" t="inlineStr"/>
       <c r="P305" t="inlineStr">
         <is>
-          <t>Raid Battles Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Raid Battles Mega Mawile and Mega Salamence in Mega Raids Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q305" t="inlineStr">
@@ -13168,7 +13168,7 @@
       <c r="D306" t="inlineStr"/>
       <c r="E306" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles</t>
+          <t>Mega Mawile and Mega Salamence in Mega Raids</t>
         </is>
       </c>
       <c r="F306" t="inlineStr">
@@ -13187,7 +13187,7 @@
       <c r="O306" t="inlineStr"/>
       <c r="P306" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Mega Mawile and Mega Salamence in Mega Raids Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q306" t="inlineStr">
@@ -13207,7 +13207,7 @@
       <c r="D307" t="inlineStr"/>
       <c r="E307" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles</t>
+          <t>Mega Mawile and Mega Salamence in Mega Raids</t>
         </is>
       </c>
       <c r="F307" t="inlineStr">
@@ -13226,7 +13226,7 @@
       <c r="O307" t="inlineStr"/>
       <c r="P307" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Mega Mawile and Mega Salamence in Mega Raids Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q307" t="inlineStr">
@@ -13246,7 +13246,7 @@
       <c r="D308" t="inlineStr"/>
       <c r="E308" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles</t>
+          <t>Mega Mawile and Mega Salamence in Mega Raids</t>
         </is>
       </c>
       <c r="F308" t="inlineStr">
@@ -13265,7 +13265,7 @@
       <c r="O308" t="inlineStr"/>
       <c r="P308" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) in 5-star Raid Battles Tue, Oct 14, at 10:00 AM Local Time</t>
+          <t>Mega Mawile and Mega Salamence in Mega Raids Tue, Oct 14, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q308" t="inlineStr">
@@ -13285,12 +13285,12 @@
       <c r="D309" t="inlineStr"/>
       <c r="E309" t="inlineStr">
         <is>
-          <t>Mega Mawile and Mega Salamence in Mega Raids</t>
+          <t>Master Premier and Great League Remix | Tales of Transformation</t>
         </is>
       </c>
       <c r="F309" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G309" t="inlineStr"/>
@@ -13304,7 +13304,7 @@
       <c r="O309" t="inlineStr"/>
       <c r="P309" t="inlineStr">
         <is>
-          <t>Raid Battles Mega Mawile and Mega Salamence in Mega Raids Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>GO Battle League Master Premier and Great League Remix | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q309" t="inlineStr">
@@ -13324,12 +13324,12 @@
       <c r="D310" t="inlineStr"/>
       <c r="E310" t="inlineStr">
         <is>
-          <t>Mega Mawile and Mega Salamence in Mega Raids</t>
+          <t>Master Premier and Great League Remix | Tales of Transformation</t>
         </is>
       </c>
       <c r="F310" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G310" t="inlineStr"/>
@@ -13343,7 +13343,7 @@
       <c r="O310" t="inlineStr"/>
       <c r="P310" t="inlineStr">
         <is>
-          <t>Mega Mawile and Mega Salamence in Mega Raids Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Master Premier and Great League Remix | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q310" t="inlineStr">
@@ -13363,12 +13363,12 @@
       <c r="D311" t="inlineStr"/>
       <c r="E311" t="inlineStr">
         <is>
-          <t>Mega Mawile and Mega Salamence in Mega Raids</t>
+          <t>Master Premier and Great League Remix | Tales of Transformation</t>
         </is>
       </c>
       <c r="F311" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G311" t="inlineStr"/>
@@ -13382,7 +13382,7 @@
       <c r="O311" t="inlineStr"/>
       <c r="P311" t="inlineStr">
         <is>
-          <t>Mega Mawile and Mega Salamence in Mega Raids Tue, Oct 14, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Master Premier and Great League Remix | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q311" t="inlineStr">
@@ -13402,12 +13402,12 @@
       <c r="D312" t="inlineStr"/>
       <c r="E312" t="inlineStr">
         <is>
-          <t>Mega Mawile and Mega Salamence in Mega Raids</t>
+          <t>Master Premier and Great League Remix | Tales of Transformation</t>
         </is>
       </c>
       <c r="F312" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G312" t="inlineStr"/>
@@ -13421,7 +13421,7 @@
       <c r="O312" t="inlineStr"/>
       <c r="P312" t="inlineStr">
         <is>
-          <t>Mega Mawile and Mega Salamence in Mega Raids Tue, Oct 14, at 10:00 AM Local Time</t>
+          <t>Master Premier and Great League Remix | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q312" t="inlineStr">
@@ -13441,12 +13441,12 @@
       <c r="D313" t="inlineStr"/>
       <c r="E313" t="inlineStr">
         <is>
-          <t>Master Premier and Great League Remix | Tales of Transformation</t>
+          <t>Petilil Spotlight Hour</t>
         </is>
       </c>
       <c r="F313" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G313" t="inlineStr"/>
@@ -13460,7 +13460,7 @@
       <c r="O313" t="inlineStr"/>
       <c r="P313" t="inlineStr">
         <is>
-          <t>GO Battle League Master Premier and Great League Remix | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Pokémon Spotlight Hour Petilil Spotlight Hour Tue, Oct 14, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q313" t="inlineStr">
@@ -13480,12 +13480,12 @@
       <c r="D314" t="inlineStr"/>
       <c r="E314" t="inlineStr">
         <is>
-          <t>Master Premier and Great League Remix | Tales of Transformation</t>
+          <t>Petilil Spotlight Hour</t>
         </is>
       </c>
       <c r="F314" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G314" t="inlineStr"/>
@@ -13499,7 +13499,7 @@
       <c r="O314" t="inlineStr"/>
       <c r="P314" t="inlineStr">
         <is>
-          <t>Master Premier and Great League Remix | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Petilil Spotlight Hour Tue, Oct 14, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q314" t="inlineStr">
@@ -13519,12 +13519,12 @@
       <c r="D315" t="inlineStr"/>
       <c r="E315" t="inlineStr">
         <is>
-          <t>Master Premier and Great League Remix | Tales of Transformation</t>
+          <t>Petilil Spotlight Hour</t>
         </is>
       </c>
       <c r="F315" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G315" t="inlineStr"/>
@@ -13538,7 +13538,7 @@
       <c r="O315" t="inlineStr"/>
       <c r="P315" t="inlineStr">
         <is>
-          <t>Master Premier and Great League Remix | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Petilil Spotlight Hour Tue, Oct 14, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q315" t="inlineStr">
@@ -13558,12 +13558,12 @@
       <c r="D316" t="inlineStr"/>
       <c r="E316" t="inlineStr">
         <is>
-          <t>Master Premier and Great League Remix | Tales of Transformation</t>
+          <t>Petilil Spotlight Hour</t>
         </is>
       </c>
       <c r="F316" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G316" t="inlineStr"/>
@@ -13577,7 +13577,7 @@
       <c r="O316" t="inlineStr"/>
       <c r="P316" t="inlineStr">
         <is>
-          <t>Master Premier and Great League Remix | Tales of Transformation Calculating...</t>
+          <t>Petilil Spotlight Hour Tue, Oct 14, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q316" t="inlineStr">
@@ -13597,12 +13597,12 @@
       <c r="D317" t="inlineStr"/>
       <c r="E317" t="inlineStr">
         <is>
-          <t>Petilil Spotlight Hour</t>
+          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F317" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G317" t="inlineStr"/>
@@ -13616,7 +13616,7 @@
       <c r="O317" t="inlineStr"/>
       <c r="P317" t="inlineStr">
         <is>
-          <t>Pokémon Spotlight Hour Petilil Spotlight Hour Tue, Oct 14, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Raid Hour Deoxys (Attack &amp; Speed Forme) Raid Hour Wed, Oct 15, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q317" t="inlineStr">
@@ -13636,12 +13636,12 @@
       <c r="D318" t="inlineStr"/>
       <c r="E318" t="inlineStr">
         <is>
-          <t>Petilil Spotlight Hour</t>
+          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F318" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G318" t="inlineStr"/>
@@ -13655,7 +13655,7 @@
       <c r="O318" t="inlineStr"/>
       <c r="P318" t="inlineStr">
         <is>
-          <t>Petilil Spotlight Hour Tue, Oct 14, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour Wed, Oct 15, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q318" t="inlineStr">
@@ -13675,12 +13675,12 @@
       <c r="D319" t="inlineStr"/>
       <c r="E319" t="inlineStr">
         <is>
-          <t>Petilil Spotlight Hour</t>
+          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F319" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G319" t="inlineStr"/>
@@ -13694,7 +13694,7 @@
       <c r="O319" t="inlineStr"/>
       <c r="P319" t="inlineStr">
         <is>
-          <t>Petilil Spotlight Hour Tue, Oct 14, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour Wed, Oct 15, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q319" t="inlineStr">
@@ -13714,12 +13714,12 @@
       <c r="D320" t="inlineStr"/>
       <c r="E320" t="inlineStr">
         <is>
-          <t>Petilil Spotlight Hour</t>
+          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F320" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G320" t="inlineStr"/>
@@ -13733,7 +13733,7 @@
       <c r="O320" t="inlineStr"/>
       <c r="P320" t="inlineStr">
         <is>
-          <t>Petilil Spotlight Hour Tue, Oct 14, at 6:00 PM Local Time</t>
+          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour Wed, Oct 15, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q320" t="inlineStr">
@@ -13753,12 +13753,12 @@
       <c r="D321" t="inlineStr"/>
       <c r="E321" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour</t>
+          <t>Pokémon Legends: Z-A Celebration Event</t>
         </is>
       </c>
       <c r="F321" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G321" t="inlineStr"/>
@@ -13772,7 +13772,7 @@
       <c r="O321" t="inlineStr"/>
       <c r="P321" t="inlineStr">
         <is>
-          <t>Raid Hour Deoxys (Attack &amp; Speed Forme) Raid Hour Wed, Oct 15, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Event Pokémon Legends: Z-A Celebration Event Thu, Oct 16, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q321" t="inlineStr">
@@ -13792,12 +13792,12 @@
       <c r="D322" t="inlineStr"/>
       <c r="E322" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour</t>
+          <t>Pokémon Legends: Z-A Celebration Event</t>
         </is>
       </c>
       <c r="F322" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G322" t="inlineStr"/>
@@ -13811,7 +13811,7 @@
       <c r="O322" t="inlineStr"/>
       <c r="P322" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour Wed, Oct 15, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Pokémon Legends: Z-A Celebration Event Thu, Oct 16, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q322" t="inlineStr">
@@ -13831,12 +13831,12 @@
       <c r="D323" t="inlineStr"/>
       <c r="E323" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour</t>
+          <t>Pokémon Legends: Z-A Celebration Event</t>
         </is>
       </c>
       <c r="F323" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G323" t="inlineStr"/>
@@ -13850,7 +13850,7 @@
       <c r="O323" t="inlineStr"/>
       <c r="P323" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour Wed, Oct 15, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Pokémon Legends: Z-A Celebration Event Thu, Oct 16, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q323" t="inlineStr">
@@ -13870,12 +13870,12 @@
       <c r="D324" t="inlineStr"/>
       <c r="E324" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour</t>
+          <t>Pokémon Legends: Z-A Celebration Event</t>
         </is>
       </c>
       <c r="F324" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G324" t="inlineStr"/>
@@ -13889,7 +13889,7 @@
       <c r="O324" t="inlineStr"/>
       <c r="P324" t="inlineStr">
         <is>
-          <t>Deoxys (Attack &amp; Speed Forme) Raid Hour Wed, Oct 15, at 6:00 PM Local Time</t>
+          <t>Pokémon Legends: Z-A Celebration Event Thu, Oct 16, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q324" t="inlineStr">
@@ -13909,12 +13909,12 @@
       <c r="D325" t="inlineStr"/>
       <c r="E325" t="inlineStr">
         <is>
-          <t>Pokémon Legends: Z-A Celebration Event</t>
+          <t>Mega Rayquaza Raid Day</t>
         </is>
       </c>
       <c r="F325" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G325" t="inlineStr"/>
@@ -13928,7 +13928,7 @@
       <c r="O325" t="inlineStr"/>
       <c r="P325" t="inlineStr">
         <is>
-          <t>Event Pokémon Legends: Z-A Celebration Event Thu, Oct 16, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Raid Day Mega Rayquaza Raid Day Sat, Oct 18, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q325" t="inlineStr">
@@ -13948,12 +13948,12 @@
       <c r="D326" t="inlineStr"/>
       <c r="E326" t="inlineStr">
         <is>
-          <t>Pokémon Legends: Z-A Celebration Event</t>
+          <t>Mega Rayquaza Raid Day</t>
         </is>
       </c>
       <c r="F326" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G326" t="inlineStr"/>
@@ -13967,7 +13967,7 @@
       <c r="O326" t="inlineStr"/>
       <c r="P326" t="inlineStr">
         <is>
-          <t>Pokémon Legends: Z-A Celebration Event Thu, Oct 16, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Mega Rayquaza Raid Day Sat, Oct 18, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q326" t="inlineStr">
@@ -13987,12 +13987,12 @@
       <c r="D327" t="inlineStr"/>
       <c r="E327" t="inlineStr">
         <is>
-          <t>Pokémon Legends: Z-A Celebration Event</t>
+          <t>Mega Rayquaza Raid Day</t>
         </is>
       </c>
       <c r="F327" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G327" t="inlineStr"/>
@@ -14006,7 +14006,7 @@
       <c r="O327" t="inlineStr"/>
       <c r="P327" t="inlineStr">
         <is>
-          <t>Pokémon Legends: Z-A Celebration Event Thu, Oct 16, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Mega Rayquaza Raid Day Sat, Oct 18, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q327" t="inlineStr">
@@ -14026,12 +14026,12 @@
       <c r="D328" t="inlineStr"/>
       <c r="E328" t="inlineStr">
         <is>
-          <t>Pokémon Legends: Z-A Celebration Event</t>
+          <t>Mega Rayquaza Raid Day</t>
         </is>
       </c>
       <c r="F328" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G328" t="inlineStr"/>
@@ -14045,7 +14045,7 @@
       <c r="O328" t="inlineStr"/>
       <c r="P328" t="inlineStr">
         <is>
-          <t>Pokémon Legends: Z-A Celebration Event Thu, Oct 16, at 10:00 AM Local Time</t>
+          <t>Mega Rayquaza Raid Day Sat, Oct 18, at 2:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q328" t="inlineStr">
@@ -14065,12 +14065,12 @@
       <c r="D329" t="inlineStr"/>
       <c r="E329" t="inlineStr">
         <is>
-          <t>Mega Rayquaza Raid Day</t>
+          <t>Dynamax Gastly during Max Monday</t>
         </is>
       </c>
       <c r="F329" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G329" t="inlineStr"/>
@@ -14084,7 +14084,7 @@
       <c r="O329" t="inlineStr"/>
       <c r="P329" t="inlineStr">
         <is>
-          <t>Raid Day Mega Rayquaza Raid Day Sat, Oct 18, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Max Mondays Dynamax Gastly during Max Monday Mon, Oct 20, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q329" t="inlineStr">
@@ -14104,12 +14104,12 @@
       <c r="D330" t="inlineStr"/>
       <c r="E330" t="inlineStr">
         <is>
-          <t>Mega Rayquaza Raid Day</t>
+          <t>Dynamax Gastly during Max Monday</t>
         </is>
       </c>
       <c r="F330" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G330" t="inlineStr"/>
@@ -14123,7 +14123,7 @@
       <c r="O330" t="inlineStr"/>
       <c r="P330" t="inlineStr">
         <is>
-          <t>Mega Rayquaza Raid Day Sat, Oct 18, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Dynamax Gastly during Max Monday Mon, Oct 20, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q330" t="inlineStr">
@@ -14143,12 +14143,12 @@
       <c r="D331" t="inlineStr"/>
       <c r="E331" t="inlineStr">
         <is>
-          <t>Mega Rayquaza Raid Day</t>
+          <t>Dynamax Gastly during Max Monday</t>
         </is>
       </c>
       <c r="F331" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G331" t="inlineStr"/>
@@ -14162,7 +14162,7 @@
       <c r="O331" t="inlineStr"/>
       <c r="P331" t="inlineStr">
         <is>
-          <t>Mega Rayquaza Raid Day Sat, Oct 18, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Dynamax Gastly during Max Monday Mon, Oct 20, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q331" t="inlineStr">
@@ -14182,12 +14182,12 @@
       <c r="D332" t="inlineStr"/>
       <c r="E332" t="inlineStr">
         <is>
-          <t>Mega Rayquaza Raid Day</t>
+          <t>Dynamax Gastly during Max Monday</t>
         </is>
       </c>
       <c r="F332" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G332" t="inlineStr"/>
@@ -14201,7 +14201,7 @@
       <c r="O332" t="inlineStr"/>
       <c r="P332" t="inlineStr">
         <is>
-          <t>Mega Rayquaza Raid Day Sat, Oct 18, at 2:00 PM Local Time</t>
+          <t>Dynamax Gastly during Max Monday Mon, Oct 20, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q332" t="inlineStr">
@@ -14221,7 +14221,7 @@
       <c r="D333" t="inlineStr"/>
       <c r="E333" t="inlineStr">
         <is>
-          <t>Dynamax Gastly during Max Monday</t>
+          <t>GO Pass: Halloween 2025</t>
         </is>
       </c>
       <c r="F333" t="inlineStr">
@@ -14240,7 +14240,7 @@
       <c r="O333" t="inlineStr"/>
       <c r="P333" t="inlineStr">
         <is>
-          <t>Max Mondays Dynamax Gastly during Max Monday Mon, Oct 20, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>GO Pass GO Pass: Halloween 2025 Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q333" t="inlineStr">
@@ -14260,7 +14260,7 @@
       <c r="D334" t="inlineStr"/>
       <c r="E334" t="inlineStr">
         <is>
-          <t>Dynamax Gastly during Max Monday</t>
+          <t>GO Pass: Halloween 2025</t>
         </is>
       </c>
       <c r="F334" t="inlineStr">
@@ -14279,7 +14279,7 @@
       <c r="O334" t="inlineStr"/>
       <c r="P334" t="inlineStr">
         <is>
-          <t>Dynamax Gastly during Max Monday Mon, Oct 20, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>GO Pass: Halloween 2025 Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q334" t="inlineStr">
@@ -14299,7 +14299,7 @@
       <c r="D335" t="inlineStr"/>
       <c r="E335" t="inlineStr">
         <is>
-          <t>Dynamax Gastly during Max Monday</t>
+          <t>GO Pass: Halloween 2025</t>
         </is>
       </c>
       <c r="F335" t="inlineStr">
@@ -14318,7 +14318,7 @@
       <c r="O335" t="inlineStr"/>
       <c r="P335" t="inlineStr">
         <is>
-          <t>Dynamax Gastly during Max Monday Mon, Oct 20, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>GO Pass: Halloween 2025 Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q335" t="inlineStr">
@@ -14338,7 +14338,7 @@
       <c r="D336" t="inlineStr"/>
       <c r="E336" t="inlineStr">
         <is>
-          <t>Dynamax Gastly during Max Monday</t>
+          <t>GO Pass: Halloween 2025</t>
         </is>
       </c>
       <c r="F336" t="inlineStr">
@@ -14357,7 +14357,7 @@
       <c r="O336" t="inlineStr"/>
       <c r="P336" t="inlineStr">
         <is>
-          <t>Dynamax Gastly during Max Monday Mon, Oct 20, at 6:00 PM Local Time</t>
+          <t>GO Pass: Halloween 2025 Tue, Oct 21, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q336" t="inlineStr">
@@ -14377,7 +14377,7 @@
       <c r="D337" t="inlineStr"/>
       <c r="E337" t="inlineStr">
         <is>
-          <t>GO Pass: Halloween 2025</t>
+          <t>Halloween 2025 Part I</t>
         </is>
       </c>
       <c r="F337" t="inlineStr">
@@ -14396,7 +14396,7 @@
       <c r="O337" t="inlineStr"/>
       <c r="P337" t="inlineStr">
         <is>
-          <t>GO Pass GO Pass: Halloween 2025 Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Event Halloween 2025 Part I Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q337" t="inlineStr">
@@ -14416,7 +14416,7 @@
       <c r="D338" t="inlineStr"/>
       <c r="E338" t="inlineStr">
         <is>
-          <t>GO Pass: Halloween 2025</t>
+          <t>Halloween 2025 Part I</t>
         </is>
       </c>
       <c r="F338" t="inlineStr">
@@ -14435,7 +14435,7 @@
       <c r="O338" t="inlineStr"/>
       <c r="P338" t="inlineStr">
         <is>
-          <t>GO Pass: Halloween 2025 Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Halloween 2025 Part I Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q338" t="inlineStr">
@@ -14455,7 +14455,7 @@
       <c r="D339" t="inlineStr"/>
       <c r="E339" t="inlineStr">
         <is>
-          <t>GO Pass: Halloween 2025</t>
+          <t>Halloween 2025 Part I</t>
         </is>
       </c>
       <c r="F339" t="inlineStr">
@@ -14474,7 +14474,7 @@
       <c r="O339" t="inlineStr"/>
       <c r="P339" t="inlineStr">
         <is>
-          <t>GO Pass: Halloween 2025 Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Halloween 2025 Part I Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q339" t="inlineStr">
@@ -14494,7 +14494,7 @@
       <c r="D340" t="inlineStr"/>
       <c r="E340" t="inlineStr">
         <is>
-          <t>GO Pass: Halloween 2025</t>
+          <t>Halloween 2025 Part I</t>
         </is>
       </c>
       <c r="F340" t="inlineStr">
@@ -14513,7 +14513,7 @@
       <c r="O340" t="inlineStr"/>
       <c r="P340" t="inlineStr">
         <is>
-          <t>GO Pass: Halloween 2025 Tue, Oct 21, at 10:00 AM Local Time</t>
+          <t>Halloween 2025 Part I Tue, Oct 21, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q340" t="inlineStr">
@@ -14533,12 +14533,12 @@
       <c r="D341" t="inlineStr"/>
       <c r="E341" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part I</t>
+          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F341" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G341" t="inlineStr"/>
@@ -14552,7 +14552,7 @@
       <c r="O341" t="inlineStr"/>
       <c r="P341" t="inlineStr">
         <is>
-          <t>Event Halloween 2025 Part I Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Raid Battles Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q341" t="inlineStr">
@@ -14572,12 +14572,12 @@
       <c r="D342" t="inlineStr"/>
       <c r="E342" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part I</t>
+          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F342" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G342" t="inlineStr"/>
@@ -14591,7 +14591,7 @@
       <c r="O342" t="inlineStr"/>
       <c r="P342" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part I Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q342" t="inlineStr">
@@ -14611,12 +14611,12 @@
       <c r="D343" t="inlineStr"/>
       <c r="E343" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part I</t>
+          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F343" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G343" t="inlineStr"/>
@@ -14630,7 +14630,7 @@
       <c r="O343" t="inlineStr"/>
       <c r="P343" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part I Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q343" t="inlineStr">
@@ -14650,12 +14650,12 @@
       <c r="D344" t="inlineStr"/>
       <c r="E344" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part I</t>
+          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F344" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G344" t="inlineStr"/>
@@ -14669,7 +14669,7 @@
       <c r="O344" t="inlineStr"/>
       <c r="P344" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part I Tue, Oct 21, at 10:00 AM Local Time</t>
+          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles Tue, Oct 21, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q344" t="inlineStr">
@@ -14689,7 +14689,7 @@
       <c r="D345" t="inlineStr"/>
       <c r="E345" t="inlineStr">
         <is>
-          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles</t>
+          <t>Mega Houndoom and Mega Absol in Mega Raids</t>
         </is>
       </c>
       <c r="F345" t="inlineStr">
@@ -14708,7 +14708,7 @@
       <c r="O345" t="inlineStr"/>
       <c r="P345" t="inlineStr">
         <is>
-          <t>Raid Battles Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Raid Battles Mega Houndoom and Mega Absol in Mega Raids Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q345" t="inlineStr">
@@ -14728,7 +14728,7 @@
       <c r="D346" t="inlineStr"/>
       <c r="E346" t="inlineStr">
         <is>
-          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles</t>
+          <t>Mega Houndoom and Mega Absol in Mega Raids</t>
         </is>
       </c>
       <c r="F346" t="inlineStr">
@@ -14747,7 +14747,7 @@
       <c r="O346" t="inlineStr"/>
       <c r="P346" t="inlineStr">
         <is>
-          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Mega Houndoom and Mega Absol in Mega Raids Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q346" t="inlineStr">
@@ -14767,7 +14767,7 @@
       <c r="D347" t="inlineStr"/>
       <c r="E347" t="inlineStr">
         <is>
-          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles</t>
+          <t>Mega Houndoom and Mega Absol in Mega Raids</t>
         </is>
       </c>
       <c r="F347" t="inlineStr">
@@ -14786,7 +14786,7 @@
       <c r="O347" t="inlineStr"/>
       <c r="P347" t="inlineStr">
         <is>
-          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Mega Houndoom and Mega Absol in Mega Raids Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q347" t="inlineStr">
@@ -14806,7 +14806,7 @@
       <c r="D348" t="inlineStr"/>
       <c r="E348" t="inlineStr">
         <is>
-          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles</t>
+          <t>Mega Houndoom and Mega Absol in Mega Raids</t>
         </is>
       </c>
       <c r="F348" t="inlineStr">
@@ -14825,7 +14825,7 @@
       <c r="O348" t="inlineStr"/>
       <c r="P348" t="inlineStr">
         <is>
-          <t>Genesect (Douse &amp; Shock Drive) in 5-star Raid Battles Tue, Oct 21, at 10:00 AM Local Time</t>
+          <t>Mega Houndoom and Mega Absol in Mega Raids Tue, Oct 21, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q348" t="inlineStr">
@@ -14845,12 +14845,12 @@
       <c r="D349" t="inlineStr"/>
       <c r="E349" t="inlineStr">
         <is>
-          <t>Mega Houndoom and Mega Absol in Mega Raids</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F349" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G349" t="inlineStr"/>
@@ -14864,7 +14864,7 @@
       <c r="O349" t="inlineStr"/>
       <c r="P349" t="inlineStr">
         <is>
-          <t>Raid Battles Mega Houndoom and Mega Absol in Mega Raids Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>GO Battle League Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q349" t="inlineStr">
@@ -14884,12 +14884,12 @@
       <c r="D350" t="inlineStr"/>
       <c r="E350" t="inlineStr">
         <is>
-          <t>Mega Houndoom and Mega Absol in Mega Raids</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F350" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G350" t="inlineStr"/>
@@ -14903,7 +14903,7 @@
       <c r="O350" t="inlineStr"/>
       <c r="P350" t="inlineStr">
         <is>
-          <t>Mega Houndoom and Mega Absol in Mega Raids Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q350" t="inlineStr">
@@ -14923,12 +14923,12 @@
       <c r="D351" t="inlineStr"/>
       <c r="E351" t="inlineStr">
         <is>
-          <t>Mega Houndoom and Mega Absol in Mega Raids</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F351" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G351" t="inlineStr"/>
@@ -14942,7 +14942,7 @@
       <c r="O351" t="inlineStr"/>
       <c r="P351" t="inlineStr">
         <is>
-          <t>Mega Houndoom and Mega Absol in Mega Raids Tue, Oct 21, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q351" t="inlineStr">
@@ -14962,12 +14962,12 @@
       <c r="D352" t="inlineStr"/>
       <c r="E352" t="inlineStr">
         <is>
-          <t>Mega Houndoom and Mega Absol in Mega Raids</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F352" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G352" t="inlineStr"/>
@@ -14981,7 +14981,7 @@
       <c r="O352" t="inlineStr"/>
       <c r="P352" t="inlineStr">
         <is>
-          <t>Mega Houndoom and Mega Absol in Mega Raids Tue, Oct 21, at 10:00 AM Local Time</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q352" t="inlineStr">
@@ -15001,12 +15001,12 @@
       <c r="D353" t="inlineStr"/>
       <c r="E353" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Gastly Spotlight Hour</t>
         </is>
       </c>
       <c r="F353" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G353" t="inlineStr"/>
@@ -15020,7 +15020,7 @@
       <c r="O353" t="inlineStr"/>
       <c r="P353" t="inlineStr">
         <is>
-          <t>GO Battle League Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Pokémon Spotlight Hour Gastly Spotlight Hour Tue, Oct 21, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q353" t="inlineStr">
@@ -15040,12 +15040,12 @@
       <c r="D354" t="inlineStr"/>
       <c r="E354" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Gastly Spotlight Hour</t>
         </is>
       </c>
       <c r="F354" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G354" t="inlineStr"/>
@@ -15059,7 +15059,7 @@
       <c r="O354" t="inlineStr"/>
       <c r="P354" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Gastly Spotlight Hour Tue, Oct 21, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q354" t="inlineStr">
@@ -15079,12 +15079,12 @@
       <c r="D355" t="inlineStr"/>
       <c r="E355" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Gastly Spotlight Hour</t>
         </is>
       </c>
       <c r="F355" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G355" t="inlineStr"/>
@@ -15098,7 +15098,7 @@
       <c r="O355" t="inlineStr"/>
       <c r="P355" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Gastly Spotlight Hour Tue, Oct 21, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q355" t="inlineStr">
@@ -15118,12 +15118,12 @@
       <c r="D356" t="inlineStr"/>
       <c r="E356" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Gastly Spotlight Hour</t>
         </is>
       </c>
       <c r="F356" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G356" t="inlineStr"/>
@@ -15137,7 +15137,7 @@
       <c r="O356" t="inlineStr"/>
       <c r="P356" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating...</t>
+          <t>Gastly Spotlight Hour Tue, Oct 21, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q356" t="inlineStr">
@@ -15157,12 +15157,12 @@
       <c r="D357" t="inlineStr"/>
       <c r="E357" t="inlineStr">
         <is>
-          <t>Gastly Spotlight Hour</t>
+          <t>Genesect Raid Hour</t>
         </is>
       </c>
       <c r="F357" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G357" t="inlineStr"/>
@@ -15176,7 +15176,7 @@
       <c r="O357" t="inlineStr"/>
       <c r="P357" t="inlineStr">
         <is>
-          <t>Pokémon Spotlight Hour Gastly Spotlight Hour Tue, Oct 21, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Raid Hour Genesect Raid Hour Wed, Oct 22, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q357" t="inlineStr">
@@ -15196,12 +15196,12 @@
       <c r="D358" t="inlineStr"/>
       <c r="E358" t="inlineStr">
         <is>
-          <t>Gastly Spotlight Hour</t>
+          <t>Genesect Raid Hour</t>
         </is>
       </c>
       <c r="F358" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G358" t="inlineStr"/>
@@ -15215,7 +15215,7 @@
       <c r="O358" t="inlineStr"/>
       <c r="P358" t="inlineStr">
         <is>
-          <t>Gastly Spotlight Hour Tue, Oct 21, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Genesect Raid Hour Wed, Oct 22, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q358" t="inlineStr">
@@ -15235,12 +15235,12 @@
       <c r="D359" t="inlineStr"/>
       <c r="E359" t="inlineStr">
         <is>
-          <t>Gastly Spotlight Hour</t>
+          <t>Genesect Raid Hour</t>
         </is>
       </c>
       <c r="F359" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G359" t="inlineStr"/>
@@ -15254,7 +15254,7 @@
       <c r="O359" t="inlineStr"/>
       <c r="P359" t="inlineStr">
         <is>
-          <t>Gastly Spotlight Hour Tue, Oct 21, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Genesect Raid Hour Wed, Oct 22, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q359" t="inlineStr">
@@ -15274,12 +15274,12 @@
       <c r="D360" t="inlineStr"/>
       <c r="E360" t="inlineStr">
         <is>
-          <t>Gastly Spotlight Hour</t>
+          <t>Genesect Raid Hour</t>
         </is>
       </c>
       <c r="F360" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G360" t="inlineStr"/>
@@ -15293,7 +15293,7 @@
       <c r="O360" t="inlineStr"/>
       <c r="P360" t="inlineStr">
         <is>
-          <t>Gastly Spotlight Hour Tue, Oct 21, at 6:00 PM Local Time</t>
+          <t>Genesect Raid Hour Wed, Oct 22, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q360" t="inlineStr">
@@ -15313,12 +15313,12 @@
       <c r="D361" t="inlineStr"/>
       <c r="E361" t="inlineStr">
         <is>
-          <t>Genesect Raid Hour</t>
+          <t>GO Battle Weekend: Tales of Transformation</t>
         </is>
       </c>
       <c r="F361" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G361" t="inlineStr"/>
@@ -15332,7 +15332,7 @@
       <c r="O361" t="inlineStr"/>
       <c r="P361" t="inlineStr">
         <is>
-          <t>Raid Hour Genesect Raid Hour Wed, Oct 22, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Event GO Battle Weekend: Tales of Transformation Sat, Oct 25, at 12:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q361" t="inlineStr">
@@ -15352,12 +15352,12 @@
       <c r="D362" t="inlineStr"/>
       <c r="E362" t="inlineStr">
         <is>
-          <t>Genesect Raid Hour</t>
+          <t>GO Battle Weekend: Tales of Transformation</t>
         </is>
       </c>
       <c r="F362" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G362" t="inlineStr"/>
@@ -15371,7 +15371,7 @@
       <c r="O362" t="inlineStr"/>
       <c r="P362" t="inlineStr">
         <is>
-          <t>Genesect Raid Hour Wed, Oct 22, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>GO Battle Weekend: Tales of Transformation Sat, Oct 25, at 12:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q362" t="inlineStr">
@@ -15391,12 +15391,12 @@
       <c r="D363" t="inlineStr"/>
       <c r="E363" t="inlineStr">
         <is>
-          <t>Genesect Raid Hour</t>
+          <t>GO Battle Weekend: Tales of Transformation</t>
         </is>
       </c>
       <c r="F363" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G363" t="inlineStr"/>
@@ -15410,7 +15410,7 @@
       <c r="O363" t="inlineStr"/>
       <c r="P363" t="inlineStr">
         <is>
-          <t>Genesect Raid Hour Wed, Oct 22, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>GO Battle Weekend: Tales of Transformation Sat, Oct 25, at 12:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q363" t="inlineStr">
@@ -15430,12 +15430,12 @@
       <c r="D364" t="inlineStr"/>
       <c r="E364" t="inlineStr">
         <is>
-          <t>Genesect Raid Hour</t>
+          <t>GO Battle Weekend: Tales of Transformation</t>
         </is>
       </c>
       <c r="F364" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G364" t="inlineStr"/>
@@ -15449,7 +15449,7 @@
       <c r="O364" t="inlineStr"/>
       <c r="P364" t="inlineStr">
         <is>
-          <t>Genesect Raid Hour Wed, Oct 22, at 6:00 PM Local Time</t>
+          <t>GO Battle Weekend: Tales of Transformation Sat, Oct 25, at 12:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q364" t="inlineStr">
@@ -15469,7 +15469,7 @@
       <c r="D365" t="inlineStr"/>
       <c r="E365" t="inlineStr">
         <is>
-          <t>GO Battle Weekend: Tales of Transformation</t>
+          <t>Halloween 2025 Part II</t>
         </is>
       </c>
       <c r="F365" t="inlineStr">
@@ -15488,7 +15488,7 @@
       <c r="O365" t="inlineStr"/>
       <c r="P365" t="inlineStr">
         <is>
-          <t>Event GO Battle Weekend: Tales of Transformation Sat, Oct 25, at 12:00 AM Local Time Starts: Calculating...</t>
+          <t>Event Halloween 2025 Part II Mon, Oct 27, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q365" t="inlineStr">
@@ -15508,7 +15508,7 @@
       <c r="D366" t="inlineStr"/>
       <c r="E366" t="inlineStr">
         <is>
-          <t>GO Battle Weekend: Tales of Transformation</t>
+          <t>Halloween 2025 Part II</t>
         </is>
       </c>
       <c r="F366" t="inlineStr">
@@ -15527,7 +15527,7 @@
       <c r="O366" t="inlineStr"/>
       <c r="P366" t="inlineStr">
         <is>
-          <t>GO Battle Weekend: Tales of Transformation Sat, Oct 25, at 12:00 AM Local Time Starts: Calculating...</t>
+          <t>Halloween 2025 Part II Mon, Oct 27, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q366" t="inlineStr">
@@ -15547,7 +15547,7 @@
       <c r="D367" t="inlineStr"/>
       <c r="E367" t="inlineStr">
         <is>
-          <t>GO Battle Weekend: Tales of Transformation</t>
+          <t>Halloween 2025 Part II</t>
         </is>
       </c>
       <c r="F367" t="inlineStr">
@@ -15566,7 +15566,7 @@
       <c r="O367" t="inlineStr"/>
       <c r="P367" t="inlineStr">
         <is>
-          <t>GO Battle Weekend: Tales of Transformation Sat, Oct 25, at 12:00 AM Local Time Starts: Calculating...</t>
+          <t>Halloween 2025 Part II Mon, Oct 27, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q367" t="inlineStr">
@@ -15586,7 +15586,7 @@
       <c r="D368" t="inlineStr"/>
       <c r="E368" t="inlineStr">
         <is>
-          <t>GO Battle Weekend: Tales of Transformation</t>
+          <t>Halloween 2025 Part II</t>
         </is>
       </c>
       <c r="F368" t="inlineStr">
@@ -15605,7 +15605,7 @@
       <c r="O368" t="inlineStr"/>
       <c r="P368" t="inlineStr">
         <is>
-          <t>GO Battle Weekend: Tales of Transformation Sat, Oct 25, at 12:00 AM Local Time</t>
+          <t>Halloween 2025 Part II Mon, Oct 27, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q368" t="inlineStr">
@@ -15625,7 +15625,7 @@
       <c r="D369" t="inlineStr"/>
       <c r="E369" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part II</t>
+          <t>Dynamax Woobat during Max Monday</t>
         </is>
       </c>
       <c r="F369" t="inlineStr">
@@ -15644,7 +15644,7 @@
       <c r="O369" t="inlineStr"/>
       <c r="P369" t="inlineStr">
         <is>
-          <t>Event Halloween 2025 Part II Mon, Oct 27, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Max Mondays Dynamax Woobat during Max Monday Mon, Oct 27, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q369" t="inlineStr">
@@ -15664,7 +15664,7 @@
       <c r="D370" t="inlineStr"/>
       <c r="E370" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part II</t>
+          <t>Dynamax Woobat during Max Monday</t>
         </is>
       </c>
       <c r="F370" t="inlineStr">
@@ -15683,7 +15683,7 @@
       <c r="O370" t="inlineStr"/>
       <c r="P370" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part II Mon, Oct 27, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Dynamax Woobat during Max Monday Mon, Oct 27, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q370" t="inlineStr">
@@ -15703,7 +15703,7 @@
       <c r="D371" t="inlineStr"/>
       <c r="E371" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part II</t>
+          <t>Dynamax Woobat during Max Monday</t>
         </is>
       </c>
       <c r="F371" t="inlineStr">
@@ -15722,7 +15722,7 @@
       <c r="O371" t="inlineStr"/>
       <c r="P371" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part II Mon, Oct 27, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Dynamax Woobat during Max Monday Mon, Oct 27, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q371" t="inlineStr">
@@ -15742,7 +15742,7 @@
       <c r="D372" t="inlineStr"/>
       <c r="E372" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part II</t>
+          <t>Dynamax Woobat during Max Monday</t>
         </is>
       </c>
       <c r="F372" t="inlineStr">
@@ -15761,7 +15761,7 @@
       <c r="O372" t="inlineStr"/>
       <c r="P372" t="inlineStr">
         <is>
-          <t>Halloween 2025 Part II Mon, Oct 27, at 10:00 AM Local Time</t>
+          <t>Dynamax Woobat during Max Monday Mon, Oct 27, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q372" t="inlineStr">
@@ -15781,12 +15781,12 @@
       <c r="D373" t="inlineStr"/>
       <c r="E373" t="inlineStr">
         <is>
-          <t>Dynamax Woobat during Max Monday</t>
+          <t>Giratina (Altered Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F373" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G373" t="inlineStr"/>
@@ -15800,7 +15800,7 @@
       <c r="O373" t="inlineStr"/>
       <c r="P373" t="inlineStr">
         <is>
-          <t>Max Mondays Dynamax Woobat during Max Monday Mon, Oct 27, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Raid Battles Giratina (Altered Forme) in 5-star Raid Battles Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q373" t="inlineStr">
@@ -15820,12 +15820,12 @@
       <c r="D374" t="inlineStr"/>
       <c r="E374" t="inlineStr">
         <is>
-          <t>Dynamax Woobat during Max Monday</t>
+          <t>Giratina (Altered Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F374" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G374" t="inlineStr"/>
@@ -15839,7 +15839,7 @@
       <c r="O374" t="inlineStr"/>
       <c r="P374" t="inlineStr">
         <is>
-          <t>Dynamax Woobat during Max Monday Mon, Oct 27, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Giratina (Altered Forme) in 5-star Raid Battles Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q374" t="inlineStr">
@@ -15859,12 +15859,12 @@
       <c r="D375" t="inlineStr"/>
       <c r="E375" t="inlineStr">
         <is>
-          <t>Dynamax Woobat during Max Monday</t>
+          <t>Giratina (Altered Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F375" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G375" t="inlineStr"/>
@@ -15878,7 +15878,7 @@
       <c r="O375" t="inlineStr"/>
       <c r="P375" t="inlineStr">
         <is>
-          <t>Dynamax Woobat during Max Monday Mon, Oct 27, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Giratina (Altered Forme) in 5-star Raid Battles Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q375" t="inlineStr">
@@ -15898,12 +15898,12 @@
       <c r="D376" t="inlineStr"/>
       <c r="E376" t="inlineStr">
         <is>
-          <t>Dynamax Woobat during Max Monday</t>
+          <t>Giratina (Altered Forme) in 5-star Raid Battles</t>
         </is>
       </c>
       <c r="F376" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G376" t="inlineStr"/>
@@ -15917,7 +15917,7 @@
       <c r="O376" t="inlineStr"/>
       <c r="P376" t="inlineStr">
         <is>
-          <t>Dynamax Woobat during Max Monday Mon, Oct 27, at 6:00 PM Local Time</t>
+          <t>Giratina (Altered Forme) in 5-star Raid Battles Tue, Oct 28, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q376" t="inlineStr">
@@ -15937,7 +15937,7 @@
       <c r="D377" t="inlineStr"/>
       <c r="E377" t="inlineStr">
         <is>
-          <t>Giratina (Altered Forme) in 5-star Raid Battles</t>
+          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids</t>
         </is>
       </c>
       <c r="F377" t="inlineStr">
@@ -15956,7 +15956,7 @@
       <c r="O377" t="inlineStr"/>
       <c r="P377" t="inlineStr">
         <is>
-          <t>Raid Battles Giratina (Altered Forme) in 5-star Raid Battles Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Raid Battles Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q377" t="inlineStr">
@@ -15976,7 +15976,7 @@
       <c r="D378" t="inlineStr"/>
       <c r="E378" t="inlineStr">
         <is>
-          <t>Giratina (Altered Forme) in 5-star Raid Battles</t>
+          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids</t>
         </is>
       </c>
       <c r="F378" t="inlineStr">
@@ -15995,7 +15995,7 @@
       <c r="O378" t="inlineStr"/>
       <c r="P378" t="inlineStr">
         <is>
-          <t>Giratina (Altered Forme) in 5-star Raid Battles Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q378" t="inlineStr">
@@ -16015,7 +16015,7 @@
       <c r="D379" t="inlineStr"/>
       <c r="E379" t="inlineStr">
         <is>
-          <t>Giratina (Altered Forme) in 5-star Raid Battles</t>
+          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids</t>
         </is>
       </c>
       <c r="F379" t="inlineStr">
@@ -16034,7 +16034,7 @@
       <c r="O379" t="inlineStr"/>
       <c r="P379" t="inlineStr">
         <is>
-          <t>Giratina (Altered Forme) in 5-star Raid Battles Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q379" t="inlineStr">
@@ -16054,7 +16054,7 @@
       <c r="D380" t="inlineStr"/>
       <c r="E380" t="inlineStr">
         <is>
-          <t>Giratina (Altered Forme) in 5-star Raid Battles</t>
+          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids</t>
         </is>
       </c>
       <c r="F380" t="inlineStr">
@@ -16073,7 +16073,7 @@
       <c r="O380" t="inlineStr"/>
       <c r="P380" t="inlineStr">
         <is>
-          <t>Giratina (Altered Forme) in 5-star Raid Battles Tue, Oct 28, at 10:00 AM Local Time</t>
+          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids Tue, Oct 28, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q380" t="inlineStr">
@@ -16093,12 +16093,12 @@
       <c r="D381" t="inlineStr"/>
       <c r="E381" t="inlineStr">
         <is>
-          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids</t>
+          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F381" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G381" t="inlineStr"/>
@@ -16112,7 +16112,7 @@
       <c r="O381" t="inlineStr"/>
       <c r="P381" t="inlineStr">
         <is>
-          <t>Raid Battles Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>GO Battle League Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q381" t="inlineStr">
@@ -16132,12 +16132,12 @@
       <c r="D382" t="inlineStr"/>
       <c r="E382" t="inlineStr">
         <is>
-          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids</t>
+          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F382" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G382" t="inlineStr"/>
@@ -16151,7 +16151,7 @@
       <c r="O382" t="inlineStr"/>
       <c r="P382" t="inlineStr">
         <is>
-          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q382" t="inlineStr">
@@ -16171,12 +16171,12 @@
       <c r="D383" t="inlineStr"/>
       <c r="E383" t="inlineStr">
         <is>
-          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids</t>
+          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F383" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G383" t="inlineStr"/>
@@ -16190,7 +16190,7 @@
       <c r="O383" t="inlineStr"/>
       <c r="P383" t="inlineStr">
         <is>
-          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids Tue, Oct 28, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q383" t="inlineStr">
@@ -16210,12 +16210,12 @@
       <c r="D384" t="inlineStr"/>
       <c r="E384" t="inlineStr">
         <is>
-          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids</t>
+          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F384" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G384" t="inlineStr"/>
@@ -16229,7 +16229,7 @@
       <c r="O384" t="inlineStr"/>
       <c r="P384" t="inlineStr">
         <is>
-          <t>Mega Gengar, Mega Sableye, and Mega Banette in Mega Raids Tue, Oct 28, at 10:00 AM Local Time</t>
+          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q384" t="inlineStr">
@@ -16249,12 +16249,12 @@
       <c r="D385" t="inlineStr"/>
       <c r="E385" t="inlineStr">
         <is>
-          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation</t>
+          <t>Sinistea Spotlight Hour</t>
         </is>
       </c>
       <c r="F385" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G385" t="inlineStr"/>
@@ -16268,7 +16268,7 @@
       <c r="O385" t="inlineStr"/>
       <c r="P385" t="inlineStr">
         <is>
-          <t>GO Battle League Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Pokémon Spotlight Hour Sinistea Spotlight Hour Tue, Oct 28, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q385" t="inlineStr">
@@ -16288,12 +16288,12 @@
       <c r="D386" t="inlineStr"/>
       <c r="E386" t="inlineStr">
         <is>
-          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation</t>
+          <t>Sinistea Spotlight Hour</t>
         </is>
       </c>
       <c r="F386" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G386" t="inlineStr"/>
@@ -16307,7 +16307,7 @@
       <c r="O386" t="inlineStr"/>
       <c r="P386" t="inlineStr">
         <is>
-          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Sinistea Spotlight Hour Tue, Oct 28, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q386" t="inlineStr">
@@ -16327,12 +16327,12 @@
       <c r="D387" t="inlineStr"/>
       <c r="E387" t="inlineStr">
         <is>
-          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation</t>
+          <t>Sinistea Spotlight Hour</t>
         </is>
       </c>
       <c r="F387" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G387" t="inlineStr"/>
@@ -16346,7 +16346,7 @@
       <c r="O387" t="inlineStr"/>
       <c r="P387" t="inlineStr">
         <is>
-          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Sinistea Spotlight Hour Tue, Oct 28, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q387" t="inlineStr">
@@ -16366,12 +16366,12 @@
       <c r="D388" t="inlineStr"/>
       <c r="E388" t="inlineStr">
         <is>
-          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation</t>
+          <t>Sinistea Spotlight Hour</t>
         </is>
       </c>
       <c r="F388" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="G388" t="inlineStr"/>
@@ -16385,7 +16385,7 @@
       <c r="O388" t="inlineStr"/>
       <c r="P388" t="inlineStr">
         <is>
-          <t>Great League and Halloween Cup: Great League Edition | Tales of Transformation Calculating...</t>
+          <t>Sinistea Spotlight Hour Tue, Oct 28, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q388" t="inlineStr">
@@ -16405,12 +16405,12 @@
       <c r="D389" t="inlineStr"/>
       <c r="E389" t="inlineStr">
         <is>
-          <t>Sinistea Spotlight Hour</t>
+          <t>Giratina (Origin Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F389" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G389" t="inlineStr"/>
@@ -16424,7 +16424,7 @@
       <c r="O389" t="inlineStr"/>
       <c r="P389" t="inlineStr">
         <is>
-          <t>Pokémon Spotlight Hour Sinistea Spotlight Hour Tue, Oct 28, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Raid Hour Giratina (Origin Forme) Raid Hour Wed, Oct 29, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q389" t="inlineStr">
@@ -16444,12 +16444,12 @@
       <c r="D390" t="inlineStr"/>
       <c r="E390" t="inlineStr">
         <is>
-          <t>Sinistea Spotlight Hour</t>
+          <t>Giratina (Origin Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F390" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G390" t="inlineStr"/>
@@ -16463,7 +16463,7 @@
       <c r="O390" t="inlineStr"/>
       <c r="P390" t="inlineStr">
         <is>
-          <t>Sinistea Spotlight Hour Tue, Oct 28, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Giratina (Origin Forme) Raid Hour Wed, Oct 29, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q390" t="inlineStr">
@@ -16483,12 +16483,12 @@
       <c r="D391" t="inlineStr"/>
       <c r="E391" t="inlineStr">
         <is>
-          <t>Sinistea Spotlight Hour</t>
+          <t>Giratina (Origin Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F391" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G391" t="inlineStr"/>
@@ -16502,7 +16502,7 @@
       <c r="O391" t="inlineStr"/>
       <c r="P391" t="inlineStr">
         <is>
-          <t>Sinistea Spotlight Hour Tue, Oct 28, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Giratina (Origin Forme) Raid Hour Wed, Oct 29, at 6:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q391" t="inlineStr">
@@ -16522,12 +16522,12 @@
       <c r="D392" t="inlineStr"/>
       <c r="E392" t="inlineStr">
         <is>
-          <t>Sinistea Spotlight Hour</t>
+          <t>Giratina (Origin Forme) Raid Hour</t>
         </is>
       </c>
       <c r="F392" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G392" t="inlineStr"/>
@@ -16541,7 +16541,7 @@
       <c r="O392" t="inlineStr"/>
       <c r="P392" t="inlineStr">
         <is>
-          <t>Sinistea Spotlight Hour Tue, Oct 28, at 6:00 PM Local Time</t>
+          <t>Giratina (Origin Forme) Raid Hour Wed, Oct 29, at 6:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q392" t="inlineStr">
@@ -16561,12 +16561,12 @@
       <c r="D393" t="inlineStr"/>
       <c r="E393" t="inlineStr">
         <is>
-          <t>Giratina (Origin Forme) Raid Hour</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F393" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G393" t="inlineStr"/>
@@ -16580,7 +16580,7 @@
       <c r="O393" t="inlineStr"/>
       <c r="P393" t="inlineStr">
         <is>
-          <t>Raid Hour Giratina (Origin Forme) Raid Hour Wed, Oct 29, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>GO Battle League Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q393" t="inlineStr">
@@ -16600,12 +16600,12 @@
       <c r="D394" t="inlineStr"/>
       <c r="E394" t="inlineStr">
         <is>
-          <t>Giratina (Origin Forme) Raid Hour</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F394" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G394" t="inlineStr"/>
@@ -16619,7 +16619,7 @@
       <c r="O394" t="inlineStr"/>
       <c r="P394" t="inlineStr">
         <is>
-          <t>Giratina (Origin Forme) Raid Hour Wed, Oct 29, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q394" t="inlineStr">
@@ -16639,12 +16639,12 @@
       <c r="D395" t="inlineStr"/>
       <c r="E395" t="inlineStr">
         <is>
-          <t>Giratina (Origin Forme) Raid Hour</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F395" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G395" t="inlineStr"/>
@@ -16658,7 +16658,7 @@
       <c r="O395" t="inlineStr"/>
       <c r="P395" t="inlineStr">
         <is>
-          <t>Giratina (Origin Forme) Raid Hour Wed, Oct 29, at 6:00 PM Local Time Starts: Calculating...</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q395" t="inlineStr">
@@ -16678,12 +16678,12 @@
       <c r="D396" t="inlineStr"/>
       <c r="E396" t="inlineStr">
         <is>
-          <t>Giratina (Origin Forme) Raid Hour</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F396" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G396" t="inlineStr"/>
@@ -16697,7 +16697,7 @@
       <c r="O396" t="inlineStr"/>
       <c r="P396" t="inlineStr">
         <is>
-          <t>Giratina (Origin Forme) Raid Hour Wed, Oct 29, at 6:00 PM Local Time</t>
+          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q396" t="inlineStr">
@@ -16717,7 +16717,7 @@
       <c r="D397" t="inlineStr"/>
       <c r="E397" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
+          <t>Pokémon GO Wild Area: Nagasaki</t>
         </is>
       </c>
       <c r="F397" t="inlineStr">
@@ -16736,7 +16736,7 @@
       <c r="O397" t="inlineStr"/>
       <c r="P397" t="inlineStr">
         <is>
-          <t>GO Battle League Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Wild Area Pokémon GO Wild Area: Nagasaki Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q397" t="inlineStr">
@@ -16756,7 +16756,7 @@
       <c r="D398" t="inlineStr"/>
       <c r="E398" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
+          <t>Pokémon GO Wild Area: Nagasaki</t>
         </is>
       </c>
       <c r="F398" t="inlineStr">
@@ -16775,7 +16775,7 @@
       <c r="O398" t="inlineStr"/>
       <c r="P398" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Pokémon GO Wild Area: Nagasaki Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q398" t="inlineStr">
@@ -16795,7 +16795,7 @@
       <c r="D399" t="inlineStr"/>
       <c r="E399" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
+          <t>Pokémon GO Wild Area: Nagasaki</t>
         </is>
       </c>
       <c r="F399" t="inlineStr">
@@ -16814,7 +16814,7 @@
       <c r="O399" t="inlineStr"/>
       <c r="P399" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Pokémon GO Wild Area: Nagasaki Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q399" t="inlineStr">
@@ -16834,7 +16834,7 @@
       <c r="D400" t="inlineStr"/>
       <c r="E400" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation</t>
+          <t>Pokémon GO Wild Area: Nagasaki</t>
         </is>
       </c>
       <c r="F400" t="inlineStr">
@@ -16853,7 +16853,7 @@
       <c r="O400" t="inlineStr"/>
       <c r="P400" t="inlineStr">
         <is>
-          <t>Ultra League and Jungle Cup: Great League Edition | Tales of Transformation Calculating...</t>
+          <t>Pokémon GO Wild Area: Nagasaki Calculating...</t>
         </is>
       </c>
       <c r="Q400" t="inlineStr">
@@ -16873,7 +16873,7 @@
       <c r="D401" t="inlineStr"/>
       <c r="E401" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Nagasaki</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F401" t="inlineStr">
@@ -16892,7 +16892,7 @@
       <c r="O401" t="inlineStr"/>
       <c r="P401" t="inlineStr">
         <is>
-          <t>Wild Area Pokémon GO Wild Area: Nagasaki Calculating... Starts: Calculating...</t>
+          <t>GO Battle League Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q401" t="inlineStr">
@@ -16912,7 +16912,7 @@
       <c r="D402" t="inlineStr"/>
       <c r="E402" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Nagasaki</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F402" t="inlineStr">
@@ -16931,7 +16931,7 @@
       <c r="O402" t="inlineStr"/>
       <c r="P402" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Nagasaki Calculating... Starts: Calculating...</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q402" t="inlineStr">
@@ -16951,7 +16951,7 @@
       <c r="D403" t="inlineStr"/>
       <c r="E403" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Nagasaki</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F403" t="inlineStr">
@@ -16970,7 +16970,7 @@
       <c r="O403" t="inlineStr"/>
       <c r="P403" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Nagasaki Calculating... Starts: Calculating...</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q403" t="inlineStr">
@@ -16990,7 +16990,7 @@
       <c r="D404" t="inlineStr"/>
       <c r="E404" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Nagasaki</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F404" t="inlineStr">
@@ -17009,7 +17009,7 @@
       <c r="O404" t="inlineStr"/>
       <c r="P404" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Nagasaki Calculating...</t>
+          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q404" t="inlineStr">
@@ -17029,7 +17029,7 @@
       <c r="D405" t="inlineStr"/>
       <c r="E405" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Pokémon GO Wild Area: Global</t>
         </is>
       </c>
       <c r="F405" t="inlineStr">
@@ -17048,7 +17048,7 @@
       <c r="O405" t="inlineStr"/>
       <c r="P405" t="inlineStr">
         <is>
-          <t>GO Battle League Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Wild Area Pokémon GO Wild Area: Global Sat, Nov 15, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q405" t="inlineStr">
@@ -17068,7 +17068,7 @@
       <c r="D406" t="inlineStr"/>
       <c r="E406" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Pokémon GO Wild Area: Global</t>
         </is>
       </c>
       <c r="F406" t="inlineStr">
@@ -17087,7 +17087,7 @@
       <c r="O406" t="inlineStr"/>
       <c r="P406" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Pokémon GO Wild Area: Global Sat, Nov 15, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q406" t="inlineStr">
@@ -17107,7 +17107,7 @@
       <c r="D407" t="inlineStr"/>
       <c r="E407" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Pokémon GO Wild Area: Global</t>
         </is>
       </c>
       <c r="F407" t="inlineStr">
@@ -17126,7 +17126,7 @@
       <c r="O407" t="inlineStr"/>
       <c r="P407" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Pokémon GO Wild Area: Global Sat, Nov 15, at 10:00 AM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q407" t="inlineStr">
@@ -17146,7 +17146,7 @@
       <c r="D408" t="inlineStr"/>
       <c r="E408" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation</t>
+          <t>Pokémon GO Wild Area: Global</t>
         </is>
       </c>
       <c r="F408" t="inlineStr">
@@ -17165,7 +17165,7 @@
       <c r="O408" t="inlineStr"/>
       <c r="P408" t="inlineStr">
         <is>
-          <t>Great League, Ultra League, and Master League | Tales of Transformation Calculating...</t>
+          <t>Pokémon GO Wild Area: Global Sat, Nov 15, at 10:00 AM Local Time</t>
         </is>
       </c>
       <c r="Q408" t="inlineStr">
@@ -17185,12 +17185,12 @@
       <c r="D409" t="inlineStr"/>
       <c r="E409" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Global</t>
+          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F409" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G409" t="inlineStr"/>
@@ -17204,7 +17204,7 @@
       <c r="O409" t="inlineStr"/>
       <c r="P409" t="inlineStr">
         <is>
-          <t>Wild Area Pokémon GO Wild Area: Global Sat, Nov 15, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>GO Battle League 2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q409" t="inlineStr">
@@ -17224,12 +17224,12 @@
       <c r="D410" t="inlineStr"/>
       <c r="E410" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Global</t>
+          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F410" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G410" t="inlineStr"/>
@@ -17243,7 +17243,7 @@
       <c r="O410" t="inlineStr"/>
       <c r="P410" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Global Sat, Nov 15, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q410" t="inlineStr">
@@ -17263,12 +17263,12 @@
       <c r="D411" t="inlineStr"/>
       <c r="E411" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Global</t>
+          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F411" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G411" t="inlineStr"/>
@@ -17282,7 +17282,7 @@
       <c r="O411" t="inlineStr"/>
       <c r="P411" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Global Sat, Nov 15, at 10:00 AM Local Time Starts: Calculating...</t>
+          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q411" t="inlineStr">
@@ -17302,12 +17302,12 @@
       <c r="D412" t="inlineStr"/>
       <c r="E412" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Global</t>
+          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation</t>
         </is>
       </c>
       <c r="F412" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G412" t="inlineStr"/>
@@ -17321,7 +17321,7 @@
       <c r="O412" t="inlineStr"/>
       <c r="P412" t="inlineStr">
         <is>
-          <t>Pokémon GO Wild Area: Global Sat, Nov 15, at 10:00 AM Local Time</t>
+          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q412" t="inlineStr">
@@ -17341,12 +17341,12 @@
       <c r="D413" t="inlineStr"/>
       <c r="E413" t="inlineStr">
         <is>
-          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation</t>
+          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F413" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G413" t="inlineStr"/>
@@ -17360,7 +17360,7 @@
       <c r="O413" t="inlineStr"/>
       <c r="P413" t="inlineStr">
         <is>
-          <t>GO Battle League 2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>GO Battle League Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q413" t="inlineStr">
@@ -17380,12 +17380,12 @@
       <c r="D414" t="inlineStr"/>
       <c r="E414" t="inlineStr">
         <is>
-          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation</t>
+          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F414" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G414" t="inlineStr"/>
@@ -17399,7 +17399,7 @@
       <c r="O414" t="inlineStr"/>
       <c r="P414" t="inlineStr">
         <is>
-          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q414" t="inlineStr">
@@ -17419,12 +17419,12 @@
       <c r="D415" t="inlineStr"/>
       <c r="E415" t="inlineStr">
         <is>
-          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation</t>
+          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F415" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G415" t="inlineStr"/>
@@ -17438,7 +17438,7 @@
       <c r="O415" t="inlineStr"/>
       <c r="P415" t="inlineStr">
         <is>
-          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q415" t="inlineStr">
@@ -17458,12 +17458,12 @@
       <c r="D416" t="inlineStr"/>
       <c r="E416" t="inlineStr">
         <is>
-          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation</t>
+          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation</t>
         </is>
       </c>
       <c r="F416" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G416" t="inlineStr"/>
@@ -17477,7 +17477,7 @@
       <c r="O416" t="inlineStr"/>
       <c r="P416" t="inlineStr">
         <is>
-          <t>2025 Championship Series Cup and Master League: Mega Edition | Tales of Transformation Calculating...</t>
+          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating...</t>
         </is>
       </c>
       <c r="Q416" t="inlineStr">
@@ -17497,12 +17497,12 @@
       <c r="D417" t="inlineStr"/>
       <c r="E417" t="inlineStr">
         <is>
-          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation</t>
+          <t>November Community Day</t>
         </is>
       </c>
       <c r="F417" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Community Day</t>
         </is>
       </c>
       <c r="G417" t="inlineStr"/>
@@ -17516,7 +17516,7 @@
       <c r="O417" t="inlineStr"/>
       <c r="P417" t="inlineStr">
         <is>
-          <t>GO Battle League Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>Community Day November Community Day Sun, Nov 30, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q417" t="inlineStr">
@@ -17536,12 +17536,12 @@
       <c r="D418" t="inlineStr"/>
       <c r="E418" t="inlineStr">
         <is>
-          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation</t>
+          <t>November Community Day</t>
         </is>
       </c>
       <c r="F418" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Community Day</t>
         </is>
       </c>
       <c r="G418" t="inlineStr"/>
@@ -17555,7 +17555,7 @@
       <c r="O418" t="inlineStr"/>
       <c r="P418" t="inlineStr">
         <is>
-          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>November Community Day Sun, Nov 30, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q418" t="inlineStr">
@@ -17575,12 +17575,12 @@
       <c r="D419" t="inlineStr"/>
       <c r="E419" t="inlineStr">
         <is>
-          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation</t>
+          <t>November Community Day</t>
         </is>
       </c>
       <c r="F419" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Community Day</t>
         </is>
       </c>
       <c r="G419" t="inlineStr"/>
@@ -17594,7 +17594,7 @@
       <c r="O419" t="inlineStr"/>
       <c r="P419" t="inlineStr">
         <is>
-          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating... Starts: Calculating...</t>
+          <t>November Community Day Sun, Nov 30, at 2:00 PM Local Time Starts: Calculating...</t>
         </is>
       </c>
       <c r="Q419" t="inlineStr">
@@ -17614,12 +17614,12 @@
       <c r="D420" t="inlineStr"/>
       <c r="E420" t="inlineStr">
         <is>
-          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation</t>
+          <t>November Community Day</t>
         </is>
       </c>
       <c r="F420" t="inlineStr">
         <is>
-          <t>Event/News</t>
+          <t>Community Day</t>
         </is>
       </c>
       <c r="G420" t="inlineStr"/>
@@ -17633,7 +17633,7 @@
       <c r="O420" t="inlineStr"/>
       <c r="P420" t="inlineStr">
         <is>
-          <t>Catch Cup: Tales of Transformation: Great Edition, Ultra League, and Master League | Tales of Transformation Calculating...</t>
+          <t>November Community Day Sun, Nov 30, at 2:00 PM Local Time</t>
         </is>
       </c>
       <c r="Q420" t="inlineStr">
@@ -17653,12 +17653,12 @@
       <c r="D421" t="inlineStr"/>
       <c r="E421" t="inlineStr">
         <is>
-          <t>November Community Day</t>
+          <t>Raid NOW</t>
         </is>
       </c>
       <c r="F421" t="inlineStr">
         <is>
-          <t>Community Day</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G421" t="inlineStr"/>
@@ -17672,12 +17672,12 @@
       <c r="O421" t="inlineStr"/>
       <c r="P421" t="inlineStr">
         <is>
-          <t>Community Day November Community Day Sun, Nov 30, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Raid NOW From Leek Duck | Powered by GO FRIEND General Information It has been reported that the registration information (Trainer Name, Trainer Level, Trainer Code) is incorrect. Please check again. HOST HOST Auto join Raids you are joining (Latest 2) MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rpl_maxuser'] }} {{ val1['cnt'] }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} No.{{ val1['rpl_id'] }} No.{{ val1['rpl_id'] }} TL{{ val1['rpl_level'] }} {{ val1['rpl_glevel'] }} {{ ((val1['rpl_gescore'] == -1)?0:val1['rpl_gescore']) }} {{ aryPokemon[value]['raidbbs_short_name_en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} FULL Host TL 5 30 35 40 45 Host Rating - 0 {{ i }} MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['ti</t>
         </is>
       </c>
       <c r="Q421" t="inlineStr">
         <is>
-          <t>2024-06-01_events.html</t>
+          <t>2024-06-01_raid-now.html</t>
         </is>
       </c>
     </row>
@@ -17692,12 +17692,12 @@
       <c r="D422" t="inlineStr"/>
       <c r="E422" t="inlineStr">
         <is>
-          <t>November Community Day</t>
+          <t>Raids you are joining (Latest 2)</t>
         </is>
       </c>
       <c r="F422" t="inlineStr">
         <is>
-          <t>Community Day</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G422" t="inlineStr"/>
@@ -17711,12 +17711,12 @@
       <c r="O422" t="inlineStr"/>
       <c r="P422" t="inlineStr">
         <is>
-          <t>November Community Day Sun, Nov 30, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>General Information It has been reported that the registration information (Trainer Name, Trainer Level, Trainer Code) is incorrect. Please check again. HOST HOST Auto join Raids you are joining (Latest 2) MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rpl_maxuser'] }} {{ val1['cnt'] }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} No.{{ val1['rpl_id'] }} No.{{ val1['rpl_id'] }} TL{{ val1['rpl_level'] }} {{ val1['rpl_glevel'] }} {{ ((val1['rpl_gescore'] == -1)?0:val1['rpl_gescore']) }} {{ aryPokemon[value]['raidbbs_short_name_en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} FULL Host TL 5 30 35 40 45 Host Rating - 0 {{ i }} MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rp</t>
         </is>
       </c>
       <c r="Q422" t="inlineStr">
         <is>
-          <t>2024-06-01_events.html</t>
+          <t>2024-06-01_raid-now.html</t>
         </is>
       </c>
     </row>
@@ -17731,12 +17731,12 @@
       <c r="D423" t="inlineStr"/>
       <c r="E423" t="inlineStr">
         <is>
-          <t>November Community Day</t>
+          <t>Raids you are joining (Latest 2)</t>
         </is>
       </c>
       <c r="F423" t="inlineStr">
         <is>
-          <t>Community Day</t>
+          <t>Raid/Mega</t>
         </is>
       </c>
       <c r="G423" t="inlineStr"/>
@@ -17750,12 +17750,12 @@
       <c r="O423" t="inlineStr"/>
       <c r="P423" t="inlineStr">
         <is>
-          <t>November Community Day Sun, Nov 30, at 2:00 PM Local Time Starts: Calculating...</t>
+          <t>Raids you are joining (Latest 2) MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rpl_maxuser'] }} {{ val1['cnt'] }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} No.{{ val1['rpl_id'] }} No.{{ val1['rpl_id'] }} TL{{ val1['rpl_level'] }} {{ val1['rpl_glevel'] }} {{ ((val1['rpl_gescore'] == -1)?0:val1['rpl_gescore']) }}</t>
         </is>
       </c>
       <c r="Q423" t="inlineStr">
         <is>
-          <t>2024-06-01_events.html</t>
+          <t>2024-06-01_raid-now.html</t>
         </is>
       </c>
     </row>
@@ -17770,12 +17770,12 @@
       <c r="D424" t="inlineStr"/>
       <c r="E424" t="inlineStr">
         <is>
-          <t>November Community Day</t>
+          <t>まとめて評価</t>
         </is>
       </c>
       <c r="F424" t="inlineStr">
         <is>
-          <t>Community Day</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G424" t="inlineStr"/>
@@ -17789,12 +17789,12 @@
       <c r="O424" t="inlineStr"/>
       <c r="P424" t="inlineStr">
         <is>
-          <t>November Community Day Sun, Nov 30, at 2:00 PM Local Time</t>
+          <t>まとめて評価 Can't rate</t>
         </is>
       </c>
       <c r="Q424" t="inlineStr">
         <is>
-          <t>2024-06-01_events.html</t>
+          <t>2024-06-01_raid-now.html</t>
         </is>
       </c>
     </row>
@@ -17809,12 +17809,12 @@
       <c r="D425" t="inlineStr"/>
       <c r="E425" t="inlineStr">
         <is>
-          <t>Raid NOW</t>
+          <t>Bonuses</t>
         </is>
       </c>
       <c r="F425" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G425" t="inlineStr"/>
@@ -17828,12 +17828,12 @@
       <c r="O425" t="inlineStr"/>
       <c r="P425" t="inlineStr">
         <is>
-          <t>Raid NOW From Leek Duck | Powered by GO FRIEND General Information It has been reported that the registration information (Trainer Name, Trainer Level, Trainer Code) is incorrect. Please check again. HOST HOST Auto join Raids you are joining (Latest 2) MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rpl_maxuser'] }} {{ val1['cnt'] }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} No.{{ val1['rpl_id'] }} No.{{ val1['rpl_id'] }} TL{{ val1['rpl_level'] }} {{ val1['rpl_glevel'] }} {{ ((val1['rpl_gescore'] == -1)?0:val1['rpl_gescore']) }} {{ aryPokemon[value]['raidbbs_short_name_en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} FULL Host TL 5 30 35 40 45 Host Rating - 0 {{ i }} MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['ti</t>
+          <t>Bonuses 4× Stardust from win rewards. (This does not include end-of-set rewards.) The maximum number of sets you can play per day will increase from five to 20—for a total of 100 battles—from 12:00 a.m. to 11:59 p.m. local time. Free battle-themed Timed Research will be available. Rewards include glasses for your avatar inspired by Clemont. Pokémon encountered via GO Battle League rewards will have a wider variance of Attack, Defense, and HP. Active Leagues The following leagues will be active. Great League Ultra League Master League</t>
         </is>
       </c>
       <c r="Q425" t="inlineStr">
         <is>
-          <t>2024-06-01_raid-now.html</t>
+          <t>2024-06-01_event-go-battle-weekend-tales-of-transformation-sun-oct-26-at-1159-pm-local-time-ends-calculating.html</t>
         </is>
       </c>
     </row>
@@ -17848,12 +17848,12 @@
       <c r="D426" t="inlineStr"/>
       <c r="E426" t="inlineStr">
         <is>
-          <t>Raids you are joining (Latest 2)</t>
+          <t>For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area?</t>
         </is>
       </c>
       <c r="F426" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G426" t="inlineStr"/>
@@ -17867,12 +17867,12 @@
       <c r="O426" t="inlineStr"/>
       <c r="P426" t="inlineStr">
         <is>
-          <t>General Information It has been reported that the registration information (Trainer Name, Trainer Level, Trainer Code) is incorrect. Please check again. HOST HOST Auto join Raids you are joining (Latest 2) MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rpl_maxuser'] }} {{ val1['cnt'] }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} No.{{ val1['rpl_id'] }} No.{{ val1['rpl_id'] }} TL{{ val1['rpl_level'] }} {{ val1['rpl_glevel'] }} {{ ((val1['rpl_gescore'] == -1)?0:val1['rpl_gescore']) }} {{ aryPokemon[value]['raidbbs_short_name_en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} {{ aryPokemon[value]['en'] }} FULL Host TL 5 30 35 40 45 Host Rating - 0 {{ i }} MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rp</t>
+          <t xml:space="preserve">For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area? In this next chapter of Pokémon GO Wild Area, get ready to test your skills once again as you encounter Dark- and Fairy-type Pokémon, including Grimmsnarl, the Bulk Up Pokémon! Plus, exceptionally powerful Pokémon known as mighty Pokémon are appearing in the wild—use GO Wild Area–exclusive GO Safari Balls to improve your odds of catching these rare Pokémon. All event gameplay is exclusive to ticket holders. Tickets for Pokémon GO Wild Area: Nagasaki are now available on the Niantic events portal . Live Event Ticket - ¥3,600 (including applicable taxes and fees) Location: A citywide experience across Nagasaki City, Japan Dates: November 7, 8, or 9, 2025 Time: 9:00 a.m. – 5:00 p.m. JST Tickets for Pokémon GO Wild Area: Nagasaki include one day of event gameplay, and attendees may purchase add-ons that extend the gameplay for an additional day. One-day tickets are ¥3,600 (or the equivalent pricing tier in your local currency, including applicable taxes and fees). Event gameplay will be available only at the date, time, and location specified on your ticket. Note: Tickets to this event are </t>
         </is>
       </c>
       <c r="Q426" t="inlineStr">
         <is>
-          <t>2024-06-01_raid-now.html</t>
+          <t>2024-06-01_wild-area-pokmon-go-wild-area-nagasaki-calculating-ends-calculating.html</t>
         </is>
       </c>
     </row>
@@ -17887,12 +17887,12 @@
       <c r="D427" t="inlineStr"/>
       <c r="E427" t="inlineStr">
         <is>
-          <t>Raids you are joining (Latest 2)</t>
+          <t>For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area?</t>
         </is>
       </c>
       <c r="F427" t="inlineStr">
         <is>
-          <t>Raid/Mega</t>
+          <t>Event/News</t>
         </is>
       </c>
       <c r="G427" t="inlineStr"/>
@@ -17906,166 +17906,10 @@
       <c r="O427" t="inlineStr"/>
       <c r="P427" t="inlineStr">
         <is>
-          <t>Raids you are joining (Latest 2) MY POST JOINED {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp20'] }} {{ aryPokemon[aryRaidList[key1]['rpl_pokemon']]['maxcp25'] }} {{ val1['time'] }} Expired {{ val1['cnt'] }} / {{ val1['rpl_maxuser'] }} {{ val1['cnt'] }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} {{ (val1['rpl_pokemon'] ? aryPokemon[val1['rpl_pokemon']]['en'] : 'unknown') }} No.{{ val1['rpl_id'] }} No.{{ val1['rpl_id'] }} TL{{ val1['rpl_level'] }} {{ val1['rpl_glevel'] }} {{ ((val1['rpl_gescore'] == -1)?0:val1['rpl_gescore']) }}</t>
+          <t>For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area? Trainers around the world can gear up for a worldwide adventure during Pokémon GO Wild Area: Global, available in-game for two days only! Looking to enhance your GO Wild Area weekend with exclusive Special Research, additional bonuses, and an increased chance of encountering Shiny Pokémon? Purchase a global event ticket from the Pokémon GO Web Store! Event Tickets Tickets for Pokémon GO Wild Area: Global are available now in the in-game Shop and Pokémon Go Web Store for $11.99 USD . Purchase your ticket on the Pokémon GO Web Store for a new avatar item! Trainers who purchase their Pokémon GO Wild Area: Global ticket on the Pokémon GO Web Store will receive a special avatar item—the Flower Crown! You can purchase your ticket on the web store until the last day of the event to receive this avatar item. Pokémon GO Wild Area: Nagasaki For details on the in-person event in Nagasaki, Japan, click here .</t>
         </is>
       </c>
       <c r="Q427" t="inlineStr">
-        <is>
-          <t>2024-06-01_raid-now.html</t>
-        </is>
-      </c>
-    </row>
-    <row r="428">
-      <c r="A428" t="inlineStr">
-        <is>
-          <t>Leek Duck</t>
-        </is>
-      </c>
-      <c r="B428" t="inlineStr"/>
-      <c r="C428" t="inlineStr"/>
-      <c r="D428" t="inlineStr"/>
-      <c r="E428" t="inlineStr">
-        <is>
-          <t>まとめて評価</t>
-        </is>
-      </c>
-      <c r="F428" t="inlineStr">
-        <is>
-          <t>Event/News</t>
-        </is>
-      </c>
-      <c r="G428" t="inlineStr"/>
-      <c r="H428" t="inlineStr"/>
-      <c r="I428" t="inlineStr"/>
-      <c r="J428" t="inlineStr"/>
-      <c r="K428" t="inlineStr"/>
-      <c r="L428" t="inlineStr"/>
-      <c r="M428" t="inlineStr"/>
-      <c r="N428" t="inlineStr"/>
-      <c r="O428" t="inlineStr"/>
-      <c r="P428" t="inlineStr">
-        <is>
-          <t>まとめて評価 Can't rate</t>
-        </is>
-      </c>
-      <c r="Q428" t="inlineStr">
-        <is>
-          <t>2024-06-01_raid-now.html</t>
-        </is>
-      </c>
-    </row>
-    <row r="429">
-      <c r="A429" t="inlineStr">
-        <is>
-          <t>Leek Duck</t>
-        </is>
-      </c>
-      <c r="B429" t="inlineStr"/>
-      <c r="C429" t="inlineStr"/>
-      <c r="D429" t="inlineStr"/>
-      <c r="E429" t="inlineStr">
-        <is>
-          <t>Bonuses</t>
-        </is>
-      </c>
-      <c r="F429" t="inlineStr">
-        <is>
-          <t>Event/News</t>
-        </is>
-      </c>
-      <c r="G429" t="inlineStr"/>
-      <c r="H429" t="inlineStr"/>
-      <c r="I429" t="inlineStr"/>
-      <c r="J429" t="inlineStr"/>
-      <c r="K429" t="inlineStr"/>
-      <c r="L429" t="inlineStr"/>
-      <c r="M429" t="inlineStr"/>
-      <c r="N429" t="inlineStr"/>
-      <c r="O429" t="inlineStr"/>
-      <c r="P429" t="inlineStr">
-        <is>
-          <t>Bonuses 4× Stardust from win rewards. (This does not include end-of-set rewards.) The maximum number of sets you can play per day will increase from five to 20—for a total of 100 battles—from 12:00 a.m. to 11:59 p.m. local time. Free battle-themed Timed Research will be available. Rewards include glasses for your avatar inspired by Clemont. Pokémon encountered via GO Battle League rewards will have a wider variance of Attack, Defense, and HP. Active Leagues The following leagues will be active. Great League Ultra League Master League</t>
-        </is>
-      </c>
-      <c r="Q429" t="inlineStr">
-        <is>
-          <t>2024-06-01_event-go-battle-weekend-tales-of-transformation-sun-oct-26-at-1159-pm-local-time-ends-calculating.html</t>
-        </is>
-      </c>
-    </row>
-    <row r="430">
-      <c r="A430" t="inlineStr">
-        <is>
-          <t>Leek Duck</t>
-        </is>
-      </c>
-      <c r="B430" t="inlineStr"/>
-      <c r="C430" t="inlineStr"/>
-      <c r="D430" t="inlineStr"/>
-      <c r="E430" t="inlineStr">
-        <is>
-          <t>For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area?</t>
-        </is>
-      </c>
-      <c r="F430" t="inlineStr">
-        <is>
-          <t>Event/News</t>
-        </is>
-      </c>
-      <c r="G430" t="inlineStr"/>
-      <c r="H430" t="inlineStr"/>
-      <c r="I430" t="inlineStr"/>
-      <c r="J430" t="inlineStr"/>
-      <c r="K430" t="inlineStr"/>
-      <c r="L430" t="inlineStr"/>
-      <c r="M430" t="inlineStr"/>
-      <c r="N430" t="inlineStr"/>
-      <c r="O430" t="inlineStr"/>
-      <c r="P430" t="inlineStr">
-        <is>
-          <t xml:space="preserve">For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area? In this next chapter of Pokémon GO Wild Area, get ready to test your skills once again as you encounter Dark- and Fairy-type Pokémon, including Grimmsnarl, the Bulk Up Pokémon! Plus, exceptionally powerful Pokémon known as mighty Pokémon are appearing in the wild—use GO Wild Area–exclusive GO Safari Balls to improve your odds of catching these rare Pokémon. All event gameplay is exclusive to ticket holders. Tickets for Pokémon GO Wild Area: Nagasaki are now available on the Niantic events portal . Live Event Ticket - ¥3,600 (including applicable taxes and fees) Location: A citywide experience across Nagasaki City, Japan Dates: November 7, 8, or 9, 2025 Time: 9:00 a.m. – 5:00 p.m. JST Tickets for Pokémon GO Wild Area: Nagasaki include one day of event gameplay, and attendees may purchase add-ons that extend the gameplay for an additional day. One-day tickets are ¥3,600 (or the equivalent pricing tier in your local currency, including applicable taxes and fees). Event gameplay will be available only at the date, time, and location specified on your ticket. Note: Tickets to this event are </t>
-        </is>
-      </c>
-      <c r="Q430" t="inlineStr">
-        <is>
-          <t>2024-06-01_wild-area-pokmon-go-wild-area-nagasaki-calculating-ends-calculating.html</t>
-        </is>
-      </c>
-    </row>
-    <row r="431">
-      <c r="A431" t="inlineStr">
-        <is>
-          <t>Leek Duck</t>
-        </is>
-      </c>
-      <c r="B431" t="inlineStr"/>
-      <c r="C431" t="inlineStr"/>
-      <c r="D431" t="inlineStr"/>
-      <c r="E431" t="inlineStr">
-        <is>
-          <t>For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area?</t>
-        </is>
-      </c>
-      <c r="F431" t="inlineStr">
-        <is>
-          <t>Event/News</t>
-        </is>
-      </c>
-      <c r="G431" t="inlineStr"/>
-      <c r="H431" t="inlineStr"/>
-      <c r="I431" t="inlineStr"/>
-      <c r="J431" t="inlineStr"/>
-      <c r="K431" t="inlineStr"/>
-      <c r="L431" t="inlineStr"/>
-      <c r="M431" t="inlineStr"/>
-      <c r="N431" t="inlineStr"/>
-      <c r="O431" t="inlineStr"/>
-      <c r="P431" t="inlineStr">
-        <is>
-          <t>For the brave, adventure awaits around every corner—are you ready to venture into the Wild Area? Trainers around the world can gear up for a worldwide adventure during Pokémon GO Wild Area: Global, available in-game for two days only! Looking to enhance your GO Wild Area weekend with exclusive Special Research, additional bonuses, and an increased chance of encountering Shiny Pokémon? Purchase a global event ticket from the Pokémon GO Web Store! Event Tickets Tickets for Pokémon GO Wild Area: Global are available now in the in-game Shop and Pokémon Go Web Store for $11.99 USD . Purchase your ticket on the Pokémon GO Web Store for a new avatar item! Trainers who purchase their Pokémon GO Wild Area: Global ticket on the Pokémon GO Web Store will receive a special avatar item—the Flower Crown! You can purchase your ticket on the web store until the last day of the event to receive this avatar item. Pokémon GO Wild Area: Nagasaki For details on the in-person event in Nagasaki, Japan, click here .</t>
-        </is>
-      </c>
-      <c r="Q431" t="inlineStr">
         <is>
           <t>2024-06-01_wild-area-pokmon-go-wild-area-global-sun-nov-16-at-600-pm-local-time-ends-calculating.html</t>
         </is>

</xml_diff>